<commit_message>
Bump to 22.11.1.1 Consistent manual/test files through le_prompt
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -5,12 +5,12 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\DocSource\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA1A0EBF-7592-4536-89B4-857F85E0219B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E9E98BAA-635D-47C8-BFC5-2B62C7705890}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44460" yWindow="720" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44805" yWindow="1065" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -24,7 +24,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="613" uniqueCount="352">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="631" uniqueCount="353">
   <si>
     <t>Statement</t>
   </si>
@@ -131,24 +131,6 @@
     <t>le_prompt(message)</t>
   </si>
   <si>
-    <t>end()</t>
-  </si>
-  <si>
-    <t>end</t>
-  </si>
-  <si>
-    <t>pause()</t>
-  </si>
-  <si>
-    <t>pause</t>
-  </si>
-  <si>
-    <t>sleep(seconds)</t>
-  </si>
-  <si>
-    <t>random(n, low, high)</t>
-  </si>
-  <si>
     <t>jump(string label)</t>
   </si>
   <si>
@@ -167,19 +149,10 @@
     <t>ret()</t>
   </si>
   <si>
-    <t>ret</t>
-  </si>
-  <si>
     <t>Input File Support</t>
   </si>
   <si>
-    <t>infile_open(filename)</t>
-  </si>
-  <si>
     <t>infile_close()</t>
-  </si>
-  <si>
-    <t>infile_scale()</t>
   </si>
   <si>
     <t>infile_readline()</t>
@@ -1085,6 +1058,36 @@
   </si>
   <si>
     <t>random</t>
+  </si>
+  <si>
+    <t>sleep(double seconds)</t>
+  </si>
+  <si>
+    <t>random(int N, double low, double high)</t>
+  </si>
+  <si>
+    <t>le_pause()</t>
+  </si>
+  <si>
+    <t>le_stop()</t>
+  </si>
+  <si>
+    <t>infile_open(string filename)</t>
+  </si>
+  <si>
+    <t>infile_scale(pairs)</t>
+  </si>
+  <si>
+    <t>TEST</t>
+  </si>
+  <si>
+    <t>le_pause</t>
+  </si>
+  <si>
+    <t>le_stop</t>
+  </si>
+  <si>
+    <t>le_prompt</t>
   </si>
 </sst>
 </file>
@@ -1512,11 +1515,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AF1008"/>
+  <dimension ref="A1:AF1004"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
+      <pane ySplit="2" topLeftCell="A37" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F45" sqref="F45"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1550,7 +1553,7 @@
       <c r="G1" s="30"/>
       <c r="H1" s="30"/>
       <c r="I1" s="31" t="s">
-        <v>319</v>
+        <v>310</v>
       </c>
       <c r="J1" s="31"/>
       <c r="K1" s="30" t="s">
@@ -1581,10 +1584,10 @@
         <v>10</v>
       </c>
       <c r="I2" s="22" t="s">
-        <v>339</v>
+        <v>330</v>
       </c>
       <c r="J2" s="25" t="s">
-        <v>335</v>
+        <v>326</v>
       </c>
       <c r="K2" s="30"/>
     </row>
@@ -1613,7 +1616,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="J4" s="15"/>
     </row>
@@ -1634,7 +1637,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="J5" s="15"/>
     </row>
@@ -1655,13 +1658,13 @@
         <v>11</v>
       </c>
       <c r="I6" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="J6" s="15"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>326</v>
+        <v>317</v>
       </c>
       <c r="B7" s="4" t="s">
         <v>11</v>
@@ -1676,7 +1679,7 @@
         <v>11</v>
       </c>
       <c r="I7" s="15" t="s">
-        <v>320</v>
+        <v>311</v>
       </c>
       <c r="J7" s="15"/>
     </row>
@@ -1697,10 +1700,10 @@
         <v>11</v>
       </c>
       <c r="I8" s="26" t="s">
-        <v>323</v>
+        <v>314</v>
       </c>
       <c r="J8" s="27" t="s">
-        <v>322</v>
+        <v>313</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
@@ -1720,10 +1723,10 @@
         <v>11</v>
       </c>
       <c r="I9" s="26" t="s">
-        <v>324</v>
+        <v>315</v>
       </c>
       <c r="J9" s="27" t="s">
-        <v>325</v>
+        <v>316</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1731,25 +1734,25 @@
         <v>17</v>
       </c>
       <c r="B10" s="3" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="C10" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="D10" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="E10" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="I10" s="4" t="s">
-        <v>321</v>
+        <v>312</v>
       </c>
       <c r="J10" s="4"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>350</v>
+        <v>341</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -1771,7 +1774,7 @@
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>330</v>
+        <v>321</v>
       </c>
       <c r="B14" s="3" t="s">
         <v>11</v>
@@ -1782,12 +1785,12 @@
         <v>11</v>
       </c>
       <c r="I14" s="15" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="15" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>331</v>
+        <v>322</v>
       </c>
       <c r="B15" s="3" t="s">
         <v>11</v>
@@ -1798,15 +1801,15 @@
         <v>11</v>
       </c>
       <c r="I15" s="15" t="s">
-        <v>334</v>
+        <v>325</v>
       </c>
       <c r="J15" s="15" t="s">
-        <v>336</v>
+        <v>327</v>
       </c>
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>332</v>
+        <v>323</v>
       </c>
       <c r="B16" s="3" t="s">
         <v>11</v>
@@ -1817,7 +1820,7 @@
         <v>11</v>
       </c>
       <c r="I16" s="15" t="s">
-        <v>333</v>
+        <v>324</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1837,7 +1840,7 @@
         <v>11</v>
       </c>
       <c r="I17" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1857,7 +1860,7 @@
         <v>11</v>
       </c>
       <c r="I18" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1877,7 +1880,7 @@
         <v>11</v>
       </c>
       <c r="I19" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1897,12 +1900,12 @@
         <v>11</v>
       </c>
       <c r="I20" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="21" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>40</v>
+        <v>344</v>
       </c>
       <c r="B21" s="4" t="s">
         <v>11</v>
@@ -1913,12 +1916,12 @@
         <v>11</v>
       </c>
       <c r="I21" s="26" t="s">
-        <v>351</v>
+        <v>342</v>
       </c>
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>327</v>
+        <v>318</v>
       </c>
       <c r="B22" s="4"/>
       <c r="C22" s="4" t="s">
@@ -1931,12 +1934,12 @@
         <v>11</v>
       </c>
       <c r="I22" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>328</v>
+        <v>319</v>
       </c>
       <c r="B23" s="4"/>
       <c r="C23" s="4" t="s">
@@ -1949,12 +1952,12 @@
         <v>11</v>
       </c>
       <c r="I23" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>329</v>
+        <v>320</v>
       </c>
       <c r="B24" s="4"/>
       <c r="C24" s="4" t="s">
@@ -1967,7 +1970,7 @@
         <v>11</v>
       </c>
       <c r="I24" s="26" t="s">
-        <v>341</v>
+        <v>332</v>
       </c>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1978,7 +1981,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A26" s="17" t="s">
-        <v>349</v>
+        <v>340</v>
       </c>
       <c r="B26" s="3"/>
       <c r="C26" s="4"/>
@@ -1986,7 +1989,7 @@
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A27" s="15" t="s">
-        <v>344</v>
+        <v>335</v>
       </c>
       <c r="B27" s="3" t="s">
         <v>11</v>
@@ -2001,12 +2004,12 @@
         <v>11</v>
       </c>
       <c r="I27" s="15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>342</v>
+        <v>333</v>
       </c>
       <c r="B28" s="3" t="s">
         <v>11</v>
@@ -2021,7 +2024,7 @@
         <v>11</v>
       </c>
       <c r="I28" s="15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2041,7 +2044,7 @@
         <v>11</v>
       </c>
       <c r="I29" s="15" t="s">
-        <v>346</v>
+        <v>337</v>
       </c>
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2054,7 +2057,7 @@
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A31" s="17" t="s">
-        <v>348</v>
+        <v>339</v>
       </c>
       <c r="B31" s="4"/>
       <c r="C31" s="4"/>
@@ -2064,7 +2067,7 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>343</v>
+        <v>334</v>
       </c>
       <c r="B32" s="4" t="s">
         <v>11</v>
@@ -2079,12 +2082,12 @@
         <v>11</v>
       </c>
       <c r="I32" s="15" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>345</v>
+        <v>336</v>
       </c>
       <c r="B33" s="4" t="s">
         <v>11</v>
@@ -2099,7 +2102,7 @@
         <v>11</v>
       </c>
       <c r="I33" s="26" t="s">
-        <v>347</v>
+        <v>338</v>
       </c>
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2117,261 +2120,320 @@
       <c r="C35" s="4"/>
       <c r="D35" s="3"/>
     </row>
-    <row r="36" spans="1:32" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:32" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>33</v>
+        <v>345</v>
       </c>
       <c r="B36" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C36" s="4"/>
-      <c r="D36" s="3" t="s">
+      <c r="C36" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="D36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E36" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I36" s="15" t="s">
+        <v>350</v>
       </c>
     </row>
     <row r="37" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>35</v>
+        <v>346</v>
       </c>
       <c r="B37" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C37" s="4"/>
-      <c r="D37" s="3" t="s">
+      <c r="C37" s="4" t="s">
         <v>11</v>
+      </c>
+      <c r="D37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E37" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I37" s="15" t="s">
+        <v>351</v>
       </c>
     </row>
     <row r="38" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="15" t="s">
-        <v>36</v>
-      </c>
-      <c r="B38" s="3" t="s">
+        <v>34</v>
+      </c>
+      <c r="B38" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C38" s="4"/>
-      <c r="D38" s="3" t="s">
+      <c r="C38" s="4" t="s">
         <v>11</v>
       </c>
-    </row>
-    <row r="39" spans="1:32" ht="15" x14ac:dyDescent="0.2">
+      <c r="D38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="E38" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I38" s="15" t="s">
+        <v>352</v>
+      </c>
+    </row>
+    <row r="39" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>37</v>
+        <v>33</v>
       </c>
       <c r="B39" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C39" s="4"/>
-      <c r="D39" s="4"/>
+      <c r="C39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I39" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="40" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>38</v>
+        <v>35</v>
       </c>
       <c r="B40" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C40" s="4"/>
-      <c r="D40" s="4"/>
+      <c r="C40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D40" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I40" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="41" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>39</v>
-      </c>
-      <c r="B41" s="3" t="s">
+        <v>36</v>
+      </c>
+      <c r="B41" s="7"/>
+      <c r="C41" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="C41" s="4"/>
-      <c r="D41" s="3" t="s">
+      <c r="D41" s="8" t="s">
         <v>11</v>
       </c>
+      <c r="E41" s="9"/>
+      <c r="F41" s="9"/>
+      <c r="G41" s="9"/>
+      <c r="H41" s="9"/>
+      <c r="I41" t="s">
+        <v>349</v>
+      </c>
+      <c r="J41" s="9"/>
+      <c r="K41" s="9"/>
+      <c r="L41" s="9"/>
+      <c r="M41" s="9"/>
+      <c r="N41" s="9"/>
+      <c r="O41" s="9"/>
+      <c r="P41" s="9"/>
+      <c r="Q41" s="9"/>
+      <c r="R41" s="9"/>
+      <c r="S41" s="9"/>
+      <c r="T41" s="9"/>
+      <c r="U41" s="9"/>
+      <c r="V41" s="9"/>
+      <c r="W41" s="9"/>
+      <c r="X41" s="9"/>
+      <c r="Y41" s="9"/>
+      <c r="Z41" s="9"/>
+      <c r="AA41" s="9"/>
+      <c r="AB41" s="9"/>
+      <c r="AC41" s="9"/>
+      <c r="AD41" s="9"/>
+      <c r="AE41" s="9"/>
+      <c r="AF41" s="9"/>
     </row>
     <row r="42" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>40</v>
+        <v>37</v>
       </c>
       <c r="B42" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C42" s="4"/>
       <c r="D42" s="4"/>
+      <c r="I42" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>41</v>
+        <v>38</v>
       </c>
       <c r="B43" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C43" s="4"/>
-      <c r="D43" s="4"/>
+      <c r="C43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D43" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I43" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="44" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>42</v>
-      </c>
-      <c r="B44" s="7"/>
+        <v>39</v>
+      </c>
+      <c r="B44" s="3"/>
       <c r="C44" s="8" t="s">
         <v>11</v>
       </c>
       <c r="D44" s="8" t="s">
         <v>11</v>
       </c>
-      <c r="E44" s="9"/>
-      <c r="F44" s="9"/>
-      <c r="G44" s="9"/>
-      <c r="H44" s="9"/>
-      <c r="I44" s="9"/>
-      <c r="J44" s="9"/>
-      <c r="K44" s="9"/>
-      <c r="L44" s="9"/>
-      <c r="M44" s="9"/>
-      <c r="N44" s="9"/>
-      <c r="O44" s="9"/>
-      <c r="P44" s="9"/>
-      <c r="Q44" s="9"/>
-      <c r="R44" s="9"/>
-      <c r="S44" s="9"/>
-      <c r="T44" s="9"/>
-      <c r="U44" s="9"/>
-      <c r="V44" s="9"/>
-      <c r="W44" s="9"/>
-      <c r="X44" s="9"/>
-      <c r="Y44" s="9"/>
-      <c r="Z44" s="9"/>
-      <c r="AA44" s="9"/>
-      <c r="AB44" s="9"/>
-      <c r="AC44" s="9"/>
-      <c r="AD44" s="9"/>
-      <c r="AE44" s="9"/>
-      <c r="AF44" s="9"/>
+      <c r="I44" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>43</v>
+        <v>40</v>
       </c>
       <c r="B45" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C45" s="4"/>
-      <c r="D45" s="4"/>
+      <c r="C45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D45" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I45" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="46" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>44</v>
+        <v>343</v>
       </c>
       <c r="B46" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C46" s="4"/>
-      <c r="D46" s="4"/>
+      <c r="C46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="I46" t="s">
+        <v>349</v>
+      </c>
     </row>
     <row r="47" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>45</v>
-      </c>
-      <c r="B47" s="3"/>
-      <c r="C47" s="8" t="s">
+        <v>328</v>
+      </c>
+      <c r="B47" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="8" t="s">
-        <v>11</v>
+      <c r="C47" s="4"/>
+      <c r="D47" s="4"/>
+      <c r="I47" s="29" t="s">
+        <v>331</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>46</v>
-      </c>
-      <c r="B48" s="3" t="s">
+        <v>329</v>
+      </c>
+      <c r="B48" s="4"/>
+      <c r="C48" s="4" t="s">
         <v>11</v>
       </c>
-      <c r="C48" s="4"/>
-      <c r="D48" s="4"/>
-    </row>
-    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="15" t="s">
-        <v>47</v>
-      </c>
-      <c r="B49" s="3" t="s">
+      <c r="D48" s="4" t="s">
         <v>11</v>
       </c>
+      <c r="I48" s="29" t="s">
+        <v>331</v>
+      </c>
+    </row>
+    <row r="49" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A49" s="15"/>
+      <c r="B49" s="4"/>
       <c r="C49" s="4"/>
       <c r="D49" s="4"/>
     </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A50" s="15" t="s">
-        <v>337</v>
-      </c>
-      <c r="B50" s="4" t="s">
-        <v>11</v>
-      </c>
+    <row r="50" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A50" s="17" t="s">
+        <v>41</v>
+      </c>
+      <c r="B50" s="4"/>
       <c r="C50" s="4"/>
       <c r="D50" s="4"/>
-      <c r="I50" s="29" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    </row>
+    <row r="51" spans="1:4" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>338</v>
-      </c>
-      <c r="B51" s="4"/>
-      <c r="C51" s="4" t="s">
+        <v>347</v>
+      </c>
+      <c r="B51" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="4" t="s">
-        <v>11</v>
-      </c>
-      <c r="I51" s="29" t="s">
-        <v>340</v>
-      </c>
-    </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="C51" s="4"/>
+      <c r="D51" s="4"/>
+    </row>
+    <row r="52" spans="1:4" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>34</v>
-      </c>
-      <c r="B52" s="4" t="s">
+        <v>42</v>
+      </c>
+      <c r="B52" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C52" s="4"/>
       <c r="D52" s="4"/>
     </row>
-    <row r="53" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="15"/>
-      <c r="B53" s="4"/>
+    <row r="53" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A53" s="15" t="s">
+        <v>348</v>
+      </c>
+      <c r="B53" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C53" s="4"/>
       <c r="D53" s="4"/>
     </row>
-    <row r="54" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B54" s="4"/>
+    <row r="54" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B54" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C54" s="4"/>
       <c r="D54" s="4"/>
     </row>
-    <row r="55" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="15" t="s">
-        <v>49</v>
-      </c>
-      <c r="B55" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="55" spans="1:4" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="15"/>
+      <c r="B55" s="4"/>
       <c r="C55" s="4"/>
       <c r="D55" s="4"/>
     </row>
-    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A56" s="15" t="s">
-        <v>50</v>
-      </c>
-      <c r="B56" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="56" spans="1:4" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A56" s="17" t="s">
+        <v>44</v>
+      </c>
+      <c r="B56" s="4"/>
       <c r="C56" s="4"/>
       <c r="D56" s="4"/>
     </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:4" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>51</v>
+        <v>45</v>
       </c>
       <c r="B57" s="3" t="s">
         <v>11</v>
@@ -2379,57 +2441,63 @@
       <c r="C57" s="4"/>
       <c r="D57" s="4"/>
     </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="15" t="s">
-        <v>52</v>
-      </c>
-      <c r="B58" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="58" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A58" s="5"/>
+      <c r="B58" s="4"/>
       <c r="C58" s="4"/>
       <c r="D58" s="4"/>
     </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A59" s="15"/>
-      <c r="B59" s="4"/>
+    <row r="59" spans="1:4" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="A59" s="17" t="s">
+        <v>25</v>
+      </c>
+      <c r="B59" s="3"/>
       <c r="C59" s="4"/>
-      <c r="D59" s="4"/>
-    </row>
-    <row r="60" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A60" s="17" t="s">
-        <v>53</v>
-      </c>
-      <c r="B60" s="4"/>
+      <c r="D59" s="3"/>
+    </row>
+    <row r="60" spans="1:4" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A60" s="15" t="s">
+        <v>26</v>
+      </c>
+      <c r="B60" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C60" s="4"/>
-      <c r="D60" s="4"/>
-    </row>
-    <row r="61" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="D60" s="3"/>
+    </row>
+    <row r="61" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="15" t="s">
-        <v>54</v>
+        <v>27</v>
       </c>
       <c r="B61" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C61" s="4"/>
-      <c r="D61" s="4"/>
-    </row>
-    <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.25">
-      <c r="A62" s="5"/>
-      <c r="B62" s="4"/>
+      <c r="D61" s="3"/>
+    </row>
+    <row r="62" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="15" t="s">
+        <v>28</v>
+      </c>
+      <c r="B62" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C62" s="4"/>
-      <c r="D62" s="4"/>
-    </row>
-    <row r="63" spans="1:9" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A63" s="17" t="s">
-        <v>25</v>
-      </c>
-      <c r="B63" s="3"/>
+      <c r="D62" s="3"/>
+    </row>
+    <row r="63" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A63" s="15" t="s">
+        <v>29</v>
+      </c>
+      <c r="B63" s="3" t="s">
+        <v>11</v>
+      </c>
       <c r="C63" s="4"/>
       <c r="D63" s="3"/>
     </row>
-    <row r="64" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="64" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>26</v>
+        <v>30</v>
       </c>
       <c r="B64" s="3" t="s">
         <v>11</v>
@@ -2439,51 +2507,35 @@
     </row>
     <row r="65" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>27</v>
-      </c>
-      <c r="B65" s="3" t="s">
-        <v>11</v>
-      </c>
+        <v>31</v>
+      </c>
+      <c r="B65" s="3"/>
       <c r="C65" s="4"/>
       <c r="D65" s="3"/>
     </row>
-    <row r="66" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A66" s="15" t="s">
-        <v>28</v>
-      </c>
-      <c r="B66" s="3" t="s">
-        <v>11</v>
-      </c>
+    <row r="66" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A66" s="5"/>
+      <c r="B66" s="4"/>
       <c r="C66" s="4"/>
-      <c r="D66" s="3"/>
-    </row>
-    <row r="67" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A67" s="15" t="s">
-        <v>29</v>
-      </c>
-      <c r="B67" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="D66" s="4"/>
+    </row>
+    <row r="67" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A67" s="5"/>
+      <c r="B67" s="4"/>
       <c r="C67" s="4"/>
-      <c r="D67" s="3"/>
-    </row>
-    <row r="68" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A68" s="15" t="s">
-        <v>30</v>
-      </c>
-      <c r="B68" s="3" t="s">
-        <v>11</v>
-      </c>
+      <c r="D67" s="4"/>
+    </row>
+    <row r="68" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A68" s="5"/>
+      <c r="B68" s="4"/>
       <c r="C68" s="4"/>
-      <c r="D68" s="3"/>
-    </row>
-    <row r="69" spans="1:4" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A69" s="15" t="s">
-        <v>31</v>
-      </c>
-      <c r="B69" s="3"/>
+      <c r="D68" s="4"/>
+    </row>
+    <row r="69" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A69" s="5"/>
+      <c r="B69" s="4"/>
       <c r="C69" s="4"/>
-      <c r="D69" s="3"/>
+      <c r="D69" s="4"/>
     </row>
     <row r="70" spans="1:4" ht="15" x14ac:dyDescent="0.25">
       <c r="A70" s="5"/>
@@ -8094,30 +8146,6 @@
       <c r="B1004" s="4"/>
       <c r="C1004" s="4"/>
       <c r="D1004" s="4"/>
-    </row>
-    <row r="1005" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1005" s="5"/>
-      <c r="B1005" s="4"/>
-      <c r="C1005" s="4"/>
-      <c r="D1005" s="4"/>
-    </row>
-    <row r="1006" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1006" s="5"/>
-      <c r="B1006" s="4"/>
-      <c r="C1006" s="4"/>
-      <c r="D1006" s="4"/>
-    </row>
-    <row r="1007" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1007" s="5"/>
-      <c r="B1007" s="4"/>
-      <c r="C1007" s="4"/>
-      <c r="D1007" s="4"/>
-    </row>
-    <row r="1008" spans="1:4" ht="15" x14ac:dyDescent="0.25">
-      <c r="A1008" s="5"/>
-      <c r="B1008" s="4"/>
-      <c r="C1008" s="4"/>
-      <c r="D1008" s="4"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8163,7 +8191,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="32" t="s">
-        <v>315</v>
+        <v>306</v>
       </c>
       <c r="C1" s="30" t="s">
         <v>1</v>
@@ -8250,7 +8278,7 @@
     </row>
     <row r="3" spans="1:31" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A3" s="17" t="s">
-        <v>55</v>
+        <v>46</v>
       </c>
       <c r="B3" s="10"/>
       <c r="C3" s="11"/>
@@ -8263,7 +8291,7 @@
     </row>
     <row r="4" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>56</v>
+        <v>47</v>
       </c>
       <c r="B4" s="10"/>
       <c r="C4" s="11" t="s">
@@ -8288,7 +8316,7 @@
     </row>
     <row r="6" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>57</v>
+        <v>48</v>
       </c>
       <c r="B6" s="13"/>
       <c r="C6" s="11"/>
@@ -8301,13 +8329,13 @@
     </row>
     <row r="7" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>58</v>
+        <v>49</v>
       </c>
       <c r="B7" s="10" t="s">
-        <v>59</v>
+        <v>50</v>
       </c>
       <c r="C7" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D7" s="12"/>
       <c r="E7" s="12"/>
@@ -8318,13 +8346,13 @@
     </row>
     <row r="8" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>61</v>
+        <v>52</v>
       </c>
       <c r="B8" s="10">
         <v>98</v>
       </c>
       <c r="C8" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D8" s="12"/>
       <c r="E8" s="12"/>
@@ -8335,13 +8363,13 @@
     </row>
     <row r="9" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>62</v>
+        <v>53</v>
       </c>
       <c r="B9" s="10">
         <v>99</v>
       </c>
       <c r="C9" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D9" s="12"/>
       <c r="E9" s="12"/>
@@ -8362,7 +8390,7 @@
     </row>
     <row r="11" spans="1:31" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>63</v>
+        <v>54</v>
       </c>
       <c r="B11" s="10"/>
       <c r="C11" s="11"/>
@@ -8375,7 +8403,7 @@
     </row>
     <row r="12" spans="1:31" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>64</v>
+        <v>55</v>
       </c>
       <c r="B12" s="10"/>
       <c r="C12" s="11" t="s">
@@ -8398,7 +8426,7 @@
     </row>
     <row r="14" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>65</v>
+        <v>56</v>
       </c>
       <c r="B14" s="10"/>
       <c r="C14" s="11" t="s">
@@ -8413,7 +8441,7 @@
     </row>
     <row r="15" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>66</v>
+        <v>57</v>
       </c>
       <c r="B15" s="10"/>
       <c r="C15" s="11" t="s">
@@ -8428,7 +8456,7 @@
     </row>
     <row r="16" spans="1:31" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>67</v>
+        <v>58</v>
       </c>
       <c r="B16" s="10"/>
       <c r="C16" s="11" t="s">
@@ -8441,12 +8469,12 @@
       <c r="H16" s="11"/>
       <c r="I16" s="11"/>
       <c r="J16" s="14" t="s">
-        <v>68</v>
+        <v>59</v>
       </c>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
       <c r="B17" s="10"/>
       <c r="C17" s="11" t="s">
@@ -8461,7 +8489,7 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>70</v>
+        <v>61</v>
       </c>
       <c r="B18" s="10"/>
       <c r="C18" s="11" t="s">
@@ -8476,7 +8504,7 @@
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>71</v>
+        <v>62</v>
       </c>
       <c r="B19" s="10"/>
       <c r="C19" s="11" t="s">
@@ -8491,7 +8519,7 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>72</v>
+        <v>63</v>
       </c>
       <c r="B20" s="10"/>
       <c r="C20" s="11" t="s">
@@ -8506,13 +8534,13 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="B21" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C21" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D21" s="12"/>
       <c r="E21" s="12"/>
@@ -8533,7 +8561,7 @@
     </row>
     <row r="23" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A23" s="17" t="s">
-        <v>75</v>
+        <v>66</v>
       </c>
       <c r="B23" s="10"/>
       <c r="C23" s="11"/>
@@ -8546,13 +8574,13 @@
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>76</v>
+        <v>67</v>
       </c>
       <c r="B24" s="10" t="s">
-        <v>77</v>
+        <v>68</v>
       </c>
       <c r="C24" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D24" s="12"/>
       <c r="E24" s="12"/>
@@ -8563,13 +8591,13 @@
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>78</v>
+        <v>69</v>
       </c>
       <c r="B25" s="10" t="s">
-        <v>79</v>
+        <v>70</v>
       </c>
       <c r="C25" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D25" s="12"/>
       <c r="E25" s="12"/>
@@ -8580,13 +8608,13 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>80</v>
+        <v>71</v>
       </c>
       <c r="B26" s="10" t="s">
-        <v>81</v>
+        <v>72</v>
       </c>
       <c r="C26" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D26" s="12"/>
       <c r="E26" s="12"/>
@@ -8607,13 +8635,13 @@
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="15" t="s">
-        <v>82</v>
+        <v>73</v>
       </c>
       <c r="B28" s="10" t="s">
-        <v>83</v>
+        <v>74</v>
       </c>
       <c r="C28" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D28" s="12"/>
       <c r="E28" s="12"/>
@@ -8624,13 +8652,13 @@
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>84</v>
+        <v>75</v>
       </c>
       <c r="B29" s="10" t="s">
-        <v>85</v>
+        <v>76</v>
       </c>
       <c r="C29" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D29" s="12"/>
       <c r="E29" s="12"/>
@@ -8641,13 +8669,13 @@
     </row>
     <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>86</v>
+        <v>77</v>
       </c>
       <c r="B30" s="10" t="s">
-        <v>87</v>
+        <v>78</v>
       </c>
       <c r="C30" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D30" s="12"/>
       <c r="E30" s="12"/>
@@ -8668,13 +8696,13 @@
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>88</v>
+        <v>79</v>
       </c>
       <c r="B32" s="10" t="s">
-        <v>89</v>
+        <v>80</v>
       </c>
       <c r="C32" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D32" s="12"/>
       <c r="E32" s="12"/>
@@ -8685,13 +8713,13 @@
     </row>
     <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>90</v>
+        <v>81</v>
       </c>
       <c r="B33" s="10" t="s">
-        <v>91</v>
+        <v>82</v>
       </c>
       <c r="C33" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D33" s="12"/>
       <c r="E33" s="12"/>
@@ -8712,13 +8740,13 @@
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>92</v>
+        <v>83</v>
       </c>
       <c r="B35" s="10" t="s">
-        <v>93</v>
+        <v>84</v>
       </c>
       <c r="C35" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D35" s="12"/>
       <c r="E35" s="12"/>
@@ -8729,13 +8757,13 @@
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>94</v>
+        <v>85</v>
       </c>
       <c r="B36" s="10" t="s">
-        <v>95</v>
+        <v>86</v>
       </c>
       <c r="C36" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D36" s="12"/>
       <c r="E36" s="12"/>
@@ -8746,13 +8774,13 @@
     </row>
     <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>96</v>
+        <v>87</v>
       </c>
       <c r="B37" s="10" t="s">
-        <v>97</v>
+        <v>88</v>
       </c>
       <c r="C37" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D37" s="12"/>
       <c r="E37" s="12"/>
@@ -8773,7 +8801,7 @@
     </row>
     <row r="39" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A39" s="17" t="s">
-        <v>98</v>
+        <v>89</v>
       </c>
       <c r="B39" s="10"/>
       <c r="C39" s="12"/>
@@ -8786,13 +8814,13 @@
     </row>
     <row r="40" spans="1:9" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>99</v>
+        <v>90</v>
       </c>
       <c r="B40" s="10" t="s">
-        <v>100</v>
+        <v>91</v>
       </c>
       <c r="C40" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D40" s="12"/>
       <c r="E40" s="12"/>
@@ -8803,13 +8831,13 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>101</v>
+        <v>92</v>
       </c>
       <c r="B41" s="10" t="s">
-        <v>102</v>
+        <v>93</v>
       </c>
       <c r="C41" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D41" s="12"/>
       <c r="E41" s="12"/>
@@ -8820,13 +8848,13 @@
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>103</v>
+        <v>94</v>
       </c>
       <c r="B42" s="10" t="s">
-        <v>104</v>
+        <v>95</v>
       </c>
       <c r="C42" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D42" s="12"/>
       <c r="E42" s="12"/>
@@ -8837,13 +8865,13 @@
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="15" t="s">
-        <v>105</v>
+        <v>96</v>
       </c>
       <c r="B43" s="10" t="s">
-        <v>106</v>
+        <v>97</v>
       </c>
       <c r="C43" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D43" s="12"/>
       <c r="E43" s="12"/>
@@ -8854,13 +8882,13 @@
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B44" s="10" t="s">
-        <v>108</v>
+        <v>99</v>
       </c>
       <c r="C44" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D44" s="12"/>
       <c r="E44" s="12"/>
@@ -8881,7 +8909,7 @@
     </row>
     <row r="46" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A46" s="17" t="s">
-        <v>109</v>
+        <v>100</v>
       </c>
       <c r="B46" s="10"/>
       <c r="C46" s="11"/>
@@ -8894,13 +8922,13 @@
     </row>
     <row r="47" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A47" s="15" t="s">
-        <v>110</v>
+        <v>101</v>
       </c>
       <c r="B47" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C47" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D47" s="12"/>
       <c r="E47" s="12"/>
@@ -8911,13 +8939,13 @@
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>112</v>
+        <v>103</v>
       </c>
       <c r="B48" s="10" t="s">
-        <v>111</v>
+        <v>102</v>
       </c>
       <c r="C48" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D48" s="12"/>
       <c r="E48" s="12"/>
@@ -8928,13 +8956,13 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>113</v>
+        <v>104</v>
       </c>
       <c r="B49" s="10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C49" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D49" s="12"/>
       <c r="E49" s="12"/>
@@ -8945,13 +8973,13 @@
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>115</v>
+        <v>106</v>
       </c>
       <c r="B50" s="10" t="s">
-        <v>114</v>
+        <v>105</v>
       </c>
       <c r="C50" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D50" s="12"/>
       <c r="E50" s="12"/>
@@ -8962,13 +8990,13 @@
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>116</v>
+        <v>107</v>
       </c>
       <c r="B51" s="10" t="s">
-        <v>117</v>
+        <v>108</v>
       </c>
       <c r="C51" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D51" s="12"/>
       <c r="E51" s="12"/>
@@ -8979,13 +9007,13 @@
     </row>
     <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>118</v>
+        <v>109</v>
       </c>
       <c r="B52" s="10" t="s">
-        <v>119</v>
+        <v>110</v>
       </c>
       <c r="C52" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D52" s="12"/>
       <c r="E52" s="12"/>
@@ -9006,11 +9034,11 @@
     </row>
     <row r="54" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A54" s="17" t="s">
-        <v>120</v>
+        <v>111</v>
       </c>
       <c r="B54" s="13"/>
       <c r="C54" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D54" s="12"/>
       <c r="E54" s="12"/>
@@ -9021,13 +9049,13 @@
     </row>
     <row r="55" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>121</v>
+        <v>112</v>
       </c>
       <c r="B55" s="10" t="s">
-        <v>122</v>
+        <v>113</v>
       </c>
       <c r="C55" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D55" s="12"/>
       <c r="E55" s="12"/>
@@ -9038,13 +9066,13 @@
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>123</v>
+        <v>114</v>
       </c>
       <c r="B56" s="10" t="s">
-        <v>124</v>
+        <v>115</v>
       </c>
       <c r="C56" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D56" s="12"/>
       <c r="E56" s="12"/>
@@ -9055,13 +9083,13 @@
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>125</v>
+        <v>116</v>
       </c>
       <c r="B57" s="10" t="s">
-        <v>126</v>
+        <v>117</v>
       </c>
       <c r="C57" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D57" s="12"/>
       <c r="E57" s="12"/>
@@ -9072,13 +9100,13 @@
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>127</v>
+        <v>118</v>
       </c>
       <c r="B58" s="10" t="s">
-        <v>128</v>
+        <v>119</v>
       </c>
       <c r="C58" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D58" s="12"/>
       <c r="E58" s="12"/>
@@ -9089,13 +9117,13 @@
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>129</v>
+        <v>120</v>
       </c>
       <c r="B59" s="10" t="s">
-        <v>130</v>
+        <v>121</v>
       </c>
       <c r="C59" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D59" s="12"/>
       <c r="E59" s="12"/>
@@ -9106,13 +9134,13 @@
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>131</v>
+        <v>122</v>
       </c>
       <c r="B60" s="10" t="s">
-        <v>132</v>
+        <v>123</v>
       </c>
       <c r="C60" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D60" s="12"/>
       <c r="E60" s="12"/>
@@ -9133,7 +9161,7 @@
     </row>
     <row r="62" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A62" s="17" t="s">
-        <v>133</v>
+        <v>124</v>
       </c>
       <c r="B62" s="10"/>
       <c r="C62" s="11"/>
@@ -9146,13 +9174,13 @@
     </row>
     <row r="63" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>134</v>
+        <v>125</v>
       </c>
       <c r="B63" s="10" t="s">
-        <v>135</v>
+        <v>126</v>
       </c>
       <c r="C63" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D63" s="12"/>
       <c r="E63" s="12"/>
@@ -9163,13 +9191,13 @@
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>136</v>
+        <v>127</v>
       </c>
       <c r="B64" s="10" t="s">
-        <v>137</v>
+        <v>128</v>
       </c>
       <c r="C64" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D64" s="12"/>
       <c r="E64" s="12"/>
@@ -9180,13 +9208,13 @@
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>138</v>
+        <v>129</v>
       </c>
       <c r="B65" s="10" t="s">
-        <v>139</v>
+        <v>130</v>
       </c>
       <c r="C65" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D65" s="12"/>
       <c r="E65" s="12"/>
@@ -9197,13 +9225,13 @@
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="15" t="s">
-        <v>140</v>
+        <v>131</v>
       </c>
       <c r="B66" s="10" t="s">
-        <v>141</v>
+        <v>132</v>
       </c>
       <c r="C66" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D66" s="12"/>
       <c r="E66" s="12"/>
@@ -9214,13 +9242,13 @@
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="15" t="s">
-        <v>142</v>
+        <v>133</v>
       </c>
       <c r="B67" s="10" t="s">
-        <v>143</v>
+        <v>134</v>
       </c>
       <c r="C67" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D67" s="12"/>
       <c r="E67" s="12"/>
@@ -9231,13 +9259,13 @@
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="15" t="s">
-        <v>144</v>
+        <v>135</v>
       </c>
       <c r="B68" s="10" t="s">
-        <v>145</v>
+        <v>136</v>
       </c>
       <c r="C68" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D68" s="12"/>
       <c r="E68" s="12"/>
@@ -9248,13 +9276,13 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="15" t="s">
-        <v>146</v>
+        <v>137</v>
       </c>
       <c r="B69" s="10" t="s">
-        <v>147</v>
+        <v>138</v>
       </c>
       <c r="C69" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D69" s="12"/>
       <c r="E69" s="12"/>
@@ -9265,13 +9293,13 @@
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="15" t="s">
-        <v>148</v>
+        <v>139</v>
       </c>
       <c r="B70" s="10" t="s">
-        <v>149</v>
+        <v>140</v>
       </c>
       <c r="C70" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D70" s="12"/>
       <c r="E70" s="12"/>
@@ -9282,13 +9310,13 @@
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>150</v>
+        <v>141</v>
       </c>
       <c r="B71" s="10" t="s">
-        <v>151</v>
+        <v>142</v>
       </c>
       <c r="C71" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D71" s="12"/>
       <c r="E71" s="12"/>
@@ -9299,13 +9327,13 @@
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>152</v>
+        <v>143</v>
       </c>
       <c r="B72" s="10" t="s">
-        <v>74</v>
+        <v>65</v>
       </c>
       <c r="C72" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D72" s="12"/>
       <c r="E72" s="12"/>
@@ -9316,13 +9344,13 @@
     </row>
     <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>153</v>
+        <v>144</v>
       </c>
       <c r="B73" s="10" t="s">
-        <v>154</v>
+        <v>145</v>
       </c>
       <c r="C73" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D73" s="12"/>
       <c r="E73" s="12"/>
@@ -9343,7 +9371,7 @@
     </row>
     <row r="75" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A75" s="17" t="s">
-        <v>155</v>
+        <v>146</v>
       </c>
       <c r="B75" s="10"/>
       <c r="C75" s="11"/>
@@ -9356,13 +9384,13 @@
     </row>
     <row r="76" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A76" s="15" t="s">
-        <v>156</v>
+        <v>147</v>
       </c>
       <c r="B76" s="10" t="s">
-        <v>157</v>
+        <v>148</v>
       </c>
       <c r="C76" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D76" s="12"/>
       <c r="E76" s="12"/>
@@ -9373,13 +9401,13 @@
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="15" t="s">
-        <v>158</v>
+        <v>149</v>
       </c>
       <c r="B77" s="10" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C77" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D77" s="12"/>
       <c r="E77" s="12"/>
@@ -9390,13 +9418,13 @@
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="15" t="s">
-        <v>160</v>
+        <v>151</v>
       </c>
       <c r="B78" s="10" t="s">
-        <v>161</v>
+        <v>152</v>
       </c>
       <c r="C78" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D78" s="12"/>
       <c r="E78" s="12"/>
@@ -9407,13 +9435,13 @@
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="15" t="s">
-        <v>162</v>
+        <v>153</v>
       </c>
       <c r="B79" s="10" t="s">
-        <v>163</v>
+        <v>154</v>
       </c>
       <c r="C79" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D79" s="12"/>
       <c r="E79" s="12"/>
@@ -9424,13 +9452,13 @@
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="15" t="s">
-        <v>164</v>
+        <v>155</v>
       </c>
       <c r="B80" s="10" t="s">
-        <v>165</v>
+        <v>156</v>
       </c>
       <c r="C80" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D80" s="12"/>
       <c r="E80" s="12"/>
@@ -9441,13 +9469,13 @@
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="15" t="s">
-        <v>166</v>
+        <v>157</v>
       </c>
       <c r="B81" s="10" t="s">
-        <v>167</v>
+        <v>158</v>
       </c>
       <c r="C81" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D81" s="12"/>
       <c r="E81" s="12"/>
@@ -9458,13 +9486,13 @@
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="15" t="s">
-        <v>168</v>
+        <v>159</v>
       </c>
       <c r="B82" s="10" t="s">
-        <v>169</v>
+        <v>160</v>
       </c>
       <c r="C82" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D82" s="12"/>
       <c r="E82" s="12"/>
@@ -9475,13 +9503,13 @@
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="15" t="s">
-        <v>170</v>
+        <v>161</v>
       </c>
       <c r="B83" s="10" t="s">
-        <v>171</v>
+        <v>162</v>
       </c>
       <c r="C83" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D83" s="12"/>
       <c r="E83" s="12"/>
@@ -9492,13 +9520,13 @@
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="15" t="s">
-        <v>172</v>
+        <v>163</v>
       </c>
       <c r="B84" s="10" t="s">
-        <v>173</v>
+        <v>164</v>
       </c>
       <c r="C84" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D84" s="12"/>
       <c r="E84" s="12"/>
@@ -9509,13 +9537,13 @@
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="15" t="s">
-        <v>174</v>
+        <v>165</v>
       </c>
       <c r="B85" s="10" t="s">
-        <v>175</v>
+        <v>166</v>
       </c>
       <c r="C85" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D85" s="12"/>
       <c r="E85" s="12"/>
@@ -9526,13 +9554,13 @@
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="15" t="s">
-        <v>176</v>
+        <v>167</v>
       </c>
       <c r="B86" s="10" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="C86" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D86" s="12"/>
       <c r="E86" s="12"/>
@@ -9543,13 +9571,13 @@
     </row>
     <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A87" s="15" t="s">
-        <v>178</v>
+        <v>169</v>
       </c>
       <c r="B87" s="10" t="s">
-        <v>179</v>
+        <v>170</v>
       </c>
       <c r="C87" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D87" s="12"/>
       <c r="E87" s="12"/>
@@ -9570,7 +9598,7 @@
     </row>
     <row r="89" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A89" s="17" t="s">
-        <v>180</v>
+        <v>171</v>
       </c>
       <c r="B89" s="13"/>
       <c r="C89" s="12"/>
@@ -9583,13 +9611,13 @@
     </row>
     <row r="90" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A90" s="15" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="B90" s="10" t="s">
-        <v>182</v>
+        <v>173</v>
       </c>
       <c r="C90" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D90" s="12"/>
       <c r="E90" s="12"/>
@@ -9602,13 +9630,13 @@
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="15" t="s">
-        <v>183</v>
+        <v>174</v>
       </c>
       <c r="B91" s="10" t="s">
-        <v>184</v>
+        <v>175</v>
       </c>
       <c r="C91" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D91" s="12"/>
       <c r="E91" s="12"/>
@@ -9621,13 +9649,13 @@
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="15" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B92" s="10" t="s">
-        <v>186</v>
+        <v>177</v>
       </c>
       <c r="C92" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D92" s="12"/>
       <c r="E92" s="12"/>
@@ -9640,13 +9668,13 @@
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="15" t="s">
-        <v>187</v>
+        <v>178</v>
       </c>
       <c r="B93" s="10" t="s">
-        <v>188</v>
+        <v>179</v>
       </c>
       <c r="C93" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D93" s="12"/>
       <c r="E93" s="12"/>
@@ -9659,13 +9687,13 @@
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="15" t="s">
-        <v>189</v>
+        <v>180</v>
       </c>
       <c r="B94" s="10" t="s">
-        <v>190</v>
+        <v>181</v>
       </c>
       <c r="C94" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D94" s="12"/>
       <c r="E94" s="12"/>
@@ -9678,13 +9706,13 @@
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="15" t="s">
-        <v>191</v>
+        <v>182</v>
       </c>
       <c r="B95" s="10" t="s">
-        <v>192</v>
+        <v>183</v>
       </c>
       <c r="C95" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D95" s="12"/>
       <c r="E95" s="12"/>
@@ -9697,13 +9725,13 @@
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="15" t="s">
-        <v>193</v>
+        <v>184</v>
       </c>
       <c r="B96" s="10" t="s">
-        <v>194</v>
+        <v>185</v>
       </c>
       <c r="C96" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D96" s="12"/>
       <c r="E96" s="12"/>
@@ -9716,13 +9744,13 @@
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="15" t="s">
-        <v>195</v>
+        <v>186</v>
       </c>
       <c r="B97" s="10" t="s">
-        <v>196</v>
+        <v>187</v>
       </c>
       <c r="C97" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D97" s="12"/>
       <c r="E97" s="12"/>
@@ -9745,7 +9773,7 @@
     </row>
     <row r="99" spans="1:9" ht="17.25" thickBot="1" x14ac:dyDescent="0.25">
       <c r="A99" s="17" t="s">
-        <v>197</v>
+        <v>188</v>
       </c>
       <c r="B99" s="13"/>
       <c r="C99" s="12"/>
@@ -9758,13 +9786,13 @@
     </row>
     <row r="100" spans="1:9" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A100" s="15" t="s">
-        <v>198</v>
+        <v>189</v>
       </c>
       <c r="B100" s="10" t="s">
-        <v>199</v>
+        <v>190</v>
       </c>
       <c r="C100" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D100" s="12"/>
       <c r="E100" s="12"/>
@@ -9775,13 +9803,13 @@
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="15" t="s">
-        <v>200</v>
+        <v>191</v>
       </c>
       <c r="B101" s="10" t="s">
-        <v>201</v>
+        <v>192</v>
       </c>
       <c r="C101" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D101" s="12"/>
       <c r="E101" s="12"/>
@@ -9792,13 +9820,13 @@
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="15" t="s">
-        <v>202</v>
+        <v>193</v>
       </c>
       <c r="B102" s="10" t="s">
-        <v>203</v>
+        <v>194</v>
       </c>
       <c r="C102" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D102" s="12"/>
       <c r="E102" s="12"/>
@@ -9809,13 +9837,13 @@
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="15" t="s">
-        <v>204</v>
+        <v>195</v>
       </c>
       <c r="B103" s="10" t="s">
-        <v>205</v>
+        <v>196</v>
       </c>
       <c r="C103" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D103" s="12"/>
       <c r="E103" s="12"/>
@@ -9826,13 +9854,13 @@
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="15" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B104" s="10" t="s">
-        <v>207</v>
+        <v>198</v>
       </c>
       <c r="C104" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D104" s="12"/>
       <c r="E104" s="12"/>
@@ -9843,13 +9871,13 @@
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="15" t="s">
-        <v>208</v>
+        <v>199</v>
       </c>
       <c r="B105" s="10" t="s">
-        <v>209</v>
+        <v>200</v>
       </c>
       <c r="C105" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D105" s="12"/>
       <c r="E105" s="12"/>
@@ -9860,13 +9888,13 @@
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="15" t="s">
-        <v>210</v>
+        <v>201</v>
       </c>
       <c r="B106" s="10" t="s">
-        <v>211</v>
+        <v>202</v>
       </c>
       <c r="C106" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D106" s="12"/>
       <c r="E106" s="12"/>
@@ -9877,13 +9905,13 @@
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="15" t="s">
-        <v>212</v>
+        <v>203</v>
       </c>
       <c r="B107" s="10" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C107" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D107" s="12"/>
       <c r="E107" s="12"/>
@@ -9894,13 +9922,13 @@
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="15" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
       <c r="B108" s="10" t="s">
-        <v>215</v>
+        <v>206</v>
       </c>
       <c r="C108" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D108" s="12"/>
       <c r="E108" s="12"/>
@@ -9911,13 +9939,13 @@
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="15" t="s">
-        <v>216</v>
+        <v>207</v>
       </c>
       <c r="B109" s="10" t="s">
-        <v>217</v>
+        <v>208</v>
       </c>
       <c r="C109" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D109" s="12"/>
       <c r="E109" s="12"/>
@@ -9928,13 +9956,13 @@
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="15" t="s">
-        <v>218</v>
+        <v>209</v>
       </c>
       <c r="B110" s="10" t="s">
-        <v>219</v>
+        <v>210</v>
       </c>
       <c r="C110" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D110" s="12"/>
       <c r="E110" s="12"/>
@@ -9945,13 +9973,13 @@
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="15" t="s">
-        <v>220</v>
+        <v>211</v>
       </c>
       <c r="B111" s="10" t="s">
-        <v>221</v>
+        <v>212</v>
       </c>
       <c r="C111" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D111" s="12"/>
       <c r="E111" s="12"/>
@@ -9962,13 +9990,13 @@
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="15" t="s">
-        <v>222</v>
+        <v>213</v>
       </c>
       <c r="B112" s="10" t="s">
-        <v>223</v>
+        <v>214</v>
       </c>
       <c r="C112" s="11" t="s">
-        <v>60</v>
+        <v>51</v>
       </c>
       <c r="D112" s="12"/>
       <c r="E112" s="12"/>
@@ -19742,7 +19770,7 @@
     </row>
     <row r="3" spans="1:30" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="21" t="s">
-        <v>316</v>
+        <v>307</v>
       </c>
       <c r="B3" s="18"/>
       <c r="C3" s="18"/>
@@ -19776,7 +19804,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>224</v>
+        <v>215</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -19786,7 +19814,7 @@
     </row>
     <row r="5" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>225</v>
+        <v>216</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -19796,7 +19824,7 @@
     </row>
     <row r="6" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>226</v>
+        <v>217</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -19807,7 +19835,7 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>227</v>
+        <v>218</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
@@ -19817,7 +19845,7 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>228</v>
+        <v>219</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -19833,7 +19861,7 @@
     </row>
     <row r="10" spans="1:30" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="16" t="s">
-        <v>317</v>
+        <v>308</v>
       </c>
       <c r="B10" s="4"/>
       <c r="C10" s="4"/>
@@ -19842,7 +19870,7 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>229</v>
+        <v>220</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -19852,7 +19880,7 @@
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>230</v>
+        <v>221</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -19862,7 +19890,7 @@
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>231</v>
+        <v>222</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -19872,7 +19900,7 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>232</v>
+        <v>223</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -19882,7 +19910,7 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>233</v>
+        <v>224</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>
@@ -25673,132 +25701,132 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>234</v>
+        <v>225</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>235</v>
+        <v>226</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>236</v>
+        <v>227</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>237</v>
+        <v>228</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>238</v>
+        <v>229</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>239</v>
+        <v>230</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>240</v>
+        <v>231</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>241</v>
+        <v>232</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>242</v>
+        <v>233</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>243</v>
+        <v>234</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>244</v>
+        <v>235</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>245</v>
+        <v>236</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>246</v>
+        <v>237</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>251</v>
+        <v>242</v>
       </c>
     </row>
     <row r="15" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="15" t="s">
-        <v>252</v>
+        <v>243</v>
       </c>
     </row>
     <row r="16" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="15" t="s">
-        <v>253</v>
+        <v>244</v>
       </c>
     </row>
     <row r="17" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="15" t="s">
-        <v>254</v>
+        <v>245</v>
       </c>
     </row>
     <row r="18" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="15" t="s">
-        <v>255</v>
+        <v>246</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>256</v>
+        <v>247</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>257</v>
+        <v>248</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>258</v>
+        <v>249</v>
       </c>
     </row>
     <row r="28" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="24" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="23" t="s">
-        <v>247</v>
+        <v>238</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="23" t="s">
-        <v>248</v>
+        <v>239</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="23" t="s">
-        <v>249</v>
+        <v>240</v>
       </c>
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="23" t="s">
-        <v>250</v>
+        <v>241</v>
       </c>
     </row>
   </sheetData>
@@ -25825,112 +25853,112 @@
   <sheetData>
     <row r="1" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A1" s="15" t="s">
-        <v>259</v>
+        <v>250</v>
       </c>
     </row>
     <row r="2" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A2" s="15" t="s">
-        <v>260</v>
+        <v>251</v>
       </c>
     </row>
     <row r="3" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A3" s="15" t="s">
-        <v>261</v>
+        <v>252</v>
       </c>
     </row>
     <row r="4" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="15" t="s">
-        <v>262</v>
+        <v>253</v>
       </c>
     </row>
     <row r="5" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A5" s="15" t="s">
-        <v>263</v>
+        <v>254</v>
       </c>
     </row>
     <row r="6" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A6" s="15" t="s">
-        <v>264</v>
+        <v>255</v>
       </c>
     </row>
     <row r="7" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="15" t="s">
-        <v>265</v>
+        <v>256</v>
       </c>
     </row>
     <row r="8" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="15" t="s">
-        <v>266</v>
+        <v>257</v>
       </c>
     </row>
     <row r="9" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="15" t="s">
-        <v>267</v>
+        <v>258</v>
       </c>
     </row>
     <row r="10" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="15" t="s">
-        <v>268</v>
+        <v>259</v>
       </c>
     </row>
     <row r="11" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="15" t="s">
-        <v>269</v>
+        <v>260</v>
       </c>
     </row>
     <row r="12" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="15" t="s">
-        <v>270</v>
+        <v>261</v>
       </c>
     </row>
     <row r="13" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="15" t="s">
-        <v>271</v>
+        <v>262</v>
       </c>
     </row>
     <row r="14" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="15" t="s">
-        <v>272</v>
+        <v>263</v>
       </c>
     </row>
     <row r="19" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="15" t="s">
-        <v>277</v>
+        <v>268</v>
       </c>
     </row>
     <row r="20" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="15" t="s">
-        <v>278</v>
+        <v>269</v>
       </c>
     </row>
     <row r="21" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="15" t="s">
-        <v>279</v>
+        <v>270</v>
       </c>
     </row>
     <row r="22" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="15" t="s">
-        <v>280</v>
+        <v>271</v>
       </c>
     </row>
     <row r="23" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="15" t="s">
-        <v>281</v>
+        <v>272</v>
       </c>
     </row>
     <row r="24" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="15" t="s">
-        <v>282</v>
+        <v>273</v>
       </c>
     </row>
     <row r="25" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="15" t="s">
-        <v>283</v>
+        <v>274</v>
       </c>
     </row>
     <row r="26" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="15" t="s">
-        <v>284</v>
+        <v>275</v>
       </c>
     </row>
     <row r="27" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25941,12 +25969,12 @@
     </row>
     <row r="29" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="15" t="s">
-        <v>285</v>
+        <v>276</v>
       </c>
     </row>
     <row r="30" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="15" t="s">
-        <v>286</v>
+        <v>277</v>
       </c>
     </row>
     <row r="31" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -25954,32 +25982,32 @@
     </row>
     <row r="32" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="15" t="s">
-        <v>287</v>
+        <v>278</v>
       </c>
     </row>
     <row r="33" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A33" s="15" t="s">
-        <v>288</v>
+        <v>279</v>
       </c>
     </row>
     <row r="34" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="15" t="s">
-        <v>289</v>
+        <v>280</v>
       </c>
     </row>
     <row r="35" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="15" t="s">
-        <v>290</v>
+        <v>281</v>
       </c>
     </row>
     <row r="36" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="15" t="s">
-        <v>291</v>
+        <v>282</v>
       </c>
     </row>
     <row r="37" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A37" s="15" t="s">
-        <v>292</v>
+        <v>283</v>
       </c>
     </row>
     <row r="38" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -25987,22 +26015,22 @@
     </row>
     <row r="39" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="15" t="s">
-        <v>293</v>
+        <v>284</v>
       </c>
     </row>
     <row r="40" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="15" t="s">
-        <v>294</v>
+        <v>285</v>
       </c>
     </row>
     <row r="41" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="15" t="s">
-        <v>295</v>
+        <v>286</v>
       </c>
     </row>
     <row r="42" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="15" t="s">
-        <v>296</v>
+        <v>287</v>
       </c>
     </row>
     <row r="43" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -26010,17 +26038,17 @@
     </row>
     <row r="44" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="15" t="s">
-        <v>297</v>
+        <v>288</v>
       </c>
     </row>
     <row r="45" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="15" t="s">
-        <v>298</v>
+        <v>289</v>
       </c>
     </row>
     <row r="46" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="15" t="s">
-        <v>299</v>
+        <v>290</v>
       </c>
     </row>
     <row r="47" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -26028,67 +26056,67 @@
     </row>
     <row r="48" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="15" t="s">
-        <v>300</v>
+        <v>291</v>
       </c>
     </row>
     <row r="49" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="15" t="s">
-        <v>301</v>
+        <v>292</v>
       </c>
     </row>
     <row r="50" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="15" t="s">
-        <v>302</v>
+        <v>293</v>
       </c>
     </row>
     <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="15" t="s">
-        <v>303</v>
+        <v>294</v>
       </c>
     </row>
     <row r="52" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="15" t="s">
-        <v>304</v>
+        <v>295</v>
       </c>
     </row>
     <row r="53" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="15" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="54" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="15" t="s">
-        <v>306</v>
+        <v>297</v>
       </c>
     </row>
     <row r="55" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="15" t="s">
-        <v>307</v>
+        <v>298</v>
       </c>
     </row>
     <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="15" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="57" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="15" t="s">
-        <v>308</v>
+        <v>299</v>
       </c>
     </row>
     <row r="58" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="15" t="s">
-        <v>309</v>
+        <v>300</v>
       </c>
     </row>
     <row r="59" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="15" t="s">
-        <v>305</v>
+        <v>296</v>
       </c>
     </row>
     <row r="60" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="15" t="s">
-        <v>310</v>
+        <v>301</v>
       </c>
     </row>
     <row r="61" spans="1:1" ht="15" x14ac:dyDescent="0.2">
@@ -26096,47 +26124,47 @@
     </row>
     <row r="62" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="15" t="s">
-        <v>311</v>
+        <v>302</v>
       </c>
     </row>
     <row r="63" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="15" t="s">
-        <v>312</v>
+        <v>303</v>
       </c>
     </row>
     <row r="64" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="15" t="s">
-        <v>313</v>
+        <v>304</v>
       </c>
     </row>
     <row r="65" spans="1:1" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="15" t="s">
-        <v>314</v>
+        <v>305</v>
       </c>
     </row>
     <row r="70" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A70" s="24" t="s">
-        <v>318</v>
+        <v>309</v>
       </c>
     </row>
     <row r="71" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A71" s="15" t="s">
-        <v>273</v>
+        <v>264</v>
       </c>
     </row>
     <row r="72" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="15" t="s">
-        <v>274</v>
+        <v>265</v>
       </c>
     </row>
     <row r="73" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="15" t="s">
-        <v>275</v>
+        <v>266</v>
       </c>
     </row>
     <row r="74" spans="1:1" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="15" t="s">
-        <v>276</v>
+        <v>267</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Split out gocator_ functions so they are callable from Java and Python directly
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{551D77CB-0CD7-4385-9471-A6F821680DF5}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070362F9-EB6F-4838-9C03-BCEE3FE57FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44805" yWindow="1065" windowWidth="30420" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44595" yWindow="1725" windowWidth="30420" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="736" uniqueCount="278">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="279">
   <si>
     <t>Statement</t>
   </si>
@@ -862,6 +862,9 @@
   </si>
   <si>
     <t>N/A</t>
+  </si>
+  <si>
+    <t>THESE NEED WORK IN JAVA AND PYTHON</t>
   </si>
 </sst>
 </file>
@@ -1047,6 +1050,15 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
+      <alignment vertical="top"/>
+    </xf>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
+      <alignment vertical="top" wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1058,15 +1070,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="1" xfId="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="2" xfId="2" applyFill="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="3" applyAlignment="1">
-      <alignment vertical="top" wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1312,30 +1315,30 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11" s="16" customFormat="1" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="32" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="32"/>
-      <c r="D1" s="32"/>
-      <c r="E1" s="31" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="34" t="s">
         <v>3</v>
       </c>
     </row>
     <row r="2" spans="1:11" s="16" customFormat="1" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="21" t="s">
         <v>4</v>
       </c>
@@ -1363,7 +1366,7 @@
       <c r="J2" s="21" t="s">
         <v>221</v>
       </c>
-      <c r="K2" s="31"/>
+      <c r="K2" s="34"/>
     </row>
     <row r="3" spans="1:11" ht="15.75" customHeight="1" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="14" t="s">
@@ -8194,7 +8197,7 @@
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="E90" sqref="E90:E97"/>
+      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8214,28 +8217,28 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:33" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="33" t="s">
+      <c r="B1" s="36" t="s">
         <v>208</v>
       </c>
-      <c r="C1" s="31" t="s">
+      <c r="C1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31"/>
-      <c r="F1" s="31" t="s">
+      <c r="D1" s="34"/>
+      <c r="E1" s="34"/>
+      <c r="F1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31"/>
-      <c r="J1" s="31" t="s">
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34"/>
+      <c r="J1" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="K1" s="31"/>
-      <c r="L1" s="31" t="s">
+      <c r="K1" s="34"/>
+      <c r="L1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="M1" s="1"/>
@@ -8261,8 +8264,8 @@
       <c r="AG1" s="1"/>
     </row>
     <row r="2" spans="1:33" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
-      <c r="B2" s="34"/>
+      <c r="A2" s="34"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="17" t="s">
         <v>4</v>
       </c>
@@ -8290,7 +8293,7 @@
       <c r="K2" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="L2" s="31"/>
+      <c r="L2" s="34"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
       <c r="O2" s="1"/>
@@ -8337,8 +8340,12 @@
       <c r="C4" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D4" s="10"/>
-      <c r="E4" s="10"/>
+      <c r="D4" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E4" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F4" s="10"/>
       <c r="G4" s="10"/>
       <c r="H4" s="10"/>
@@ -8384,7 +8391,9 @@
       <c r="C7" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D7" s="10"/>
+      <c r="D7" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E7" s="10" t="s">
         <v>11</v>
       </c>
@@ -8405,7 +8414,9 @@
       <c r="C8" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D8" s="10"/>
+      <c r="D8" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E8" s="10" t="s">
         <v>11</v>
       </c>
@@ -8426,7 +8437,9 @@
       <c r="C9" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D9" s="10"/>
+      <c r="D9" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E9" s="10" t="s">
         <v>11</v>
       </c>
@@ -8461,7 +8474,7 @@
       <c r="G11" s="27"/>
       <c r="H11" s="27"/>
       <c r="I11" s="27"/>
-      <c r="J11" s="36"/>
+      <c r="J11" s="32"/>
       <c r="K11" s="14"/>
       <c r="L11" s="14"/>
     </row>
@@ -8473,7 +8486,9 @@
       <c r="C12" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D12" s="10"/>
+      <c r="D12" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E12" s="10" t="s">
         <v>11</v>
       </c>
@@ -8482,6 +8497,9 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="22"/>
+      <c r="L12" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
@@ -8489,8 +8507,10 @@
       </c>
       <c r="B13" s="4"/>
       <c r="C13" s="4"/>
-      <c r="D13" s="4"/>
       <c r="J13" s="22"/>
+      <c r="L13" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
@@ -8508,6 +8528,9 @@
       <c r="I14" s="10"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
+      <c r="L14" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -8517,7 +8540,9 @@
       <c r="C15" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D15" s="10"/>
+      <c r="D15" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E15" s="10" t="s">
         <v>11</v>
       </c>
@@ -8527,6 +8552,9 @@
       <c r="I15" s="10"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
+      <c r="L15" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
@@ -8544,6 +8572,9 @@
       <c r="I16" s="9"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
+      <c r="L16" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
@@ -8561,6 +8592,9 @@
       <c r="I17" s="10"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
+      <c r="L17" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
@@ -8578,6 +8612,9 @@
       <c r="I18" s="10"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
+      <c r="L18" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
@@ -8587,7 +8624,9 @@
       <c r="C19" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D19" s="10"/>
+      <c r="D19" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E19" s="10" t="s">
         <v>11</v>
       </c>
@@ -8597,6 +8636,9 @@
       <c r="I19" s="10"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
+      <c r="L19" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
@@ -8606,7 +8648,9 @@
       <c r="C20" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D20" s="10"/>
+      <c r="D20" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E20" s="10" t="s">
         <v>11</v>
       </c>
@@ -8616,6 +8660,9 @@
       <c r="I20" s="10"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
+      <c r="L20" t="s">
+        <v>278</v>
+      </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="13" t="s">
@@ -8627,7 +8674,9 @@
       <c r="C21" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D21" s="10"/>
+      <c r="D21" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E21" s="10" t="s">
         <v>11</v>
       </c>
@@ -8676,7 +8725,9 @@
       <c r="C24" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D24" s="10"/>
+      <c r="D24" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E24" s="10" t="s">
         <v>11</v>
       </c>
@@ -8697,7 +8748,9 @@
       <c r="C25" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D25" s="10"/>
+      <c r="D25" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E25" s="10" t="s">
         <v>11</v>
       </c>
@@ -8718,7 +8771,9 @@
       <c r="C26" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D26" s="10"/>
+      <c r="D26" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E26" s="10" t="s">
         <v>11</v>
       </c>
@@ -8751,7 +8806,9 @@
       <c r="C28" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D28" s="10"/>
+      <c r="D28" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E28" s="10" t="s">
         <v>11</v>
       </c>
@@ -8772,7 +8829,9 @@
       <c r="C29" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D29" s="10"/>
+      <c r="D29" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E29" s="10" t="s">
         <v>11</v>
       </c>
@@ -8793,7 +8852,9 @@
       <c r="C30" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D30" s="10"/>
+      <c r="D30" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E30" s="10" t="s">
         <v>11</v>
       </c>
@@ -8826,7 +8887,9 @@
       <c r="C32" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D32" s="10"/>
+      <c r="D32" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E32" s="10" t="s">
         <v>11</v>
       </c>
@@ -8847,7 +8910,9 @@
       <c r="C33" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D33" s="10"/>
+      <c r="D33" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E33" s="10" t="s">
         <v>11</v>
       </c>
@@ -8880,7 +8945,9 @@
       <c r="C35" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D35" s="10"/>
+      <c r="D35" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E35" s="10" t="s">
         <v>11</v>
       </c>
@@ -8901,7 +8968,9 @@
       <c r="C36" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D36" s="10"/>
+      <c r="D36" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E36" s="10" t="s">
         <v>11</v>
       </c>
@@ -8922,7 +8991,9 @@
       <c r="C37" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D37" s="10"/>
+      <c r="D37" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E37" s="10" t="s">
         <v>11</v>
       </c>
@@ -8971,7 +9042,9 @@
       <c r="C40" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D40" s="10"/>
+      <c r="D40" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E40" s="10" t="s">
         <v>11</v>
       </c>
@@ -8992,7 +9065,9 @@
       <c r="C41" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D41" s="10"/>
+      <c r="D41" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E41" s="10" t="s">
         <v>11</v>
       </c>
@@ -9013,7 +9088,9 @@
       <c r="C42" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D42" s="10"/>
+      <c r="D42" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E42" s="10" t="s">
         <v>11</v>
       </c>
@@ -9034,7 +9111,9 @@
       <c r="C43" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D43" s="10"/>
+      <c r="D43" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E43" s="10" t="s">
         <v>11</v>
       </c>
@@ -9055,7 +9134,9 @@
       <c r="C44" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D44" s="10"/>
+      <c r="D44" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E44" s="10" t="s">
         <v>11</v>
       </c>
@@ -9102,7 +9183,9 @@
       <c r="C47" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D47" s="10"/>
+      <c r="D47" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E47" s="10" t="s">
         <v>11</v>
       </c>
@@ -9122,7 +9205,9 @@
       <c r="C48" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D48" s="10"/>
+      <c r="D48" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E48" s="10" t="s">
         <v>11</v>
       </c>
@@ -9142,7 +9227,9 @@
       <c r="C49" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D49" s="10"/>
+      <c r="D49" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E49" s="10" t="s">
         <v>11</v>
       </c>
@@ -9162,7 +9249,9 @@
       <c r="C50" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D50" s="10"/>
+      <c r="D50" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E50" s="10" t="s">
         <v>11</v>
       </c>
@@ -9182,7 +9271,9 @@
       <c r="C51" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D51" s="10"/>
+      <c r="D51" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E51" s="10" t="s">
         <v>11</v>
       </c>
@@ -9201,7 +9292,9 @@
       <c r="C52" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D52" s="10"/>
+      <c r="D52" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E52" s="10" t="s">
         <v>11</v>
       </c>
@@ -9247,7 +9340,9 @@
       <c r="C55" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D55" s="10"/>
+      <c r="D55" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E55" s="10" t="s">
         <v>11</v>
       </c>
@@ -9267,7 +9362,9 @@
       <c r="C56" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D56" s="10"/>
+      <c r="D56" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E56" s="10" t="s">
         <v>11</v>
       </c>
@@ -9287,7 +9384,9 @@
       <c r="C57" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D57" s="10"/>
+      <c r="D57" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E57" s="10" t="s">
         <v>11</v>
       </c>
@@ -9307,7 +9406,9 @@
       <c r="C58" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D58" s="10"/>
+      <c r="D58" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E58" s="10" t="s">
         <v>11</v>
       </c>
@@ -9327,7 +9428,9 @@
       <c r="C59" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D59" s="10"/>
+      <c r="D59" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E59" s="10" t="s">
         <v>11</v>
       </c>
@@ -9346,7 +9449,9 @@
       <c r="C60" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D60" s="10"/>
+      <c r="D60" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E60" s="10" t="s">
         <v>11</v>
       </c>
@@ -9914,7 +10019,7 @@
       <c r="L89" s="14"/>
     </row>
     <row r="90" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A90" s="37" t="s">
+      <c r="A90" s="33" t="s">
         <v>156</v>
       </c>
       <c r="B90" s="8" t="s">
@@ -9923,7 +10028,9 @@
       <c r="C90" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D90" s="10"/>
+      <c r="D90" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E90" s="10" t="s">
         <v>11</v>
       </c>
@@ -9935,7 +10042,7 @@
       <c r="I90" s="10"/>
     </row>
     <row r="91" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A91" s="37" t="s">
+      <c r="A91" s="33" t="s">
         <v>158</v>
       </c>
       <c r="B91" s="8" t="s">
@@ -9944,7 +10051,9 @@
       <c r="C91" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D91" s="10"/>
+      <c r="D91" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E91" s="10" t="s">
         <v>11</v>
       </c>
@@ -9956,7 +10065,7 @@
       <c r="I91" s="10"/>
     </row>
     <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A92" s="37" t="s">
+      <c r="A92" s="33" t="s">
         <v>160</v>
       </c>
       <c r="B92" s="8" t="s">
@@ -9965,7 +10074,9 @@
       <c r="C92" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D92" s="10"/>
+      <c r="D92" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E92" s="10" t="s">
         <v>11</v>
       </c>
@@ -9977,7 +10088,7 @@
       <c r="I92" s="10"/>
     </row>
     <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A93" s="37" t="s">
+      <c r="A93" s="33" t="s">
         <v>162</v>
       </c>
       <c r="B93" s="8" t="s">
@@ -9986,7 +10097,9 @@
       <c r="C93" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D93" s="10"/>
+      <c r="D93" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E93" s="10" t="s">
         <v>11</v>
       </c>
@@ -9998,7 +10111,7 @@
       <c r="I93" s="10"/>
     </row>
     <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A94" s="37" t="s">
+      <c r="A94" s="33" t="s">
         <v>164</v>
       </c>
       <c r="B94" s="8" t="s">
@@ -10007,7 +10120,9 @@
       <c r="C94" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D94" s="10"/>
+      <c r="D94" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E94" s="10" t="s">
         <v>11</v>
       </c>
@@ -10019,7 +10134,7 @@
       <c r="I94" s="10"/>
     </row>
     <row r="95" spans="1:12" ht="30" x14ac:dyDescent="0.2">
-      <c r="A95" s="37" t="s">
+      <c r="A95" s="33" t="s">
         <v>166</v>
       </c>
       <c r="B95" s="8" t="s">
@@ -10028,7 +10143,9 @@
       <c r="C95" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D95" s="10"/>
+      <c r="D95" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E95" s="10" t="s">
         <v>11</v>
       </c>
@@ -10040,7 +10157,7 @@
       <c r="I95" s="10"/>
     </row>
     <row r="96" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A96" s="37" t="s">
+      <c r="A96" s="33" t="s">
         <v>168</v>
       </c>
       <c r="B96" s="8" t="s">
@@ -10049,7 +10166,9 @@
       <c r="C96" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D96" s="10"/>
+      <c r="D96" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E96" s="10" t="s">
         <v>11</v>
       </c>
@@ -10070,7 +10189,9 @@
       <c r="C97" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D97" s="10"/>
+      <c r="D97" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E97" s="10" t="s">
         <v>11</v>
       </c>
@@ -10108,7 +10229,7 @@
       <c r="L99" s="14"/>
     </row>
     <row r="100" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="37" t="s">
+      <c r="A100" s="33" t="s">
         <v>275</v>
       </c>
       <c r="B100" s="8" t="s">
@@ -10117,7 +10238,9 @@
       <c r="C100" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D100" s="10"/>
+      <c r="D100" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E100" s="10" t="s">
         <v>11</v>
       </c>
@@ -10139,7 +10262,9 @@
       <c r="C101" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D101" s="10"/>
+      <c r="D101" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E101" s="10" t="s">
         <v>11</v>
       </c>
@@ -10161,7 +10286,9 @@
       <c r="C102" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D102" s="10"/>
+      <c r="D102" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E102" s="10" t="s">
         <v>11</v>
       </c>
@@ -10183,7 +10310,9 @@
       <c r="C103" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D103" s="10"/>
+      <c r="D103" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E103" s="10" t="s">
         <v>11</v>
       </c>
@@ -10205,7 +10334,9 @@
       <c r="C104" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D104" s="10"/>
+      <c r="D104" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E104" s="10" t="s">
         <v>11</v>
       </c>
@@ -10227,7 +10358,9 @@
       <c r="C105" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D105" s="10"/>
+      <c r="D105" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E105" s="10" t="s">
         <v>11</v>
       </c>
@@ -10249,7 +10382,9 @@
       <c r="C106" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D106" s="10"/>
+      <c r="D106" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E106" s="10" t="s">
         <v>11</v>
       </c>
@@ -10271,7 +10406,9 @@
       <c r="C107" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D107" s="10"/>
+      <c r="D107" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E107" s="10" t="s">
         <v>11</v>
       </c>
@@ -10293,7 +10430,9 @@
       <c r="C108" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D108" s="10"/>
+      <c r="D108" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E108" s="10" t="s">
         <v>11</v>
       </c>
@@ -10315,7 +10454,9 @@
       <c r="C109" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D109" s="10"/>
+      <c r="D109" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E109" s="10" t="s">
         <v>11</v>
       </c>
@@ -10337,7 +10478,9 @@
       <c r="C110" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D110" s="10"/>
+      <c r="D110" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E110" s="10" t="s">
         <v>11</v>
       </c>
@@ -10359,7 +10502,9 @@
       <c r="C111" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D111" s="10"/>
+      <c r="D111" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E111" s="10" t="s">
         <v>11</v>
       </c>
@@ -10381,7 +10526,9 @@
       <c r="C112" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D112" s="10"/>
+      <c r="D112" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="E112" s="10" t="s">
         <v>11</v>
       </c>
@@ -20055,7 +20202,7 @@
   <sheetViews>
     <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H23" sqref="H23"/>
+      <selection pane="bottomLeft" activeCell="F23" sqref="F23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -20074,25 +20221,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:32" ht="16.5" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A1" s="31" t="s">
+      <c r="A1" s="34" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="31" t="s">
+      <c r="B1" s="34" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="31"/>
-      <c r="D1" s="31"/>
-      <c r="E1" s="31" t="s">
+      <c r="C1" s="34"/>
+      <c r="D1" s="34"/>
+      <c r="E1" s="34" t="s">
         <v>2</v>
       </c>
-      <c r="F1" s="31"/>
-      <c r="G1" s="31"/>
-      <c r="H1" s="31"/>
-      <c r="I1" s="31" t="s">
+      <c r="F1" s="34"/>
+      <c r="G1" s="34"/>
+      <c r="H1" s="34"/>
+      <c r="I1" s="34" t="s">
         <v>211</v>
       </c>
-      <c r="J1" s="31"/>
-      <c r="K1" s="31" t="s">
+      <c r="J1" s="34"/>
+      <c r="K1" s="34" t="s">
         <v>3</v>
       </c>
       <c r="L1" s="1"/>
@@ -20118,7 +20265,7 @@
       <c r="AF1" s="1"/>
     </row>
     <row r="2" spans="1:32" ht="33" thickTop="1" thickBot="1" x14ac:dyDescent="0.25">
-      <c r="A2" s="31"/>
+      <c r="A2" s="34"/>
       <c r="B2" s="17" t="s">
         <v>4</v>
       </c>
@@ -20146,7 +20293,7 @@
       <c r="J2" s="29" t="s">
         <v>221</v>
       </c>
-      <c r="K2" s="31"/>
+      <c r="K2" s="34"/>
       <c r="L2" s="1"/>
       <c r="M2" s="1"/>
       <c r="N2" s="1"/>
@@ -20212,8 +20359,12 @@
       <c r="B4" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C4" s="4"/>
-      <c r="D4" s="4"/>
+      <c r="C4" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D4" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I4" s="13"/>
       <c r="J4" s="13"/>
     </row>
@@ -20224,8 +20375,12 @@
       <c r="B5" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C5" s="4"/>
-      <c r="D5" s="4"/>
+      <c r="C5" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D5" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I5" s="13"/>
       <c r="J5" s="13"/>
     </row>
@@ -20236,8 +20391,12 @@
       <c r="B6" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C6" s="4"/>
-      <c r="D6" s="4"/>
+      <c r="C6" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D6" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I6" s="16"/>
       <c r="J6" s="16"/>
       <c r="K6" s="12"/>
@@ -20249,8 +20408,12 @@
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C7" s="4"/>
-      <c r="D7" s="4"/>
+      <c r="C7" s="4" t="s">
+        <v>277</v>
+      </c>
+      <c r="D7" s="4" t="s">
+        <v>277</v>
+      </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
@@ -20261,8 +20424,12 @@
       <c r="B8" s="3" t="s">
         <v>11</v>
       </c>
-      <c r="C8" s="4"/>
-      <c r="D8" s="4"/>
+      <c r="C8" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="D8" s="4" t="s">
+        <v>11</v>
+      </c>
       <c r="I8" s="16"/>
       <c r="J8" s="16"/>
     </row>
@@ -20278,9 +20445,9 @@
       <c r="A10" s="14" t="s">
         <v>210</v>
       </c>
-      <c r="B10" s="35"/>
-      <c r="C10" s="35"/>
-      <c r="D10" s="35"/>
+      <c r="B10" s="31"/>
+      <c r="C10" s="31"/>
+      <c r="D10" s="31"/>
       <c r="E10" s="14"/>
       <c r="F10" s="14"/>
       <c r="G10" s="14"/>

</xml_diff>

<commit_message>
Finished up universal support for all commands in Java and Python
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{070362F9-EB6F-4838-9C03-BCEE3FE57FCB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EEABE3-A180-4A3A-A025-C0D8121DD17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44595" yWindow="1725" windowWidth="30420" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44595" yWindow="1725" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="279">
   <si>
     <t>Statement</t>
   </si>
@@ -169,9 +169,6 @@
   </si>
   <si>
     <t>move_linear(pos_name)</t>
-  </si>
-  <si>
-    <t>move_relative(x,y) DEPRECATED for movel_incr_part</t>
   </si>
   <si>
     <t>move_tool_home()</t>
@@ -864,7 +861,10 @@
     <t>N/A</t>
   </si>
   <si>
-    <t>THESE NEED WORK IN JAVA AND PYTHON</t>
+    <t>???</t>
+  </si>
+  <si>
+    <t>DEPRECATE FOR exec_lescript???</t>
   </si>
 </sst>
 </file>
@@ -1294,9 +1294,9 @@
   </sheetPr>
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="I2" sqref="I1:J1048576"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1330,7 +1330,7 @@
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
       <c r="I1" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J1" s="34"/>
       <c r="K1" s="34" t="s">
@@ -1361,10 +1361,10 @@
         <v>10</v>
       </c>
       <c r="I2" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J2" s="21" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K2" s="34"/>
     </row>
@@ -1400,7 +1400,7 @@
         <v>11</v>
       </c>
       <c r="I4" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J4" s="13"/>
     </row>
@@ -1421,7 +1421,7 @@
         <v>11</v>
       </c>
       <c r="I5" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J5" s="13"/>
     </row>
@@ -1442,13 +1442,13 @@
         <v>11</v>
       </c>
       <c r="I6" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J6" s="13"/>
     </row>
     <row r="7" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="13" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B7" s="10" t="s">
         <v>11</v>
@@ -1463,13 +1463,13 @@
         <v>11</v>
       </c>
       <c r="I7" s="13" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="J7" s="13"/>
     </row>
     <row r="8" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="13" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="B8" s="10" t="s">
         <v>11</v>
@@ -1484,18 +1484,18 @@
         <v>11</v>
       </c>
       <c r="I8" s="22" t="s">
+        <v>266</v>
+      </c>
+      <c r="J8" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="J8" s="23" t="s">
-        <v>268</v>
-      </c>
       <c r="K8" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B9" s="10" t="s">
         <v>11</v>
@@ -1510,18 +1510,18 @@
         <v>11</v>
       </c>
       <c r="I9" s="22" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="J9" s="23" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="K9" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B10" s="10" t="s">
         <v>11</v>
@@ -1536,18 +1536,18 @@
         <v>11</v>
       </c>
       <c r="I10" s="22" t="s">
+        <v>214</v>
+      </c>
+      <c r="J10" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="J10" s="23" t="s">
-        <v>216</v>
-      </c>
       <c r="K10" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="B11" s="10" t="s">
         <v>11</v>
@@ -1562,15 +1562,15 @@
         <v>11</v>
       </c>
       <c r="I11" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K11" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="12" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="13" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B12" s="10" t="s">
         <v>11</v>
@@ -1585,15 +1585,15 @@
         <v>11</v>
       </c>
       <c r="I12" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K12" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="13" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B13" s="10" t="s">
         <v>11</v>
@@ -1608,10 +1608,10 @@
         <v>11</v>
       </c>
       <c r="I13" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="K13" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="14" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
@@ -1637,42 +1637,53 @@
     </row>
     <row r="16" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B16" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C16" s="10"/>
-      <c r="D16" s="10"/>
+      <c r="C16" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D16" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="E16" s="25" t="s">
         <v>11</v>
       </c>
       <c r="I16" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="17" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B17" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="C17" s="10"/>
-      <c r="D17" s="10"/>
+      <c r="C17" s="10" t="s">
+        <v>277</v>
+      </c>
+      <c r="D17" s="10" t="s">
+        <v>277</v>
+      </c>
       <c r="E17" s="25" t="s">
         <v>11</v>
       </c>
       <c r="I17" s="13" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="J17" s="13" t="s">
-        <v>222</v>
+        <v>221</v>
+      </c>
+      <c r="K17" s="13" t="s">
+        <v>278</v>
       </c>
     </row>
     <row r="18" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B18" s="10" t="s">
         <v>11</v>
@@ -1683,7 +1694,7 @@
         <v>11</v>
       </c>
       <c r="I18" s="13" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
     </row>
     <row r="19" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1703,7 +1714,7 @@
         <v>11</v>
       </c>
       <c r="I19" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="20" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1723,7 +1734,7 @@
         <v>11</v>
       </c>
       <c r="I20" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="21" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1743,7 +1754,7 @@
         <v>11</v>
       </c>
       <c r="I21" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="22" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1763,12 +1774,12 @@
         <v>11</v>
       </c>
       <c r="I22" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="23" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="13" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B23" s="10" t="s">
         <v>11</v>
@@ -1779,12 +1790,12 @@
         <v>11</v>
       </c>
       <c r="I23" s="22" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
     </row>
     <row r="24" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B24" s="10"/>
       <c r="C24" s="10" t="s">
@@ -1797,12 +1808,12 @@
         <v>11</v>
       </c>
       <c r="I24" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="25" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B25" s="10"/>
       <c r="C25" s="10" t="s">
@@ -1815,12 +1826,12 @@
         <v>11</v>
       </c>
       <c r="I25" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="26" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="13" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B26" s="10"/>
       <c r="C26" s="10" t="s">
@@ -1833,7 +1844,7 @@
         <v>11</v>
       </c>
       <c r="I26" s="22" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
     </row>
     <row r="27" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1844,7 +1855,7 @@
     </row>
     <row r="28" spans="1:11" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A28" s="15" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B28" s="27"/>
       <c r="C28" s="27"/>
@@ -1859,7 +1870,7 @@
     </row>
     <row r="29" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B29" s="10" t="s">
         <v>11</v>
@@ -1874,12 +1885,12 @@
         <v>11</v>
       </c>
       <c r="I29" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="30" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="13" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B30" s="10" t="s">
         <v>11</v>
@@ -1894,7 +1905,7 @@
         <v>11</v>
       </c>
       <c r="I30" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="31" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1914,7 +1925,7 @@
         <v>11</v>
       </c>
       <c r="I31" s="13" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
     </row>
     <row r="32" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -1927,7 +1938,7 @@
     </row>
     <row r="33" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A33" s="15" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B33" s="27"/>
       <c r="C33" s="27"/>
@@ -1942,7 +1953,7 @@
     </row>
     <row r="34" spans="1:32" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A34" s="13" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B34" s="10" t="s">
         <v>11</v>
@@ -1957,12 +1968,12 @@
         <v>11</v>
       </c>
       <c r="I34" s="13" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="35" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B35" s="10" t="s">
         <v>11</v>
@@ -1977,7 +1988,7 @@
         <v>11</v>
       </c>
       <c r="I35" s="22" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
     </row>
     <row r="36" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2004,7 +2015,7 @@
     </row>
     <row r="38" spans="1:32" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A38" s="13" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B38" s="10" t="s">
         <v>11</v>
@@ -2019,12 +2030,12 @@
         <v>11</v>
       </c>
       <c r="I38" s="13" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
     </row>
     <row r="39" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="13" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B39" s="10" t="s">
         <v>11</v>
@@ -2039,7 +2050,7 @@
         <v>11</v>
       </c>
       <c r="I39" s="13" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
     </row>
     <row r="40" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2059,7 +2070,7 @@
         <v>11</v>
       </c>
       <c r="I40" s="13" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
     </row>
     <row r="41" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2079,7 +2090,7 @@
         <v>11</v>
       </c>
       <c r="I41" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="42" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2099,7 +2110,7 @@
         <v>11</v>
       </c>
       <c r="I42" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="43" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2122,7 +2133,7 @@
       <c r="G43" s="7"/>
       <c r="H43" s="7"/>
       <c r="I43" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="J43" s="7"/>
       <c r="K43" s="7"/>
@@ -2161,7 +2172,7 @@
         <v>11</v>
       </c>
       <c r="I44" s="13" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
     </row>
     <row r="45" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2181,7 +2192,7 @@
         <v>11</v>
       </c>
       <c r="I45" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="46" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2201,7 +2212,7 @@
         <v>11</v>
       </c>
       <c r="I46" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="47" spans="1:32" ht="15" x14ac:dyDescent="0.2">
@@ -2221,12 +2232,12 @@
         <v>11</v>
       </c>
       <c r="I47" s="13" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
     </row>
     <row r="48" spans="1:32" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="13" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B48" s="10" t="s">
         <v>11</v>
@@ -2241,12 +2252,12 @@
         <v>11</v>
       </c>
       <c r="I48" s="13" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
     </row>
     <row r="49" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B49" s="10" t="s">
         <v>11</v>
@@ -2257,12 +2268,12 @@
         <v>11</v>
       </c>
       <c r="I49" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="50" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="13" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B50" s="10"/>
       <c r="C50" s="10" t="s">
@@ -2275,7 +2286,7 @@
         <v>11</v>
       </c>
       <c r="I50" s="13" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
     </row>
     <row r="51" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -2301,7 +2312,7 @@
     </row>
     <row r="53" spans="1:11" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A53" s="13" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B53" s="10" t="s">
         <v>11</v>
@@ -2316,15 +2327,15 @@
         <v>11</v>
       </c>
       <c r="I53" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K53" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="54" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="13" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B54" s="10" t="s">
         <v>11</v>
@@ -2339,15 +2350,15 @@
         <v>11</v>
       </c>
       <c r="I54" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K54" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="55" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B55" s="10" t="s">
         <v>11</v>
@@ -2362,15 +2373,15 @@
         <v>11</v>
       </c>
       <c r="I55" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K55" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="56" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B56" s="10" t="s">
         <v>11</v>
@@ -2385,10 +2396,10 @@
         <v>11</v>
       </c>
       <c r="I56" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K56" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="57" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2408,10 +2419,10 @@
         <v>11</v>
       </c>
       <c r="I57" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K57" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="58" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
@@ -2431,10 +2442,10 @@
         <v>11</v>
       </c>
       <c r="I58" s="22" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="K58" s="22" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
     </row>
     <row r="59" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2460,7 +2471,7 @@
     </row>
     <row r="61" spans="1:11" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A61" s="13" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B61" s="10" t="s">
         <v>11</v>
@@ -2471,7 +2482,7 @@
         <v>11</v>
       </c>
       <c r="I61" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="62" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -2487,7 +2498,7 @@
         <v>11</v>
       </c>
       <c r="I62" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="63" spans="1:11" ht="15" x14ac:dyDescent="0.2">
@@ -2503,12 +2514,12 @@
         <v>11</v>
       </c>
       <c r="I63" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="64" spans="1:11" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B64" s="10" t="s">
         <v>11</v>
@@ -2519,7 +2530,7 @@
         <v>11</v>
       </c>
       <c r="I64" s="13" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
     </row>
     <row r="65" spans="1:11" ht="15" x14ac:dyDescent="0.25">
@@ -2545,7 +2556,7 @@
     </row>
     <row r="67" spans="1:11" thickTop="1" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="B67" s="10" t="s">
         <v>11</v>
@@ -8193,11 +8204,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AG1076"/>
+  <dimension ref="A1:AG1075"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H16" sqref="H16"/>
+      <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -8221,7 +8232,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="36" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="C1" s="34" t="s">
         <v>1</v>
@@ -8235,7 +8246,7 @@
       <c r="H1" s="34"/>
       <c r="I1" s="34"/>
       <c r="J1" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="K1" s="34"/>
       <c r="L1" s="34" t="s">
@@ -8288,10 +8299,10 @@
         <v>10</v>
       </c>
       <c r="J2" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="K2" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="L2" s="34"/>
       <c r="M2" s="1"/>
@@ -8497,20 +8508,22 @@
       <c r="H12" s="10"/>
       <c r="I12" s="10"/>
       <c r="J12" s="22"/>
-      <c r="L12" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="13" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="13" t="s">
         <v>16</v>
       </c>
       <c r="B13" s="4"/>
-      <c r="C13" s="4"/>
+      <c r="C13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D13" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E13" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="J13" s="22"/>
-      <c r="L13" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="14" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="13" t="s">
@@ -8520,17 +8533,18 @@
       <c r="C14" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D14" s="10"/>
-      <c r="E14" s="10"/>
+      <c r="D14" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E14" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F14" s="10"/>
       <c r="G14" s="10"/>
       <c r="H14" s="10"/>
       <c r="I14" s="10"/>
       <c r="J14" s="16"/>
       <c r="K14" s="16"/>
-      <c r="L14" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="15" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="13" t="s">
@@ -8552,9 +8566,6 @@
       <c r="I15" s="10"/>
       <c r="J15" s="16"/>
       <c r="K15" s="16"/>
-      <c r="L15" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="16" spans="1:33" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="13" t="s">
@@ -8564,17 +8575,18 @@
       <c r="C16" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D16" s="10"/>
-      <c r="E16" s="10"/>
-      <c r="F16" s="9"/>
-      <c r="G16" s="9"/>
-      <c r="H16" s="9"/>
-      <c r="I16" s="9"/>
+      <c r="D16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E16" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F16" s="10"/>
+      <c r="G16" s="10"/>
+      <c r="H16" s="10"/>
+      <c r="I16" s="10"/>
       <c r="J16" s="16"/>
       <c r="K16" s="16"/>
-      <c r="L16" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="17" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="13" t="s">
@@ -8584,17 +8596,18 @@
       <c r="C17" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D17" s="10"/>
-      <c r="E17" s="10"/>
+      <c r="D17" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E17" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F17" s="10"/>
       <c r="G17" s="10"/>
       <c r="H17" s="10"/>
       <c r="I17" s="10"/>
       <c r="J17" s="16"/>
       <c r="K17" s="16"/>
-      <c r="L17" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="18" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="13" t="s">
@@ -8604,17 +8617,18 @@
       <c r="C18" s="9" t="s">
         <v>11</v>
       </c>
-      <c r="D18" s="10"/>
-      <c r="E18" s="10"/>
+      <c r="D18" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E18" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F18" s="10"/>
       <c r="G18" s="10"/>
       <c r="H18" s="10"/>
       <c r="I18" s="10"/>
       <c r="J18" s="16"/>
       <c r="K18" s="16"/>
-      <c r="L18" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="19" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="13" t="s">
@@ -8636,16 +8650,15 @@
       <c r="I19" s="10"/>
       <c r="J19" s="16"/>
       <c r="K19" s="16"/>
-      <c r="L19" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="20" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="13" t="s">
         <v>53</v>
       </c>
-      <c r="B20" s="8"/>
-      <c r="C20" s="9" t="s">
+      <c r="B20" s="8" t="s">
+        <v>54</v>
+      </c>
+      <c r="C20" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D20" s="10" t="s">
@@ -8660,26 +8673,12 @@
       <c r="I20" s="10"/>
       <c r="J20" s="16"/>
       <c r="K20" s="16"/>
-      <c r="L20" t="s">
-        <v>278</v>
-      </c>
     </row>
     <row r="21" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="13" t="s">
-        <v>54</v>
-      </c>
-      <c r="B21" s="8" t="s">
-        <v>55</v>
-      </c>
-      <c r="C21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D21" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E21" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B21" s="8"/>
+      <c r="C21" s="9"/>
+      <c r="D21" s="10"/>
+      <c r="E21" s="10"/>
       <c r="F21" s="10"/>
       <c r="G21" s="10"/>
       <c r="H21" s="10"/>
@@ -8687,40 +8686,51 @@
       <c r="J21" s="16"/>
       <c r="K21" s="16"/>
     </row>
-    <row r="22" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B22" s="8"/>
-      <c r="C22" s="9"/>
-      <c r="D22" s="10"/>
-      <c r="E22" s="10"/>
-      <c r="F22" s="10"/>
-      <c r="G22" s="10"/>
-      <c r="H22" s="10"/>
-      <c r="I22" s="10"/>
-      <c r="J22" s="16"/>
-      <c r="K22" s="16"/>
-    </row>
-    <row r="23" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A23" s="15" t="s">
+    <row r="22" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A22" s="15" t="s">
+        <v>55</v>
+      </c>
+      <c r="B22" s="27"/>
+      <c r="C22" s="27"/>
+      <c r="D22" s="27"/>
+      <c r="E22" s="27"/>
+      <c r="F22" s="27"/>
+      <c r="G22" s="27"/>
+      <c r="H22" s="27"/>
+      <c r="I22" s="27"/>
+      <c r="J22" s="19"/>
+      <c r="K22" s="19"/>
+      <c r="L22" s="14"/>
+    </row>
+    <row r="23" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A23" s="13" t="s">
         <v>56</v>
       </c>
-      <c r="B23" s="27"/>
-      <c r="C23" s="27"/>
-      <c r="D23" s="27"/>
-      <c r="E23" s="27"/>
-      <c r="F23" s="27"/>
-      <c r="G23" s="27"/>
-      <c r="H23" s="27"/>
-      <c r="I23" s="27"/>
-      <c r="J23" s="19"/>
-      <c r="K23" s="19"/>
-      <c r="L23" s="14"/>
-    </row>
-    <row r="24" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B23" s="8" t="s">
+        <v>57</v>
+      </c>
+      <c r="C23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E23" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F23" s="10"/>
+      <c r="G23" s="10"/>
+      <c r="H23" s="10"/>
+      <c r="I23" s="10"/>
+      <c r="J23" s="16"/>
+      <c r="K23" s="16"/>
+    </row>
+    <row r="24" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="13" t="s">
-        <v>57</v>
+        <v>58</v>
       </c>
       <c r="B24" s="8" t="s">
-        <v>58</v>
+        <v>59</v>
       </c>
       <c r="C24" s="10" t="s">
         <v>11</v>
@@ -8740,10 +8750,10 @@
     </row>
     <row r="25" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="13" t="s">
-        <v>59</v>
+        <v>60</v>
       </c>
       <c r="B25" s="8" t="s">
-        <v>60</v>
+        <v>61</v>
       </c>
       <c r="C25" s="10" t="s">
         <v>11</v>
@@ -8762,21 +8772,10 @@
       <c r="K25" s="16"/>
     </row>
     <row r="26" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="13" t="s">
-        <v>61</v>
-      </c>
-      <c r="B26" s="8" t="s">
-        <v>62</v>
-      </c>
-      <c r="C26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D26" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E26" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B26" s="8"/>
+      <c r="C26" s="9"/>
+      <c r="D26" s="10"/>
+      <c r="E26" s="10"/>
       <c r="F26" s="10"/>
       <c r="G26" s="10"/>
       <c r="H26" s="10"/>
@@ -8785,10 +8784,21 @@
       <c r="K26" s="16"/>
     </row>
     <row r="27" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B27" s="8"/>
-      <c r="C27" s="9"/>
-      <c r="D27" s="10"/>
-      <c r="E27" s="10"/>
+      <c r="A27" s="13" t="s">
+        <v>62</v>
+      </c>
+      <c r="B27" s="8" t="s">
+        <v>63</v>
+      </c>
+      <c r="C27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D27" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E27" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F27" s="10"/>
       <c r="G27" s="10"/>
       <c r="H27" s="10"/>
@@ -8798,10 +8808,10 @@
     </row>
     <row r="28" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="13" t="s">
-        <v>63</v>
+        <v>64</v>
       </c>
       <c r="B28" s="8" t="s">
-        <v>64</v>
+        <v>65</v>
       </c>
       <c r="C28" s="10" t="s">
         <v>11</v>
@@ -8821,10 +8831,10 @@
     </row>
     <row r="29" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="13" t="s">
-        <v>65</v>
+        <v>66</v>
       </c>
       <c r="B29" s="8" t="s">
-        <v>66</v>
+        <v>67</v>
       </c>
       <c r="C29" s="10" t="s">
         <v>11</v>
@@ -8843,21 +8853,10 @@
       <c r="K29" s="16"/>
     </row>
     <row r="30" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="13" t="s">
-        <v>67</v>
-      </c>
-      <c r="B30" s="8" t="s">
-        <v>68</v>
-      </c>
-      <c r="C30" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D30" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E30" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B30" s="8"/>
+      <c r="C30" s="9"/>
+      <c r="D30" s="10"/>
+      <c r="E30" s="10"/>
       <c r="F30" s="10"/>
       <c r="G30" s="10"/>
       <c r="H30" s="10"/>
@@ -8866,10 +8865,21 @@
       <c r="K30" s="16"/>
     </row>
     <row r="31" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B31" s="8"/>
-      <c r="C31" s="9"/>
-      <c r="D31" s="10"/>
-      <c r="E31" s="10"/>
+      <c r="A31" s="13" t="s">
+        <v>68</v>
+      </c>
+      <c r="B31" s="8" t="s">
+        <v>69</v>
+      </c>
+      <c r="C31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D31" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E31" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F31" s="10"/>
       <c r="G31" s="10"/>
       <c r="H31" s="10"/>
@@ -8879,10 +8889,10 @@
     </row>
     <row r="32" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="13" t="s">
-        <v>69</v>
+        <v>70</v>
       </c>
       <c r="B32" s="8" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C32" s="10" t="s">
         <v>11</v>
@@ -8901,21 +8911,10 @@
       <c r="K32" s="16"/>
     </row>
     <row r="33" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="13" t="s">
-        <v>71</v>
-      </c>
-      <c r="B33" s="8" t="s">
-        <v>72</v>
-      </c>
-      <c r="C33" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D33" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E33" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B33" s="8"/>
+      <c r="C33" s="9"/>
+      <c r="D33" s="10"/>
+      <c r="E33" s="10"/>
       <c r="F33" s="10"/>
       <c r="G33" s="10"/>
       <c r="H33" s="10"/>
@@ -8924,10 +8923,21 @@
       <c r="K33" s="16"/>
     </row>
     <row r="34" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B34" s="8"/>
-      <c r="C34" s="9"/>
-      <c r="D34" s="10"/>
-      <c r="E34" s="10"/>
+      <c r="A34" s="13" t="s">
+        <v>72</v>
+      </c>
+      <c r="B34" s="8" t="s">
+        <v>73</v>
+      </c>
+      <c r="C34" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D34" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E34" s="10" t="s">
+        <v>11</v>
+      </c>
       <c r="F34" s="10"/>
       <c r="G34" s="10"/>
       <c r="H34" s="10"/>
@@ -8937,10 +8947,10 @@
     </row>
     <row r="35" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="13" t="s">
-        <v>73</v>
+        <v>74</v>
       </c>
       <c r="B35" s="8" t="s">
-        <v>74</v>
+        <v>75</v>
       </c>
       <c r="C35" s="10" t="s">
         <v>11</v>
@@ -8960,10 +8970,10 @@
     </row>
     <row r="36" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="13" t="s">
-        <v>75</v>
+        <v>76</v>
       </c>
       <c r="B36" s="8" t="s">
-        <v>76</v>
+        <v>77</v>
       </c>
       <c r="C36" s="10" t="s">
         <v>11</v>
@@ -8982,21 +8992,10 @@
       <c r="K36" s="16"/>
     </row>
     <row r="37" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A37" s="13" t="s">
-        <v>77</v>
-      </c>
-      <c r="B37" s="8" t="s">
-        <v>78</v>
-      </c>
-      <c r="C37" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D37" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E37" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B37" s="11"/>
+      <c r="C37" s="9"/>
+      <c r="D37" s="10"/>
+      <c r="E37" s="10"/>
       <c r="F37" s="10"/>
       <c r="G37" s="10"/>
       <c r="H37" s="10"/>
@@ -9004,40 +9003,51 @@
       <c r="J37" s="16"/>
       <c r="K37" s="16"/>
     </row>
-    <row r="38" spans="1:12" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="B38" s="11"/>
-      <c r="C38" s="9"/>
-      <c r="D38" s="10"/>
-      <c r="E38" s="10"/>
-      <c r="F38" s="10"/>
-      <c r="G38" s="10"/>
-      <c r="H38" s="10"/>
-      <c r="I38" s="10"/>
-      <c r="J38" s="16"/>
-      <c r="K38" s="16"/>
-    </row>
-    <row r="39" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A39" s="15" t="s">
+    <row r="38" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A38" s="15" t="s">
+        <v>78</v>
+      </c>
+      <c r="B38" s="27"/>
+      <c r="C38" s="27"/>
+      <c r="D38" s="27"/>
+      <c r="E38" s="27"/>
+      <c r="F38" s="27"/>
+      <c r="G38" s="27"/>
+      <c r="H38" s="27"/>
+      <c r="I38" s="27"/>
+      <c r="J38" s="14"/>
+      <c r="K38" s="14"/>
+      <c r="L38" s="14"/>
+    </row>
+    <row r="39" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A39" s="13" t="s">
         <v>79</v>
       </c>
-      <c r="B39" s="27"/>
-      <c r="C39" s="27"/>
-      <c r="D39" s="27"/>
-      <c r="E39" s="27"/>
-      <c r="F39" s="27"/>
-      <c r="G39" s="27"/>
-      <c r="H39" s="27"/>
-      <c r="I39" s="27"/>
-      <c r="J39" s="14"/>
-      <c r="K39" s="14"/>
-      <c r="L39" s="14"/>
-    </row>
-    <row r="40" spans="1:12" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B39" s="8" t="s">
+        <v>80</v>
+      </c>
+      <c r="C39" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D39" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E39" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F39" s="10"/>
+      <c r="G39" s="10"/>
+      <c r="H39" s="10"/>
+      <c r="I39" s="10"/>
+      <c r="J39" s="16"/>
+      <c r="K39" s="16"/>
+    </row>
+    <row r="40" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="13" t="s">
-        <v>80</v>
+        <v>81</v>
       </c>
       <c r="B40" s="8" t="s">
-        <v>81</v>
+        <v>82</v>
       </c>
       <c r="C40" s="10" t="s">
         <v>11</v>
@@ -9057,10 +9067,10 @@
     </row>
     <row r="41" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="13" t="s">
-        <v>82</v>
+        <v>83</v>
       </c>
       <c r="B41" s="8" t="s">
-        <v>83</v>
+        <v>84</v>
       </c>
       <c r="C41" s="10" t="s">
         <v>11</v>
@@ -9080,10 +9090,10 @@
     </row>
     <row r="42" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="13" t="s">
-        <v>84</v>
+        <v>85</v>
       </c>
       <c r="B42" s="8" t="s">
-        <v>85</v>
+        <v>86</v>
       </c>
       <c r="C42" s="10" t="s">
         <v>11</v>
@@ -9098,15 +9108,15 @@
       <c r="G42" s="10"/>
       <c r="H42" s="10"/>
       <c r="I42" s="10"/>
-      <c r="J42" s="16"/>
-      <c r="K42" s="16"/>
+      <c r="J42" s="13"/>
+      <c r="K42" s="7"/>
     </row>
     <row r="43" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="13" t="s">
-        <v>86</v>
+        <v>87</v>
       </c>
       <c r="B43" s="8" t="s">
-        <v>87</v>
+        <v>88</v>
       </c>
       <c r="C43" s="10" t="s">
         <v>11</v>
@@ -9122,63 +9132,62 @@
       <c r="H43" s="10"/>
       <c r="I43" s="10"/>
       <c r="J43" s="13"/>
-      <c r="K43" s="7"/>
     </row>
     <row r="44" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="13" t="s">
-        <v>88</v>
-      </c>
-      <c r="B44" s="8" t="s">
-        <v>89</v>
-      </c>
-      <c r="C44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D44" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E44" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B44" s="8"/>
+      <c r="C44" s="9"/>
+      <c r="D44" s="10"/>
+      <c r="E44" s="10"/>
       <c r="F44" s="10"/>
       <c r="G44" s="10"/>
       <c r="H44" s="10"/>
       <c r="I44" s="10"/>
       <c r="J44" s="13"/>
     </row>
-    <row r="45" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B45" s="8"/>
-      <c r="C45" s="9"/>
-      <c r="D45" s="10"/>
-      <c r="E45" s="10"/>
-      <c r="F45" s="10"/>
-      <c r="G45" s="10"/>
-      <c r="H45" s="10"/>
-      <c r="I45" s="10"/>
-      <c r="J45" s="13"/>
-    </row>
-    <row r="46" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A46" s="15" t="s">
+    <row r="45" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A45" s="15" t="s">
+        <v>89</v>
+      </c>
+      <c r="B45" s="27"/>
+      <c r="C45" s="27"/>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27"/>
+      <c r="F45" s="27"/>
+      <c r="G45" s="27"/>
+      <c r="H45" s="27"/>
+      <c r="I45" s="27"/>
+      <c r="J45" s="14"/>
+      <c r="K45" s="14"/>
+      <c r="L45" s="14"/>
+    </row>
+    <row r="46" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A46" s="13" t="s">
         <v>90</v>
       </c>
-      <c r="B46" s="27"/>
-      <c r="C46" s="27"/>
-      <c r="D46" s="27"/>
-      <c r="E46" s="27"/>
-      <c r="F46" s="27"/>
-      <c r="G46" s="27"/>
-      <c r="H46" s="27"/>
-      <c r="I46" s="27"/>
-      <c r="J46" s="14"/>
-      <c r="K46" s="14"/>
-      <c r="L46" s="14"/>
-    </row>
-    <row r="47" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B46" s="8" t="s">
+        <v>91</v>
+      </c>
+      <c r="C46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E46" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F46" s="10"/>
+      <c r="G46" s="10"/>
+      <c r="H46" s="10"/>
+      <c r="I46" s="10"/>
+      <c r="J46" s="13"/>
+    </row>
+    <row r="47" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="13" t="s">
+        <v>92</v>
+      </c>
+      <c r="B47" s="8" t="s">
         <v>91</v>
-      </c>
-      <c r="B47" s="8" t="s">
-        <v>92</v>
       </c>
       <c r="C47" s="10" t="s">
         <v>11</v>
@@ -9200,7 +9209,7 @@
         <v>93</v>
       </c>
       <c r="B48" s="8" t="s">
-        <v>92</v>
+        <v>94</v>
       </c>
       <c r="C48" s="10" t="s">
         <v>11</v>
@@ -9219,10 +9228,10 @@
     </row>
     <row r="49" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="13" t="s">
+        <v>95</v>
+      </c>
+      <c r="B49" s="8" t="s">
         <v>94</v>
-      </c>
-      <c r="B49" s="8" t="s">
-        <v>95</v>
       </c>
       <c r="C49" s="10" t="s">
         <v>11</v>
@@ -9244,7 +9253,7 @@
         <v>96</v>
       </c>
       <c r="B50" s="8" t="s">
-        <v>95</v>
+        <v>97</v>
       </c>
       <c r="C50" s="10" t="s">
         <v>11</v>
@@ -9259,14 +9268,13 @@
       <c r="G50" s="10"/>
       <c r="H50" s="10"/>
       <c r="I50" s="10"/>
-      <c r="J50" s="13"/>
     </row>
     <row r="51" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="13" t="s">
-        <v>97</v>
+        <v>98</v>
       </c>
       <c r="B51" s="8" t="s">
-        <v>98</v>
+        <v>99</v>
       </c>
       <c r="C51" s="10" t="s">
         <v>11</v>
@@ -9283,56 +9291,57 @@
       <c r="I51" s="10"/>
     </row>
     <row r="52" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="13" t="s">
-        <v>99</v>
-      </c>
-      <c r="B52" s="8" t="s">
-        <v>100</v>
-      </c>
-      <c r="C52" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D52" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E52" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B52" s="11"/>
+      <c r="C52" s="10"/>
+      <c r="D52" s="10"/>
+      <c r="E52" s="10"/>
       <c r="F52" s="10"/>
       <c r="G52" s="10"/>
       <c r="H52" s="10"/>
       <c r="I52" s="10"/>
-    </row>
-    <row r="53" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B53" s="11"/>
-      <c r="C53" s="10"/>
-      <c r="D53" s="10"/>
-      <c r="E53" s="10"/>
-      <c r="F53" s="10"/>
-      <c r="G53" s="10"/>
-      <c r="H53" s="10"/>
-      <c r="I53" s="10"/>
-      <c r="J53" s="22"/>
-    </row>
-    <row r="54" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A54" s="15" t="s">
+      <c r="J52" s="22"/>
+    </row>
+    <row r="53" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A53" s="15" t="s">
+        <v>100</v>
+      </c>
+      <c r="B53" s="27"/>
+      <c r="C53" s="27"/>
+      <c r="D53" s="27"/>
+      <c r="E53" s="27"/>
+      <c r="F53" s="27"/>
+      <c r="G53" s="27"/>
+      <c r="H53" s="27"/>
+      <c r="I53" s="27"/>
+      <c r="J53" s="14"/>
+      <c r="K53" s="14"/>
+      <c r="L53" s="14"/>
+    </row>
+    <row r="54" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A54" s="13" t="s">
+        <v>273</v>
+      </c>
+      <c r="B54" s="8" t="s">
         <v>101</v>
       </c>
-      <c r="B54" s="27"/>
-      <c r="C54" s="27"/>
-      <c r="D54" s="27"/>
-      <c r="E54" s="27"/>
-      <c r="F54" s="27"/>
-      <c r="G54" s="27"/>
-      <c r="H54" s="27"/>
-      <c r="I54" s="27"/>
-      <c r="J54" s="14"/>
-      <c r="K54" s="14"/>
-      <c r="L54" s="14"/>
-    </row>
-    <row r="55" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="C54" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D54" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E54" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F54" s="10"/>
+      <c r="G54" s="10"/>
+      <c r="H54" s="10"/>
+      <c r="I54" s="10"/>
+      <c r="J54" s="22"/>
+    </row>
+    <row r="55" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="13" t="s">
-        <v>274</v>
+        <v>272</v>
       </c>
       <c r="B55" s="8" t="s">
         <v>102</v>
@@ -9354,7 +9363,7 @@
     </row>
     <row r="56" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="13" t="s">
-        <v>273</v>
+        <v>271</v>
       </c>
       <c r="B56" s="8" t="s">
         <v>103</v>
@@ -9376,7 +9385,7 @@
     </row>
     <row r="57" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="13" t="s">
-        <v>272</v>
+        <v>270</v>
       </c>
       <c r="B57" s="8" t="s">
         <v>104</v>
@@ -9398,7 +9407,7 @@
     </row>
     <row r="58" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="13" t="s">
-        <v>271</v>
+        <v>269</v>
       </c>
       <c r="B58" s="8" t="s">
         <v>105</v>
@@ -9416,11 +9425,10 @@
       <c r="G58" s="10"/>
       <c r="H58" s="10"/>
       <c r="I58" s="10"/>
-      <c r="J58" s="22"/>
     </row>
     <row r="59" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="13" t="s">
-        <v>270</v>
+        <v>268</v>
       </c>
       <c r="B59" s="8" t="s">
         <v>106</v>
@@ -9438,70 +9446,71 @@
       <c r="G59" s="10"/>
       <c r="H59" s="10"/>
       <c r="I59" s="10"/>
+      <c r="J59" s="16"/>
+      <c r="K59" s="16"/>
     </row>
     <row r="60" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="13" t="s">
-        <v>269</v>
-      </c>
-      <c r="B60" s="8" t="s">
-        <v>107</v>
-      </c>
-      <c r="C60" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D60" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E60" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B60" s="8"/>
+      <c r="C60" s="9"/>
+      <c r="D60" s="10"/>
+      <c r="E60" s="10"/>
       <c r="F60" s="10"/>
       <c r="G60" s="10"/>
       <c r="H60" s="10"/>
       <c r="I60" s="10"/>
-      <c r="J60" s="16"/>
-      <c r="K60" s="16"/>
-    </row>
-    <row r="61" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B61" s="8"/>
-      <c r="C61" s="9"/>
-      <c r="D61" s="10"/>
-      <c r="E61" s="10"/>
-      <c r="F61" s="10"/>
-      <c r="G61" s="10"/>
-      <c r="H61" s="10"/>
-      <c r="I61" s="10"/>
-      <c r="J61" s="13"/>
-    </row>
-    <row r="62" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A62" s="15" t="s">
+      <c r="J60" s="13"/>
+    </row>
+    <row r="61" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A61" s="15" t="s">
+        <v>107</v>
+      </c>
+      <c r="B61" s="27"/>
+      <c r="C61" s="27"/>
+      <c r="D61" s="27"/>
+      <c r="E61" s="27"/>
+      <c r="F61" s="27"/>
+      <c r="G61" s="27"/>
+      <c r="H61" s="27"/>
+      <c r="I61" s="27"/>
+      <c r="J61" s="14"/>
+      <c r="K61" s="14"/>
+      <c r="L61" s="14"/>
+    </row>
+    <row r="62" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="13" t="s">
         <v>108</v>
       </c>
-      <c r="B62" s="27"/>
-      <c r="C62" s="27"/>
-      <c r="D62" s="27"/>
-      <c r="E62" s="27"/>
-      <c r="F62" s="27"/>
-      <c r="G62" s="27"/>
-      <c r="H62" s="27"/>
-      <c r="I62" s="27"/>
-      <c r="J62" s="14"/>
-      <c r="K62" s="14"/>
-      <c r="L62" s="14"/>
-    </row>
-    <row r="63" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B62" s="8" t="s">
+        <v>109</v>
+      </c>
+      <c r="C62" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D62" s="10"/>
+      <c r="E62" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F62" s="10"/>
+      <c r="G62" s="10"/>
+      <c r="H62" s="10"/>
+      <c r="I62" s="10"/>
+      <c r="J62" s="13"/>
+    </row>
+    <row r="63" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="13" t="s">
-        <v>109</v>
+        <v>110</v>
       </c>
       <c r="B63" s="8" t="s">
-        <v>110</v>
+        <v>111</v>
       </c>
       <c r="C63" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D63" s="10"/>
+      <c r="D63" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="E63" s="10" t="s">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="F63" s="10"/>
       <c r="G63" s="10"/>
@@ -9511,85 +9520,84 @@
     </row>
     <row r="64" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="13" t="s">
-        <v>111</v>
+        <v>112</v>
       </c>
       <c r="B64" s="8" t="s">
-        <v>112</v>
+        <v>113</v>
       </c>
       <c r="C64" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D64" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E64" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F64" s="10"/>
       <c r="G64" s="10"/>
       <c r="H64" s="10"/>
       <c r="I64" s="10"/>
-      <c r="J64" s="13"/>
     </row>
     <row r="65" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="13" t="s">
-        <v>113</v>
+        <v>114</v>
       </c>
       <c r="B65" s="8" t="s">
-        <v>114</v>
+        <v>115</v>
       </c>
       <c r="C65" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D65" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E65" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F65" s="10"/>
       <c r="G65" s="10"/>
       <c r="H65" s="10"/>
       <c r="I65" s="10"/>
+      <c r="J65" s="16"/>
+      <c r="K65" s="16"/>
     </row>
     <row r="66" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="13" t="s">
-        <v>115</v>
+        <v>116</v>
       </c>
       <c r="B66" s="8" t="s">
-        <v>116</v>
+        <v>117</v>
       </c>
       <c r="C66" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D66" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E66" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F66" s="10"/>
       <c r="G66" s="10"/>
       <c r="H66" s="10"/>
       <c r="I66" s="10"/>
-      <c r="J66" s="16"/>
-      <c r="K66" s="16"/>
     </row>
     <row r="67" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="13" t="s">
-        <v>117</v>
+        <v>118</v>
       </c>
       <c r="B67" s="8" t="s">
-        <v>118</v>
+        <v>119</v>
       </c>
       <c r="C67" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D67" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E67" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F67" s="10"/>
       <c r="G67" s="10"/>
@@ -9598,19 +9606,17 @@
     </row>
     <row r="68" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="13" t="s">
-        <v>119</v>
+        <v>120</v>
       </c>
       <c r="B68" s="8" t="s">
-        <v>120</v>
+        <v>121</v>
       </c>
       <c r="C68" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D68" s="10" t="s">
-        <v>277</v>
-      </c>
+      <c r="D68" s="10"/>
       <c r="E68" s="10" t="s">
-        <v>277</v>
+        <v>11</v>
       </c>
       <c r="F68" s="10"/>
       <c r="G68" s="10"/>
@@ -9619,10 +9625,10 @@
     </row>
     <row r="69" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="13" t="s">
-        <v>121</v>
+        <v>122</v>
       </c>
       <c r="B69" s="8" t="s">
-        <v>122</v>
+        <v>123</v>
       </c>
       <c r="C69" s="10" t="s">
         <v>11</v>
@@ -9638,10 +9644,10 @@
     </row>
     <row r="70" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="13" t="s">
-        <v>123</v>
+        <v>124</v>
       </c>
       <c r="B70" s="8" t="s">
-        <v>124</v>
+        <v>125</v>
       </c>
       <c r="C70" s="10" t="s">
         <v>11</v>
@@ -9657,10 +9663,10 @@
     </row>
     <row r="71" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="13" t="s">
-        <v>125</v>
+        <v>126</v>
       </c>
       <c r="B71" s="8" t="s">
-        <v>126</v>
+        <v>54</v>
       </c>
       <c r="C71" s="10" t="s">
         <v>11</v>
@@ -9679,14 +9685,16 @@
         <v>127</v>
       </c>
       <c r="B72" s="8" t="s">
-        <v>55</v>
+        <v>128</v>
       </c>
       <c r="C72" s="10" t="s">
         <v>11</v>
       </c>
-      <c r="D72" s="10"/>
+      <c r="D72" s="10" t="s">
+        <v>276</v>
+      </c>
       <c r="E72" s="10" t="s">
-        <v>11</v>
+        <v>276</v>
       </c>
       <c r="F72" s="10"/>
       <c r="G72" s="10"/>
@@ -9694,67 +9702,67 @@
       <c r="I72" s="10"/>
     </row>
     <row r="73" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="13" t="s">
-        <v>128</v>
-      </c>
-      <c r="B73" s="8" t="s">
-        <v>129</v>
-      </c>
-      <c r="C73" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D73" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="E73" s="10" t="s">
-        <v>277</v>
-      </c>
+      <c r="B73" s="11"/>
+      <c r="C73" s="10"/>
+      <c r="D73" s="10"/>
+      <c r="E73" s="10"/>
       <c r="F73" s="10"/>
       <c r="G73" s="10"/>
       <c r="H73" s="10"/>
       <c r="I73" s="10"/>
     </row>
-    <row r="74" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B74" s="11"/>
-      <c r="C74" s="10"/>
-      <c r="D74" s="10"/>
-      <c r="E74" s="10"/>
-      <c r="F74" s="10"/>
-      <c r="G74" s="10"/>
-      <c r="H74" s="10"/>
-      <c r="I74" s="10"/>
-    </row>
-    <row r="75" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A75" s="15" t="s">
+    <row r="74" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A74" s="15" t="s">
+        <v>129</v>
+      </c>
+      <c r="B74" s="27"/>
+      <c r="C74" s="27"/>
+      <c r="D74" s="27"/>
+      <c r="E74" s="27"/>
+      <c r="F74" s="27"/>
+      <c r="G74" s="27"/>
+      <c r="H74" s="27"/>
+      <c r="I74" s="27"/>
+      <c r="J74" s="14"/>
+      <c r="K74" s="14"/>
+      <c r="L74" s="14"/>
+    </row>
+    <row r="75" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="13" t="s">
         <v>130</v>
       </c>
-      <c r="B75" s="27"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
-      <c r="G75" s="27"/>
-      <c r="H75" s="27"/>
-      <c r="I75" s="27"/>
-      <c r="J75" s="14"/>
-      <c r="K75" s="14"/>
-      <c r="L75" s="14"/>
-    </row>
-    <row r="76" spans="1:12" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B75" s="8" t="s">
+        <v>131</v>
+      </c>
+      <c r="C75" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D75" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="E75" s="10" t="s">
+        <v>276</v>
+      </c>
+      <c r="F75" s="10"/>
+      <c r="G75" s="10"/>
+      <c r="H75" s="10"/>
+      <c r="I75" s="10"/>
+    </row>
+    <row r="76" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="13" t="s">
-        <v>131</v>
+        <v>132</v>
       </c>
       <c r="B76" s="8" t="s">
-        <v>132</v>
+        <v>133</v>
       </c>
       <c r="C76" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D76" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E76" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F76" s="10"/>
       <c r="G76" s="10"/>
@@ -9763,19 +9771,19 @@
     </row>
     <row r="77" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="13" t="s">
-        <v>133</v>
+        <v>134</v>
       </c>
       <c r="B77" s="8" t="s">
-        <v>134</v>
+        <v>135</v>
       </c>
       <c r="C77" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D77" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E77" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F77" s="10"/>
       <c r="G77" s="10"/>
@@ -9784,19 +9792,19 @@
     </row>
     <row r="78" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="13" t="s">
-        <v>135</v>
+        <v>136</v>
       </c>
       <c r="B78" s="8" t="s">
-        <v>136</v>
+        <v>137</v>
       </c>
       <c r="C78" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D78" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E78" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F78" s="10"/>
       <c r="G78" s="10"/>
@@ -9805,19 +9813,19 @@
     </row>
     <row r="79" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="13" t="s">
-        <v>137</v>
+        <v>138</v>
       </c>
       <c r="B79" s="8" t="s">
-        <v>138</v>
+        <v>139</v>
       </c>
       <c r="C79" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D79" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E79" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F79" s="10"/>
       <c r="G79" s="10"/>
@@ -9826,19 +9834,19 @@
     </row>
     <row r="80" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="13" t="s">
-        <v>139</v>
+        <v>140</v>
       </c>
       <c r="B80" s="8" t="s">
-        <v>140</v>
+        <v>141</v>
       </c>
       <c r="C80" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D80" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E80" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F80" s="10"/>
       <c r="G80" s="10"/>
@@ -9847,19 +9855,19 @@
     </row>
     <row r="81" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="13" t="s">
-        <v>141</v>
+        <v>142</v>
       </c>
       <c r="B81" s="8" t="s">
-        <v>142</v>
+        <v>143</v>
       </c>
       <c r="C81" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D81" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E81" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F81" s="10"/>
       <c r="G81" s="10"/>
@@ -9868,19 +9876,19 @@
     </row>
     <row r="82" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="13" t="s">
-        <v>143</v>
+        <v>144</v>
       </c>
       <c r="B82" s="8" t="s">
-        <v>144</v>
+        <v>145</v>
       </c>
       <c r="C82" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D82" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E82" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F82" s="10"/>
       <c r="G82" s="10"/>
@@ -9889,19 +9897,19 @@
     </row>
     <row r="83" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="13" t="s">
-        <v>145</v>
+        <v>146</v>
       </c>
       <c r="B83" s="8" t="s">
-        <v>146</v>
+        <v>147</v>
       </c>
       <c r="C83" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D83" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E83" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F83" s="10"/>
       <c r="G83" s="10"/>
@@ -9910,19 +9918,19 @@
     </row>
     <row r="84" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="13" t="s">
-        <v>147</v>
+        <v>148</v>
       </c>
       <c r="B84" s="8" t="s">
-        <v>148</v>
+        <v>149</v>
       </c>
       <c r="C84" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D84" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E84" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F84" s="10"/>
       <c r="G84" s="10"/>
@@ -9931,19 +9939,19 @@
     </row>
     <row r="85" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="13" t="s">
-        <v>149</v>
+        <v>150</v>
       </c>
       <c r="B85" s="8" t="s">
-        <v>150</v>
+        <v>151</v>
       </c>
       <c r="C85" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D85" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E85" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F85" s="10"/>
       <c r="G85" s="10"/>
@@ -9952,19 +9960,19 @@
     </row>
     <row r="86" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="13" t="s">
-        <v>151</v>
+        <v>152</v>
       </c>
       <c r="B86" s="8" t="s">
-        <v>152</v>
+        <v>153</v>
       </c>
       <c r="C86" s="10" t="s">
         <v>11</v>
       </c>
       <c r="D86" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="E86" s="10" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="F86" s="10"/>
       <c r="G86" s="10"/>
@@ -9972,58 +9980,60 @@
       <c r="I86" s="10"/>
     </row>
     <row r="87" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="13" t="s">
-        <v>153</v>
-      </c>
-      <c r="B87" s="8" t="s">
-        <v>154</v>
-      </c>
-      <c r="C87" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D87" s="10" t="s">
-        <v>277</v>
-      </c>
-      <c r="E87" s="10" t="s">
-        <v>277</v>
-      </c>
+      <c r="B87" s="11"/>
+      <c r="C87" s="10"/>
+      <c r="D87" s="10"/>
+      <c r="E87" s="10"/>
       <c r="F87" s="10"/>
       <c r="G87" s="10"/>
       <c r="H87" s="10"/>
       <c r="I87" s="10"/>
     </row>
-    <row r="88" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B88" s="11"/>
-      <c r="C88" s="10"/>
-      <c r="D88" s="10"/>
-      <c r="E88" s="10"/>
-      <c r="F88" s="10"/>
-      <c r="G88" s="10"/>
-      <c r="H88" s="10"/>
-      <c r="I88" s="10"/>
-    </row>
-    <row r="89" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A89" s="15" t="s">
+    <row r="88" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A88" s="15" t="s">
+        <v>154</v>
+      </c>
+      <c r="B88" s="27"/>
+      <c r="C88" s="27"/>
+      <c r="D88" s="27"/>
+      <c r="E88" s="27"/>
+      <c r="F88" s="27"/>
+      <c r="G88" s="27"/>
+      <c r="H88" s="27"/>
+      <c r="I88" s="27"/>
+      <c r="J88" s="14"/>
+      <c r="K88" s="14"/>
+      <c r="L88" s="14"/>
+    </row>
+    <row r="89" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A89" s="33" t="s">
         <v>155</v>
       </c>
-      <c r="B89" s="27"/>
-      <c r="C89" s="27"/>
-      <c r="D89" s="27"/>
-      <c r="E89" s="27"/>
-      <c r="F89" s="27"/>
-      <c r="G89" s="27"/>
-      <c r="H89" s="27"/>
-      <c r="I89" s="27"/>
-      <c r="J89" s="14"/>
-      <c r="K89" s="14"/>
-      <c r="L89" s="14"/>
-    </row>
-    <row r="90" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B89" s="8" t="s">
+        <v>156</v>
+      </c>
+      <c r="C89" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D89" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E89" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F89" s="10"/>
+      <c r="G89" s="9" t="s">
+        <v>11</v>
+      </c>
+      <c r="H89" s="10"/>
+      <c r="I89" s="10"/>
+    </row>
+    <row r="90" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A90" s="33" t="s">
-        <v>156</v>
+        <v>157</v>
       </c>
       <c r="B90" s="8" t="s">
-        <v>157</v>
+        <v>158</v>
       </c>
       <c r="C90" s="10" t="s">
         <v>11</v>
@@ -10043,10 +10053,10 @@
     </row>
     <row r="91" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A91" s="33" t="s">
-        <v>158</v>
+        <v>159</v>
       </c>
       <c r="B91" s="8" t="s">
-        <v>159</v>
+        <v>160</v>
       </c>
       <c r="C91" s="10" t="s">
         <v>11</v>
@@ -10066,10 +10076,10 @@
     </row>
     <row r="92" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A92" s="33" t="s">
-        <v>160</v>
+        <v>161</v>
       </c>
       <c r="B92" s="8" t="s">
-        <v>161</v>
+        <v>162</v>
       </c>
       <c r="C92" s="10" t="s">
         <v>11</v>
@@ -10089,10 +10099,10 @@
     </row>
     <row r="93" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A93" s="33" t="s">
-        <v>162</v>
+        <v>163</v>
       </c>
       <c r="B93" s="8" t="s">
-        <v>163</v>
+        <v>164</v>
       </c>
       <c r="C93" s="10" t="s">
         <v>11</v>
@@ -10112,10 +10122,10 @@
     </row>
     <row r="94" spans="1:12" ht="30" x14ac:dyDescent="0.2">
       <c r="A94" s="33" t="s">
-        <v>164</v>
+        <v>165</v>
       </c>
       <c r="B94" s="8" t="s">
-        <v>165</v>
+        <v>166</v>
       </c>
       <c r="C94" s="10" t="s">
         <v>11</v>
@@ -10133,12 +10143,12 @@
       <c r="H94" s="10"/>
       <c r="I94" s="10"/>
     </row>
-    <row r="95" spans="1:12" ht="30" x14ac:dyDescent="0.2">
+    <row r="95" spans="1:12" ht="45" x14ac:dyDescent="0.2">
       <c r="A95" s="33" t="s">
-        <v>166</v>
+        <v>167</v>
       </c>
       <c r="B95" s="8" t="s">
-        <v>167</v>
+        <v>168</v>
       </c>
       <c r="C95" s="10" t="s">
         <v>11</v>
@@ -10156,12 +10166,12 @@
       <c r="H95" s="10"/>
       <c r="I95" s="10"/>
     </row>
-    <row r="96" spans="1:12" ht="45" x14ac:dyDescent="0.2">
-      <c r="A96" s="33" t="s">
-        <v>168</v>
+    <row r="96" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A96" s="13" t="s">
+        <v>169</v>
       </c>
       <c r="B96" s="8" t="s">
-        <v>169</v>
+        <v>170</v>
       </c>
       <c r="C96" s="10" t="s">
         <v>11</v>
@@ -10180,60 +10190,61 @@
       <c r="I96" s="10"/>
     </row>
     <row r="97" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="13" t="s">
-        <v>170</v>
-      </c>
-      <c r="B97" s="8" t="s">
-        <v>171</v>
-      </c>
-      <c r="C97" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D97" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E97" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B97" s="11"/>
+      <c r="C97" s="10"/>
+      <c r="D97" s="10"/>
+      <c r="E97" s="10"/>
       <c r="F97" s="10"/>
-      <c r="G97" s="9" t="s">
-        <v>11</v>
-      </c>
+      <c r="G97" s="10"/>
       <c r="H97" s="10"/>
       <c r="I97" s="10"/>
     </row>
-    <row r="98" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="B98" s="11"/>
-      <c r="C98" s="10"/>
-      <c r="D98" s="10"/>
-      <c r="E98" s="10"/>
-      <c r="F98" s="10"/>
-      <c r="G98" s="10"/>
-      <c r="H98" s="10"/>
-      <c r="I98" s="10"/>
-    </row>
-    <row r="99" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
-      <c r="A99" s="15" t="s">
+    <row r="98" spans="1:12" ht="17.25" thickBot="1" x14ac:dyDescent="0.3">
+      <c r="A98" s="15" t="s">
+        <v>171</v>
+      </c>
+      <c r="B98" s="27"/>
+      <c r="C98" s="27"/>
+      <c r="D98" s="27"/>
+      <c r="E98" s="27"/>
+      <c r="F98" s="27"/>
+      <c r="G98" s="27"/>
+      <c r="H98" s="27"/>
+      <c r="I98" s="27"/>
+      <c r="J98" s="14"/>
+      <c r="K98" s="14"/>
+      <c r="L98" s="14"/>
+    </row>
+    <row r="99" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="A99" s="33" t="s">
+        <v>274</v>
+      </c>
+      <c r="B99" s="8" t="s">
         <v>172</v>
       </c>
-      <c r="B99" s="27"/>
-      <c r="C99" s="27"/>
-      <c r="D99" s="27"/>
-      <c r="E99" s="27"/>
-      <c r="F99" s="27"/>
-      <c r="G99" s="27"/>
-      <c r="H99" s="27"/>
-      <c r="I99" s="27"/>
-      <c r="J99" s="14"/>
-      <c r="K99" s="14"/>
-      <c r="L99" s="14"/>
-    </row>
-    <row r="100" spans="1:12" ht="30.75" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="A100" s="33" t="s">
+      <c r="C99" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="D99" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="E99" s="10" t="s">
+        <v>11</v>
+      </c>
+      <c r="F99" s="10"/>
+      <c r="G99" s="10"/>
+      <c r="H99" s="10"/>
+      <c r="I99" s="10"/>
+      <c r="J99" t="s">
         <v>275</v>
       </c>
+    </row>
+    <row r="100" spans="1:12" ht="15" x14ac:dyDescent="0.2">
+      <c r="A100" s="13" t="s">
+        <v>173</v>
+      </c>
       <c r="B100" s="8" t="s">
-        <v>173</v>
+        <v>174</v>
       </c>
       <c r="C100" s="10" t="s">
         <v>11</v>
@@ -10249,15 +10260,15 @@
       <c r="H100" s="10"/>
       <c r="I100" s="10"/>
       <c r="J100" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="101" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="13" t="s">
-        <v>174</v>
+        <v>175</v>
       </c>
       <c r="B101" s="8" t="s">
-        <v>175</v>
+        <v>176</v>
       </c>
       <c r="C101" s="10" t="s">
         <v>11</v>
@@ -10273,15 +10284,15 @@
       <c r="H101" s="10"/>
       <c r="I101" s="10"/>
       <c r="J101" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="102" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="13" t="s">
-        <v>176</v>
+        <v>177</v>
       </c>
       <c r="B102" s="8" t="s">
-        <v>177</v>
+        <v>178</v>
       </c>
       <c r="C102" s="10" t="s">
         <v>11</v>
@@ -10297,15 +10308,15 @@
       <c r="H102" s="10"/>
       <c r="I102" s="10"/>
       <c r="J102" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="103" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="13" t="s">
-        <v>178</v>
+        <v>179</v>
       </c>
       <c r="B103" s="8" t="s">
-        <v>179</v>
+        <v>180</v>
       </c>
       <c r="C103" s="10" t="s">
         <v>11</v>
@@ -10321,15 +10332,15 @@
       <c r="H103" s="10"/>
       <c r="I103" s="10"/>
       <c r="J103" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="104" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="13" t="s">
-        <v>180</v>
+        <v>181</v>
       </c>
       <c r="B104" s="8" t="s">
-        <v>181</v>
+        <v>182</v>
       </c>
       <c r="C104" s="10" t="s">
         <v>11</v>
@@ -10345,15 +10356,15 @@
       <c r="H104" s="10"/>
       <c r="I104" s="10"/>
       <c r="J104" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="105" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="13" t="s">
-        <v>182</v>
+        <v>183</v>
       </c>
       <c r="B105" s="8" t="s">
-        <v>183</v>
+        <v>184</v>
       </c>
       <c r="C105" s="10" t="s">
         <v>11</v>
@@ -10369,15 +10380,15 @@
       <c r="H105" s="10"/>
       <c r="I105" s="10"/>
       <c r="J105" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="106" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="13" t="s">
-        <v>184</v>
+        <v>185</v>
       </c>
       <c r="B106" s="8" t="s">
-        <v>185</v>
+        <v>186</v>
       </c>
       <c r="C106" s="10" t="s">
         <v>11</v>
@@ -10393,15 +10404,15 @@
       <c r="H106" s="10"/>
       <c r="I106" s="10"/>
       <c r="J106" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="107" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="13" t="s">
-        <v>186</v>
+        <v>187</v>
       </c>
       <c r="B107" s="8" t="s">
-        <v>187</v>
+        <v>188</v>
       </c>
       <c r="C107" s="10" t="s">
         <v>11</v>
@@ -10417,15 +10428,15 @@
       <c r="H107" s="10"/>
       <c r="I107" s="10"/>
       <c r="J107" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="108" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="13" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="B108" s="8" t="s">
-        <v>189</v>
+        <v>190</v>
       </c>
       <c r="C108" s="10" t="s">
         <v>11</v>
@@ -10441,15 +10452,15 @@
       <c r="H108" s="10"/>
       <c r="I108" s="10"/>
       <c r="J108" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="109" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="13" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
       <c r="B109" s="8" t="s">
-        <v>191</v>
+        <v>192</v>
       </c>
       <c r="C109" s="10" t="s">
         <v>11</v>
@@ -10465,15 +10476,15 @@
       <c r="H109" s="10"/>
       <c r="I109" s="10"/>
       <c r="J109" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="110" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="13" t="s">
-        <v>192</v>
+        <v>193</v>
       </c>
       <c r="B110" s="8" t="s">
-        <v>193</v>
+        <v>194</v>
       </c>
       <c r="C110" s="10" t="s">
         <v>11</v>
@@ -10489,15 +10500,15 @@
       <c r="H110" s="10"/>
       <c r="I110" s="10"/>
       <c r="J110" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="111" spans="1:12" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="13" t="s">
-        <v>194</v>
+        <v>195</v>
       </c>
       <c r="B111" s="8" t="s">
-        <v>195</v>
+        <v>196</v>
       </c>
       <c r="C111" s="10" t="s">
         <v>11</v>
@@ -10513,32 +10524,18 @@
       <c r="H111" s="10"/>
       <c r="I111" s="10"/>
       <c r="J111" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
     </row>
     <row r="112" spans="1:12" ht="15" x14ac:dyDescent="0.2">
-      <c r="A112" s="13" t="s">
-        <v>196</v>
-      </c>
-      <c r="B112" s="8" t="s">
-        <v>197</v>
-      </c>
-      <c r="C112" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="D112" s="10" t="s">
-        <v>11</v>
-      </c>
-      <c r="E112" s="10" t="s">
-        <v>11</v>
-      </c>
+      <c r="B112" s="9"/>
+      <c r="C112" s="9"/>
+      <c r="D112" s="10"/>
+      <c r="E112" s="10"/>
       <c r="F112" s="10"/>
       <c r="G112" s="10"/>
       <c r="H112" s="10"/>
       <c r="I112" s="10"/>
-      <c r="J112" t="s">
-        <v>276</v>
-      </c>
     </row>
     <row r="113" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B113" s="9"/>
@@ -10591,8 +10588,8 @@
       <c r="I117" s="10"/>
     </row>
     <row r="118" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B118" s="9"/>
-      <c r="C118" s="9"/>
+      <c r="B118" s="10"/>
+      <c r="C118" s="10"/>
       <c r="D118" s="10"/>
       <c r="E118" s="10"/>
       <c r="F118" s="10"/>
@@ -10611,8 +10608,8 @@
       <c r="I119" s="10"/>
     </row>
     <row r="120" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B120" s="10"/>
-      <c r="C120" s="10"/>
+      <c r="B120" s="9"/>
+      <c r="C120" s="9"/>
       <c r="D120" s="10"/>
       <c r="E120" s="10"/>
       <c r="F120" s="10"/>
@@ -10621,8 +10618,8 @@
       <c r="I120" s="10"/>
     </row>
     <row r="121" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B121" s="9"/>
-      <c r="C121" s="9"/>
+      <c r="B121" s="10"/>
+      <c r="C121" s="10"/>
       <c r="D121" s="10"/>
       <c r="E121" s="10"/>
       <c r="F121" s="10"/>
@@ -10641,8 +10638,8 @@
       <c r="I122" s="10"/>
     </row>
     <row r="123" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B123" s="10"/>
-      <c r="C123" s="10"/>
+      <c r="B123" s="9"/>
+      <c r="C123" s="9"/>
       <c r="D123" s="10"/>
       <c r="E123" s="10"/>
       <c r="F123" s="10"/>
@@ -10661,7 +10658,7 @@
       <c r="I124" s="10"/>
     </row>
     <row r="125" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B125" s="9"/>
+      <c r="B125" s="10"/>
       <c r="C125" s="9"/>
       <c r="D125" s="10"/>
       <c r="E125" s="10"/>
@@ -10702,7 +10699,7 @@
     </row>
     <row r="129" spans="2:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B129" s="10"/>
-      <c r="C129" s="9"/>
+      <c r="C129" s="10"/>
       <c r="D129" s="10"/>
       <c r="E129" s="10"/>
       <c r="F129" s="10"/>
@@ -20169,16 +20166,6 @@
       <c r="G1075" s="10"/>
       <c r="H1075" s="10"/>
       <c r="I1075" s="10"/>
-    </row>
-    <row r="1076" spans="2:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B1076" s="10"/>
-      <c r="C1076" s="10"/>
-      <c r="D1076" s="10"/>
-      <c r="E1076" s="10"/>
-      <c r="F1076" s="10"/>
-      <c r="G1076" s="10"/>
-      <c r="H1076" s="10"/>
-      <c r="I1076" s="10"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -20207,7 +20194,7 @@
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="57.85546875" customWidth="1"/>
+    <col min="1" max="1" width="64.5703125" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" customWidth="1"/>
@@ -20236,7 +20223,7 @@
       <c r="G1" s="34"/>
       <c r="H1" s="34"/>
       <c r="I1" s="34" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="J1" s="34"/>
       <c r="K1" s="34" t="s">
@@ -20288,10 +20275,10 @@
         <v>10</v>
       </c>
       <c r="I2" s="30" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="J2" s="29" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="K2" s="34"/>
       <c r="L2" s="1"/>
@@ -20318,7 +20305,7 @@
     </row>
     <row r="3" spans="1:32" ht="18" thickTop="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A3" s="19" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="B3" s="19"/>
       <c r="C3" s="19"/>
@@ -20354,7 +20341,7 @@
     </row>
     <row r="4" spans="1:32" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A4" s="2" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B4" s="3" t="s">
         <v>11</v>
@@ -20370,7 +20357,7 @@
     </row>
     <row r="5" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="2" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="B5" s="3" t="s">
         <v>11</v>
@@ -20386,7 +20373,7 @@
     </row>
     <row r="6" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="2" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="B6" s="3" t="s">
         <v>11</v>
@@ -20403,23 +20390,23 @@
     </row>
     <row r="7" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="2" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="B7" s="3" t="s">
         <v>11</v>
       </c>
       <c r="C7" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="D7" s="4" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="I7" s="16"/>
       <c r="J7" s="16"/>
     </row>
     <row r="8" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="2" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="B8" s="3" t="s">
         <v>11</v>
@@ -20443,7 +20430,7 @@
     </row>
     <row r="10" spans="1:32" ht="15.75" customHeight="1" thickBot="1" x14ac:dyDescent="0.3">
       <c r="A10" s="14" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="B10" s="31"/>
       <c r="C10" s="31"/>
@@ -20458,7 +20445,7 @@
     </row>
     <row r="11" spans="1:32" ht="15.75" customHeight="1" thickTop="1" x14ac:dyDescent="0.25">
       <c r="A11" s="2" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="B11" s="4"/>
       <c r="C11" s="4"/>
@@ -20470,7 +20457,7 @@
     </row>
     <row r="12" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="2" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="B12" s="4"/>
       <c r="C12" s="4"/>
@@ -20482,7 +20469,7 @@
     </row>
     <row r="13" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="2" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B13" s="3"/>
       <c r="C13" s="4"/>
@@ -20494,7 +20481,7 @@
     </row>
     <row r="14" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="2" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B14" s="3"/>
       <c r="C14" s="4"/>
@@ -20506,7 +20493,7 @@
     </row>
     <row r="15" spans="1:32" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="2" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B15" s="3"/>
       <c r="C15" s="4"/>

</xml_diff>

<commit_message>
Remove URL detection from all code windows. exec_lescript testing
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{C3EEABE3-A180-4A3A-A025-C0D8121DD17B}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E4E3AB4A-3F1A-4B8C-92E9-4BF6D9D8D0A3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44595" yWindow="1725" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="42675" yWindow="930" windowWidth="30420" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="817" uniqueCount="279">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="814" uniqueCount="280">
   <si>
     <t>Statement</t>
   </si>
@@ -865,6 +865,9 @@
   </si>
   <si>
     <t>DEPRECATE FOR exec_lescript???</t>
+  </si>
+  <si>
+    <t>exec_lescript</t>
   </si>
 </sst>
 </file>
@@ -1294,9 +1297,9 @@
   </sheetPr>
   <dimension ref="A1:AF1004"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A6" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G22" sqref="G22"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A39" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="K10" sqref="K10"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1484,14 +1487,12 @@
         <v>11</v>
       </c>
       <c r="I8" s="22" t="s">
-        <v>266</v>
+        <v>279</v>
       </c>
       <c r="J8" s="23" t="s">
         <v>267</v>
       </c>
-      <c r="K8" s="22" t="s">
-        <v>266</v>
-      </c>
+      <c r="K8" s="22"/>
     </row>
     <row r="9" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="13" t="s">
@@ -1515,9 +1516,7 @@
       <c r="J9" s="23" t="s">
         <v>212</v>
       </c>
-      <c r="K9" s="22" t="s">
-        <v>266</v>
-      </c>
+      <c r="K9" s="22"/>
     </row>
     <row r="10" spans="1:11" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="13" t="s">
@@ -1541,9 +1540,7 @@
       <c r="J10" s="23" t="s">
         <v>215</v>
       </c>
-      <c r="K10" s="22" t="s">
-        <v>266</v>
-      </c>
+      <c r="K10" s="22"/>
     </row>
     <row r="11" spans="1:11" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="13" t="s">
@@ -8206,7 +8203,7 @@
   </sheetPr>
   <dimension ref="A1:AG1075"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="H14" sqref="H14"/>
     </sheetView>

</xml_diff>

<commit_message>
Testing and individual function cleanup
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{6D9D1B52-9819-4E23-881D-3D067D22DBBA}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1E498A99-32F9-47BE-8BA6-EA1335C01FEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="42675" yWindow="930" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="44790" yWindow="1770" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="811" uniqueCount="280">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="808" uniqueCount="283">
   <si>
     <t>Statement</t>
   </si>
@@ -840,9 +840,6 @@
     <t>???</t>
   </si>
   <si>
-    <t>DEPRECATE FOR exec_lescript???</t>
-  </si>
-  <si>
     <t>exec_lescript</t>
   </si>
   <si>
@@ -868,6 +865,18 @@
   </si>
   <si>
     <t>assertNotEqual(var_name, value)</t>
+  </si>
+  <si>
+    <t>execline_lescript</t>
+  </si>
+  <si>
+    <t>execline_java</t>
+  </si>
+  <si>
+    <t>execline_python</t>
+  </si>
+  <si>
+    <t>CONTINUE FROM HERE</t>
   </si>
 </sst>
 </file>
@@ -1314,8 +1323,8 @@
   <dimension ref="A1:AC1006"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A36" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G50" sqref="G50"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="H17" sqref="H17"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1340,7 +1349,7 @@
       <c r="C1" s="35"/>
       <c r="D1" s="35"/>
       <c r="E1" s="13" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>204</v>
@@ -1487,7 +1496,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="30" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="G8" s="31" t="s">
         <v>259</v>
@@ -1559,12 +1568,10 @@
         <v>6</v>
       </c>
       <c r="F11" s="30" t="s">
-        <v>258</v>
+        <v>279</v>
       </c>
       <c r="G11" s="21"/>
-      <c r="H11" s="30" t="s">
-        <v>258</v>
-      </c>
+      <c r="H11" s="30"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="22" t="s">
@@ -1583,12 +1590,10 @@
         <v>6</v>
       </c>
       <c r="F12" s="30" t="s">
-        <v>258</v>
+        <v>280</v>
       </c>
       <c r="G12" s="21"/>
-      <c r="H12" s="30" t="s">
-        <v>258</v>
-      </c>
+      <c r="H12" s="30"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="22" t="s">
@@ -1607,12 +1612,10 @@
         <v>6</v>
       </c>
       <c r="F13" s="30" t="s">
-        <v>258</v>
+        <v>281</v>
       </c>
       <c r="G13" s="21"/>
-      <c r="H13" s="30" t="s">
-        <v>258</v>
-      </c>
+      <c r="H13" s="30"/>
     </row>
     <row r="14" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="19"/>
@@ -1656,7 +1659,9 @@
         <v>212</v>
       </c>
       <c r="G16" s="21"/>
-      <c r="H16" s="21"/>
+      <c r="H16" s="21" t="s">
+        <v>282</v>
+      </c>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="22" t="s">
@@ -1680,9 +1685,7 @@
       <c r="G17" s="22" t="s">
         <v>215</v>
       </c>
-      <c r="H17" s="22" t="s">
-        <v>270</v>
-      </c>
+      <c r="H17" s="22"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="22" t="s">
@@ -2305,7 +2308,7 @@
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="22" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B49" s="29" t="s">
         <v>6</v>
@@ -2323,7 +2326,7 @@
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="22" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B50" s="29" t="s">
         <v>6</v>
@@ -2341,7 +2344,7 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="22" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B51" s="29"/>
       <c r="C51" s="29" t="s">
@@ -2361,7 +2364,7 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="22" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B52" s="29"/>
       <c r="C52" s="29" t="s">
@@ -8348,7 +8351,7 @@
       <c r="D1" s="12"/>
       <c r="E1" s="12"/>
       <c r="F1" s="13" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="G1" s="12" t="s">
         <v>204</v>
@@ -17301,7 +17304,7 @@
       <c r="C1" s="12"/>
       <c r="D1" s="12"/>
       <c r="E1" s="13" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="F1" s="12" t="s">
         <v>204</v>
@@ -17576,7 +17579,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="19" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B15" s="20"/>
       <c r="C15" s="20"/>

</xml_diff>

<commit_message>
grind accel was double not int- fixed Doc updates Robot and Grind parameter updates
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{54D96A46-84AE-45F0-A547-298E62EA5FC2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2A0E3C-EB90-4E9E-9E22-67728D348C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="44790" yWindow="1770" windowWidth="30420" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="49365" yWindow="1155" windowWidth="24810" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="803" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="283">
   <si>
     <t>Statement</t>
   </si>
@@ -165,12 +165,6 @@
     <t>select_tool(tool_name)</t>
   </si>
   <si>
-    <t>set_part_geometry(FLAT|CYLINDER|SPHERE, diam_mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">free_drive(0=OFF|1=ON) </t>
-  </si>
-  <si>
     <t>30,19</t>
   </si>
   <si>
@@ -528,74 +522,37 @@
     <t>35,1</t>
   </si>
   <si>
-    <t>grind_touch_retract(touch_retract_mm)</t>
-  </si>
-  <si>
     <t>35,2</t>
   </si>
   <si>
-    <t>grind_touch_speed(touch_speed_mm/s)</t>
-  </si>
-  <si>
     <t>35,3</t>
   </si>
   <si>
-    <t>grind_force_dwell(dwell_time_ms)</t>
-  </si>
-  <si>
     <t>35,4</t>
   </si>
   <si>
-    <t>grind_max_wait(max_time_before_retract_ms)</t>
-  </si>
-  <si>
     <t>35,5</t>
   </si>
   <si>
-    <t>grind_max_blend_radius(grind_blend_radius_mm)</t>
-  </si>
-  <si>
     <t>35,6</t>
   </si>
   <si>
-    <t>grind_trial_speed(trial_speed_mm/s)</t>
-  </si>
-  <si>
     <t>35,7</t>
   </si>
   <si>
-    <t>grind_linear_accel(accel_mm/s^2)</t>
-  </si>
-  <si>
     <t>35,8</t>
   </si>
   <si>
-    <t>grind_point_frequency(point_frequency_hz)</t>
-  </si>
-  <si>
     <t>35,9</t>
   </si>
   <si>
-    <t>grind_jog_speed(trial_speed_mm/s)</t>
-  </si>
-  <si>
     <t>35,10</t>
   </si>
   <si>
-    <t>grind_jog_accel(accel_mm/s^2)</t>
-  </si>
-  <si>
     <t>35,11</t>
   </si>
   <si>
-    <t>grind_force_mode_damping(damping:
-0.0 – 1.0)</t>
-  </si>
-  <si>
     <t>35,12</t>
-  </si>
-  <si>
-    <t>grind_force_mode_gain_scaling(scaling: 0.0 – 2.0)</t>
   </si>
   <si>
     <t>35,13</t>
@@ -802,81 +759,123 @@
     <t>int le_write_sysvar(string var_name, string value)</t>
   </si>
   <si>
-    <t>MUST TEST</t>
-  </si>
-  <si>
     <t>LEScript1.txt
 LEScript2.txt</t>
   </si>
   <si>
-    <t>set_part_geometry_N(int n, double diam_mm)</t>
-  </si>
-  <si>
-    <t>set_joint_accel(double accel_dpss)</t>
-  </si>
-  <si>
-    <t>set_joint_speed(double speed_dps)</t>
-  </si>
-  <si>
     <t>set_blend_radius(double blend_radius_mm)</t>
   </si>
   <si>
-    <t>set_linear_accel(double accel_mmpss)</t>
-  </si>
-  <si>
-    <t>set_linear_speed(double speed_mmps)</t>
-  </si>
-  <si>
-    <t>grind_contact_enable(0=Touch OFF,Grind OFF |
+    <t>N/A</t>
+  </si>
+  <si>
+    <t>exec_lescript</t>
+  </si>
+  <si>
+    <t>In User Manual</t>
+  </si>
+  <si>
+    <t>In UR Manual</t>
+  </si>
+  <si>
+    <t>In Gocator Manual</t>
+  </si>
+  <si>
+    <t>end_operation()</t>
+  </si>
+  <si>
+    <t>assertTrue(bool condition)</t>
+  </si>
+  <si>
+    <t>assertFalse(bool condition)</t>
+  </si>
+  <si>
+    <t>assertEqual(var_name, value)</t>
+  </si>
+  <si>
+    <t>assertNotEqual(var_name, value)</t>
+  </si>
+  <si>
+    <t>execline_lescript</t>
+  </si>
+  <si>
+    <t>execline_java</t>
+  </si>
+  <si>
+    <t>execline_python</t>
+  </si>
+  <si>
+    <t>grind_trial_speed(int trial_speed_mm/s)</t>
+  </si>
+  <si>
+    <t>grind_linear_accel(int accel_mm/s^2)</t>
+  </si>
+  <si>
+    <t>set_robot_parameters</t>
+  </si>
+  <si>
+    <t>set_grind_parameters</t>
+  </si>
+  <si>
+    <t>grind_contact_enable(int 0=Touch OFF,Grind OFF |
 1=Touch ON,Grind OFF | 2=Touch ON,Grind ON)</t>
   </si>
   <si>
-    <t>ints or doubles??</t>
-  </si>
-  <si>
-    <t>N/A</t>
-  </si>
-  <si>
-    <t>exec_lescript</t>
-  </si>
-  <si>
-    <t>In User Manual</t>
-  </si>
-  <si>
-    <t>In UR Manual</t>
-  </si>
-  <si>
-    <t>In Gocator Manual</t>
-  </si>
-  <si>
-    <t>end_operation()</t>
-  </si>
-  <si>
-    <t>assertTrue(bool condition)</t>
-  </si>
-  <si>
-    <t>assertFalse(bool condition)</t>
-  </si>
-  <si>
-    <t>assertEqual(var_name, value)</t>
-  </si>
-  <si>
-    <t>assertNotEqual(var_name, value)</t>
-  </si>
-  <si>
-    <t>execline_lescript</t>
-  </si>
-  <si>
-    <t>execline_java</t>
-  </si>
-  <si>
-    <t>execline_python</t>
-  </si>
-  <si>
-    <t>PICK UP HERE</t>
-  </si>
-  <si>
-    <t>LEScript OK… need Java and Python</t>
+    <t>Update Manual ints or doubles</t>
+  </si>
+  <si>
+    <t>set_linear_speed(int speed_mmps)</t>
+  </si>
+  <si>
+    <t>set_linear_accel(int accel_mmpss)</t>
+  </si>
+  <si>
+    <t>set_joint_speed(int speed_dps)</t>
+  </si>
+  <si>
+    <t>set_joint_accel(int accel_dpss)</t>
+  </si>
+  <si>
+    <t>set_part_geometry(string FLAT|CYLINDER|SPHERE, double diam_mm)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_drive(int 0=OFF|1=ON) </t>
+  </si>
+  <si>
+    <t>set_part_geometry_N(int n, double diam_mm) FOR TESTING ONLY</t>
+  </si>
+  <si>
+    <t>SEQUENCE OK?</t>
+  </si>
+  <si>
+    <t>grind_touch_retract(int touch_retract_mm)</t>
+  </si>
+  <si>
+    <t>grind_touch_speed(int touch_speed_mm/s)</t>
+  </si>
+  <si>
+    <t>grind_force_dwell(int dwell_time_ms)</t>
+  </si>
+  <si>
+    <t>grind_max_wait(int max_time_before_retract_ms)</t>
+  </si>
+  <si>
+    <t>grind_max_blend_radius(double grind_blend_radius_mm)</t>
+  </si>
+  <si>
+    <t>grind_point_frequency(int point_frequency_hz)</t>
+  </si>
+  <si>
+    <t>grind_jog_speed(int trial_speed_mm/s)</t>
+  </si>
+  <si>
+    <t>grind_jog_accel(int accel_mm/s^2)</t>
+  </si>
+  <si>
+    <t>grind_force_mode_damping(double damping: 0.0 – 1.0)</t>
+  </si>
+  <si>
+    <t>grind_force_mode_gain_scaling(double scaling: 0.0 – 2.0)</t>
   </si>
 </sst>
 </file>
@@ -1001,7 +1000,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="41">
+  <cellXfs count="39">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1070,18 +1069,9 @@
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="top"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="7" fillId="0" borderId="3" xfId="3" applyBorder="1" applyAlignment="1">
       <alignment vertical="top" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="3" xfId="2" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
@@ -1098,6 +1088,9 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1322,9 +1315,9 @@
   </sheetPr>
   <dimension ref="A1:AC1006"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A27" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="H57" sqref="H57"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1333,34 +1326,34 @@
     <col min="2" max="2" width="10.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="11" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="11" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="38" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
-    <col min="8" max="8" width="42.42578125" customWidth="1"/>
+    <col min="8" max="8" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="39" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="39"/>
-      <c r="D1" s="39"/>
-      <c r="E1" s="40" t="s">
-        <v>270</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="37" t="s">
+        <v>248</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1370,14 +1363,14 @@
       <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="13" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="38"/>
+        <v>200</v>
+      </c>
+      <c r="H2" s="35"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1386,7 +1379,7 @@
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
-      <c r="E3" s="33"/>
+      <c r="E3" s="25"/>
       <c r="F3" s="16"/>
       <c r="G3" s="16"/>
       <c r="H3" s="16"/>
@@ -1408,7 +1401,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19"/>
@@ -1430,7 +1423,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="19"/>
@@ -1452,14 +1445,14 @@
         <v>6</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>250</v>
+        <v>236</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>6</v>
@@ -1474,14 +1467,14 @@
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>205</v>
+        <v>191</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>248</v>
+        <v>234</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>6</v>
@@ -1496,16 +1489,16 @@
         <v>6</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>269</v>
+        <v>247</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>259</v>
+        <v>244</v>
       </c>
       <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>251</v>
+        <v>237</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>6</v>
@@ -1520,16 +1513,16 @@
         <v>6</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>207</v>
+        <v>193</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>206</v>
+        <v>192</v>
       </c>
       <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>249</v>
+        <v>235</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>6</v>
@@ -1544,16 +1537,16 @@
         <v>6</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>208</v>
+        <v>194</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>209</v>
+        <v>195</v>
       </c>
       <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>247</v>
+        <v>233</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>6</v>
@@ -1568,14 +1561,14 @@
         <v>6</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>278</v>
+        <v>256</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>253</v>
+        <v>239</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>6</v>
@@ -1590,14 +1583,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>279</v>
+        <v>257</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>254</v>
+        <v>240</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>6</v>
@@ -1612,7 +1605,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>280</v>
+        <v>258</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="28"/>
@@ -1622,7 +1615,7 @@
       <c r="B14" s="27"/>
       <c r="C14" s="27"/>
       <c r="D14" s="27"/>
-      <c r="E14" s="34"/>
+      <c r="E14" s="32"/>
       <c r="F14" s="19"/>
       <c r="G14" s="19"/>
       <c r="H14" s="19"/>
@@ -1634,63 +1627,63 @@
       <c r="B15" s="25"/>
       <c r="C15" s="25"/>
       <c r="D15" s="25"/>
-      <c r="E15" s="33"/>
+      <c r="E15" s="25"/>
       <c r="F15" s="16"/>
       <c r="G15" s="16"/>
       <c r="H15" s="16"/>
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>210</v>
+        <v>196</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C16" s="27"/>
       <c r="D16" s="27"/>
-      <c r="E16" s="35" t="s">
+      <c r="E16" s="32" t="s">
         <v>6</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>252</v>
+        <v>238</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C17" s="27"/>
       <c r="D17" s="27"/>
-      <c r="E17" s="35" t="s">
+      <c r="E17" s="32" t="s">
         <v>6</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>213</v>
+        <v>199</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>215</v>
+        <v>201</v>
       </c>
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>211</v>
+        <v>197</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C18" s="27"/>
       <c r="D18" s="27"/>
-      <c r="E18" s="35" t="s">
+      <c r="E18" s="32" t="s">
         <v>6</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>212</v>
+        <v>198</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
@@ -1712,7 +1705,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
@@ -1734,7 +1727,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
@@ -1756,7 +1749,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
@@ -1778,14 +1771,14 @@
         <v>6</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>229</v>
+        <v>215</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>6</v>
@@ -1796,14 +1789,14 @@
         <v>6</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>227</v>
+        <v>213</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>255</v>
+        <v>241</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27" t="s">
@@ -1816,14 +1809,14 @@
         <v>6</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>256</v>
+        <v>242</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27" t="s">
@@ -1836,14 +1829,14 @@
         <v>6</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>257</v>
+        <v>243</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27" t="s">
@@ -1856,7 +1849,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>218</v>
+        <v>204</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
@@ -1866,26 +1859,26 @@
       <c r="B27" s="27"/>
       <c r="C27" s="27"/>
       <c r="D27" s="27"/>
-      <c r="E27" s="34"/>
+      <c r="E27" s="32"/>
       <c r="F27" s="19"/>
       <c r="G27" s="19"/>
       <c r="H27" s="19"/>
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>226</v>
+        <v>212</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
       <c r="D28" s="25"/>
-      <c r="E28" s="33"/>
+      <c r="E28" s="25"/>
       <c r="F28" s="16"/>
       <c r="G28" s="16"/>
       <c r="H28" s="16"/>
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>221</v>
+        <v>207</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>6</v>
@@ -1900,14 +1893,14 @@
         <v>6</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>219</v>
+        <v>205</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>6</v>
@@ -1922,7 +1915,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
@@ -1944,7 +1937,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>223</v>
+        <v>209</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -1961,7 +1954,7 @@
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>225</v>
+        <v>211</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="25"/>
@@ -1973,7 +1966,7 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>220</v>
+        <v>206</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>6</v>
@@ -1988,14 +1981,14 @@
         <v>6</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>222</v>
+        <v>208</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>6</v>
@@ -2010,7 +2003,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>224</v>
+        <v>210</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -2032,14 +2025,14 @@
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
       <c r="D37" s="25"/>
-      <c r="E37" s="33"/>
+      <c r="E37" s="25"/>
       <c r="F37" s="16"/>
       <c r="G37" s="16"/>
       <c r="H37" s="16"/>
     </row>
     <row r="38" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>230</v>
+        <v>216</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>6</v>
@@ -2054,14 +2047,14 @@
         <v>6</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>234</v>
+        <v>220</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>231</v>
+        <v>217</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>6</v>
@@ -2076,7 +2069,7 @@
         <v>6</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>235</v>
+        <v>221</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
@@ -2098,7 +2091,7 @@
         <v>6</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>236</v>
+        <v>222</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
@@ -2120,7 +2113,7 @@
         <v>6</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
@@ -2142,7 +2135,7 @@
         <v>6</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
@@ -2151,23 +2144,23 @@
       <c r="A43" s="20" t="s">
         <v>24</v>
       </c>
-      <c r="B43" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="36" t="s">
+      <c r="B43" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E43" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>237</v>
-      </c>
-      <c r="G43" s="31"/>
-      <c r="H43" s="31"/>
+        <v>223</v>
+      </c>
+      <c r="G43" s="30"/>
+      <c r="H43" s="30"/>
       <c r="I43" s="6"/>
       <c r="J43" s="6"/>
       <c r="K43" s="6"/>
@@ -2203,7 +2196,7 @@
         <v>6</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>237</v>
+        <v>223</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
@@ -2225,7 +2218,7 @@
         <v>6</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
@@ -2237,17 +2230,17 @@
       <c r="B46" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C46" s="36" t="s">
-        <v>6</v>
-      </c>
-      <c r="D46" s="36" t="s">
+      <c r="C46" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D46" s="33" t="s">
         <v>6</v>
       </c>
       <c r="E46" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G46" s="19"/>
       <c r="H46" s="19"/>
@@ -2269,14 +2262,14 @@
         <v>6</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>238</v>
+        <v>224</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>228</v>
+        <v>214</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>6</v>
@@ -2291,14 +2284,14 @@
         <v>6</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>239</v>
+        <v>225</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="19"/>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>276</v>
+        <v>254</v>
       </c>
       <c r="B49" s="27" t="s">
         <v>6</v>
@@ -2309,14 +2302,14 @@
         <v>6</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>277</v>
+        <v>255</v>
       </c>
       <c r="B50" s="27" t="s">
         <v>6</v>
@@ -2327,14 +2320,14 @@
         <v>6</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>274</v>
+        <v>252</v>
       </c>
       <c r="B51" s="27"/>
       <c r="C51" s="27" t="s">
@@ -2347,14 +2340,14 @@
         <v>6</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G51" s="19"/>
       <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>275</v>
+        <v>253</v>
       </c>
       <c r="B52" s="27"/>
       <c r="C52" s="27" t="s">
@@ -2367,7 +2360,7 @@
         <v>6</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>217</v>
+        <v>203</v>
       </c>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
@@ -2377,7 +2370,7 @@
       <c r="B53" s="27"/>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
-      <c r="E53" s="34"/>
+      <c r="E53" s="32"/>
       <c r="F53" s="19"/>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
@@ -2389,14 +2382,14 @@
       <c r="B54" s="25"/>
       <c r="C54" s="25"/>
       <c r="D54" s="25"/>
-      <c r="E54" s="33"/>
+      <c r="E54" s="25"/>
       <c r="F54" s="16"/>
       <c r="G54" s="16"/>
       <c r="H54" s="16"/>
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>240</v>
+        <v>226</v>
       </c>
       <c r="B55" s="27" t="s">
         <v>6</v>
@@ -2411,16 +2404,14 @@
         <v>6</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G55" s="19"/>
-      <c r="H55" s="28" t="s">
-        <v>281</v>
-      </c>
+      <c r="H55" s="28"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>241</v>
+        <v>227</v>
       </c>
       <c r="B56" s="27" t="s">
         <v>6</v>
@@ -2435,16 +2426,14 @@
         <v>6</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G56" s="19"/>
-      <c r="H56" s="28" t="s">
-        <v>282</v>
-      </c>
+      <c r="H56" s="28"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>242</v>
+        <v>228</v>
       </c>
       <c r="B57" s="27" t="s">
         <v>6</v>
@@ -2459,16 +2448,14 @@
         <v>6</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G57" s="19"/>
-      <c r="H57" s="28" t="s">
-        <v>258</v>
-      </c>
+      <c r="H57" s="28"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>243</v>
+        <v>229</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>6</v>
@@ -2483,12 +2470,10 @@
         <v>6</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G58" s="19"/>
-      <c r="H58" s="28" t="s">
-        <v>258</v>
-      </c>
+      <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
@@ -2507,12 +2492,10 @@
         <v>6</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G59" s="19"/>
-      <c r="H59" s="28" t="s">
-        <v>258</v>
-      </c>
+      <c r="H59" s="28"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
@@ -2531,19 +2514,17 @@
         <v>6</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>245</v>
+        <v>231</v>
       </c>
       <c r="G60" s="19"/>
-      <c r="H60" s="28" t="s">
-        <v>258</v>
-      </c>
+      <c r="H60" s="28"/>
     </row>
     <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="37"/>
+      <c r="A61" s="34"/>
       <c r="B61" s="27"/>
       <c r="C61" s="27"/>
       <c r="D61" s="27"/>
-      <c r="E61" s="34"/>
+      <c r="E61" s="32"/>
       <c r="F61" s="19"/>
       <c r="G61" s="19"/>
       <c r="H61" s="19"/>
@@ -2555,14 +2536,14 @@
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
       <c r="D62" s="25"/>
-      <c r="E62" s="33"/>
+      <c r="E62" s="25"/>
       <c r="F62" s="16"/>
       <c r="G62" s="16"/>
       <c r="H62" s="16"/>
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>232</v>
+        <v>218</v>
       </c>
       <c r="B63" s="27" t="s">
         <v>6</v>
@@ -2573,7 +2554,7 @@
         <v>6</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
@@ -2591,7 +2572,7 @@
         <v>6</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
@@ -2609,14 +2590,14 @@
         <v>6</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>233</v>
+        <v>219</v>
       </c>
       <c r="B66" s="27" t="s">
         <v>6</v>
@@ -2627,17 +2608,17 @@
         <v>6</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>244</v>
+        <v>230</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="37"/>
+      <c r="A67" s="34"/>
       <c r="B67" s="27"/>
       <c r="C67" s="27"/>
       <c r="D67" s="27"/>
-      <c r="E67" s="34"/>
+      <c r="E67" s="32"/>
       <c r="F67" s="19"/>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
@@ -2649,21 +2630,23 @@
       <c r="B68" s="25"/>
       <c r="C68" s="25"/>
       <c r="D68" s="25"/>
-      <c r="E68" s="33"/>
+      <c r="E68" s="25"/>
       <c r="F68" s="16"/>
       <c r="G68" s="16"/>
       <c r="H68" s="16"/>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>246</v>
+        <v>232</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="27"/>
-      <c r="E69" s="34"/>
+      <c r="E69" s="32" t="s">
+        <v>246</v>
+      </c>
       <c r="F69" s="19"/>
       <c r="G69" s="19"/>
       <c r="H69" s="19"/>
@@ -8310,14 +8293,14 @@
   </sheetPr>
   <dimension ref="A1:AD1075"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="J21" sqref="J21"/>
+      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="70.5703125" style="9" customWidth="1"/>
+    <col min="1" max="1" width="83.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
@@ -8329,25 +8312,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="40" t="s">
-        <v>201</v>
-      </c>
-      <c r="C1" s="38" t="s">
+      <c r="B1" s="37" t="s">
+        <v>187</v>
+      </c>
+      <c r="C1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="38"/>
-      <c r="E1" s="38"/>
-      <c r="F1" s="40" t="s">
-        <v>271</v>
-      </c>
-      <c r="G1" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="H1" s="38"/>
-      <c r="I1" s="38" t="s">
+      <c r="D1" s="35"/>
+      <c r="E1" s="35"/>
+      <c r="F1" s="37" t="s">
+        <v>249</v>
+      </c>
+      <c r="G1" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="H1" s="35"/>
+      <c r="I1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1"/>
@@ -8373,8 +8356,8 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
-      <c r="B2" s="40"/>
+      <c r="A2" s="35"/>
+      <c r="B2" s="37"/>
       <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
@@ -8384,14 +8367,14 @@
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="40"/>
+      <c r="F2" s="37"/>
       <c r="G2" s="13" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="I2" s="38"/>
+        <v>200</v>
+      </c>
+      <c r="I2" s="35"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -8422,8 +8405,10 @@
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="25"/>
-      <c r="G3" s="16"/>
+      <c r="F3" s="25" t="s">
+        <v>272</v>
+      </c>
+      <c r="G3" s="20"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
@@ -8466,7 +8451,7 @@
       <c r="D6" s="25"/>
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
-      <c r="G6" s="24"/>
+      <c r="G6" s="20"/>
       <c r="H6" s="24"/>
       <c r="I6" s="16"/>
     </row>
@@ -8508,7 +8493,7 @@
         <v>6</v>
       </c>
       <c r="F8" s="27"/>
-      <c r="G8" s="28"/>
+      <c r="G8" s="20"/>
       <c r="H8" s="29"/>
       <c r="I8" s="19"/>
     </row>
@@ -8529,7 +8514,7 @@
         <v>6</v>
       </c>
       <c r="F9" s="27"/>
-      <c r="G9" s="28"/>
+      <c r="G9" s="20"/>
       <c r="H9" s="29"/>
       <c r="I9" s="19"/>
     </row>
@@ -8540,7 +8525,7 @@
       <c r="D10" s="27"/>
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
-      <c r="G10" s="28"/>
+      <c r="G10" s="20"/>
       <c r="H10" s="29"/>
       <c r="I10" s="19"/>
     </row>
@@ -8553,13 +8538,13 @@
       <c r="D11" s="25"/>
       <c r="E11" s="25"/>
       <c r="F11" s="25"/>
-      <c r="G11" s="30"/>
+      <c r="G11" s="20"/>
       <c r="H11" s="16"/>
       <c r="I11" s="16"/>
     </row>
     <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>41</v>
+        <v>46</v>
       </c>
       <c r="B12" s="26"/>
       <c r="C12" s="27" t="s">
@@ -8572,15 +8557,15 @@
         <v>6</v>
       </c>
       <c r="F12" s="27"/>
-      <c r="G12" s="28"/>
-      <c r="H12" s="19"/>
+      <c r="G12" s="20"/>
+      <c r="H12" s="21"/>
       <c r="I12" s="19"/>
     </row>
     <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B13" s="18"/>
+        <v>269</v>
+      </c>
+      <c r="B13" s="26"/>
       <c r="C13" s="27" t="s">
         <v>6</v>
       </c>
@@ -8590,14 +8575,14 @@
       <c r="E13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="19"/>
-      <c r="G13" s="28"/>
-      <c r="H13" s="19"/>
+      <c r="F13" s="27"/>
+      <c r="G13" s="20"/>
+      <c r="H13" s="21"/>
       <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="B14" s="26"/>
       <c r="C14" s="27" t="s">
@@ -8610,15 +8595,15 @@
         <v>6</v>
       </c>
       <c r="F14" s="27"/>
-      <c r="G14" s="21"/>
-      <c r="H14" s="21"/>
+      <c r="G14" s="20"/>
+      <c r="H14" s="19"/>
       <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B15" s="26"/>
+        <v>11</v>
+      </c>
+      <c r="B15" s="18"/>
       <c r="C15" s="27" t="s">
         <v>6</v>
       </c>
@@ -8628,14 +8613,14 @@
       <c r="E15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="27"/>
-      <c r="G15" s="21"/>
-      <c r="H15" s="21"/>
+      <c r="F15" s="19"/>
+      <c r="G15" s="20"/>
+      <c r="H15" s="19"/>
       <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="B16" s="26"/>
       <c r="C16" s="27" t="s">
@@ -8648,13 +8633,13 @@
         <v>6</v>
       </c>
       <c r="F16" s="27"/>
-      <c r="G16" s="21"/>
+      <c r="G16" s="20"/>
       <c r="H16" s="21"/>
       <c r="I16" s="19"/>
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="B17" s="26"/>
       <c r="C17" s="27" t="s">
@@ -8667,13 +8652,13 @@
         <v>6</v>
       </c>
       <c r="F17" s="27"/>
-      <c r="G17" s="21"/>
+      <c r="G17" s="20"/>
       <c r="H17" s="21"/>
       <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B18" s="26"/>
       <c r="C18" s="27" t="s">
@@ -8686,13 +8671,13 @@
         <v>6</v>
       </c>
       <c r="F18" s="27"/>
-      <c r="G18" s="21"/>
+      <c r="G18" s="20"/>
       <c r="H18" s="21"/>
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="B19" s="26"/>
       <c r="C19" s="27" t="s">
@@ -8705,16 +8690,16 @@
         <v>6</v>
       </c>
       <c r="F19" s="27"/>
-      <c r="G19" s="21"/>
+      <c r="G19" s="20"/>
       <c r="H19" s="21"/>
       <c r="I19" s="19"/>
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>48</v>
+        <v>270</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>6</v>
@@ -8726,7 +8711,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="27"/>
-      <c r="G20" s="21"/>
+      <c r="G20" s="20"/>
       <c r="H20" s="21"/>
       <c r="I20" s="19"/>
     </row>
@@ -8737,29 +8722,29 @@
       <c r="D21" s="27"/>
       <c r="E21" s="27"/>
       <c r="F21" s="27"/>
-      <c r="G21" s="21"/>
+      <c r="G21" s="20"/>
       <c r="H21" s="21"/>
       <c r="I21" s="19"/>
     </row>
     <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A22" s="24" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B22" s="25"/>
       <c r="C22" s="25"/>
       <c r="D22" s="25"/>
       <c r="E22" s="25"/>
       <c r="F22" s="25"/>
-      <c r="G22" s="15"/>
+      <c r="G22" s="20"/>
       <c r="H22" s="15"/>
       <c r="I22" s="16"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>6</v>
@@ -8771,16 +8756,16 @@
         <v>6</v>
       </c>
       <c r="F23" s="27"/>
-      <c r="G23" s="21"/>
+      <c r="G23" s="20"/>
       <c r="H23" s="21"/>
       <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="B24" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C24" s="27" t="s">
         <v>6</v>
@@ -8792,16 +8777,16 @@
         <v>6</v>
       </c>
       <c r="F24" s="27"/>
-      <c r="G24" s="21"/>
+      <c r="G24" s="20"/>
       <c r="H24" s="21"/>
       <c r="I24" s="19"/>
     </row>
     <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B25" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C25" s="27" t="s">
         <v>6</v>
@@ -8813,7 +8798,7 @@
         <v>6</v>
       </c>
       <c r="F25" s="27"/>
-      <c r="G25" s="21"/>
+      <c r="G25" s="20"/>
       <c r="H25" s="21"/>
       <c r="I25" s="19"/>
     </row>
@@ -8824,16 +8809,16 @@
       <c r="D26" s="27"/>
       <c r="E26" s="27"/>
       <c r="F26" s="27"/>
-      <c r="G26" s="21"/>
+      <c r="G26" s="20"/>
       <c r="H26" s="21"/>
       <c r="I26" s="19"/>
     </row>
     <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>6</v>
@@ -8845,16 +8830,16 @@
         <v>6</v>
       </c>
       <c r="F27" s="27"/>
-      <c r="G27" s="21"/>
+      <c r="G27" s="20"/>
       <c r="H27" s="21"/>
       <c r="I27" s="19"/>
     </row>
     <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>6</v>
@@ -8866,16 +8851,16 @@
         <v>6</v>
       </c>
       <c r="F28" s="27"/>
-      <c r="G28" s="21"/>
+      <c r="G28" s="20"/>
       <c r="H28" s="21"/>
       <c r="I28" s="19"/>
     </row>
     <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>61</v>
+        <v>59</v>
       </c>
       <c r="B29" s="26" t="s">
-        <v>62</v>
+        <v>60</v>
       </c>
       <c r="C29" s="27" t="s">
         <v>6</v>
@@ -8887,7 +8872,7 @@
         <v>6</v>
       </c>
       <c r="F29" s="27"/>
-      <c r="G29" s="21"/>
+      <c r="G29" s="20"/>
       <c r="H29" s="21"/>
       <c r="I29" s="19"/>
     </row>
@@ -8898,16 +8883,16 @@
       <c r="D30" s="27"/>
       <c r="E30" s="27"/>
       <c r="F30" s="27"/>
-      <c r="G30" s="21"/>
+      <c r="G30" s="20"/>
       <c r="H30" s="21"/>
       <c r="I30" s="19"/>
     </row>
     <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>63</v>
+        <v>61</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -8919,16 +8904,16 @@
         <v>6</v>
       </c>
       <c r="F31" s="27"/>
-      <c r="G31" s="21"/>
+      <c r="G31" s="20"/>
       <c r="H31" s="21"/>
       <c r="I31" s="19"/>
     </row>
     <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>66</v>
+        <v>64</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -8940,7 +8925,7 @@
         <v>6</v>
       </c>
       <c r="F32" s="27"/>
-      <c r="G32" s="21"/>
+      <c r="G32" s="20"/>
       <c r="H32" s="21"/>
       <c r="I32" s="19"/>
     </row>
@@ -8951,16 +8936,16 @@
       <c r="D33" s="27"/>
       <c r="E33" s="27"/>
       <c r="F33" s="27"/>
-      <c r="G33" s="21"/>
+      <c r="G33" s="20"/>
       <c r="H33" s="21"/>
       <c r="I33" s="19"/>
     </row>
     <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>67</v>
+        <v>65</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>68</v>
+        <v>66</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>6</v>
@@ -8972,16 +8957,16 @@
         <v>6</v>
       </c>
       <c r="F34" s="27"/>
-      <c r="G34" s="21"/>
+      <c r="G34" s="20"/>
       <c r="H34" s="21"/>
       <c r="I34" s="19"/>
     </row>
     <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>69</v>
+        <v>67</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>70</v>
+        <v>68</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>6</v>
@@ -8993,16 +8978,16 @@
         <v>6</v>
       </c>
       <c r="F35" s="27"/>
-      <c r="G35" s="21"/>
+      <c r="G35" s="20"/>
       <c r="H35" s="21"/>
       <c r="I35" s="19"/>
     </row>
     <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>71</v>
+        <v>69</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>72</v>
+        <v>70</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>6</v>
@@ -9014,7 +8999,7 @@
         <v>6</v>
       </c>
       <c r="F36" s="27"/>
-      <c r="G36" s="21"/>
+      <c r="G36" s="20"/>
       <c r="H36" s="21"/>
       <c r="I36" s="19"/>
     </row>
@@ -9025,29 +9010,29 @@
       <c r="D37" s="27"/>
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
-      <c r="G37" s="21"/>
+      <c r="G37" s="20"/>
       <c r="H37" s="21"/>
       <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>73</v>
+        <v>71</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
       <c r="D38" s="25"/>
       <c r="E38" s="25"/>
       <c r="F38" s="25"/>
-      <c r="G38" s="16"/>
+      <c r="G38" s="20"/>
       <c r="H38" s="16"/>
       <c r="I38" s="16"/>
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>74</v>
+        <v>72</v>
       </c>
       <c r="B39" s="26" t="s">
-        <v>75</v>
+        <v>73</v>
       </c>
       <c r="C39" s="27" t="s">
         <v>6</v>
@@ -9059,16 +9044,16 @@
         <v>6</v>
       </c>
       <c r="F39" s="27"/>
-      <c r="G39" s="21"/>
+      <c r="G39" s="20"/>
       <c r="H39" s="21"/>
       <c r="I39" s="19"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>76</v>
+        <v>74</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>77</v>
+        <v>75</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>6</v>
@@ -9080,16 +9065,16 @@
         <v>6</v>
       </c>
       <c r="F40" s="27"/>
-      <c r="G40" s="21"/>
+      <c r="G40" s="20"/>
       <c r="H40" s="21"/>
       <c r="I40" s="19"/>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>78</v>
+        <v>76</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>79</v>
+        <v>77</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>6</v>
@@ -9101,16 +9086,16 @@
         <v>6</v>
       </c>
       <c r="F41" s="27"/>
-      <c r="G41" s="21"/>
+      <c r="G41" s="20"/>
       <c r="H41" s="21"/>
       <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>80</v>
+        <v>78</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>81</v>
+        <v>79</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>6</v>
@@ -9123,15 +9108,15 @@
       </c>
       <c r="F42" s="27"/>
       <c r="G42" s="20"/>
-      <c r="H42" s="31"/>
+      <c r="H42" s="30"/>
       <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>82</v>
+        <v>80</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>83</v>
+        <v>81</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>6</v>
@@ -9160,23 +9145,23 @@
     </row>
     <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A45" s="24" t="s">
-        <v>84</v>
+        <v>82</v>
       </c>
       <c r="B45" s="25"/>
       <c r="C45" s="25"/>
       <c r="D45" s="25"/>
       <c r="E45" s="25"/>
       <c r="F45" s="25"/>
-      <c r="G45" s="16"/>
+      <c r="G45" s="20"/>
       <c r="H45" s="16"/>
       <c r="I45" s="16"/>
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>85</v>
+        <v>83</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>6</v>
@@ -9194,10 +9179,10 @@
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>87</v>
+        <v>85</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>86</v>
+        <v>84</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>6</v>
@@ -9215,10 +9200,10 @@
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>88</v>
+        <v>86</v>
       </c>
       <c r="B48" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C48" s="27" t="s">
         <v>6</v>
@@ -9236,10 +9221,10 @@
     </row>
     <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="B49" s="26" t="s">
-        <v>89</v>
+        <v>87</v>
       </c>
       <c r="C49" s="27" t="s">
         <v>6</v>
@@ -9257,10 +9242,10 @@
     </row>
     <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
       <c r="B50" s="26" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C50" s="27" t="s">
         <v>6</v>
@@ -9272,16 +9257,16 @@
         <v>6</v>
       </c>
       <c r="F50" s="27"/>
-      <c r="G50" s="19"/>
+      <c r="G50" s="20"/>
       <c r="H50" s="19"/>
       <c r="I50" s="19"/>
     </row>
     <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
       <c r="B51" s="26" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C51" s="27" t="s">
         <v>6</v>
@@ -9293,7 +9278,7 @@
         <v>6</v>
       </c>
       <c r="F51" s="27"/>
-      <c r="G51" s="19"/>
+      <c r="G51" s="20"/>
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
     </row>
@@ -9304,20 +9289,20 @@
       <c r="D52" s="27"/>
       <c r="E52" s="27"/>
       <c r="F52" s="27"/>
-      <c r="G52" s="28"/>
+      <c r="G52" s="20"/>
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
     </row>
     <row r="53" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A53" s="24" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
       <c r="B53" s="25"/>
       <c r="C53" s="25"/>
       <c r="D53" s="25"/>
       <c r="E53" s="25"/>
       <c r="F53" s="25"/>
-      <c r="G53" s="16"/>
+      <c r="G53" s="20"/>
       <c r="H53" s="16"/>
       <c r="I53" s="16"/>
     </row>
@@ -9326,7 +9311,7 @@
         <v>265</v>
       </c>
       <c r="B54" s="26" t="s">
-        <v>96</v>
+        <v>94</v>
       </c>
       <c r="C54" s="27" t="s">
         <v>6</v>
@@ -9337,17 +9322,23 @@
       <c r="E54" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F54" s="27"/>
-      <c r="G54" s="28"/>
+      <c r="F54" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G54" s="20" t="s">
+        <v>261</v>
+      </c>
       <c r="H54" s="19"/>
-      <c r="I54" s="19"/>
+      <c r="I54" s="19" t="s">
+        <v>264</v>
+      </c>
     </row>
     <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>264</v>
+        <v>266</v>
       </c>
       <c r="B55" s="26" t="s">
-        <v>97</v>
+        <v>95</v>
       </c>
       <c r="C55" s="27" t="s">
         <v>6</v>
@@ -9358,17 +9349,21 @@
       <c r="E55" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F55" s="27"/>
-      <c r="G55" s="28"/>
+      <c r="F55" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G55" s="20" t="s">
+        <v>261</v>
+      </c>
       <c r="H55" s="19"/>
       <c r="I55" s="19"/>
     </row>
     <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>263</v>
+        <v>245</v>
       </c>
       <c r="B56" s="26" t="s">
-        <v>98</v>
+        <v>96</v>
       </c>
       <c r="C56" s="27" t="s">
         <v>6</v>
@@ -9379,17 +9374,21 @@
       <c r="E56" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F56" s="27"/>
-      <c r="G56" s="28"/>
+      <c r="F56" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G56" s="20" t="s">
+        <v>261</v>
+      </c>
       <c r="H56" s="19"/>
       <c r="I56" s="19"/>
     </row>
     <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>262</v>
+        <v>267</v>
       </c>
       <c r="B57" s="26" t="s">
-        <v>99</v>
+        <v>97</v>
       </c>
       <c r="C57" s="27" t="s">
         <v>6</v>
@@ -9400,38 +9399,46 @@
       <c r="E57" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F57" s="27"/>
-      <c r="G57" s="28"/>
+      <c r="F57" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G57" s="20" t="s">
+        <v>261</v>
+      </c>
       <c r="H57" s="19"/>
       <c r="I57" s="19"/>
     </row>
     <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
+        <v>268</v>
+      </c>
+      <c r="B58" s="26" t="s">
+        <v>98</v>
+      </c>
+      <c r="C58" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D58" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E58" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F58" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G58" s="20" t="s">
         <v>261</v>
       </c>
-      <c r="B58" s="26" t="s">
-        <v>100</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="27"/>
-      <c r="G58" s="19"/>
       <c r="H58" s="19"/>
       <c r="I58" s="19"/>
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>260</v>
+        <v>271</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>101</v>
+        <v>99</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>6</v>
@@ -9442,8 +9449,12 @@
       <c r="E59" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F59" s="27"/>
-      <c r="G59" s="21"/>
+      <c r="F59" s="27" t="s">
+        <v>246</v>
+      </c>
+      <c r="G59" s="20" t="s">
+        <v>261</v>
+      </c>
       <c r="H59" s="21"/>
       <c r="I59" s="19"/>
     </row>
@@ -9460,23 +9471,23 @@
     </row>
     <row r="61" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A61" s="24" t="s">
-        <v>102</v>
+        <v>100</v>
       </c>
       <c r="B61" s="25"/>
       <c r="C61" s="25"/>
       <c r="D61" s="25"/>
       <c r="E61" s="25"/>
       <c r="F61" s="25"/>
-      <c r="G61" s="16"/>
+      <c r="G61" s="20"/>
       <c r="H61" s="16"/>
       <c r="I61" s="16"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>103</v>
+        <v>101</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>104</v>
+        <v>102</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>6</v>
@@ -9492,19 +9503,19 @@
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>105</v>
+        <v>103</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>106</v>
+        <v>104</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E63" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F63" s="27"/>
       <c r="G63" s="20"/>
@@ -9513,94 +9524,94 @@
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>107</v>
+        <v>105</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>108</v>
+        <v>106</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E64" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F64" s="27"/>
-      <c r="G64" s="19"/>
+      <c r="G64" s="20"/>
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>109</v>
+        <v>107</v>
       </c>
       <c r="B65" s="26" t="s">
-        <v>110</v>
+        <v>108</v>
       </c>
       <c r="C65" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D65" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E65" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F65" s="27"/>
-      <c r="G65" s="21"/>
+      <c r="G65" s="20"/>
       <c r="H65" s="21"/>
       <c r="I65" s="19"/>
     </row>
     <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
       <c r="B66" s="26" t="s">
-        <v>112</v>
+        <v>110</v>
       </c>
       <c r="C66" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D66" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E66" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F66" s="27"/>
-      <c r="G66" s="19"/>
+      <c r="G66" s="20"/>
       <c r="H66" s="19"/>
       <c r="I66" s="19"/>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>113</v>
+        <v>111</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>114</v>
+        <v>112</v>
       </c>
       <c r="C67" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D67" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E67" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F67" s="27"/>
-      <c r="G67" s="19"/>
+      <c r="G67" s="20"/>
       <c r="H67" s="19"/>
       <c r="I67" s="19"/>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>115</v>
+        <v>113</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>116</v>
+        <v>114</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>6</v>
@@ -9610,16 +9621,16 @@
         <v>6</v>
       </c>
       <c r="F68" s="27"/>
-      <c r="G68" s="19"/>
+      <c r="G68" s="20"/>
       <c r="H68" s="19"/>
       <c r="I68" s="19"/>
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>117</v>
+        <v>115</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>118</v>
+        <v>116</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>6</v>
@@ -9629,16 +9640,16 @@
         <v>6</v>
       </c>
       <c r="F69" s="27"/>
-      <c r="G69" s="19"/>
+      <c r="G69" s="20"/>
       <c r="H69" s="19"/>
       <c r="I69" s="19"/>
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A70" s="20" t="s">
-        <v>119</v>
+        <v>117</v>
       </c>
       <c r="B70" s="26" t="s">
-        <v>120</v>
+        <v>118</v>
       </c>
       <c r="C70" s="27" t="s">
         <v>6</v>
@@ -9648,16 +9659,16 @@
         <v>6</v>
       </c>
       <c r="F70" s="27"/>
-      <c r="G70" s="19"/>
+      <c r="G70" s="20"/>
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
     </row>
     <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A71" s="20" t="s">
-        <v>121</v>
+        <v>119</v>
       </c>
       <c r="B71" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C71" s="27" t="s">
         <v>6</v>
@@ -9667,28 +9678,28 @@
         <v>6</v>
       </c>
       <c r="F71" s="27"/>
-      <c r="G71" s="19"/>
+      <c r="G71" s="20"/>
       <c r="H71" s="19"/>
       <c r="I71" s="19"/>
     </row>
     <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>122</v>
+        <v>120</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>123</v>
+        <v>121</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F72" s="27"/>
-      <c r="G72" s="19"/>
+      <c r="G72" s="20"/>
       <c r="H72" s="19"/>
       <c r="I72" s="19"/>
     </row>
@@ -9699,272 +9710,272 @@
       <c r="D73" s="27"/>
       <c r="E73" s="27"/>
       <c r="F73" s="27"/>
-      <c r="G73" s="19"/>
+      <c r="G73" s="20"/>
       <c r="H73" s="19"/>
       <c r="I73" s="19"/>
     </row>
     <row r="74" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A74" s="24" t="s">
-        <v>124</v>
+        <v>122</v>
       </c>
       <c r="B74" s="25"/>
       <c r="C74" s="25"/>
       <c r="D74" s="25"/>
       <c r="E74" s="25"/>
       <c r="F74" s="25"/>
-      <c r="G74" s="16"/>
+      <c r="G74" s="20"/>
       <c r="H74" s="16"/>
       <c r="I74" s="16"/>
     </row>
     <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A75" s="20" t="s">
-        <v>125</v>
+        <v>123</v>
       </c>
       <c r="B75" s="26" t="s">
-        <v>126</v>
+        <v>124</v>
       </c>
       <c r="C75" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D75" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E75" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F75" s="27"/>
-      <c r="G75" s="19"/>
+      <c r="G75" s="20"/>
       <c r="H75" s="19"/>
       <c r="I75" s="19"/>
     </row>
     <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A76" s="20" t="s">
-        <v>127</v>
+        <v>125</v>
       </c>
       <c r="B76" s="26" t="s">
-        <v>128</v>
+        <v>126</v>
       </c>
       <c r="C76" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D76" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E76" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F76" s="27"/>
-      <c r="G76" s="19"/>
+      <c r="G76" s="20"/>
       <c r="H76" s="19"/>
       <c r="I76" s="19"/>
     </row>
     <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A77" s="20" t="s">
-        <v>129</v>
+        <v>127</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>130</v>
+        <v>128</v>
       </c>
       <c r="C77" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F77" s="27"/>
-      <c r="G77" s="19"/>
+      <c r="G77" s="20"/>
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
     </row>
     <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A78" s="20" t="s">
-        <v>131</v>
+        <v>129</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>132</v>
+        <v>130</v>
       </c>
       <c r="C78" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F78" s="27"/>
-      <c r="G78" s="19"/>
+      <c r="G78" s="20"/>
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
     </row>
     <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="20" t="s">
-        <v>133</v>
+        <v>131</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>134</v>
+        <v>132</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F79" s="27"/>
-      <c r="G79" s="19"/>
+      <c r="G79" s="20"/>
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
     </row>
     <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A80" s="20" t="s">
-        <v>135</v>
+        <v>133</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>136</v>
+        <v>134</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F80" s="27"/>
-      <c r="G80" s="19"/>
+      <c r="G80" s="20"/>
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
     </row>
     <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="20" t="s">
-        <v>137</v>
+        <v>135</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>138</v>
+        <v>136</v>
       </c>
       <c r="C81" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F81" s="27"/>
-      <c r="G81" s="19"/>
+      <c r="G81" s="20"/>
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
     </row>
     <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A82" s="20" t="s">
-        <v>139</v>
+        <v>137</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F82" s="27"/>
-      <c r="G82" s="19"/>
+      <c r="G82" s="20"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
     </row>
     <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A83" s="20" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>142</v>
+        <v>140</v>
       </c>
       <c r="C83" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D83" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F83" s="27"/>
-      <c r="G83" s="19"/>
+      <c r="G83" s="20"/>
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
     </row>
     <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="20" t="s">
-        <v>143</v>
+        <v>141</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>144</v>
+        <v>142</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F84" s="27"/>
-      <c r="G84" s="19"/>
+      <c r="G84" s="20"/>
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
-        <v>145</v>
+        <v>143</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>146</v>
+        <v>144</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F85" s="27"/>
-      <c r="G85" s="19"/>
+      <c r="G85" s="20"/>
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A86" s="20" t="s">
-        <v>147</v>
+        <v>145</v>
       </c>
       <c r="B86" s="26" t="s">
-        <v>148</v>
+        <v>146</v>
       </c>
       <c r="C86" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D86" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E86" s="27" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="F86" s="27"/>
-      <c r="G86" s="19"/>
+      <c r="G86" s="20"/>
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
     </row>
@@ -9975,29 +9986,29 @@
       <c r="D87" s="27"/>
       <c r="E87" s="27"/>
       <c r="F87" s="27"/>
-      <c r="G87" s="19"/>
+      <c r="G87" s="20"/>
       <c r="H87" s="19"/>
       <c r="I87" s="19"/>
     </row>
     <row r="88" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A88" s="24" t="s">
-        <v>149</v>
+        <v>147</v>
       </c>
       <c r="B88" s="25"/>
       <c r="C88" s="25"/>
       <c r="D88" s="25"/>
       <c r="E88" s="25"/>
       <c r="F88" s="25"/>
-      <c r="G88" s="16"/>
+      <c r="G88" s="20"/>
       <c r="H88" s="16"/>
       <c r="I88" s="16"/>
     </row>
     <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A89" s="32" t="s">
-        <v>150</v>
+      <c r="A89" s="31" t="s">
+        <v>148</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>151</v>
+        <v>149</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>6</v>
@@ -10011,16 +10022,15 @@
       <c r="F89" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G89" s="19"/>
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A90" s="32" t="s">
-        <v>152</v>
+      <c r="A90" s="31" t="s">
+        <v>150</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>153</v>
+        <v>151</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>6</v>
@@ -10034,16 +10044,16 @@
       <c r="F90" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G90" s="19"/>
+      <c r="G90" s="20"/>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
     <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A91" s="32" t="s">
-        <v>154</v>
+      <c r="A91" s="31" t="s">
+        <v>152</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>155</v>
+        <v>153</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>6</v>
@@ -10057,16 +10067,16 @@
       <c r="F91" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G91" s="19"/>
+      <c r="G91" s="20"/>
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
     <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A92" s="32" t="s">
-        <v>156</v>
+      <c r="A92" s="31" t="s">
+        <v>154</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>157</v>
+        <v>155</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>6</v>
@@ -10080,16 +10090,16 @@
       <c r="F92" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G92" s="19"/>
+      <c r="G92" s="20"/>
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
     <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A93" s="32" t="s">
-        <v>158</v>
+      <c r="A93" s="31" t="s">
+        <v>156</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>159</v>
+        <v>157</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>6</v>
@@ -10103,16 +10113,16 @@
       <c r="F93" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G93" s="19"/>
+      <c r="G93" s="20"/>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
     <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A94" s="32" t="s">
-        <v>160</v>
+      <c r="A94" s="31" t="s">
+        <v>158</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>161</v>
+        <v>159</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>6</v>
@@ -10126,16 +10136,16 @@
       <c r="F94" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G94" s="19"/>
+      <c r="G94" s="20"/>
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
     <row r="95" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A95" s="32" t="s">
-        <v>162</v>
+      <c r="A95" s="31" t="s">
+        <v>160</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>163</v>
+        <v>161</v>
       </c>
       <c r="C95" s="27" t="s">
         <v>6</v>
@@ -10149,16 +10159,16 @@
       <c r="F95" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G95" s="19"/>
+      <c r="G95" s="20"/>
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>164</v>
+        <v>162</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>165</v>
+        <v>163</v>
       </c>
       <c r="C96" s="27" t="s">
         <v>6</v>
@@ -10172,7 +10182,7 @@
       <c r="F96" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G96" s="19"/>
+      <c r="G96" s="20"/>
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
@@ -10183,29 +10193,29 @@
       <c r="D97" s="27"/>
       <c r="E97" s="27"/>
       <c r="F97" s="27"/>
-      <c r="G97" s="19"/>
+      <c r="G97" s="20"/>
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A98" s="24" t="s">
-        <v>166</v>
+        <v>164</v>
       </c>
       <c r="B98" s="25"/>
       <c r="C98" s="25"/>
       <c r="D98" s="25"/>
       <c r="E98" s="25"/>
       <c r="F98" s="25"/>
-      <c r="G98" s="16"/>
+      <c r="G98" s="20"/>
       <c r="H98" s="16"/>
       <c r="I98" s="16"/>
     </row>
     <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A99" s="32" t="s">
-        <v>266</v>
+      <c r="A99" s="31" t="s">
+        <v>263</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>167</v>
+        <v>165</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>6</v>
@@ -10216,19 +10226,19 @@
       <c r="E99" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F99" s="27"/>
-      <c r="G99" s="19" t="s">
-        <v>267</v>
-      </c>
+      <c r="F99" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G99" s="20"/>
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="20" t="s">
-        <v>168</v>
+        <v>273</v>
       </c>
       <c r="B100" s="26" t="s">
-        <v>169</v>
+        <v>166</v>
       </c>
       <c r="C100" s="27" t="s">
         <v>6</v>
@@ -10239,19 +10249,21 @@
       <c r="E100" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F100" s="27"/>
-      <c r="G100" s="19" t="s">
-        <v>267</v>
+      <c r="F100" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G100" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H100" s="19"/>
       <c r="I100" s="19"/>
     </row>
     <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A101" s="20" t="s">
-        <v>170</v>
+        <v>274</v>
       </c>
       <c r="B101" s="26" t="s">
-        <v>171</v>
+        <v>167</v>
       </c>
       <c r="C101" s="27" t="s">
         <v>6</v>
@@ -10262,19 +10274,21 @@
       <c r="E101" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F101" s="27"/>
-      <c r="G101" s="19" t="s">
-        <v>267</v>
+      <c r="F101" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G101" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H101" s="19"/>
       <c r="I101" s="19"/>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
-        <v>172</v>
+        <v>275</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>173</v>
+        <v>168</v>
       </c>
       <c r="C102" s="27" t="s">
         <v>6</v>
@@ -10285,19 +10299,21 @@
       <c r="E102" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F102" s="27"/>
-      <c r="G102" s="19" t="s">
-        <v>267</v>
+      <c r="F102" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G102" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
-        <v>174</v>
+        <v>276</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>175</v>
+        <v>169</v>
       </c>
       <c r="C103" s="27" t="s">
         <v>6</v>
@@ -10308,19 +10324,21 @@
       <c r="E103" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F103" s="27"/>
-      <c r="G103" s="19" t="s">
-        <v>267</v>
+      <c r="F103" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G103" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
-        <v>176</v>
+        <v>277</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>177</v>
+        <v>170</v>
       </c>
       <c r="C104" s="27" t="s">
         <v>6</v>
@@ -10331,19 +10349,21 @@
       <c r="E104" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F104" s="27"/>
-      <c r="G104" s="19" t="s">
-        <v>267</v>
+      <c r="F104" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G104" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
-        <v>178</v>
+        <v>259</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>179</v>
+        <v>171</v>
       </c>
       <c r="C105" s="27" t="s">
         <v>6</v>
@@ -10354,19 +10374,21 @@
       <c r="E105" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F105" s="27"/>
-      <c r="G105" s="19" t="s">
-        <v>267</v>
+      <c r="F105" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G105" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
-        <v>180</v>
+        <v>260</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>181</v>
+        <v>172</v>
       </c>
       <c r="C106" s="27" t="s">
         <v>6</v>
@@ -10377,19 +10399,21 @@
       <c r="E106" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F106" s="27"/>
-      <c r="G106" s="19" t="s">
-        <v>267</v>
+      <c r="F106" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G106" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
-        <v>182</v>
+        <v>278</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>183</v>
+        <v>173</v>
       </c>
       <c r="C107" s="27" t="s">
         <v>6</v>
@@ -10400,19 +10424,21 @@
       <c r="E107" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F107" s="27"/>
-      <c r="G107" s="19" t="s">
-        <v>267</v>
+      <c r="F107" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G107" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
-        <v>184</v>
+        <v>279</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="C108" s="27" t="s">
         <v>6</v>
@@ -10423,19 +10449,21 @@
       <c r="E108" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F108" s="27"/>
-      <c r="G108" s="19" t="s">
-        <v>267</v>
+      <c r="F108" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G108" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
-        <v>186</v>
+        <v>280</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>187</v>
+        <v>175</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>6</v>
@@ -10446,19 +10474,21 @@
       <c r="E109" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F109" s="27"/>
-      <c r="G109" s="19" t="s">
-        <v>267</v>
+      <c r="F109" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G109" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A110" s="20" t="s">
-        <v>188</v>
+      <c r="A110" s="31" t="s">
+        <v>281</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>189</v>
+        <v>176</v>
       </c>
       <c r="C110" s="27" t="s">
         <v>6</v>
@@ -10469,19 +10499,21 @@
       <c r="E110" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F110" s="27"/>
-      <c r="G110" s="19" t="s">
-        <v>267</v>
+      <c r="F110" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G110" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
-        <v>190</v>
+        <v>282</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>191</v>
+        <v>177</v>
       </c>
       <c r="C111" s="27" t="s">
         <v>6</v>
@@ -10492,9 +10524,11 @@
       <c r="E111" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F111" s="27"/>
-      <c r="G111" s="19" t="s">
-        <v>267</v>
+      <c r="F111" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G111" s="20" t="s">
+        <v>262</v>
       </c>
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
@@ -17257,6 +17291,7 @@
     <mergeCell ref="F1:F2"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" horizontalDpi="300" verticalDpi="300" r:id="rId1"/>
 </worksheet>
 </file>
 
@@ -17285,22 +17320,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="38" t="s">
+      <c r="A1" s="35" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
+      <c r="B1" s="35" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="38"/>
-      <c r="D1" s="38"/>
-      <c r="E1" s="40" t="s">
-        <v>272</v>
-      </c>
-      <c r="F1" s="38" t="s">
-        <v>204</v>
-      </c>
-      <c r="G1" s="38"/>
-      <c r="H1" s="38" t="s">
+      <c r="C1" s="35"/>
+      <c r="D1" s="35"/>
+      <c r="E1" s="37" t="s">
+        <v>250</v>
+      </c>
+      <c r="F1" s="35" t="s">
+        <v>190</v>
+      </c>
+      <c r="G1" s="35"/>
+      <c r="H1" s="35" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1"/>
@@ -17326,7 +17361,7 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="38"/>
+      <c r="A2" s="35"/>
       <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
@@ -17336,14 +17371,14 @@
       <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="40"/>
+      <c r="E2" s="37"/>
       <c r="F2" s="13" t="s">
-        <v>216</v>
+        <v>202</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>214</v>
-      </c>
-      <c r="H2" s="38"/>
+        <v>200</v>
+      </c>
+      <c r="H2" s="35"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -17368,7 +17403,7 @@
     </row>
     <row r="3" spans="1:29" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>202</v>
+        <v>188</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -17401,7 +17436,7 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>192</v>
+        <v>178</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>6</v>
@@ -17419,7 +17454,7 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>193</v>
+        <v>179</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>6</v>
@@ -17437,7 +17472,7 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>194</v>
+        <v>180</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>6</v>
@@ -17455,16 +17490,16 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>195</v>
+        <v>181</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>268</v>
+        <v>246</v>
       </c>
       <c r="E7" s="19"/>
       <c r="F7" s="21"/>
@@ -17473,7 +17508,7 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>196</v>
+        <v>182</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>6</v>
@@ -17501,7 +17536,7 @@
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>203</v>
+        <v>189</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -17513,7 +17548,7 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>197</v>
+        <v>183</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -17527,7 +17562,7 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>198</v>
+        <v>184</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -17541,7 +17576,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>199</v>
+        <v>185</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -17555,7 +17590,7 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>200</v>
+        <v>186</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -17569,7 +17604,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>273</v>
+        <v>251</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>

</xml_diff>

<commit_message>
All 3 manuals updated.
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2E2A0E3C-EB90-4E9E-9E22-67728D348C9C}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC09BF8-0876-48A6-84A5-0F1A02E008A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="49365" yWindow="1155" windowWidth="24810" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48015" yWindow="1950" windowWidth="24810" windowHeight="19560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="824" uniqueCount="283">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="284">
   <si>
     <t>Statement</t>
   </si>
@@ -57,9 +57,6 @@
     <t>Variable Management</t>
   </si>
   <si>
-    <t>system_position(pos_name, True|False)</t>
-  </si>
-  <si>
     <t>var_name = value</t>
   </si>
   <si>
@@ -123,12 +120,6 @@
     <t>Internal</t>
   </si>
   <si>
-    <t>Dashboard Communication</t>
-  </si>
-  <si>
-    <t>ur_dashboard(message, timeout_ms)</t>
-  </si>
-  <si>
     <t>PolyScope Communication</t>
   </si>
   <si>
@@ -144,36 +135,18 @@
     <t>robot_program_exit()</t>
   </si>
   <si>
-    <t>Position and Tool Interface</t>
-  </si>
-  <si>
-    <t>save_position(pos_name)</t>
-  </si>
-  <si>
-    <t>move_joint(pos_name)</t>
-  </si>
-  <si>
-    <t>move_linear(pos_name)</t>
-  </si>
-  <si>
     <t>move_tool_home()</t>
   </si>
   <si>
     <t>move_tool_mount()</t>
   </si>
   <si>
-    <t>select_tool(tool_name)</t>
-  </si>
-  <si>
     <t>30,19</t>
   </si>
   <si>
     <t>Core Motion</t>
   </si>
   <si>
-    <t>movej(j1,j2,j3,j4,j5,j6)</t>
-  </si>
-  <si>
     <t>1,16</t>
   </si>
   <si>
@@ -189,9 +162,6 @@
     <t>1,13</t>
   </si>
   <si>
-    <t>movel(x,y,z,rx,ry,rz)</t>
-  </si>
-  <si>
     <t>1,17</t>
   </si>
   <si>
@@ -219,9 +189,6 @@
     <t>1,15</t>
   </si>
   <si>
-    <t>set_tcp(x_m, y_m, z_m, rx_m, ry_m, rz_m)</t>
-  </si>
-  <si>
     <t>30,20</t>
   </si>
   <si>
@@ -231,30 +198,15 @@
     <t>1,18</t>
   </si>
   <si>
-    <t>set_payload(mass_kg, cog_x_m, cog_y_m, cog_z_m)</t>
-  </si>
-  <si>
     <t>30,21</t>
   </si>
   <si>
-    <t>Movel Incremental</t>
-  </si>
-  <si>
-    <t>movel_incr_base(dx,dy,dx,drx,dry,drz)</t>
-  </si>
-  <si>
     <t>1,20</t>
   </si>
   <si>
-    <t>movel_incr_tool(dx,dy,dx,drx,dry,drz)</t>
-  </si>
-  <si>
     <t>1,21</t>
   </si>
   <si>
-    <t>movel_incr_part(dx,dy,dx,drx,dry,drz)</t>
-  </si>
-  <si>
     <t>1,22</t>
   </si>
   <si>
@@ -270,40 +222,22 @@
     <t>1,31</t>
   </si>
   <si>
-    <t>Movel Relative</t>
-  </si>
-  <si>
-    <t>movel_rel_set_tool_origin(x,y,z,rx,ry,rz)</t>
-  </si>
-  <si>
     <t>1,40</t>
   </si>
   <si>
     <t>movel_rel_set_tool_origin_here()</t>
   </si>
   <si>
-    <t>movel_rel_set_part_origin(x,y,z,rx,ry,rz)</t>
-  </si>
-  <si>
     <t>1,41</t>
   </si>
   <si>
     <t>movel_rel_set_part_origin_here()</t>
   </si>
   <si>
-    <t>movel_rel_tool(x,y,z,rx,ry,rz)</t>
-  </si>
-  <si>
     <t>1,42</t>
   </si>
   <si>
-    <t>movel_rel_part(x,y,z,rx,ry,rz)</t>
-  </si>
-  <si>
     <t>1,43</t>
-  </si>
-  <si>
-    <t>Set Robot Variables</t>
   </si>
   <si>
     <t>30,1</t>
@@ -672,9 +606,6 @@
     <t>sleep(double seconds)</t>
   </si>
   <si>
-    <t>random(int N, double low, double high)</t>
-  </si>
-  <si>
     <t>le_pause()</t>
   </si>
   <si>
@@ -763,9 +694,6 @@
 LEScript2.txt</t>
   </si>
   <si>
-    <t>set_blend_radius(double blend_radius_mm)</t>
-  </si>
-  <si>
     <t>N/A</t>
   </si>
   <si>
@@ -842,12 +770,6 @@
     <t xml:space="preserve">free_drive(int 0=OFF|1=ON) </t>
   </si>
   <si>
-    <t>set_part_geometry_N(int n, double diam_mm) FOR TESTING ONLY</t>
-  </si>
-  <si>
-    <t>SEQUENCE OK?</t>
-  </si>
-  <si>
     <t>grind_touch_retract(int touch_retract_mm)</t>
   </si>
   <si>
@@ -876,6 +798,87 @@
   </si>
   <si>
     <t>grind_force_mode_gain_scaling(double scaling: 0.0 – 2.0)</t>
+  </si>
+  <si>
+    <t>select_tool(string tool_name)</t>
+  </si>
+  <si>
+    <t>save_position(string pos_name)</t>
+  </si>
+  <si>
+    <t>system_position(string pos_name, boolean True|False)</t>
+  </si>
+  <si>
+    <t>move_joint(string pos_name)</t>
+  </si>
+  <si>
+    <t>move_linear(strig pos_name)</t>
+  </si>
+  <si>
+    <t>Position System</t>
+  </si>
+  <si>
+    <t>Tool System</t>
+  </si>
+  <si>
+    <t>Management</t>
+  </si>
+  <si>
+    <t>Move Incremental</t>
+  </si>
+  <si>
+    <t>Move Relative</t>
+  </si>
+  <si>
+    <t>THIS IS MORE COMPLEX</t>
+  </si>
+  <si>
+    <t>string ur_dashboard(string message, int timeout_ms)</t>
+  </si>
+  <si>
+    <t>movej(float j1,j2,j3,j4,j5,j6)</t>
+  </si>
+  <si>
+    <t>movel(float x,y,z,rx,ry,rz)</t>
+  </si>
+  <si>
+    <t>movel_incr_base(float dx,dy,dx,drx,dry,drz)</t>
+  </si>
+  <si>
+    <t>movel_incr_tool(float dx,dy,dx,drx,dry,drz)</t>
+  </si>
+  <si>
+    <t>movel_incr_part(float dx,dy,dx,drx,dry,drz)</t>
+  </si>
+  <si>
+    <t>movel_rel_set_tool_origin(float x,y,z,rx,ry,rz)</t>
+  </si>
+  <si>
+    <t>movel_rel_set_part_origin(float x,y,z,rx,ry,rz)</t>
+  </si>
+  <si>
+    <t>movel_rel_tool(float x,y,z,rx,ry,rz)</t>
+  </si>
+  <si>
+    <t>movel_rel_part(float x,y,z,rx,ry,rz)</t>
+  </si>
+  <si>
+    <t>set_blend_radius(float blend_radius_mm)</t>
+  </si>
+  <si>
+    <t>set_part_geometry_N(int n, float diam_mm) FOR TESTING ONLY</t>
+  </si>
+  <si>
+    <t>random(int N, float low, float high)</t>
+  </si>
+  <si>
+    <t>Set Motion Variables</t>
+  </si>
+  <si>
+    <t>set_tcp(float x_m, y_m, z_m, rx_m, ry_m, rz_m)</t>
+  </si>
+  <si>
+    <t>set_payload(float mass_kg, float cog_x_m, float cog_y_m, float cog_z_m)</t>
   </si>
 </sst>
 </file>
@@ -1000,7 +1003,7 @@
       <alignment vertical="top"/>
     </xf>
   </cellStyleXfs>
-  <cellXfs count="39">
+  <cellXfs count="40">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
@@ -1080,6 +1083,9 @@
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1089,8 +1095,8 @@
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1316,8 +1322,8 @@
   <dimension ref="A1:AC1006"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A42" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G82" sqref="G82"/>
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1326,34 +1332,34 @@
     <col min="2" max="2" width="10.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="11" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="11" customWidth="1"/>
-    <col min="5" max="5" width="13.42578125" style="38" customWidth="1"/>
+    <col min="5" max="5" width="13.42578125" style="35" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
     <col min="7" max="7" width="27.28515625" customWidth="1"/>
     <col min="8" max="8" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="37" t="s">
-        <v>248</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="38" t="s">
+        <v>224</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1363,14 +1369,14 @@
       <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="37"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="13" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="35"/>
+        <v>178</v>
+      </c>
+      <c r="H2" s="36"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1401,7 +1407,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19"/>
@@ -1423,7 +1429,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="19"/>
@@ -1445,14 +1451,14 @@
         <v>6</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>236</v>
+        <v>213</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>6</v>
@@ -1467,14 +1473,14 @@
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>191</v>
+        <v>169</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>234</v>
+        <v>211</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>6</v>
@@ -1489,16 +1495,16 @@
         <v>6</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>247</v>
+        <v>223</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>244</v>
+        <v>221</v>
       </c>
       <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>237</v>
+        <v>214</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>6</v>
@@ -1513,16 +1519,16 @@
         <v>6</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>193</v>
+        <v>171</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>192</v>
+        <v>170</v>
       </c>
       <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>235</v>
+        <v>212</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>6</v>
@@ -1537,16 +1543,16 @@
         <v>6</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>194</v>
+        <v>172</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>195</v>
+        <v>173</v>
       </c>
       <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>233</v>
+        <v>210</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>6</v>
@@ -1561,14 +1567,14 @@
         <v>6</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>239</v>
+        <v>216</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>6</v>
@@ -1583,14 +1589,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>240</v>
+        <v>217</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>6</v>
@@ -1605,7 +1611,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="28"/>
@@ -1634,7 +1640,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>196</v>
+        <v>174</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>6</v>
@@ -1645,14 +1651,14 @@
         <v>6</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>238</v>
+        <v>215</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>6</v>
@@ -1663,16 +1669,16 @@
         <v>6</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>199</v>
+        <v>177</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>201</v>
+        <v>179</v>
       </c>
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>197</v>
+        <v>175</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>6</v>
@@ -1683,14 +1689,14 @@
         <v>6</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>198</v>
+        <v>176</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
     </row>
     <row r="19" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A19" s="20" t="s">
-        <v>12</v>
+        <v>11</v>
       </c>
       <c r="B19" s="27" t="s">
         <v>6</v>
@@ -1705,14 +1711,14 @@
         <v>6</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
     </row>
     <row r="20" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>13</v>
+        <v>12</v>
       </c>
       <c r="B20" s="27" t="s">
         <v>6</v>
@@ -1727,14 +1733,14 @@
         <v>6</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
     </row>
     <row r="21" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>14</v>
+        <v>13</v>
       </c>
       <c r="B21" s="27" t="s">
         <v>6</v>
@@ -1749,14 +1755,14 @@
         <v>6</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
     </row>
     <row r="22" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>15</v>
+        <v>14</v>
       </c>
       <c r="B22" s="27" t="s">
         <v>6</v>
@@ -1771,14 +1777,14 @@
         <v>6</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>215</v>
+        <v>280</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>6</v>
@@ -1789,14 +1795,14 @@
         <v>6</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>213</v>
+        <v>191</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>241</v>
+        <v>218</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27" t="s">
@@ -1809,14 +1815,14 @@
         <v>6</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>242</v>
+        <v>219</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27" t="s">
@@ -1829,14 +1835,14 @@
         <v>6</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>243</v>
+        <v>220</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27" t="s">
@@ -1849,7 +1855,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>204</v>
+        <v>182</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
@@ -1866,7 +1872,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>212</v>
+        <v>190</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -1878,7 +1884,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>207</v>
+        <v>185</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>6</v>
@@ -1893,14 +1899,14 @@
         <v>6</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>205</v>
+        <v>183</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>6</v>
@@ -1915,14 +1921,14 @@
         <v>6</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
     </row>
     <row r="31" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="B31" s="27" t="s">
         <v>6</v>
@@ -1937,7 +1943,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>209</v>
+        <v>187</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -1954,7 +1960,7 @@
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>211</v>
+        <v>189</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="25"/>
@@ -1966,7 +1972,7 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>206</v>
+        <v>184</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>6</v>
@@ -1981,14 +1987,14 @@
         <v>6</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>208</v>
+        <v>186</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>6</v>
@@ -2003,7 +2009,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>210</v>
+        <v>188</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -2020,7 +2026,7 @@
     </row>
     <row r="37" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>20</v>
+        <v>19</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
@@ -2032,7 +2038,7 @@
     </row>
     <row r="38" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>216</v>
+        <v>193</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>6</v>
@@ -2047,14 +2053,14 @@
         <v>6</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>220</v>
+        <v>197</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>217</v>
+        <v>194</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>6</v>
@@ -2069,14 +2075,14 @@
         <v>6</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>221</v>
+        <v>198</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>6</v>
@@ -2091,14 +2097,14 @@
         <v>6</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>222</v>
+        <v>199</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>21</v>
+        <v>20</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>6</v>
@@ -2113,14 +2119,14 @@
         <v>6</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>23</v>
+        <v>22</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>6</v>
@@ -2135,14 +2141,14 @@
         <v>6</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
     </row>
     <row r="43" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>24</v>
+        <v>23</v>
       </c>
       <c r="B43" s="33" t="s">
         <v>6</v>
@@ -2157,7 +2163,7 @@
         <v>6</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="G43" s="30"/>
       <c r="H43" s="30"/>
@@ -2185,7 +2191,7 @@
     </row>
     <row r="44" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>25</v>
+        <v>24</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>6</v>
@@ -2196,14 +2202,14 @@
         <v>6</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>223</v>
+        <v>200</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>26</v>
+        <v>25</v>
       </c>
       <c r="B45" s="27" t="s">
         <v>6</v>
@@ -2218,14 +2224,14 @@
         <v>6</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
     </row>
     <row r="46" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="B46" s="27" t="s">
         <v>6</v>
@@ -2240,14 +2246,14 @@
         <v>6</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="G46" s="19"/>
       <c r="H46" s="19"/>
     </row>
     <row r="47" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="B47" s="27" t="s">
         <v>6</v>
@@ -2262,14 +2268,14 @@
         <v>6</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>224</v>
+        <v>201</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>214</v>
+        <v>192</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>6</v>
@@ -2284,14 +2290,14 @@
         <v>6</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>225</v>
+        <v>202</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="19"/>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>254</v>
+        <v>230</v>
       </c>
       <c r="B49" s="27" t="s">
         <v>6</v>
@@ -2302,14 +2308,14 @@
         <v>6</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>255</v>
+        <v>231</v>
       </c>
       <c r="B50" s="27" t="s">
         <v>6</v>
@@ -2320,14 +2326,14 @@
         <v>6</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>252</v>
+        <v>228</v>
       </c>
       <c r="B51" s="27"/>
       <c r="C51" s="27" t="s">
@@ -2340,14 +2346,14 @@
         <v>6</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="G51" s="19"/>
       <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>253</v>
+        <v>229</v>
       </c>
       <c r="B52" s="27"/>
       <c r="C52" s="27" t="s">
@@ -2360,7 +2366,7 @@
         <v>6</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>203</v>
+        <v>181</v>
       </c>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
@@ -2377,7 +2383,7 @@
     </row>
     <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A54" s="24" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="B54" s="25"/>
       <c r="C54" s="25"/>
@@ -2389,7 +2395,7 @@
     </row>
     <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>226</v>
+        <v>203</v>
       </c>
       <c r="B55" s="27" t="s">
         <v>6</v>
@@ -2404,14 +2410,14 @@
         <v>6</v>
       </c>
       <c r="F55" s="28" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G55" s="19"/>
       <c r="H55" s="28"/>
     </row>
     <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>227</v>
+        <v>204</v>
       </c>
       <c r="B56" s="27" t="s">
         <v>6</v>
@@ -2426,14 +2432,14 @@
         <v>6</v>
       </c>
       <c r="F56" s="28" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G56" s="19"/>
       <c r="H56" s="28"/>
     </row>
     <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A57" s="20" t="s">
-        <v>228</v>
+        <v>205</v>
       </c>
       <c r="B57" s="27" t="s">
         <v>6</v>
@@ -2448,14 +2454,14 @@
         <v>6</v>
       </c>
       <c r="F57" s="28" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G57" s="19"/>
       <c r="H57" s="28"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>229</v>
+        <v>206</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>6</v>
@@ -2470,14 +2476,14 @@
         <v>6</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="B59" s="27" t="s">
         <v>6</v>
@@ -2492,14 +2498,14 @@
         <v>6</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G59" s="19"/>
       <c r="H59" s="28"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>19</v>
+        <v>18</v>
       </c>
       <c r="B60" s="27" t="s">
         <v>6</v>
@@ -2514,7 +2520,7 @@
         <v>6</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>231</v>
+        <v>208</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="28"/>
@@ -2531,7 +2537,7 @@
     </row>
     <row r="62" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A62" s="24" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="B62" s="25"/>
       <c r="C62" s="25"/>
@@ -2543,7 +2549,7 @@
     </row>
     <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>218</v>
+        <v>195</v>
       </c>
       <c r="B63" s="27" t="s">
         <v>6</v>
@@ -2554,14 +2560,14 @@
         <v>6</v>
       </c>
       <c r="F63" s="20" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="G63" s="19"/>
       <c r="H63" s="19"/>
     </row>
     <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="B64" s="27" t="s">
         <v>6</v>
@@ -2572,14 +2578,14 @@
         <v>6</v>
       </c>
       <c r="F64" s="20" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
     </row>
     <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="B65" s="27" t="s">
         <v>6</v>
@@ -2590,14 +2596,14 @@
         <v>6</v>
       </c>
       <c r="F65" s="20" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="G65" s="19"/>
       <c r="H65" s="19"/>
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>219</v>
+        <v>196</v>
       </c>
       <c r="B66" s="27" t="s">
         <v>6</v>
@@ -2608,7 +2614,7 @@
         <v>6</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>230</v>
+        <v>207</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
@@ -2625,7 +2631,7 @@
     </row>
     <row r="68" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A68" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B68" s="25"/>
       <c r="C68" s="25"/>
@@ -2637,7 +2643,7 @@
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>232</v>
+        <v>209</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>6</v>
@@ -2645,7 +2651,7 @@
       <c r="C69" s="27"/>
       <c r="D69" s="27"/>
       <c r="E69" s="32" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="F69" s="19"/>
       <c r="G69" s="19"/>
@@ -8291,16 +8297,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD1075"/>
+  <dimension ref="A1:AD1077"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A6" sqref="A6"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="83.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="95.42578125" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
@@ -8312,25 +8318,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
-        <v>187</v>
-      </c>
-      <c r="C1" s="35" t="s">
+      <c r="B1" s="38" t="s">
+        <v>165</v>
+      </c>
+      <c r="C1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="35"/>
-      <c r="E1" s="35"/>
-      <c r="F1" s="37" t="s">
-        <v>249</v>
-      </c>
-      <c r="G1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="H1" s="35"/>
-      <c r="I1" s="35" t="s">
+      <c r="D1" s="36"/>
+      <c r="E1" s="36"/>
+      <c r="F1" s="38" t="s">
+        <v>225</v>
+      </c>
+      <c r="G1" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="H1" s="36"/>
+      <c r="I1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1"/>
@@ -8356,8 +8362,8 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
-      <c r="B2" s="37"/>
+      <c r="A2" s="36"/>
+      <c r="B2" s="38"/>
       <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
@@ -8367,14 +8373,14 @@
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="37"/>
+      <c r="F2" s="38"/>
       <c r="G2" s="13" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="I2" s="35"/>
+        <v>178</v>
+      </c>
+      <c r="I2" s="36"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -8399,22 +8405,20 @@
     </row>
     <row r="3" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>33</v>
+        <v>264</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
       <c r="D3" s="25"/>
       <c r="E3" s="25"/>
-      <c r="F3" s="25" t="s">
-        <v>272</v>
-      </c>
+      <c r="F3" s="25"/>
       <c r="G3" s="20"/>
       <c r="H3" s="16"/>
       <c r="I3" s="16"/>
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>34</v>
+        <v>268</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="27" t="s">
@@ -8426,7 +8430,9 @@
       <c r="E4" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F4" s="27"/>
+      <c r="F4" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G4" s="20"/>
       <c r="H4" s="20"/>
       <c r="I4" s="19"/>
@@ -8444,7 +8450,7 @@
     </row>
     <row r="6" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>35</v>
+        <v>40</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -8452,15 +8458,15 @@
       <c r="E6" s="25"/>
       <c r="F6" s="25"/>
       <c r="G6" s="20"/>
-      <c r="H6" s="24"/>
+      <c r="H6" s="15"/>
       <c r="I6" s="16"/>
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>36</v>
+        <v>269</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>37</v>
+        <v>41</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>6</v>
@@ -8471,17 +8477,19 @@
       <c r="E7" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F7" s="27"/>
+      <c r="F7" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G7" s="20"/>
-      <c r="H7" s="20"/>
+      <c r="H7" s="21"/>
       <c r="I7" s="19"/>
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>38</v>
-      </c>
-      <c r="B8" s="26">
-        <v>98</v>
+        <v>42</v>
+      </c>
+      <c r="B8" s="26" t="s">
+        <v>43</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>6</v>
@@ -8492,17 +8500,19 @@
       <c r="E8" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F8" s="27"/>
+      <c r="F8" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G8" s="20"/>
-      <c r="H8" s="29"/>
+      <c r="H8" s="21"/>
       <c r="I8" s="19"/>
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>39</v>
-      </c>
-      <c r="B9" s="26">
-        <v>99</v>
+        <v>44</v>
+      </c>
+      <c r="B9" s="26" t="s">
+        <v>45</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>6</v>
@@ -8513,12 +8523,14 @@
       <c r="E9" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F9" s="27"/>
+      <c r="F9" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G9" s="20"/>
-      <c r="H9" s="29"/>
+      <c r="H9" s="21"/>
       <c r="I9" s="19"/>
     </row>
-    <row r="10" spans="1:30" ht="15" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A10" s="20"/>
       <c r="B10" s="26"/>
       <c r="C10" s="27"/>
@@ -8526,27 +8538,39 @@
       <c r="E10" s="27"/>
       <c r="F10" s="27"/>
       <c r="G10" s="20"/>
-      <c r="H10" s="29"/>
+      <c r="H10" s="21"/>
       <c r="I10" s="19"/>
     </row>
-    <row r="11" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A11" s="24" t="s">
-        <v>40</v>
-      </c>
-      <c r="B11" s="25"/>
-      <c r="C11" s="25"/>
-      <c r="D11" s="25"/>
-      <c r="E11" s="25"/>
-      <c r="F11" s="25"/>
+    <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A11" s="20" t="s">
+        <v>270</v>
+      </c>
+      <c r="B11" s="26" t="s">
+        <v>46</v>
+      </c>
+      <c r="C11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E11" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F11" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G11" s="20"/>
-      <c r="H11" s="16"/>
-      <c r="I11" s="16"/>
-    </row>
-    <row r="12" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H11" s="21"/>
+      <c r="I11" s="19"/>
+    </row>
+    <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>46</v>
-      </c>
-      <c r="B12" s="26"/>
+        <v>62</v>
+      </c>
+      <c r="B12" s="26" t="s">
+        <v>63</v>
+      </c>
       <c r="C12" s="27" t="s">
         <v>6</v>
       </c>
@@ -8556,16 +8580,20 @@
       <c r="E12" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F12" s="27"/>
+      <c r="F12" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G12" s="20"/>
-      <c r="H12" s="21"/>
+      <c r="H12" s="30"/>
       <c r="I12" s="19"/>
     </row>
-    <row r="13" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>269</v>
-      </c>
-      <c r="B13" s="26"/>
+        <v>64</v>
+      </c>
+      <c r="B13" s="26" t="s">
+        <v>65</v>
+      </c>
       <c r="C13" s="27" t="s">
         <v>6</v>
       </c>
@@ -8575,16 +8603,20 @@
       <c r="E13" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F13" s="27"/>
+      <c r="F13" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G13" s="20"/>
-      <c r="H13" s="21"/>
+      <c r="H13" s="19"/>
       <c r="I13" s="19"/>
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>41</v>
-      </c>
-      <c r="B14" s="26"/>
+        <v>47</v>
+      </c>
+      <c r="B14" s="26" t="s">
+        <v>48</v>
+      </c>
       <c r="C14" s="27" t="s">
         <v>6</v>
       </c>
@@ -8594,16 +8626,20 @@
       <c r="E14" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F14" s="27"/>
+      <c r="F14" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G14" s="20"/>
-      <c r="H14" s="19"/>
+      <c r="H14" s="21"/>
       <c r="I14" s="19"/>
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>11</v>
-      </c>
-      <c r="B15" s="18"/>
+        <v>49</v>
+      </c>
+      <c r="B15" s="26" t="s">
+        <v>50</v>
+      </c>
       <c r="C15" s="27" t="s">
         <v>6</v>
       </c>
@@ -8613,25 +8649,19 @@
       <c r="E15" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F15" s="19"/>
+      <c r="F15" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G15" s="20"/>
-      <c r="H15" s="19"/>
+      <c r="H15" s="21"/>
       <c r="I15" s="19"/>
     </row>
     <row r="16" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A16" s="20" t="s">
-        <v>42</v>
-      </c>
+      <c r="A16" s="20"/>
       <c r="B16" s="26"/>
-      <c r="C16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D16" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E16" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="C16" s="27"/>
+      <c r="D16" s="27"/>
+      <c r="E16" s="27"/>
       <c r="F16" s="27"/>
       <c r="G16" s="20"/>
       <c r="H16" s="21"/>
@@ -8639,9 +8669,11 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>43</v>
-      </c>
-      <c r="B17" s="26"/>
+        <v>51</v>
+      </c>
+      <c r="B17" s="26" t="s">
+        <v>52</v>
+      </c>
       <c r="C17" s="27" t="s">
         <v>6</v>
       </c>
@@ -8651,16 +8683,20 @@
       <c r="E17" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F17" s="27"/>
+      <c r="F17" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G17" s="20"/>
       <c r="H17" s="21"/>
       <c r="I17" s="19"/>
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>44</v>
-      </c>
-      <c r="B18" s="26"/>
+        <v>53</v>
+      </c>
+      <c r="B18" s="26" t="s">
+        <v>54</v>
+      </c>
       <c r="C18" s="27" t="s">
         <v>6</v>
       </c>
@@ -8670,25 +8706,19 @@
       <c r="E18" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F18" s="27"/>
+      <c r="F18" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G18" s="20"/>
       <c r="H18" s="21"/>
       <c r="I18" s="19"/>
     </row>
     <row r="19" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A19" s="20" t="s">
-        <v>45</v>
-      </c>
+      <c r="A19" s="20"/>
       <c r="B19" s="26"/>
-      <c r="C19" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D19" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E19" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="C19" s="27"/>
+      <c r="D19" s="27"/>
+      <c r="E19" s="27"/>
       <c r="F19" s="27"/>
       <c r="G19" s="20"/>
       <c r="H19" s="21"/>
@@ -8696,10 +8726,10 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>270</v>
+        <v>56</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>47</v>
+        <v>57</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>6</v>
@@ -8710,41 +8740,65 @@
       <c r="E20" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F20" s="27"/>
+      <c r="F20" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G20" s="20"/>
       <c r="H20" s="21"/>
       <c r="I20" s="19"/>
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A21" s="20"/>
-      <c r="B21" s="26"/>
-      <c r="C21" s="27"/>
-      <c r="D21" s="27"/>
-      <c r="E21" s="27"/>
-      <c r="F21" s="27"/>
+      <c r="A21" s="20" t="s">
+        <v>282</v>
+      </c>
+      <c r="B21" s="26" t="s">
+        <v>55</v>
+      </c>
+      <c r="C21" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D21" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E21" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F21" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G21" s="20"/>
       <c r="H21" s="21"/>
       <c r="I21" s="19"/>
     </row>
-    <row r="22" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A22" s="24" t="s">
-        <v>48</v>
-      </c>
-      <c r="B22" s="25"/>
-      <c r="C22" s="25"/>
-      <c r="D22" s="25"/>
-      <c r="E22" s="25"/>
-      <c r="F22" s="25"/>
+    <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A22" s="20" t="s">
+        <v>283</v>
+      </c>
+      <c r="B22" s="26" t="s">
+        <v>58</v>
+      </c>
+      <c r="C22" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D22" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E22" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F22" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G22" s="20"/>
-      <c r="H22" s="15"/>
-      <c r="I22" s="16"/>
+      <c r="H22" s="21"/>
+      <c r="I22" s="19"/>
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>49</v>
+        <v>246</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>50</v>
+        <v>39</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>6</v>
@@ -8755,70 +8809,68 @@
       <c r="E23" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F23" s="27"/>
-      <c r="G23" s="20"/>
+      <c r="F23" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G23" s="20" t="s">
+        <v>267</v>
+      </c>
       <c r="H23" s="21"/>
       <c r="I23" s="19"/>
     </row>
     <row r="24" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A24" s="20" t="s">
-        <v>51</v>
-      </c>
-      <c r="B24" s="26" t="s">
-        <v>52</v>
-      </c>
-      <c r="C24" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D24" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E24" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="A24" s="20"/>
+      <c r="B24" s="26"/>
+      <c r="C24" s="27"/>
+      <c r="D24" s="27"/>
+      <c r="E24" s="27"/>
       <c r="F24" s="27"/>
       <c r="G24" s="20"/>
       <c r="H24" s="21"/>
       <c r="I24" s="19"/>
     </row>
-    <row r="25" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A25" s="20" t="s">
-        <v>53</v>
-      </c>
-      <c r="B25" s="26" t="s">
-        <v>54</v>
-      </c>
-      <c r="C25" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D25" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E25" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F25" s="27"/>
+    <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A25" s="24" t="s">
+        <v>265</v>
+      </c>
+      <c r="B25" s="25"/>
+      <c r="C25" s="25"/>
+      <c r="D25" s="25"/>
+      <c r="E25" s="25"/>
+      <c r="F25" s="25"/>
       <c r="G25" s="20"/>
-      <c r="H25" s="21"/>
-      <c r="I25" s="19"/>
+      <c r="H25" s="16"/>
+      <c r="I25" s="16"/>
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A26" s="20"/>
-      <c r="B26" s="26"/>
-      <c r="C26" s="27"/>
-      <c r="D26" s="27"/>
-      <c r="E26" s="27"/>
-      <c r="F26" s="27"/>
+      <c r="A26" s="20" t="s">
+        <v>271</v>
+      </c>
+      <c r="B26" s="26" t="s">
+        <v>59</v>
+      </c>
+      <c r="C26" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D26" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E26" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F26" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G26" s="20"/>
       <c r="H26" s="21"/>
       <c r="I26" s="19"/>
     </row>
-    <row r="27" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>55</v>
+        <v>272</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>56</v>
+        <v>60</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>6</v>
@@ -8829,17 +8881,19 @@
       <c r="E27" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F27" s="27"/>
+      <c r="F27" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G27" s="20"/>
       <c r="H27" s="21"/>
       <c r="I27" s="19"/>
     </row>
-    <row r="28" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>57</v>
+        <v>273</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>58</v>
+        <v>61</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>6</v>
@@ -8850,49 +8904,43 @@
       <c r="E28" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F28" s="27"/>
+      <c r="F28" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G28" s="20"/>
       <c r="H28" s="21"/>
       <c r="I28" s="19"/>
     </row>
-    <row r="29" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A29" s="20" t="s">
-        <v>59</v>
-      </c>
-      <c r="B29" s="26" t="s">
-        <v>60</v>
-      </c>
-      <c r="C29" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D29" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E29" s="27" t="s">
-        <v>6</v>
-      </c>
+    <row r="29" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A29" s="20"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="27"/>
+      <c r="D29" s="27"/>
+      <c r="E29" s="27"/>
       <c r="F29" s="27"/>
       <c r="G29" s="20"/>
-      <c r="H29" s="21"/>
+      <c r="H29" s="19"/>
       <c r="I29" s="19"/>
     </row>
-    <row r="30" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A30" s="20"/>
-      <c r="B30" s="26"/>
-      <c r="C30" s="27"/>
-      <c r="D30" s="27"/>
-      <c r="E30" s="27"/>
-      <c r="F30" s="27"/>
+    <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A30" s="24" t="s">
+        <v>266</v>
+      </c>
+      <c r="B30" s="25"/>
+      <c r="C30" s="25"/>
+      <c r="D30" s="25"/>
+      <c r="E30" s="25"/>
+      <c r="F30" s="25"/>
       <c r="G30" s="20"/>
-      <c r="H30" s="21"/>
-      <c r="I30" s="19"/>
-    </row>
-    <row r="31" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="H30" s="16"/>
+      <c r="I30" s="16"/>
+    </row>
+    <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>61</v>
+        <v>274</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>62</v>
+        <v>66</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -8903,17 +8951,19 @@
       <c r="E31" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F31" s="27"/>
+      <c r="F31" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G31" s="20"/>
-      <c r="H31" s="21"/>
+      <c r="H31" s="19"/>
       <c r="I31" s="19"/>
     </row>
-    <row r="32" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>63</v>
+        <v>67</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>64</v>
+        <v>66</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -8924,28 +8974,42 @@
       <c r="E32" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F32" s="27"/>
+      <c r="F32" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G32" s="20"/>
-      <c r="H32" s="21"/>
+      <c r="H32" s="19"/>
       <c r="I32" s="19"/>
     </row>
-    <row r="33" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A33" s="20"/>
-      <c r="B33" s="26"/>
-      <c r="C33" s="27"/>
-      <c r="D33" s="27"/>
-      <c r="E33" s="27"/>
-      <c r="F33" s="27"/>
+    <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A33" s="20" t="s">
+        <v>275</v>
+      </c>
+      <c r="B33" s="26" t="s">
+        <v>68</v>
+      </c>
+      <c r="C33" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D33" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E33" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F33" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G33" s="20"/>
-      <c r="H33" s="21"/>
+      <c r="H33" s="19"/>
       <c r="I33" s="19"/>
     </row>
-    <row r="34" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>65</v>
+        <v>69</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>66</v>
+        <v>68</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>6</v>
@@ -8956,17 +9020,19 @@
       <c r="E34" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F34" s="27"/>
+      <c r="F34" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G34" s="20"/>
-      <c r="H34" s="21"/>
+      <c r="H34" s="19"/>
       <c r="I34" s="19"/>
     </row>
-    <row r="35" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>67</v>
+        <v>276</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>68</v>
+        <v>70</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>6</v>
@@ -8977,17 +9043,19 @@
       <c r="E35" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F35" s="27"/>
+      <c r="F35" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G35" s="20"/>
-      <c r="H35" s="21"/>
+      <c r="H35" s="19"/>
       <c r="I35" s="19"/>
     </row>
-    <row r="36" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>69</v>
+        <v>277</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>70</v>
+        <v>71</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>6</v>
@@ -8998,12 +9066,14 @@
       <c r="E36" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F36" s="27"/>
+      <c r="F36" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G36" s="20"/>
-      <c r="H36" s="21"/>
+      <c r="H36" s="19"/>
       <c r="I36" s="19"/>
     </row>
-    <row r="37" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A37" s="20"/>
       <c r="B37" s="26"/>
       <c r="C37" s="27"/>
@@ -9011,12 +9081,12 @@
       <c r="E37" s="27"/>
       <c r="F37" s="27"/>
       <c r="G37" s="20"/>
-      <c r="H37" s="21"/>
+      <c r="H37" s="19"/>
       <c r="I37" s="19"/>
     </row>
     <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>71</v>
+        <v>263</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -9029,11 +9099,9 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>72</v>
-      </c>
-      <c r="B39" s="26" t="s">
-        <v>73</v>
-      </c>
+        <v>257</v>
+      </c>
+      <c r="B39" s="26"/>
       <c r="C39" s="27" t="s">
         <v>6</v>
       </c>
@@ -9043,210 +9111,218 @@
       <c r="E39" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F39" s="27"/>
+      <c r="F39" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G39" s="20"/>
       <c r="H39" s="21"/>
       <c r="I39" s="19"/>
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>74</v>
+        <v>83</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>75</v>
+        <v>84</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F40" s="27"/>
+        <v>222</v>
+      </c>
+      <c r="F40" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G40" s="20"/>
-      <c r="H40" s="21"/>
+      <c r="H40" s="19"/>
       <c r="I40" s="19"/>
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>76</v>
+        <v>85</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>77</v>
+        <v>86</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="27"/>
+        <v>222</v>
+      </c>
+      <c r="F41" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G41" s="20"/>
       <c r="H41" s="21"/>
       <c r="I41" s="19"/>
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>78</v>
+        <v>87</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>79</v>
+        <v>88</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F42" s="27"/>
+        <v>222</v>
+      </c>
+      <c r="F42" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G42" s="20"/>
-      <c r="H42" s="30"/>
+      <c r="H42" s="19"/>
       <c r="I42" s="19"/>
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>80</v>
+        <v>89</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>81</v>
+        <v>90</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F43" s="27"/>
+        <v>222</v>
+      </c>
+      <c r="F43" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G43" s="20"/>
       <c r="H43" s="19"/>
       <c r="I43" s="19"/>
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A44" s="20"/>
-      <c r="B44" s="26"/>
-      <c r="C44" s="27"/>
+      <c r="A44" s="20" t="s">
+        <v>91</v>
+      </c>
+      <c r="B44" s="26" t="s">
+        <v>92</v>
+      </c>
+      <c r="C44" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="D44" s="27"/>
-      <c r="E44" s="27"/>
-      <c r="F44" s="27"/>
+      <c r="E44" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F44" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G44" s="20"/>
       <c r="H44" s="19"/>
       <c r="I44" s="19"/>
     </row>
-    <row r="45" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A45" s="24" t="s">
-        <v>82</v>
-      </c>
-      <c r="B45" s="25"/>
-      <c r="C45" s="25"/>
-      <c r="D45" s="25"/>
-      <c r="E45" s="25"/>
-      <c r="F45" s="25"/>
+    <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A45" s="20" t="s">
+        <v>93</v>
+      </c>
+      <c r="B45" s="26" t="s">
+        <v>94</v>
+      </c>
+      <c r="C45" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D45" s="27"/>
+      <c r="E45" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F45" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G45" s="20"/>
-      <c r="H45" s="16"/>
-      <c r="I45" s="16"/>
+      <c r="H45" s="19"/>
+      <c r="I45" s="19"/>
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>83</v>
+        <v>95</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>84</v>
+        <v>96</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D46" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="D46" s="27"/>
       <c r="E46" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F46" s="27"/>
+      <c r="F46" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G46" s="20"/>
       <c r="H46" s="19"/>
       <c r="I46" s="19"/>
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>85</v>
+        <v>97</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>84</v>
+        <v>39</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D47" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="D47" s="27"/>
       <c r="E47" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F47" s="27"/>
+      <c r="F47" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G47" s="20"/>
       <c r="H47" s="19"/>
       <c r="I47" s="19"/>
     </row>
     <row r="48" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A48" s="20" t="s">
-        <v>86</v>
-      </c>
-      <c r="B48" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C48" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D48" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E48" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="A48" s="20"/>
+      <c r="B48" s="26"/>
+      <c r="C48" s="27"/>
+      <c r="D48" s="27"/>
+      <c r="E48" s="27"/>
       <c r="F48" s="27"/>
       <c r="G48" s="20"/>
       <c r="H48" s="19"/>
       <c r="I48" s="19"/>
     </row>
-    <row r="49" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A49" s="20" t="s">
-        <v>88</v>
-      </c>
-      <c r="B49" s="26" t="s">
-        <v>87</v>
-      </c>
-      <c r="C49" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D49" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E49" s="27" t="s">
-        <v>6</v>
-      </c>
+    <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A49" s="24" t="s">
+        <v>262</v>
+      </c>
+      <c r="B49" s="26"/>
+      <c r="C49" s="27"/>
+      <c r="D49" s="27"/>
+      <c r="E49" s="27"/>
       <c r="F49" s="27"/>
       <c r="G49" s="20"/>
-      <c r="H49" s="19"/>
+      <c r="H49" s="21"/>
       <c r="I49" s="19"/>
     </row>
-    <row r="50" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>89</v>
-      </c>
-      <c r="B50" s="26" t="s">
-        <v>90</v>
-      </c>
+        <v>245</v>
+      </c>
+      <c r="B50" s="26"/>
       <c r="C50" s="27" t="s">
         <v>6</v>
       </c>
@@ -9256,18 +9332,18 @@
       <c r="E50" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F50" s="27"/>
+      <c r="F50" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G50" s="20"/>
-      <c r="H50" s="19"/>
+      <c r="H50" s="21"/>
       <c r="I50" s="19"/>
     </row>
-    <row r="51" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>91</v>
-      </c>
-      <c r="B51" s="26" t="s">
-        <v>92</v>
-      </c>
+        <v>258</v>
+      </c>
+      <c r="B51" s="26"/>
       <c r="C51" s="27" t="s">
         <v>6</v>
       </c>
@@ -9277,42 +9353,60 @@
       <c r="E51" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F51" s="27"/>
+      <c r="F51" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G51" s="20"/>
       <c r="H51" s="19"/>
       <c r="I51" s="19"/>
     </row>
-    <row r="52" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A52" s="20"/>
-      <c r="B52" s="26"/>
-      <c r="C52" s="27"/>
-      <c r="D52" s="27"/>
-      <c r="E52" s="27"/>
-      <c r="F52" s="27"/>
+    <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A52" s="20" t="s">
+        <v>259</v>
+      </c>
+      <c r="B52" s="18"/>
+      <c r="C52" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D52" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E52" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F52" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G52" s="20"/>
       <c r="H52" s="19"/>
       <c r="I52" s="19"/>
     </row>
-    <row r="53" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A53" s="24" t="s">
-        <v>93</v>
-      </c>
-      <c r="B53" s="25"/>
-      <c r="C53" s="25"/>
-      <c r="D53" s="25"/>
-      <c r="E53" s="25"/>
-      <c r="F53" s="25"/>
+    <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A53" s="20" t="s">
+        <v>260</v>
+      </c>
+      <c r="B53" s="26"/>
+      <c r="C53" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D53" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E53" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G53" s="20"/>
-      <c r="H53" s="16"/>
-      <c r="I53" s="16"/>
-    </row>
-    <row r="54" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H53" s="21"/>
+      <c r="I53" s="19"/>
+    </row>
+    <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>265</v>
-      </c>
-      <c r="B54" s="26" t="s">
-        <v>94</v>
-      </c>
+        <v>261</v>
+      </c>
+      <c r="B54" s="26"/>
       <c r="C54" s="27" t="s">
         <v>6</v>
       </c>
@@ -9325,21 +9419,15 @@
       <c r="F54" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G54" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H54" s="19"/>
-      <c r="I54" s="19" t="s">
-        <v>264</v>
-      </c>
-    </row>
-    <row r="55" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="G54" s="20"/>
+      <c r="H54" s="21"/>
+      <c r="I54" s="19"/>
+    </row>
+    <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>266</v>
-      </c>
-      <c r="B55" s="26" t="s">
-        <v>95</v>
-      </c>
+        <v>37</v>
+      </c>
+      <c r="B55" s="26"/>
       <c r="C55" s="27" t="s">
         <v>6</v>
       </c>
@@ -9352,19 +9440,15 @@
       <c r="F55" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G55" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H55" s="19"/>
+      <c r="G55" s="20"/>
+      <c r="H55" s="21"/>
       <c r="I55" s="19"/>
     </row>
-    <row r="56" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>245</v>
-      </c>
-      <c r="B56" s="26" t="s">
-        <v>96</v>
-      </c>
+        <v>38</v>
+      </c>
+      <c r="B56" s="26"/>
       <c r="C56" s="27" t="s">
         <v>6</v>
       </c>
@@ -9377,68 +9461,40 @@
       <c r="F56" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G56" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H56" s="19"/>
+      <c r="G56" s="20"/>
+      <c r="H56" s="21"/>
       <c r="I56" s="19"/>
     </row>
-    <row r="57" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
-        <v>267</v>
-      </c>
-      <c r="B57" s="26" t="s">
-        <v>97</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G57" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H57" s="19"/>
+    <row r="57" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A57" s="20"/>
+      <c r="B57" s="26"/>
+      <c r="C57" s="27"/>
+      <c r="D57" s="27"/>
+      <c r="E57" s="27"/>
+      <c r="F57" s="27"/>
+      <c r="G57" s="20"/>
+      <c r="H57" s="21"/>
       <c r="I57" s="19"/>
     </row>
-    <row r="58" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A58" s="20" t="s">
-        <v>268</v>
-      </c>
-      <c r="B58" s="26" t="s">
-        <v>98</v>
-      </c>
-      <c r="C58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F58" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G58" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H58" s="19"/>
-      <c r="I58" s="19"/>
+    <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A58" s="24" t="s">
+        <v>281</v>
+      </c>
+      <c r="B58" s="25"/>
+      <c r="C58" s="25"/>
+      <c r="D58" s="25"/>
+      <c r="E58" s="25"/>
+      <c r="F58" s="25"/>
+      <c r="G58" s="20"/>
+      <c r="H58" s="16"/>
+      <c r="I58" s="16"/>
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>271</v>
+        <v>241</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>99</v>
+        <v>72</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>6</v>
@@ -9450,565 +9506,610 @@
         <v>6</v>
       </c>
       <c r="F59" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>261</v>
-      </c>
-      <c r="H59" s="21"/>
-      <c r="I59" s="19"/>
+        <v>237</v>
+      </c>
+      <c r="H59" s="19"/>
+      <c r="I59" s="19" t="s">
+        <v>240</v>
+      </c>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A60" s="20"/>
-      <c r="B60" s="26"/>
-      <c r="C60" s="27"/>
-      <c r="D60" s="27"/>
-      <c r="E60" s="27"/>
-      <c r="F60" s="27"/>
-      <c r="G60" s="20"/>
+      <c r="A60" s="20" t="s">
+        <v>242</v>
+      </c>
+      <c r="B60" s="26" t="s">
+        <v>73</v>
+      </c>
+      <c r="C60" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D60" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E60" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F60" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G60" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="H60" s="19"/>
       <c r="I60" s="19"/>
     </row>
-    <row r="61" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A61" s="24" t="s">
-        <v>100</v>
-      </c>
-      <c r="B61" s="25"/>
-      <c r="C61" s="25"/>
-      <c r="D61" s="25"/>
-      <c r="E61" s="25"/>
-      <c r="F61" s="25"/>
-      <c r="G61" s="20"/>
-      <c r="H61" s="16"/>
-      <c r="I61" s="16"/>
+    <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A61" s="20" t="s">
+        <v>278</v>
+      </c>
+      <c r="B61" s="26" t="s">
+        <v>74</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G61" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="H61" s="19"/>
+      <c r="I61" s="19"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>101</v>
+        <v>243</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>102</v>
+        <v>75</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D62" s="27"/>
+      <c r="D62" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="E62" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F62" s="27"/>
-      <c r="G62" s="20"/>
+      <c r="F62" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>103</v>
+        <v>244</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>104</v>
+        <v>76</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D63" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E63" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F63" s="27"/>
-      <c r="G63" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="F63" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="20" t="s">
+        <v>237</v>
+      </c>
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>105</v>
+        <v>279</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>106</v>
+        <v>77</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D64" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E64" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F64" s="27"/>
-      <c r="G64" s="20"/>
-      <c r="H64" s="19"/>
+        <v>6</v>
+      </c>
+      <c r="F64" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="G64" s="20" t="s">
+        <v>237</v>
+      </c>
+      <c r="H64" s="21"/>
       <c r="I64" s="19"/>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="20" t="s">
-        <v>107</v>
-      </c>
-      <c r="B65" s="26" t="s">
-        <v>108</v>
-      </c>
-      <c r="C65" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D65" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E65" s="27" t="s">
-        <v>246</v>
-      </c>
+      <c r="A65" s="20"/>
+      <c r="B65" s="26"/>
+      <c r="C65" s="27"/>
+      <c r="D65" s="27"/>
+      <c r="E65" s="27"/>
       <c r="F65" s="27"/>
       <c r="G65" s="20"/>
-      <c r="H65" s="21"/>
+      <c r="H65" s="19"/>
       <c r="I65" s="19"/>
     </row>
-    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A66" s="20" t="s">
-        <v>109</v>
-      </c>
-      <c r="B66" s="26" t="s">
-        <v>110</v>
-      </c>
-      <c r="C66" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D66" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E66" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F66" s="27"/>
+    <row r="66" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A66" s="24" t="s">
+        <v>78</v>
+      </c>
+      <c r="B66" s="25"/>
+      <c r="C66" s="25"/>
+      <c r="D66" s="25"/>
+      <c r="E66" s="25"/>
+      <c r="F66" s="25"/>
       <c r="G66" s="20"/>
-      <c r="H66" s="19"/>
-      <c r="I66" s="19"/>
+      <c r="H66" s="16"/>
+      <c r="I66" s="16"/>
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>111</v>
+        <v>79</v>
       </c>
       <c r="B67" s="26" t="s">
-        <v>112</v>
+        <v>80</v>
       </c>
       <c r="C67" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D67" s="27" t="s">
-        <v>246</v>
-      </c>
+      <c r="D67" s="27"/>
       <c r="E67" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F67" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F67" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G67" s="20"/>
       <c r="H67" s="19"/>
       <c r="I67" s="19"/>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>113</v>
+        <v>81</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>114</v>
+        <v>82</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D68" s="27"/>
+      <c r="D68" s="27" t="s">
+        <v>222</v>
+      </c>
       <c r="E68" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F68" s="27"/>
+        <v>222</v>
+      </c>
+      <c r="F68" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G68" s="20"/>
       <c r="H68" s="19"/>
       <c r="I68" s="19"/>
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>115</v>
+        <v>98</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>116</v>
+        <v>99</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="D69" s="27"/>
+      <c r="D69" s="27" t="s">
+        <v>222</v>
+      </c>
       <c r="E69" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F69" s="27"/>
+        <v>222</v>
+      </c>
+      <c r="F69" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G69" s="20"/>
       <c r="H69" s="19"/>
       <c r="I69" s="19"/>
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="20" t="s">
-        <v>117</v>
-      </c>
-      <c r="B70" s="26" t="s">
-        <v>118</v>
-      </c>
-      <c r="C70" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="A70" s="20"/>
+      <c r="B70" s="26"/>
+      <c r="C70" s="27"/>
       <c r="D70" s="27"/>
-      <c r="E70" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="E70" s="27"/>
       <c r="F70" s="27"/>
       <c r="G70" s="20"/>
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
     </row>
-    <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A71" s="20" t="s">
-        <v>119</v>
-      </c>
-      <c r="B71" s="26" t="s">
-        <v>47</v>
-      </c>
-      <c r="C71" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D71" s="27"/>
-      <c r="E71" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F71" s="27"/>
+    <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>32</v>
+      </c>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="25"/>
       <c r="G71" s="20"/>
-      <c r="H71" s="19"/>
-      <c r="I71" s="19"/>
-    </row>
-    <row r="72" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="H71" s="24"/>
+      <c r="I71" s="16"/>
+    </row>
+    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>120</v>
+        <v>33</v>
       </c>
       <c r="B72" s="26" t="s">
-        <v>121</v>
+        <v>34</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D72" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E72" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F72" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F72" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G72" s="20"/>
-      <c r="H72" s="19"/>
+      <c r="H72" s="20"/>
       <c r="I72" s="19"/>
     </row>
-    <row r="73" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A73" s="20"/>
-      <c r="B73" s="26"/>
-      <c r="C73" s="27"/>
-      <c r="D73" s="27"/>
-      <c r="E73" s="27"/>
-      <c r="F73" s="27"/>
+    <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A73" s="20" t="s">
+        <v>35</v>
+      </c>
+      <c r="B73" s="26">
+        <v>98</v>
+      </c>
+      <c r="C73" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D73" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E73" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F73" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G73" s="20"/>
-      <c r="H73" s="19"/>
+      <c r="H73" s="29"/>
       <c r="I73" s="19"/>
     </row>
-    <row r="74" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A74" s="24" t="s">
-        <v>122</v>
-      </c>
-      <c r="B74" s="25"/>
-      <c r="C74" s="25"/>
-      <c r="D74" s="25"/>
-      <c r="E74" s="25"/>
-      <c r="F74" s="25"/>
+    <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A74" s="20" t="s">
+        <v>36</v>
+      </c>
+      <c r="B74" s="26">
+        <v>99</v>
+      </c>
+      <c r="C74" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D74" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E74" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F74" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G74" s="20"/>
-      <c r="H74" s="16"/>
-      <c r="I74" s="16"/>
-    </row>
-    <row r="75" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A75" s="20" t="s">
-        <v>123</v>
-      </c>
-      <c r="B75" s="26" t="s">
-        <v>124</v>
-      </c>
-      <c r="C75" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D75" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E75" s="27" t="s">
-        <v>246</v>
-      </c>
+      <c r="H74" s="29"/>
+      <c r="I74" s="19"/>
+    </row>
+    <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A75" s="20"/>
+      <c r="B75" s="26"/>
+      <c r="C75" s="27"/>
+      <c r="D75" s="27"/>
+      <c r="E75" s="27"/>
       <c r="F75" s="27"/>
       <c r="G75" s="20"/>
-      <c r="H75" s="19"/>
+      <c r="H75" s="29"/>
       <c r="I75" s="19"/>
     </row>
-    <row r="76" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A76" s="20" t="s">
+    <row r="76" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A76" s="24" t="s">
         <v>125</v>
       </c>
-      <c r="B76" s="26" t="s">
-        <v>126</v>
-      </c>
-      <c r="C76" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D76" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E76" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F76" s="27"/>
+      <c r="B76" s="25"/>
+      <c r="C76" s="25"/>
+      <c r="D76" s="25"/>
+      <c r="E76" s="25"/>
+      <c r="F76" s="25"/>
       <c r="G76" s="20"/>
-      <c r="H76" s="19"/>
-      <c r="I76" s="19"/>
-    </row>
-    <row r="77" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A77" s="20" t="s">
-        <v>127</v>
+      <c r="H76" s="16"/>
+      <c r="I76" s="16"/>
+    </row>
+    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A77" s="31" t="s">
+        <v>239</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>128</v>
+        <v>143</v>
       </c>
       <c r="C77" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D77" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E77" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F77" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F77" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G77" s="20"/>
       <c r="H77" s="19"/>
       <c r="I77" s="19"/>
     </row>
-    <row r="78" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A78" s="20" t="s">
-        <v>129</v>
+    <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A78" s="31" t="s">
+        <v>126</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>130</v>
+        <v>127</v>
       </c>
       <c r="C78" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D78" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E78" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F78" s="27"/>
-      <c r="G78" s="20"/>
+        <v>6</v>
+      </c>
+      <c r="F78" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
     </row>
-    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A79" s="20" t="s">
-        <v>131</v>
+    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A79" s="31" t="s">
+        <v>128</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>132</v>
+        <v>129</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D79" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E79" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F79" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F79" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G79" s="20"/>
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
     </row>
-    <row r="80" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A80" s="20" t="s">
-        <v>133</v>
+    <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A80" s="31" t="s">
+        <v>130</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>134</v>
+        <v>131</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D80" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E80" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F80" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F80" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G80" s="20"/>
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
     </row>
-    <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A81" s="20" t="s">
-        <v>135</v>
+    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A81" s="31" t="s">
+        <v>132</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>136</v>
+        <v>133</v>
       </c>
       <c r="C81" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D81" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E81" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F81" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F81" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G81" s="20"/>
       <c r="H81" s="19"/>
       <c r="I81" s="19"/>
     </row>
-    <row r="82" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A82" s="20" t="s">
-        <v>137</v>
+    <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A82" s="31" t="s">
+        <v>134</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>138</v>
+        <v>135</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D82" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E82" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F82" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F82" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G82" s="20"/>
       <c r="H82" s="19"/>
       <c r="I82" s="19"/>
     </row>
-    <row r="83" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A83" s="20" t="s">
-        <v>139</v>
+    <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A83" s="31" t="s">
+        <v>136</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>140</v>
+        <v>137</v>
       </c>
       <c r="C83" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D83" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E83" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F83" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F83" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G83" s="20"/>
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
     </row>
-    <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A84" s="20" t="s">
-        <v>141</v>
+    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A84" s="31" t="s">
+        <v>138</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>142</v>
+        <v>139</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D84" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E84" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F84" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F84" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G84" s="20"/>
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
-        <v>143</v>
+        <v>140</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>144</v>
+        <v>141</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D85" s="27" t="s">
-        <v>246</v>
+        <v>6</v>
       </c>
       <c r="E85" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="F85" s="27"/>
+        <v>6</v>
+      </c>
+      <c r="F85" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G85" s="20"/>
       <c r="H85" s="19"/>
       <c r="I85" s="19"/>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="20" t="s">
-        <v>145</v>
-      </c>
-      <c r="B86" s="26" t="s">
-        <v>146</v>
-      </c>
-      <c r="C86" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D86" s="27" t="s">
-        <v>246</v>
-      </c>
-      <c r="E86" s="27" t="s">
-        <v>246</v>
-      </c>
+      <c r="A86" s="20"/>
+      <c r="B86" s="26"/>
+      <c r="C86" s="27"/>
+      <c r="D86" s="27"/>
+      <c r="E86" s="27"/>
       <c r="F86" s="27"/>
       <c r="G86" s="20"/>
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
     </row>
-    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A87" s="20"/>
-      <c r="B87" s="26"/>
-      <c r="C87" s="27"/>
-      <c r="D87" s="27"/>
-      <c r="E87" s="27"/>
-      <c r="F87" s="27"/>
+    <row r="87" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A87" s="24" t="s">
+        <v>142</v>
+      </c>
+      <c r="B87" s="25"/>
+      <c r="C87" s="25"/>
+      <c r="D87" s="25"/>
+      <c r="E87" s="25"/>
+      <c r="F87" s="25"/>
       <c r="G87" s="20"/>
-      <c r="H87" s="19"/>
-      <c r="I87" s="19"/>
-    </row>
-    <row r="88" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A88" s="24" t="s">
-        <v>147</v>
-      </c>
-      <c r="B88" s="25"/>
-      <c r="C88" s="25"/>
-      <c r="D88" s="25"/>
-      <c r="E88" s="25"/>
-      <c r="F88" s="25"/>
-      <c r="G88" s="20"/>
-      <c r="H88" s="16"/>
-      <c r="I88" s="16"/>
-    </row>
-    <row r="89" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A89" s="31" t="s">
-        <v>148</v>
+      <c r="H87" s="16"/>
+      <c r="I87" s="16"/>
+    </row>
+    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A88" s="20" t="s">
+        <v>247</v>
+      </c>
+      <c r="B88" s="26" t="s">
+        <v>144</v>
+      </c>
+      <c r="C88" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D88" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E88" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F88" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G88" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H88" s="19"/>
+      <c r="I88" s="19"/>
+    </row>
+    <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A89" s="20" t="s">
+        <v>248</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>149</v>
+        <v>145</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>6</v>
@@ -10021,16 +10122,19 @@
       </c>
       <c r="F89" s="27" t="s">
         <v>6</v>
+      </c>
+      <c r="G89" s="20" t="s">
+        <v>238</v>
       </c>
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
-    <row r="90" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A90" s="31" t="s">
-        <v>150</v>
+    <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A90" s="20" t="s">
+        <v>249</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>151</v>
+        <v>146</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>6</v>
@@ -10044,16 +10148,18 @@
       <c r="F90" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G90" s="20"/>
+      <c r="G90" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
-    <row r="91" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A91" s="31" t="s">
-        <v>152</v>
+    <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A91" s="20" t="s">
+        <v>250</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>6</v>
@@ -10067,16 +10173,18 @@
       <c r="F91" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G91" s="20"/>
+      <c r="G91" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
-    <row r="92" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A92" s="31" t="s">
-        <v>154</v>
+    <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A92" s="20" t="s">
+        <v>251</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>155</v>
+        <v>148</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>6</v>
@@ -10090,16 +10198,18 @@
       <c r="F92" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G92" s="20"/>
+      <c r="G92" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
-    <row r="93" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A93" s="31" t="s">
-        <v>156</v>
+    <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A93" s="20" t="s">
+        <v>235</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>157</v>
+        <v>149</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>6</v>
@@ -10113,16 +10223,18 @@
       <c r="F93" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G93" s="20"/>
+      <c r="G93" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
-    <row r="94" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A94" s="31" t="s">
-        <v>158</v>
+    <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A94" s="20" t="s">
+        <v>236</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>159</v>
+        <v>150</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>6</v>
@@ -10136,16 +10248,18 @@
       <c r="F94" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G94" s="20"/>
+      <c r="G94" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
-    <row r="95" spans="1:9" ht="45" x14ac:dyDescent="0.2">
-      <c r="A95" s="31" t="s">
-        <v>160</v>
+    <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A95" s="20" t="s">
+        <v>252</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>161</v>
+        <v>151</v>
       </c>
       <c r="C95" s="27" t="s">
         <v>6</v>
@@ -10159,16 +10273,18 @@
       <c r="F95" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G95" s="20"/>
+      <c r="G95" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>162</v>
+        <v>253</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>163</v>
+        <v>152</v>
       </c>
       <c r="C96" s="27" t="s">
         <v>6</v>
@@ -10182,40 +10298,68 @@
       <c r="F96" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G96" s="20"/>
+      <c r="G96" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A97" s="20"/>
-      <c r="B97" s="26"/>
-      <c r="C97" s="27"/>
-      <c r="D97" s="27"/>
-      <c r="E97" s="27"/>
-      <c r="F97" s="27"/>
-      <c r="G97" s="20"/>
+      <c r="A97" s="20" t="s">
+        <v>254</v>
+      </c>
+      <c r="B97" s="26" t="s">
+        <v>153</v>
+      </c>
+      <c r="C97" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D97" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E97" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F97" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G97" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
-    <row r="98" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A98" s="24" t="s">
-        <v>164</v>
-      </c>
-      <c r="B98" s="25"/>
-      <c r="C98" s="25"/>
-      <c r="D98" s="25"/>
-      <c r="E98" s="25"/>
-      <c r="F98" s="25"/>
-      <c r="G98" s="20"/>
-      <c r="H98" s="16"/>
-      <c r="I98" s="16"/>
-    </row>
-    <row r="99" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A99" s="31" t="s">
-        <v>263</v>
+    <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A98" s="31" t="s">
+        <v>255</v>
+      </c>
+      <c r="B98" s="26" t="s">
+        <v>154</v>
+      </c>
+      <c r="C98" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D98" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E98" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F98" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G98" s="20" t="s">
+        <v>238</v>
+      </c>
+      <c r="H98" s="19"/>
+      <c r="I98" s="19"/>
+    </row>
+    <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A99" s="20" t="s">
+        <v>256</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>165</v>
+        <v>155</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>6</v>
@@ -10229,423 +10373,411 @@
       <c r="F99" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G99" s="20"/>
+      <c r="G99" s="20" t="s">
+        <v>238</v>
+      </c>
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A100" s="20" t="s">
-        <v>273</v>
-      </c>
-      <c r="B100" s="26" t="s">
-        <v>166</v>
-      </c>
-      <c r="C100" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D100" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E100" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F100" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G100" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="H100" s="19"/>
-      <c r="I100" s="19"/>
-    </row>
-    <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A101" s="20" t="s">
-        <v>274</v>
-      </c>
-      <c r="B101" s="26" t="s">
-        <v>167</v>
-      </c>
-      <c r="C101" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D101" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E101" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F101" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G101" s="20" t="s">
-        <v>262</v>
-      </c>
-      <c r="H101" s="19"/>
-      <c r="I101" s="19"/>
+      <c r="B100" s="7"/>
+      <c r="C100" s="7"/>
+      <c r="D100" s="8"/>
+      <c r="E100" s="8"/>
+      <c r="F100" s="8"/>
+    </row>
+    <row r="101" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A101" s="24" t="s">
+        <v>100</v>
+      </c>
+      <c r="B101" s="25"/>
+      <c r="C101" s="25"/>
+      <c r="D101" s="25"/>
+      <c r="E101" s="25"/>
+      <c r="F101" s="25"/>
+      <c r="G101" s="20"/>
+      <c r="H101" s="16"/>
+      <c r="I101" s="16"/>
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
-        <v>275</v>
+        <v>101</v>
       </c>
       <c r="B102" s="26" t="s">
-        <v>168</v>
+        <v>102</v>
       </c>
       <c r="C102" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F102" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G102" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G102" s="20"/>
       <c r="H102" s="19"/>
       <c r="I102" s="19"/>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
-        <v>276</v>
+        <v>103</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>169</v>
+        <v>104</v>
       </c>
       <c r="C103" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F103" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G103" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G103" s="20"/>
       <c r="H103" s="19"/>
       <c r="I103" s="19"/>
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
-        <v>277</v>
+        <v>105</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>170</v>
+        <v>106</v>
       </c>
       <c r="C104" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F104" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G104" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G104" s="20"/>
       <c r="H104" s="19"/>
       <c r="I104" s="19"/>
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
-        <v>259</v>
+        <v>107</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>171</v>
+        <v>108</v>
       </c>
       <c r="C105" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F105" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G105" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G105" s="20"/>
       <c r="H105" s="19"/>
       <c r="I105" s="19"/>
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
-        <v>260</v>
+        <v>109</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>172</v>
+        <v>110</v>
       </c>
       <c r="C106" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F106" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G106" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G106" s="20"/>
       <c r="H106" s="19"/>
       <c r="I106" s="19"/>
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
-        <v>278</v>
+        <v>111</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>173</v>
+        <v>112</v>
       </c>
       <c r="C107" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F107" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G107" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G107" s="20"/>
       <c r="H107" s="19"/>
       <c r="I107" s="19"/>
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
-        <v>279</v>
+        <v>113</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>174</v>
+        <v>114</v>
       </c>
       <c r="C108" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G108" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G108" s="20"/>
       <c r="H108" s="19"/>
       <c r="I108" s="19"/>
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
-        <v>280</v>
+        <v>115</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>175</v>
+        <v>116</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F109" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G109" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G109" s="20"/>
       <c r="H109" s="19"/>
       <c r="I109" s="19"/>
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A110" s="31" t="s">
-        <v>281</v>
+      <c r="A110" s="20" t="s">
+        <v>117</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>176</v>
+        <v>118</v>
       </c>
       <c r="C110" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F110" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G110" s="20" t="s">
-        <v>262</v>
-      </c>
+        <v>222</v>
+      </c>
+      <c r="G110" s="20"/>
       <c r="H110" s="19"/>
       <c r="I110" s="19"/>
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
-        <v>282</v>
+        <v>119</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>177</v>
+        <v>120</v>
       </c>
       <c r="C111" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D111" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>6</v>
+        <v>222</v>
       </c>
       <c r="F111" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G111" s="20" t="s">
-        <v>262</v>
-      </c>
+      <c r="G111" s="20"/>
       <c r="H111" s="19"/>
       <c r="I111" s="19"/>
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B112" s="7"/>
-      <c r="C112" s="7"/>
-      <c r="D112" s="8"/>
-      <c r="E112" s="8"/>
-      <c r="F112" s="8"/>
-    </row>
-    <row r="113" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B113" s="7"/>
-      <c r="C113" s="7"/>
-      <c r="D113" s="8"/>
-      <c r="E113" s="8"/>
-      <c r="F113" s="8"/>
-    </row>
-    <row r="114" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B114" s="7"/>
-      <c r="C114" s="7"/>
-      <c r="D114" s="8"/>
-      <c r="E114" s="8"/>
-      <c r="F114" s="8"/>
-    </row>
-    <row r="115" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="A112" s="20" t="s">
+        <v>121</v>
+      </c>
+      <c r="B112" s="26" t="s">
+        <v>122</v>
+      </c>
+      <c r="C112" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D112" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E112" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="F112" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G112" s="20"/>
+      <c r="H112" s="19"/>
+      <c r="I112" s="19"/>
+    </row>
+    <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A113" s="20" t="s">
+        <v>123</v>
+      </c>
+      <c r="B113" s="26" t="s">
+        <v>124</v>
+      </c>
+      <c r="C113" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D113" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="E113" s="27" t="s">
+        <v>222</v>
+      </c>
+      <c r="F113" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G113" s="20"/>
+      <c r="H113" s="19"/>
+      <c r="I113" s="19"/>
+    </row>
+    <row r="114" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A114" s="20"/>
+      <c r="B114" s="26"/>
+      <c r="C114" s="27"/>
+      <c r="D114" s="27"/>
+      <c r="E114" s="27"/>
+      <c r="F114" s="27"/>
+      <c r="G114" s="20"/>
+      <c r="H114" s="19"/>
+      <c r="I114" s="19"/>
+    </row>
+    <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B115" s="7"/>
       <c r="C115" s="7"/>
       <c r="D115" s="8"/>
       <c r="E115" s="8"/>
       <c r="F115" s="8"/>
     </row>
-    <row r="116" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B116" s="7"/>
       <c r="C116" s="7"/>
       <c r="D116" s="8"/>
       <c r="E116" s="8"/>
       <c r="F116" s="8"/>
     </row>
-    <row r="117" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="117" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B117" s="7"/>
       <c r="C117" s="7"/>
       <c r="D117" s="8"/>
       <c r="E117" s="8"/>
       <c r="F117" s="8"/>
     </row>
-    <row r="118" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B118" s="8"/>
-      <c r="C118" s="8"/>
+    <row r="118" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B118" s="7"/>
+      <c r="C118" s="7"/>
       <c r="D118" s="8"/>
       <c r="E118" s="8"/>
       <c r="F118" s="8"/>
     </row>
-    <row r="119" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B119" s="8"/>
-      <c r="C119" s="8"/>
+    <row r="119" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B119" s="7"/>
+      <c r="C119" s="7"/>
       <c r="D119" s="8"/>
       <c r="E119" s="8"/>
       <c r="F119" s="8"/>
     </row>
-    <row r="120" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B120" s="7"/>
-      <c r="C120" s="7"/>
+    <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B120" s="8"/>
+      <c r="C120" s="8"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
     </row>
-    <row r="121" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="121" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B121" s="8"/>
       <c r="C121" s="8"/>
       <c r="D121" s="8"/>
       <c r="E121" s="8"/>
       <c r="F121" s="8"/>
     </row>
-    <row r="122" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B122" s="8"/>
-      <c r="C122" s="8"/>
+    <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B122" s="7"/>
+      <c r="C122" s="7"/>
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
     </row>
-    <row r="123" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B123" s="7"/>
-      <c r="C123" s="7"/>
+    <row r="123" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B123" s="8"/>
+      <c r="C123" s="8"/>
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
     </row>
-    <row r="124" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B124" s="7"/>
-      <c r="C124" s="7"/>
+    <row r="124" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B124" s="8"/>
+      <c r="C124" s="8"/>
       <c r="D124" s="8"/>
       <c r="E124" s="8"/>
       <c r="F124" s="8"/>
     </row>
-    <row r="125" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B125" s="8"/>
+    <row r="125" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B125" s="7"/>
       <c r="C125" s="7"/>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
     </row>
-    <row r="126" spans="2:6" ht="15" x14ac:dyDescent="0.2">
-      <c r="B126" s="8"/>
+    <row r="126" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B126" s="7"/>
       <c r="C126" s="7"/>
       <c r="D126" s="8"/>
       <c r="E126" s="8"/>
       <c r="F126" s="8"/>
     </row>
-    <row r="127" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B127" s="8"/>
       <c r="C127" s="7"/>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
       <c r="F127" s="8"/>
     </row>
-    <row r="128" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+    <row r="128" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B128" s="8"/>
       <c r="C128" s="7"/>
       <c r="D128" s="8"/>
@@ -10654,14 +10786,14 @@
     </row>
     <row r="129" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B129" s="8"/>
-      <c r="C129" s="8"/>
+      <c r="C129" s="7"/>
       <c r="D129" s="8"/>
       <c r="E129" s="8"/>
       <c r="F129" s="8"/>
     </row>
     <row r="130" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B130" s="8"/>
-      <c r="C130" s="8"/>
+      <c r="C130" s="7"/>
       <c r="D130" s="8"/>
       <c r="E130" s="8"/>
       <c r="F130" s="8"/>
@@ -17280,6 +17412,20 @@
       <c r="D1075" s="8"/>
       <c r="E1075" s="8"/>
       <c r="F1075" s="8"/>
+    </row>
+    <row r="1076" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B1076" s="8"/>
+      <c r="C1076" s="8"/>
+      <c r="D1076" s="8"/>
+      <c r="E1076" s="8"/>
+      <c r="F1076" s="8"/>
+    </row>
+    <row r="1077" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B1077" s="8"/>
+      <c r="C1077" s="8"/>
+      <c r="D1077" s="8"/>
+      <c r="E1077" s="8"/>
+      <c r="F1077" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17302,9 +17448,9 @@
   </sheetPr>
   <dimension ref="A1:AC974"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A24" sqref="A24"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -17320,22 +17466,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="35" t="s">
+      <c r="A1" s="36" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="35" t="s">
+      <c r="B1" s="36" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="35"/>
-      <c r="D1" s="35"/>
-      <c r="E1" s="37" t="s">
-        <v>250</v>
-      </c>
-      <c r="F1" s="35" t="s">
-        <v>190</v>
-      </c>
-      <c r="G1" s="35"/>
-      <c r="H1" s="35" t="s">
+      <c r="C1" s="36"/>
+      <c r="D1" s="36"/>
+      <c r="E1" s="38" t="s">
+        <v>226</v>
+      </c>
+      <c r="F1" s="36" t="s">
+        <v>168</v>
+      </c>
+      <c r="G1" s="36"/>
+      <c r="H1" s="36" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1"/>
@@ -17361,7 +17507,7 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="35"/>
+      <c r="A2" s="36"/>
       <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
@@ -17371,14 +17517,14 @@
       <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="37"/>
+      <c r="E2" s="38"/>
       <c r="F2" s="13" t="s">
-        <v>202</v>
+        <v>180</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>200</v>
-      </c>
-      <c r="H2" s="35"/>
+        <v>178</v>
+      </c>
+      <c r="H2" s="36"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -17403,7 +17549,7 @@
     </row>
     <row r="3" spans="1:29" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>188</v>
+        <v>166</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -17436,7 +17582,7 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>178</v>
+        <v>156</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>6</v>
@@ -17447,14 +17593,16 @@
       <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="19"/>
+      <c r="E4" s="39" t="s">
+        <v>6</v>
+      </c>
       <c r="F4" s="20"/>
       <c r="G4" s="20"/>
       <c r="H4" s="19"/>
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>179</v>
+        <v>157</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>6</v>
@@ -17465,14 +17613,16 @@
       <c r="D5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="19"/>
+      <c r="E5" s="39" t="s">
+        <v>6</v>
+      </c>
       <c r="F5" s="20"/>
       <c r="G5" s="20"/>
       <c r="H5" s="19"/>
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>180</v>
+        <v>158</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>6</v>
@@ -17483,32 +17633,36 @@
       <c r="D6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="19"/>
+      <c r="E6" s="39" t="s">
+        <v>6</v>
+      </c>
       <c r="F6" s="21"/>
       <c r="G6" s="21"/>
       <c r="H6" s="22"/>
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>181</v>
+        <v>159</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>246</v>
+        <v>222</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>246</v>
-      </c>
-      <c r="E7" s="19"/>
+        <v>222</v>
+      </c>
+      <c r="E7" s="39" t="s">
+        <v>6</v>
+      </c>
       <c r="F7" s="21"/>
       <c r="G7" s="21"/>
       <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>182</v>
+        <v>160</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>6</v>
@@ -17519,7 +17673,9 @@
       <c r="D8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="19"/>
+      <c r="E8" s="39" t="s">
+        <v>6</v>
+      </c>
       <c r="F8" s="21"/>
       <c r="G8" s="21"/>
       <c r="H8" s="19"/>
@@ -17536,7 +17692,7 @@
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>189</v>
+        <v>167</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -17548,7 +17704,7 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>183</v>
+        <v>161</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -17562,7 +17718,7 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>184</v>
+        <v>162</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -17576,7 +17732,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>185</v>
+        <v>163</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -17590,7 +17746,7 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>186</v>
+        <v>164</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -17604,7 +17760,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>251</v>
+        <v>227</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>

</xml_diff>

<commit_message>
stop stopif pause pauseif prompt promptif Still issues with exec continuing if Python line error
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{1AC09BF8-0876-48A6-84A5-0F1A02E008A1}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29AA93E-8DB3-4C77-8141-61124E949CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48015" yWindow="1950" windowWidth="24810" windowHeight="19560" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48015" yWindow="1950" windowWidth="24810" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="888" uniqueCount="284">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="288">
   <si>
     <t>Statement</t>
   </si>
@@ -85,9 +85,6 @@
   </si>
   <si>
     <t>label:</t>
-  </si>
-  <si>
-    <t>le_prompt(message)</t>
   </si>
   <si>
     <t>jump(string label)</t>
@@ -606,25 +603,10 @@
     <t>sleep(double seconds)</t>
   </si>
   <si>
-    <t>le_pause()</t>
-  </si>
-  <si>
-    <t>le_stop()</t>
-  </si>
-  <si>
     <t>infile_open(string filename)</t>
   </si>
   <si>
     <t>infile_scale(pairs)</t>
-  </si>
-  <si>
-    <t>le_pause</t>
-  </si>
-  <si>
-    <t>le_stop</t>
-  </si>
-  <si>
-    <t>le_prompt</t>
   </si>
   <si>
     <t>jump</t>
@@ -879,6 +861,36 @@
   </si>
   <si>
     <t>set_payload(float mass_kg, float cog_x_m, float cog_y_m, float cog_z_m)</t>
+  </si>
+  <si>
+    <t>pause()</t>
+  </si>
+  <si>
+    <t>stop()</t>
+  </si>
+  <si>
+    <t>pause</t>
+  </si>
+  <si>
+    <t>stop</t>
+  </si>
+  <si>
+    <t>prompt</t>
+  </si>
+  <si>
+    <t>pauseif(bool condition)</t>
+  </si>
+  <si>
+    <t>stopif(bool condition)</t>
+  </si>
+  <si>
+    <t>promptif(bool condition, string message)</t>
+  </si>
+  <si>
+    <t>prompt(string message)</t>
+  </si>
+  <si>
+    <t>HOW HANDLE NO ARG JAVA./PO vs. LES</t>
   </si>
 </sst>
 </file>
@@ -1086,6 +1098,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -1094,9 +1109,6 @@
     </xf>
     <xf numFmtId="0" fontId="8" fillId="0" borderId="3" xfId="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
     </xf>
   </cellXfs>
   <cellStyles count="4">
@@ -1319,11 +1331,11 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AC1006"/>
+  <dimension ref="A1:AC1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="A19" sqref="A19"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1339,27 +1351,27 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:8" s="10" customFormat="1" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="37" t="s">
+      <c r="B1" s="38" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="37"/>
-      <c r="D1" s="37"/>
-      <c r="E1" s="38" t="s">
-        <v>224</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36" t="s">
+      <c r="C1" s="38"/>
+      <c r="D1" s="38"/>
+      <c r="E1" s="39" t="s">
+        <v>218</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37" t="s">
         <v>2</v>
       </c>
     </row>
     <row r="2" spans="1:8" s="10" customFormat="1" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="36"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="14" t="s">
         <v>3</v>
       </c>
@@ -1369,14 +1381,14 @@
       <c r="D2" s="14" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="36"/>
+        <v>177</v>
+      </c>
+      <c r="H2" s="37"/>
     </row>
     <row r="3" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A3" s="16" t="s">
@@ -1407,7 +1419,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19"/>
@@ -1429,7 +1441,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="19"/>
@@ -1451,14 +1463,14 @@
         <v>6</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>213</v>
+        <v>207</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>6</v>
@@ -1473,14 +1485,14 @@
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>169</v>
+        <v>168</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>211</v>
+        <v>205</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>6</v>
@@ -1495,16 +1507,16 @@
         <v>6</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>223</v>
+        <v>217</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>221</v>
+        <v>215</v>
       </c>
       <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>214</v>
+        <v>208</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>6</v>
@@ -1519,16 +1531,16 @@
         <v>6</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>171</v>
+        <v>170</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>170</v>
+        <v>169</v>
       </c>
       <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>212</v>
+        <v>206</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>6</v>
@@ -1543,16 +1555,16 @@
         <v>6</v>
       </c>
       <c r="F10" s="28" t="s">
+        <v>171</v>
+      </c>
+      <c r="G10" s="29" t="s">
         <v>172</v>
-      </c>
-      <c r="G10" s="29" t="s">
-        <v>173</v>
       </c>
       <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>210</v>
+        <v>204</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>6</v>
@@ -1567,14 +1579,14 @@
         <v>6</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>232</v>
+        <v>226</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>216</v>
+        <v>210</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>6</v>
@@ -1589,14 +1601,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>233</v>
+        <v>227</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>217</v>
+        <v>211</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>6</v>
@@ -1611,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>234</v>
+        <v>228</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="28"/>
@@ -1640,7 +1652,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>6</v>
@@ -1651,14 +1663,14 @@
         <v>6</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>215</v>
+        <v>209</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>6</v>
@@ -1669,16 +1681,16 @@
         <v>6</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>177</v>
+        <v>176</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>179</v>
+        <v>178</v>
       </c>
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>175</v>
+        <v>174</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>6</v>
@@ -1689,7 +1701,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>176</v>
+        <v>175</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
@@ -1711,7 +1723,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
@@ -1733,7 +1745,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
@@ -1755,7 +1767,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
@@ -1777,14 +1789,14 @@
         <v>6</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>280</v>
+        <v>274</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>6</v>
@@ -1795,14 +1807,14 @@
         <v>6</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>191</v>
+        <v>190</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>218</v>
+        <v>212</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27" t="s">
@@ -1815,14 +1827,14 @@
         <v>6</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>219</v>
+        <v>213</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27" t="s">
@@ -1835,14 +1847,14 @@
         <v>6</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>220</v>
+        <v>214</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27" t="s">
@@ -1855,7 +1867,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>182</v>
+        <v>181</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
@@ -1872,7 +1884,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>190</v>
+        <v>189</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -1884,7 +1896,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>185</v>
+        <v>184</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>6</v>
@@ -1899,14 +1911,14 @@
         <v>6</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>183</v>
+        <v>182</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>6</v>
@@ -1921,7 +1933,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
@@ -1943,7 +1955,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>187</v>
+        <v>186</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -1960,7 +1972,7 @@
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>189</v>
+        <v>188</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="25"/>
@@ -1972,7 +1984,7 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>184</v>
+        <v>183</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>6</v>
@@ -1987,14 +1999,14 @@
         <v>6</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>186</v>
+        <v>185</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>6</v>
@@ -2009,7 +2021,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>188</v>
+        <v>187</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -2038,7 +2050,7 @@
     </row>
     <row r="38" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>193</v>
+        <v>278</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>6</v>
@@ -2053,14 +2065,14 @@
         <v>6</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>197</v>
+        <v>280</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>194</v>
+        <v>283</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>6</v>
@@ -2071,18 +2083,16 @@
       <c r="D39" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F39" s="20" t="s">
-        <v>198</v>
-      </c>
+      <c r="E39" s="27"/>
+      <c r="F39" s="20"/>
       <c r="G39" s="19"/>
-      <c r="H39" s="19"/>
+      <c r="H39" s="19" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="40" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>21</v>
+        <v>279</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>6</v>
@@ -2097,14 +2107,14 @@
         <v>6</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>199</v>
+        <v>281</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
     </row>
-    <row r="41" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+    <row r="41" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>20</v>
+        <v>284</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>6</v>
@@ -2115,18 +2125,16 @@
       <c r="D41" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F41" s="20" t="s">
-        <v>200</v>
-      </c>
+      <c r="E41" s="27"/>
+      <c r="F41" s="20"/>
       <c r="G41" s="19"/>
-      <c r="H41" s="19"/>
+      <c r="H41" s="19" t="s">
+        <v>287</v>
+      </c>
     </row>
     <row r="42" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>22</v>
+        <v>286</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>6</v>
@@ -2141,75 +2149,54 @@
         <v>6</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>200</v>
+        <v>282</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
     </row>
     <row r="43" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>23</v>
-      </c>
-      <c r="B43" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="C43" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="D43" s="33" t="s">
-        <v>6</v>
-      </c>
-      <c r="E43" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F43" s="20" t="s">
-        <v>200</v>
-      </c>
-      <c r="G43" s="30"/>
-      <c r="H43" s="30"/>
-      <c r="I43" s="6"/>
-      <c r="J43" s="6"/>
-      <c r="K43" s="6"/>
-      <c r="L43" s="6"/>
-      <c r="M43" s="6"/>
-      <c r="N43" s="6"/>
-      <c r="O43" s="6"/>
-      <c r="P43" s="6"/>
-      <c r="Q43" s="6"/>
-      <c r="R43" s="6"/>
-      <c r="S43" s="6"/>
-      <c r="T43" s="6"/>
-      <c r="U43" s="6"/>
-      <c r="V43" s="6"/>
-      <c r="W43" s="6"/>
-      <c r="X43" s="6"/>
-      <c r="Y43" s="6"/>
-      <c r="Z43" s="6"/>
-      <c r="AA43" s="6"/>
-      <c r="AB43" s="6"/>
-      <c r="AC43" s="6"/>
-    </row>
-    <row r="44" spans="1:29" ht="15" x14ac:dyDescent="0.2">
+        <v>285</v>
+      </c>
+      <c r="B43" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C43" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D43" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E43" s="27"/>
+      <c r="F43" s="20"/>
+      <c r="G43" s="19"/>
+      <c r="H43" s="19"/>
+    </row>
+    <row r="44" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>24</v>
+        <v>20</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C44" s="27"/>
-      <c r="D44" s="27"/>
+      <c r="C44" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D44" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="E44" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>200</v>
+        <v>194</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>25</v>
+        <v>21</v>
       </c>
       <c r="B45" s="27" t="s">
         <v>6</v>
@@ -2224,16 +2211,16 @@
         <v>6</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
     </row>
     <row r="46" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>26</v>
-      </c>
-      <c r="B46" s="27" t="s">
+        <v>22</v>
+      </c>
+      <c r="B46" s="33" t="s">
         <v>6</v>
       </c>
       <c r="C46" s="33" t="s">
@@ -2246,36 +2233,53 @@
         <v>6</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>201</v>
-      </c>
-      <c r="G46" s="19"/>
-      <c r="H46" s="19"/>
+        <v>194</v>
+      </c>
+      <c r="G46" s="30"/>
+      <c r="H46" s="30"/>
+      <c r="I46" s="6"/>
+      <c r="J46" s="6"/>
+      <c r="K46" s="6"/>
+      <c r="L46" s="6"/>
+      <c r="M46" s="6"/>
+      <c r="N46" s="6"/>
+      <c r="O46" s="6"/>
+      <c r="P46" s="6"/>
+      <c r="Q46" s="6"/>
+      <c r="R46" s="6"/>
+      <c r="S46" s="6"/>
+      <c r="T46" s="6"/>
+      <c r="U46" s="6"/>
+      <c r="V46" s="6"/>
+      <c r="W46" s="6"/>
+      <c r="X46" s="6"/>
+      <c r="Y46" s="6"/>
+      <c r="Z46" s="6"/>
+      <c r="AA46" s="6"/>
+      <c r="AB46" s="6"/>
+      <c r="AC46" s="6"/>
     </row>
     <row r="47" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>27</v>
+        <v>23</v>
       </c>
       <c r="B47" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C47" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D47" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="C47" s="27"/>
+      <c r="D47" s="27"/>
       <c r="E47" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>201</v>
+        <v>194</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>192</v>
+        <v>24</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>6</v>
@@ -2290,52 +2294,62 @@
         <v>6</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>202</v>
+        <v>195</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="19"/>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>230</v>
+        <v>25</v>
       </c>
       <c r="B49" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C49" s="27"/>
-      <c r="D49" s="27"/>
+      <c r="C49" s="33" t="s">
+        <v>6</v>
+      </c>
+      <c r="D49" s="33" t="s">
+        <v>6</v>
+      </c>
       <c r="E49" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>231</v>
+        <v>26</v>
       </c>
       <c r="B50" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C50" s="27"/>
-      <c r="D50" s="27"/>
+      <c r="C50" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D50" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="E50" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>181</v>
+        <v>195</v>
       </c>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>228</v>
-      </c>
-      <c r="B51" s="27"/>
+        <v>191</v>
+      </c>
+      <c r="B51" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="C51" s="27" t="s">
         <v>6</v>
       </c>
@@ -2346,122 +2360,112 @@
         <v>6</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>181</v>
+        <v>196</v>
       </c>
       <c r="G51" s="19"/>
       <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>229</v>
-      </c>
-      <c r="B52" s="27"/>
-      <c r="C52" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D52" s="27" t="s">
-        <v>6</v>
-      </c>
+        <v>224</v>
+      </c>
+      <c r="B52" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C52" s="27"/>
+      <c r="D52" s="27"/>
       <c r="E52" s="27" t="s">
         <v>6</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>181</v>
+        <v>180</v>
       </c>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A53" s="20"/>
-      <c r="B53" s="27"/>
+      <c r="A53" s="20" t="s">
+        <v>225</v>
+      </c>
+      <c r="B53" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="C53" s="27"/>
       <c r="D53" s="27"/>
-      <c r="E53" s="32"/>
-      <c r="F53" s="19"/>
+      <c r="E53" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F53" s="20" t="s">
+        <v>180</v>
+      </c>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
     </row>
-    <row r="54" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
-      <c r="A54" s="24" t="s">
+    <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A54" s="20" t="s">
+        <v>222</v>
+      </c>
+      <c r="B54" s="27"/>
+      <c r="C54" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D54" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E54" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F54" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G54" s="19"/>
+      <c r="H54" s="19"/>
+    </row>
+    <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A55" s="20" t="s">
+        <v>223</v>
+      </c>
+      <c r="B55" s="27"/>
+      <c r="C55" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D55" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E55" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F55" s="20" t="s">
+        <v>180</v>
+      </c>
+      <c r="G55" s="19"/>
+      <c r="H55" s="19"/>
+    </row>
+    <row r="56" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A56" s="20"/>
+      <c r="B56" s="27"/>
+      <c r="C56" s="27"/>
+      <c r="D56" s="27"/>
+      <c r="E56" s="32"/>
+      <c r="F56" s="19"/>
+      <c r="G56" s="19"/>
+      <c r="H56" s="19"/>
+    </row>
+    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
+      <c r="A57" s="24" t="s">
         <v>16</v>
       </c>
-      <c r="B54" s="25"/>
-      <c r="C54" s="25"/>
-      <c r="D54" s="25"/>
-      <c r="E54" s="25"/>
-      <c r="F54" s="16"/>
-      <c r="G54" s="16"/>
-      <c r="H54" s="16"/>
-    </row>
-    <row r="55" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A55" s="20" t="s">
-        <v>203</v>
-      </c>
-      <c r="B55" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C55" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D55" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E55" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F55" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="G55" s="19"/>
-      <c r="H55" s="28"/>
-    </row>
-    <row r="56" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A56" s="20" t="s">
-        <v>204</v>
-      </c>
-      <c r="B56" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C56" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D56" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E56" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F56" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="G56" s="19"/>
-      <c r="H56" s="28"/>
-    </row>
-    <row r="57" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A57" s="20" t="s">
-        <v>205</v>
-      </c>
-      <c r="B57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E57" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F57" s="28" t="s">
-        <v>208</v>
-      </c>
-      <c r="G57" s="19"/>
-      <c r="H57" s="28"/>
+      <c r="B57" s="25"/>
+      <c r="C57" s="25"/>
+      <c r="D57" s="25"/>
+      <c r="E57" s="25"/>
+      <c r="F57" s="16"/>
+      <c r="G57" s="16"/>
+      <c r="H57" s="16"/>
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>206</v>
+        <v>197</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>6</v>
@@ -2476,14 +2480,14 @@
         <v>6</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>17</v>
+        <v>198</v>
       </c>
       <c r="B59" s="27" t="s">
         <v>6</v>
@@ -2498,14 +2502,14 @@
         <v>6</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G59" s="19"/>
       <c r="H59" s="28"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>18</v>
+        <v>199</v>
       </c>
       <c r="B60" s="27" t="s">
         <v>6</v>
@@ -2520,90 +2524,102 @@
         <v>6</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>208</v>
+        <v>202</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="28"/>
     </row>
-    <row r="61" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A61" s="34"/>
-      <c r="B61" s="27"/>
-      <c r="C61" s="27"/>
-      <c r="D61" s="27"/>
-      <c r="E61" s="32"/>
-      <c r="F61" s="19"/>
+    <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A61" s="20" t="s">
+        <v>200</v>
+      </c>
+      <c r="B61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E61" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F61" s="28" t="s">
+        <v>202</v>
+      </c>
       <c r="G61" s="19"/>
-      <c r="H61" s="19"/>
-    </row>
-    <row r="62" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A62" s="24" t="s">
-        <v>28</v>
-      </c>
-      <c r="B62" s="25"/>
-      <c r="C62" s="25"/>
-      <c r="D62" s="25"/>
-      <c r="E62" s="25"/>
-      <c r="F62" s="16"/>
-      <c r="G62" s="16"/>
-      <c r="H62" s="16"/>
-    </row>
-    <row r="63" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="H61" s="28"/>
+    </row>
+    <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A62" s="20" t="s">
+        <v>17</v>
+      </c>
+      <c r="B62" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C62" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D62" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E62" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F62" s="28" t="s">
+        <v>202</v>
+      </c>
+      <c r="G62" s="19"/>
+      <c r="H62" s="28"/>
+    </row>
+    <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>195</v>
+        <v>18</v>
       </c>
       <c r="B63" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="C63" s="27"/>
-      <c r="D63" s="27"/>
+      <c r="C63" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D63" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="E63" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="F63" s="20" t="s">
-        <v>207</v>
+      <c r="F63" s="28" t="s">
+        <v>202</v>
       </c>
       <c r="G63" s="19"/>
-      <c r="H63" s="19"/>
-    </row>
-    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A64" s="20" t="s">
-        <v>29</v>
-      </c>
-      <c r="B64" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="H63" s="28"/>
+    </row>
+    <row r="64" spans="1:8" ht="15" x14ac:dyDescent="0.25">
+      <c r="A64" s="34"/>
+      <c r="B64" s="27"/>
       <c r="C64" s="27"/>
       <c r="D64" s="27"/>
-      <c r="E64" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F64" s="20" t="s">
-        <v>207</v>
-      </c>
+      <c r="E64" s="32"/>
+      <c r="F64" s="19"/>
       <c r="G64" s="19"/>
       <c r="H64" s="19"/>
     </row>
-    <row r="65" spans="1:8" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="20" t="s">
-        <v>30</v>
-      </c>
-      <c r="B65" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F65" s="20" t="s">
-        <v>207</v>
-      </c>
-      <c r="G65" s="19"/>
-      <c r="H65" s="19"/>
+    <row r="65" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A65" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="B65" s="25"/>
+      <c r="C65" s="25"/>
+      <c r="D65" s="25"/>
+      <c r="E65" s="25"/>
+      <c r="F65" s="16"/>
+      <c r="G65" s="16"/>
+      <c r="H65" s="16"/>
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>196</v>
+        <v>192</v>
       </c>
       <c r="B66" s="27" t="s">
         <v>6</v>
@@ -2614,66 +2630,102 @@
         <v>6</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>207</v>
+        <v>201</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
     </row>
-    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A67" s="34"/>
-      <c r="B67" s="27"/>
+    <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A67" s="20" t="s">
+        <v>28</v>
+      </c>
+      <c r="B67" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="C67" s="27"/>
       <c r="D67" s="27"/>
-      <c r="E67" s="32"/>
-      <c r="F67" s="19"/>
+      <c r="E67" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F67" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
     </row>
-    <row r="68" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A68" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B68" s="25"/>
-      <c r="C68" s="25"/>
-      <c r="D68" s="25"/>
-      <c r="E68" s="25"/>
-      <c r="F68" s="16"/>
-      <c r="G68" s="16"/>
-      <c r="H68" s="16"/>
+    <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A68" s="20" t="s">
+        <v>29</v>
+      </c>
+      <c r="B68" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C68" s="27"/>
+      <c r="D68" s="27"/>
+      <c r="E68" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F68" s="20" t="s">
+        <v>201</v>
+      </c>
+      <c r="G68" s="19"/>
+      <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>209</v>
+        <v>193</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>6</v>
       </c>
       <c r="C69" s="27"/>
       <c r="D69" s="27"/>
-      <c r="E69" s="32" t="s">
-        <v>222</v>
-      </c>
-      <c r="F69" s="19"/>
+      <c r="E69" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F69" s="20" t="s">
+        <v>201</v>
+      </c>
       <c r="G69" s="19"/>
       <c r="H69" s="19"/>
     </row>
     <row r="70" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A70" s="5"/>
-      <c r="B70" s="8"/>
-      <c r="C70" s="8"/>
-      <c r="D70" s="8"/>
-    </row>
-    <row r="71" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A71" s="5"/>
-      <c r="B71" s="8"/>
-      <c r="C71" s="8"/>
-      <c r="D71" s="8"/>
-    </row>
-    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.25">
-      <c r="A72" s="5"/>
-      <c r="B72" s="8"/>
-      <c r="C72" s="8"/>
-      <c r="D72" s="8"/>
+      <c r="A70" s="34"/>
+      <c r="B70" s="27"/>
+      <c r="C70" s="27"/>
+      <c r="D70" s="27"/>
+      <c r="E70" s="32"/>
+      <c r="F70" s="19"/>
+      <c r="G70" s="19"/>
+      <c r="H70" s="19"/>
+    </row>
+    <row r="71" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A71" s="24" t="s">
+        <v>30</v>
+      </c>
+      <c r="B71" s="25"/>
+      <c r="C71" s="25"/>
+      <c r="D71" s="25"/>
+      <c r="E71" s="25"/>
+      <c r="F71" s="16"/>
+      <c r="G71" s="16"/>
+      <c r="H71" s="16"/>
+    </row>
+    <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.2">
+      <c r="A72" s="20" t="s">
+        <v>203</v>
+      </c>
+      <c r="B72" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="C72" s="27"/>
+      <c r="D72" s="27"/>
+      <c r="E72" s="32" t="s">
+        <v>216</v>
+      </c>
+      <c r="F72" s="19"/>
+      <c r="G72" s="19"/>
+      <c r="H72" s="19"/>
     </row>
     <row r="73" spans="1:8" ht="15" x14ac:dyDescent="0.25">
       <c r="A73" s="5"/>
@@ -8278,6 +8330,24 @@
       <c r="B1006" s="8"/>
       <c r="C1006" s="8"/>
       <c r="D1006" s="8"/>
+    </row>
+    <row r="1007" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1007" s="5"/>
+      <c r="B1007" s="8"/>
+      <c r="C1007" s="8"/>
+      <c r="D1007" s="8"/>
+    </row>
+    <row r="1008" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1008" s="5"/>
+      <c r="B1008" s="8"/>
+      <c r="C1008" s="8"/>
+      <c r="D1008" s="8"/>
+    </row>
+    <row r="1009" spans="1:4" ht="15" x14ac:dyDescent="0.25">
+      <c r="A1009" s="5"/>
+      <c r="B1009" s="8"/>
+      <c r="C1009" s="8"/>
+      <c r="D1009" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="5">
@@ -8318,25 +8388,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:30" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="38" t="s">
-        <v>165</v>
-      </c>
-      <c r="C1" s="36" t="s">
+      <c r="B1" s="39" t="s">
+        <v>164</v>
+      </c>
+      <c r="C1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="D1" s="36"/>
-      <c r="E1" s="36"/>
-      <c r="F1" s="38" t="s">
-        <v>225</v>
-      </c>
-      <c r="G1" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="H1" s="36"/>
-      <c r="I1" s="36" t="s">
+      <c r="D1" s="37"/>
+      <c r="E1" s="37"/>
+      <c r="F1" s="39" t="s">
+        <v>219</v>
+      </c>
+      <c r="G1" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="H1" s="37"/>
+      <c r="I1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="J1" s="1"/>
@@ -8362,8 +8432,8 @@
       <c r="AD1" s="1"/>
     </row>
     <row r="2" spans="1:30" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="36"/>
-      <c r="B2" s="38"/>
+      <c r="A2" s="37"/>
+      <c r="B2" s="39"/>
       <c r="C2" s="12" t="s">
         <v>3</v>
       </c>
@@ -8373,14 +8443,14 @@
       <c r="E2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="F2" s="38"/>
+      <c r="F2" s="39"/>
       <c r="G2" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="I2" s="36"/>
+        <v>177</v>
+      </c>
+      <c r="I2" s="37"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
       <c r="L2" s="1"/>
@@ -8405,7 +8475,7 @@
     </row>
     <row r="3" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>264</v>
+        <v>258</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -8418,7 +8488,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>268</v>
+        <v>262</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="27" t="s">
@@ -8450,7 +8520,7 @@
     </row>
     <row r="6" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -8463,10 +8533,10 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>269</v>
+        <v>263</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>6</v>
@@ -8486,10 +8556,10 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
+        <v>41</v>
+      </c>
+      <c r="B8" s="26" t="s">
         <v>42</v>
-      </c>
-      <c r="B8" s="26" t="s">
-        <v>43</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>6</v>
@@ -8509,10 +8579,10 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
+        <v>43</v>
+      </c>
+      <c r="B9" s="26" t="s">
         <v>44</v>
-      </c>
-      <c r="B9" s="26" t="s">
-        <v>45</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>6</v>
@@ -8543,10 +8613,10 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>270</v>
+        <v>264</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>46</v>
+        <v>45</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>6</v>
@@ -8566,10 +8636,10 @@
     </row>
     <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
+        <v>61</v>
+      </c>
+      <c r="B12" s="26" t="s">
         <v>62</v>
-      </c>
-      <c r="B12" s="26" t="s">
-        <v>63</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>6</v>
@@ -8589,10 +8659,10 @@
     </row>
     <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
+        <v>63</v>
+      </c>
+      <c r="B13" s="26" t="s">
         <v>64</v>
-      </c>
-      <c r="B13" s="26" t="s">
-        <v>65</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>6</v>
@@ -8612,10 +8682,10 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
+        <v>46</v>
+      </c>
+      <c r="B14" s="26" t="s">
         <v>47</v>
-      </c>
-      <c r="B14" s="26" t="s">
-        <v>48</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>6</v>
@@ -8635,10 +8705,10 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
+        <v>48</v>
+      </c>
+      <c r="B15" s="26" t="s">
         <v>49</v>
-      </c>
-      <c r="B15" s="26" t="s">
-        <v>50</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>6</v>
@@ -8669,10 +8739,10 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
+        <v>50</v>
+      </c>
+      <c r="B17" s="26" t="s">
         <v>51</v>
-      </c>
-      <c r="B17" s="26" t="s">
-        <v>52</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>6</v>
@@ -8692,10 +8762,10 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
+        <v>52</v>
+      </c>
+      <c r="B18" s="26" t="s">
         <v>53</v>
-      </c>
-      <c r="B18" s="26" t="s">
-        <v>54</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>6</v>
@@ -8726,10 +8796,10 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
+        <v>55</v>
+      </c>
+      <c r="B20" s="26" t="s">
         <v>56</v>
-      </c>
-      <c r="B20" s="26" t="s">
-        <v>57</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>6</v>
@@ -8749,10 +8819,10 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>282</v>
+        <v>276</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>55</v>
+        <v>54</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>6</v>
@@ -8772,10 +8842,10 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>283</v>
+        <v>277</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>6</v>
@@ -8795,10 +8865,10 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>246</v>
+        <v>240</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>6</v>
@@ -8813,7 +8883,7 @@
         <v>6</v>
       </c>
       <c r="G23" s="20" t="s">
-        <v>267</v>
+        <v>261</v>
       </c>
       <c r="H23" s="21"/>
       <c r="I23" s="19"/>
@@ -8831,7 +8901,7 @@
     </row>
     <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>265</v>
+        <v>259</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -8844,10 +8914,10 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>271</v>
+        <v>265</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>59</v>
+        <v>58</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>6</v>
@@ -8867,10 +8937,10 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>272</v>
+        <v>266</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>6</v>
@@ -8890,10 +8960,10 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>273</v>
+        <v>267</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>61</v>
+        <v>60</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>6</v>
@@ -8924,7 +8994,7 @@
     </row>
     <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>266</v>
+        <v>260</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -8937,10 +9007,10 @@
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>274</v>
+        <v>268</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -8960,10 +9030,10 @@
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>67</v>
+        <v>66</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>66</v>
+        <v>65</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -8983,10 +9053,10 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>275</v>
+        <v>269</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>6</v>
@@ -9006,10 +9076,10 @@
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>69</v>
+        <v>68</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>68</v>
+        <v>67</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>6</v>
@@ -9029,10 +9099,10 @@
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>276</v>
+        <v>270</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>70</v>
+        <v>69</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>6</v>
@@ -9052,10 +9122,10 @@
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>277</v>
+        <v>271</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>71</v>
+        <v>70</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>6</v>
@@ -9086,7 +9156,7 @@
     </row>
     <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>263</v>
+        <v>257</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -9099,7 +9169,7 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>257</v>
+        <v>251</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="27" t="s">
@@ -9120,19 +9190,19 @@
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
+        <v>82</v>
+      </c>
+      <c r="B40" s="26" t="s">
         <v>83</v>
       </c>
-      <c r="B40" s="26" t="s">
-        <v>84</v>
-      </c>
       <c r="C40" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F40" s="27" t="s">
         <v>6</v>
@@ -9143,19 +9213,19 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
+        <v>84</v>
+      </c>
+      <c r="B41" s="26" t="s">
         <v>85</v>
       </c>
-      <c r="B41" s="26" t="s">
-        <v>86</v>
-      </c>
       <c r="C41" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>6</v>
@@ -9166,19 +9236,19 @@
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
+        <v>86</v>
+      </c>
+      <c r="B42" s="26" t="s">
         <v>87</v>
       </c>
-      <c r="B42" s="26" t="s">
-        <v>88</v>
-      </c>
       <c r="C42" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>6</v>
@@ -9189,19 +9259,19 @@
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
+        <v>88</v>
+      </c>
+      <c r="B43" s="26" t="s">
         <v>89</v>
       </c>
-      <c r="B43" s="26" t="s">
-        <v>90</v>
-      </c>
       <c r="C43" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>6</v>
@@ -9212,10 +9282,10 @@
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
+        <v>90</v>
+      </c>
+      <c r="B44" s="26" t="s">
         <v>91</v>
-      </c>
-      <c r="B44" s="26" t="s">
-        <v>92</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>6</v>
@@ -9233,10 +9303,10 @@
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B45" s="26" t="s">
         <v>93</v>
-      </c>
-      <c r="B45" s="26" t="s">
-        <v>94</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>6</v>
@@ -9254,10 +9324,10 @@
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
+        <v>94</v>
+      </c>
+      <c r="B46" s="26" t="s">
         <v>95</v>
-      </c>
-      <c r="B46" s="26" t="s">
-        <v>96</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>6</v>
@@ -9275,10 +9345,10 @@
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>97</v>
+        <v>96</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>6</v>
@@ -9307,7 +9377,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
-        <v>262</v>
+        <v>256</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="27"/>
@@ -9320,7 +9390,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>245</v>
+        <v>239</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="27" t="s">
@@ -9341,7 +9411,7 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>258</v>
+        <v>252</v>
       </c>
       <c r="B51" s="26"/>
       <c r="C51" s="27" t="s">
@@ -9362,7 +9432,7 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>259</v>
+        <v>253</v>
       </c>
       <c r="B52" s="18"/>
       <c r="C52" s="27" t="s">
@@ -9383,7 +9453,7 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>260</v>
+        <v>254</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="27" t="s">
@@ -9404,7 +9474,7 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>261</v>
+        <v>255</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="27" t="s">
@@ -9425,7 +9495,7 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>37</v>
+        <v>36</v>
       </c>
       <c r="B55" s="26"/>
       <c r="C55" s="27" t="s">
@@ -9446,7 +9516,7 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>38</v>
+        <v>37</v>
       </c>
       <c r="B56" s="26"/>
       <c r="C56" s="27" t="s">
@@ -9478,7 +9548,7 @@
     </row>
     <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
-        <v>281</v>
+        <v>275</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -9491,10 +9561,10 @@
     </row>
     <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>241</v>
+        <v>235</v>
       </c>
       <c r="B59" s="26" t="s">
-        <v>72</v>
+        <v>71</v>
       </c>
       <c r="C59" s="27" t="s">
         <v>6</v>
@@ -9509,19 +9579,19 @@
         <v>6</v>
       </c>
       <c r="G59" s="20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H59" s="19"/>
       <c r="I59" s="19" t="s">
-        <v>240</v>
+        <v>234</v>
       </c>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>242</v>
+        <v>236</v>
       </c>
       <c r="B60" s="26" t="s">
-        <v>73</v>
+        <v>72</v>
       </c>
       <c r="C60" s="27" t="s">
         <v>6</v>
@@ -9536,17 +9606,17 @@
         <v>6</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H60" s="19"/>
       <c r="I60" s="19"/>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>278</v>
+        <v>272</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>74</v>
+        <v>73</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>6</v>
@@ -9561,17 +9631,17 @@
         <v>6</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H61" s="19"/>
       <c r="I61" s="19"/>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>243</v>
+        <v>237</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>75</v>
+        <v>74</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>6</v>
@@ -9586,17 +9656,17 @@
         <v>6</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>244</v>
+        <v>238</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>76</v>
+        <v>75</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>6</v>
@@ -9611,17 +9681,17 @@
         <v>6</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>279</v>
+        <v>273</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>6</v>
@@ -9633,10 +9703,10 @@
         <v>6</v>
       </c>
       <c r="F64" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>237</v>
+        <v>231</v>
       </c>
       <c r="H64" s="21"/>
       <c r="I64" s="19"/>
@@ -9654,7 +9724,7 @@
     </row>
     <row r="66" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A66" s="24" t="s">
-        <v>78</v>
+        <v>77</v>
       </c>
       <c r="B66" s="25"/>
       <c r="C66" s="25"/>
@@ -9667,10 +9737,10 @@
     </row>
     <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
+        <v>78</v>
+      </c>
+      <c r="B67" s="26" t="s">
         <v>79</v>
-      </c>
-      <c r="B67" s="26" t="s">
-        <v>80</v>
       </c>
       <c r="C67" s="27" t="s">
         <v>6</v>
@@ -9688,19 +9758,19 @@
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
+        <v>80</v>
+      </c>
+      <c r="B68" s="26" t="s">
         <v>81</v>
       </c>
-      <c r="B68" s="26" t="s">
-        <v>82</v>
-      </c>
       <c r="C68" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E68" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>6</v>
@@ -9711,19 +9781,19 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
+        <v>97</v>
+      </c>
+      <c r="B69" s="26" t="s">
         <v>98</v>
       </c>
-      <c r="B69" s="26" t="s">
-        <v>99</v>
-      </c>
       <c r="C69" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F69" s="27" t="s">
         <v>6</v>
@@ -9745,7 +9815,7 @@
     </row>
     <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
@@ -9758,10 +9828,10 @@
     </row>
     <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
+        <v>32</v>
+      </c>
+      <c r="B72" s="26" t="s">
         <v>33</v>
-      </c>
-      <c r="B72" s="26" t="s">
-        <v>34</v>
       </c>
       <c r="C72" s="27" t="s">
         <v>6</v>
@@ -9781,7 +9851,7 @@
     </row>
     <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="B73" s="26">
         <v>98</v>
@@ -9804,7 +9874,7 @@
     </row>
     <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="B74" s="26">
         <v>99</v>
@@ -9838,7 +9908,7 @@
     </row>
     <row r="76" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A76" s="24" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="B76" s="25"/>
       <c r="C76" s="25"/>
@@ -9851,10 +9921,10 @@
     </row>
     <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A77" s="31" t="s">
-        <v>239</v>
+        <v>233</v>
       </c>
       <c r="B77" s="26" t="s">
-        <v>143</v>
+        <v>142</v>
       </c>
       <c r="C77" s="27" t="s">
         <v>6</v>
@@ -9874,10 +9944,10 @@
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="31" t="s">
+        <v>125</v>
+      </c>
+      <c r="B78" s="26" t="s">
         <v>126</v>
-      </c>
-      <c r="B78" s="26" t="s">
-        <v>127</v>
       </c>
       <c r="C78" s="27" t="s">
         <v>6</v>
@@ -9896,10 +9966,10 @@
     </row>
     <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
+        <v>127</v>
+      </c>
+      <c r="B79" s="26" t="s">
         <v>128</v>
-      </c>
-      <c r="B79" s="26" t="s">
-        <v>129</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>6</v>
@@ -9919,10 +9989,10 @@
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
+        <v>129</v>
+      </c>
+      <c r="B80" s="26" t="s">
         <v>130</v>
-      </c>
-      <c r="B80" s="26" t="s">
-        <v>131</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>6</v>
@@ -9942,10 +10012,10 @@
     </row>
     <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A81" s="31" t="s">
+        <v>131</v>
+      </c>
+      <c r="B81" s="26" t="s">
         <v>132</v>
-      </c>
-      <c r="B81" s="26" t="s">
-        <v>133</v>
       </c>
       <c r="C81" s="27" t="s">
         <v>6</v>
@@ -9965,10 +10035,10 @@
     </row>
     <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
+        <v>133</v>
+      </c>
+      <c r="B82" s="26" t="s">
         <v>134</v>
-      </c>
-      <c r="B82" s="26" t="s">
-        <v>135</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>6</v>
@@ -9988,10 +10058,10 @@
     </row>
     <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
+        <v>135</v>
+      </c>
+      <c r="B83" s="26" t="s">
         <v>136</v>
-      </c>
-      <c r="B83" s="26" t="s">
-        <v>137</v>
       </c>
       <c r="C83" s="27" t="s">
         <v>6</v>
@@ -10011,10 +10081,10 @@
     </row>
     <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A84" s="31" t="s">
+        <v>137</v>
+      </c>
+      <c r="B84" s="26" t="s">
         <v>138</v>
-      </c>
-      <c r="B84" s="26" t="s">
-        <v>139</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>6</v>
@@ -10034,10 +10104,10 @@
     </row>
     <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A85" s="20" t="s">
+        <v>139</v>
+      </c>
+      <c r="B85" s="26" t="s">
         <v>140</v>
-      </c>
-      <c r="B85" s="26" t="s">
-        <v>141</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>6</v>
@@ -10068,7 +10138,7 @@
     </row>
     <row r="87" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A87" s="24" t="s">
-        <v>142</v>
+        <v>141</v>
       </c>
       <c r="B87" s="25"/>
       <c r="C87" s="25"/>
@@ -10081,10 +10151,10 @@
     </row>
     <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A88" s="20" t="s">
-        <v>247</v>
+        <v>241</v>
       </c>
       <c r="B88" s="26" t="s">
-        <v>144</v>
+        <v>143</v>
       </c>
       <c r="C88" s="27" t="s">
         <v>6</v>
@@ -10099,17 +10169,17 @@
         <v>6</v>
       </c>
       <c r="G88" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H88" s="19"/>
       <c r="I88" s="19"/>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
-        <v>248</v>
+        <v>242</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>145</v>
+        <v>144</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>6</v>
@@ -10124,17 +10194,17 @@
         <v>6</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
-        <v>249</v>
+        <v>243</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>146</v>
+        <v>145</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>6</v>
@@ -10149,17 +10219,17 @@
         <v>6</v>
       </c>
       <c r="G90" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
-        <v>250</v>
+        <v>244</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>147</v>
+        <v>146</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>6</v>
@@ -10174,17 +10244,17 @@
         <v>6</v>
       </c>
       <c r="G91" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
-        <v>251</v>
+        <v>245</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>148</v>
+        <v>147</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>6</v>
@@ -10199,17 +10269,17 @@
         <v>6</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
-        <v>235</v>
+        <v>229</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>149</v>
+        <v>148</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>6</v>
@@ -10224,17 +10294,17 @@
         <v>6</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
-        <v>236</v>
+        <v>230</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>150</v>
+        <v>149</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>6</v>
@@ -10249,17 +10319,17 @@
         <v>6</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
-        <v>252</v>
+        <v>246</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>151</v>
+        <v>150</v>
       </c>
       <c r="C95" s="27" t="s">
         <v>6</v>
@@ -10274,17 +10344,17 @@
         <v>6</v>
       </c>
       <c r="G95" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>253</v>
+        <v>247</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>152</v>
+        <v>151</v>
       </c>
       <c r="C96" s="27" t="s">
         <v>6</v>
@@ -10299,17 +10369,17 @@
         <v>6</v>
       </c>
       <c r="G96" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
-        <v>254</v>
+        <v>248</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>153</v>
+        <v>152</v>
       </c>
       <c r="C97" s="27" t="s">
         <v>6</v>
@@ -10324,17 +10394,17 @@
         <v>6</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="31" t="s">
-        <v>255</v>
+        <v>249</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>154</v>
+        <v>153</v>
       </c>
       <c r="C98" s="27" t="s">
         <v>6</v>
@@ -10349,17 +10419,17 @@
         <v>6</v>
       </c>
       <c r="G98" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H98" s="19"/>
       <c r="I98" s="19"/>
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="20" t="s">
-        <v>256</v>
+        <v>250</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>155</v>
+        <v>154</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>6</v>
@@ -10374,7 +10444,7 @@
         <v>6</v>
       </c>
       <c r="G99" s="20" t="s">
-        <v>238</v>
+        <v>232</v>
       </c>
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
@@ -10388,7 +10458,7 @@
     </row>
     <row r="101" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A101" s="24" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="B101" s="25"/>
       <c r="C101" s="25"/>
@@ -10401,22 +10471,22 @@
     </row>
     <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A102" s="20" t="s">
+        <v>100</v>
+      </c>
+      <c r="B102" s="26" t="s">
         <v>101</v>
       </c>
-      <c r="B102" s="26" t="s">
-        <v>102</v>
-      </c>
       <c r="C102" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D102" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E102" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F102" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G102" s="20"/>
       <c r="H102" s="19"/>
@@ -10424,22 +10494,22 @@
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
+        <v>102</v>
+      </c>
+      <c r="B103" s="26" t="s">
         <v>103</v>
       </c>
-      <c r="B103" s="26" t="s">
-        <v>104</v>
-      </c>
       <c r="C103" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F103" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G103" s="20"/>
       <c r="H103" s="19"/>
@@ -10447,22 +10517,22 @@
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
+        <v>104</v>
+      </c>
+      <c r="B104" s="26" t="s">
         <v>105</v>
       </c>
-      <c r="B104" s="26" t="s">
-        <v>106</v>
-      </c>
       <c r="C104" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F104" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G104" s="20"/>
       <c r="H104" s="19"/>
@@ -10470,22 +10540,22 @@
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
+        <v>106</v>
+      </c>
+      <c r="B105" s="26" t="s">
         <v>107</v>
       </c>
-      <c r="B105" s="26" t="s">
-        <v>108</v>
-      </c>
       <c r="C105" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F105" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G105" s="20"/>
       <c r="H105" s="19"/>
@@ -10493,22 +10563,22 @@
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
+        <v>108</v>
+      </c>
+      <c r="B106" s="26" t="s">
         <v>109</v>
       </c>
-      <c r="B106" s="26" t="s">
-        <v>110</v>
-      </c>
       <c r="C106" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F106" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G106" s="20"/>
       <c r="H106" s="19"/>
@@ -10516,22 +10586,22 @@
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
+        <v>110</v>
+      </c>
+      <c r="B107" s="26" t="s">
         <v>111</v>
       </c>
-      <c r="B107" s="26" t="s">
-        <v>112</v>
-      </c>
       <c r="C107" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F107" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G107" s="20"/>
       <c r="H107" s="19"/>
@@ -10539,22 +10609,22 @@
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
+        <v>112</v>
+      </c>
+      <c r="B108" s="26" t="s">
         <v>113</v>
       </c>
-      <c r="B108" s="26" t="s">
-        <v>114</v>
-      </c>
       <c r="C108" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G108" s="20"/>
       <c r="H108" s="19"/>
@@ -10562,22 +10632,22 @@
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
+        <v>114</v>
+      </c>
+      <c r="B109" s="26" t="s">
         <v>115</v>
       </c>
-      <c r="B109" s="26" t="s">
-        <v>116</v>
-      </c>
       <c r="C109" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F109" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G109" s="20"/>
       <c r="H109" s="19"/>
@@ -10585,22 +10655,22 @@
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
+        <v>116</v>
+      </c>
+      <c r="B110" s="26" t="s">
         <v>117</v>
       </c>
-      <c r="B110" s="26" t="s">
-        <v>118</v>
-      </c>
       <c r="C110" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F110" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="G110" s="20"/>
       <c r="H110" s="19"/>
@@ -10608,19 +10678,19 @@
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
+        <v>118</v>
+      </c>
+      <c r="B111" s="26" t="s">
         <v>119</v>
       </c>
-      <c r="B111" s="26" t="s">
-        <v>120</v>
-      </c>
       <c r="C111" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D111" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F111" s="27" t="s">
         <v>6</v>
@@ -10631,19 +10701,19 @@
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
+        <v>120</v>
+      </c>
+      <c r="B112" s="26" t="s">
         <v>121</v>
       </c>
-      <c r="B112" s="26" t="s">
-        <v>122</v>
-      </c>
       <c r="C112" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D112" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F112" s="27" t="s">
         <v>6</v>
@@ -10654,19 +10724,19 @@
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
+        <v>122</v>
+      </c>
+      <c r="B113" s="26" t="s">
         <v>123</v>
       </c>
-      <c r="B113" s="26" t="s">
-        <v>124</v>
-      </c>
       <c r="C113" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D113" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="F113" s="27" t="s">
         <v>6</v>
@@ -17448,7 +17518,7 @@
   </sheetPr>
   <dimension ref="A1:AC974"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
@@ -17466,22 +17536,22 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:29" x14ac:dyDescent="0.2">
-      <c r="A1" s="36" t="s">
+      <c r="A1" s="37" t="s">
         <v>0</v>
       </c>
-      <c r="B1" s="36" t="s">
+      <c r="B1" s="37" t="s">
         <v>1</v>
       </c>
-      <c r="C1" s="36"/>
-      <c r="D1" s="36"/>
-      <c r="E1" s="38" t="s">
-        <v>226</v>
-      </c>
-      <c r="F1" s="36" t="s">
-        <v>168</v>
-      </c>
-      <c r="G1" s="36"/>
-      <c r="H1" s="36" t="s">
+      <c r="C1" s="37"/>
+      <c r="D1" s="37"/>
+      <c r="E1" s="39" t="s">
+        <v>220</v>
+      </c>
+      <c r="F1" s="37" t="s">
+        <v>167</v>
+      </c>
+      <c r="G1" s="37"/>
+      <c r="H1" s="37" t="s">
         <v>2</v>
       </c>
       <c r="I1" s="1"/>
@@ -17507,7 +17577,7 @@
       <c r="AC1" s="1"/>
     </row>
     <row r="2" spans="1:29" ht="31.5" x14ac:dyDescent="0.2">
-      <c r="A2" s="36"/>
+      <c r="A2" s="37"/>
       <c r="B2" s="12" t="s">
         <v>3</v>
       </c>
@@ -17517,14 +17587,14 @@
       <c r="D2" s="12" t="s">
         <v>5</v>
       </c>
-      <c r="E2" s="38"/>
+      <c r="E2" s="39"/>
       <c r="F2" s="13" t="s">
-        <v>180</v>
+        <v>179</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>178</v>
-      </c>
-      <c r="H2" s="36"/>
+        <v>177</v>
+      </c>
+      <c r="H2" s="37"/>
       <c r="I2" s="1"/>
       <c r="J2" s="1"/>
       <c r="K2" s="1"/>
@@ -17549,7 +17619,7 @@
     </row>
     <row r="3" spans="1:29" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>166</v>
+        <v>165</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -17582,7 +17652,7 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>156</v>
+        <v>155</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>6</v>
@@ -17593,7 +17663,7 @@
       <c r="D4" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E4" s="39" t="s">
+      <c r="E4" s="36" t="s">
         <v>6</v>
       </c>
       <c r="F4" s="20"/>
@@ -17602,7 +17672,7 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>157</v>
+        <v>156</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>6</v>
@@ -17613,7 +17683,7 @@
       <c r="D5" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E5" s="39" t="s">
+      <c r="E5" s="36" t="s">
         <v>6</v>
       </c>
       <c r="F5" s="20"/>
@@ -17622,7 +17692,7 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>158</v>
+        <v>157</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>6</v>
@@ -17633,7 +17703,7 @@
       <c r="D6" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E6" s="39" t="s">
+      <c r="E6" s="36" t="s">
         <v>6</v>
       </c>
       <c r="F6" s="21"/>
@@ -17642,18 +17712,18 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>159</v>
+        <v>158</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>222</v>
+        <v>216</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>222</v>
-      </c>
-      <c r="E7" s="39" t="s">
+        <v>216</v>
+      </c>
+      <c r="E7" s="36" t="s">
         <v>6</v>
       </c>
       <c r="F7" s="21"/>
@@ -17662,7 +17732,7 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>160</v>
+        <v>159</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>6</v>
@@ -17673,7 +17743,7 @@
       <c r="D8" s="18" t="s">
         <v>6</v>
       </c>
-      <c r="E8" s="39" t="s">
+      <c r="E8" s="36" t="s">
         <v>6</v>
       </c>
       <c r="F8" s="21"/>
@@ -17692,7 +17762,7 @@
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>167</v>
+        <v>166</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -17704,7 +17774,7 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>161</v>
+        <v>160</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -17718,7 +17788,7 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>162</v>
+        <v>161</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -17732,7 +17802,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>163</v>
+        <v>162</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -17746,7 +17816,7 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>164</v>
+        <v>163</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -17760,7 +17830,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>227</v>
+        <v>221</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>

</xml_diff>

<commit_message>
User manual consistency Improved interface to free_drive(...) from JoggingDialog Default positions have IsSystem specified Added clear_positions()
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{E29AA93E-8DB3-4C77-8141-61124E949CF9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D2788-939E-4B01-AE2C-99B904A2A056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48015" yWindow="1950" windowWidth="24810" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="48015" yWindow="1950" windowWidth="24810" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="902" uniqueCount="288">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="287">
   <si>
     <t>Statement</t>
   </si>
@@ -75,12 +75,6 @@
     <t>Device Management</t>
   </si>
   <si>
-    <t>le_send(device_name, message)</t>
-  </si>
-  <si>
-    <t>le_ask(device_name, message, timeout_ms)</t>
-  </si>
-  <si>
     <t>Flow Control</t>
   </si>
   <si>
@@ -207,15 +201,9 @@
     <t>1,22</t>
   </si>
   <si>
-    <t>movel_single_axis(int axis, double daxis) INCR???</t>
-  </si>
-  <si>
     <t>1,30</t>
   </si>
   <si>
-    <t>movel_rot_only(rx,ry,rz) INCR???</t>
-  </si>
-  <si>
     <t>1,31</t>
   </si>
   <si>
@@ -262,9 +250,6 @@
   </si>
   <si>
     <t>30,30</t>
-  </si>
-  <si>
-    <t>set_door_closed_input(int dig_out, int state, …)</t>
   </si>
   <si>
     <t>30,10</t>
@@ -545,22 +530,7 @@
 PythonPrint2.js</t>
   </si>
   <si>
-    <t>le_clear_variables()</t>
-  </si>
-  <si>
-    <t>le_system_variable(var_name, True|False)</t>
-  </si>
-  <si>
-    <t>le_clear_variables</t>
-  </si>
-  <si>
-    <t>le_import_variables</t>
-  </si>
-  <si>
     <t>Also Uses</t>
-  </si>
-  <si>
-    <t>import_test_data.txt</t>
   </si>
   <si>
     <t>Tested by
@@ -573,9 +543,6 @@
     <t>variables</t>
   </si>
   <si>
-    <t>le_show_console(bool show?)</t>
-  </si>
-  <si>
     <t>le_log_info(string message)</t>
   </si>
   <si>
@@ -600,15 +567,9 @@
     <t>random</t>
   </si>
   <si>
-    <t>sleep(double seconds)</t>
-  </si>
-  <si>
     <t>infile_open(string filename)</t>
   </si>
   <si>
-    <t>infile_scale(pairs)</t>
-  </si>
-  <si>
     <t>jump</t>
   </si>
   <si>
@@ -618,12 +579,6 @@
     <t>sleep</t>
   </si>
   <si>
-    <t>le_connect(device_name)</t>
-  </si>
-  <si>
-    <t>le_disconnect(device_name)</t>
-  </si>
-  <si>
     <t>le_connect_all()</t>
   </si>
   <si>
@@ -652,9 +607,6 @@
   </si>
   <si>
     <t>exec_java(string filename)</t>
-  </si>
-  <si>
-    <t>le_import_variables(string filename)</t>
   </si>
   <si>
     <t>execline_java(string line)</t>
@@ -700,12 +652,6 @@
     <t>assertFalse(bool condition)</t>
   </si>
   <si>
-    <t>assertEqual(var_name, value)</t>
-  </si>
-  <si>
-    <t>assertNotEqual(var_name, value)</t>
-  </si>
-  <si>
     <t>execline_lescript</t>
   </si>
   <si>
@@ -746,12 +692,6 @@
     <t>set_joint_accel(int accel_dpss)</t>
   </si>
   <si>
-    <t>set_part_geometry(string FLAT|CYLINDER|SPHERE, double diam_mm)</t>
-  </si>
-  <si>
-    <t xml:space="preserve">free_drive(int 0=OFF|1=ON) </t>
-  </si>
-  <si>
     <t>grind_touch_retract(int touch_retract_mm)</t>
   </si>
   <si>
@@ -785,18 +725,6 @@
     <t>select_tool(string tool_name)</t>
   </si>
   <si>
-    <t>save_position(string pos_name)</t>
-  </si>
-  <si>
-    <t>system_position(string pos_name, boolean True|False)</t>
-  </si>
-  <si>
-    <t>move_joint(string pos_name)</t>
-  </si>
-  <si>
-    <t>move_linear(strig pos_name)</t>
-  </si>
-  <si>
     <t>Position System</t>
   </si>
   <si>
@@ -812,9 +740,6 @@
     <t>Move Relative</t>
   </si>
   <si>
-    <t>THIS IS MORE COMPLEX</t>
-  </si>
-  <si>
     <t>string ur_dashboard(string message, int timeout_ms)</t>
   </si>
   <si>
@@ -890,7 +815,79 @@
     <t>prompt(string message)</t>
   </si>
   <si>
-    <t>HOW HANDLE NO ARG JAVA./PO vs. LES</t>
+    <t>le_show_console(bool show)</t>
+  </si>
+  <si>
+    <t>sleep(float seconds)</t>
+  </si>
+  <si>
+    <t>assertEqual(string var_name, string value)</t>
+  </si>
+  <si>
+    <t>assertNotEqual(string var_name, string value)</t>
+  </si>
+  <si>
+    <t>le_connect(string device_name)</t>
+  </si>
+  <si>
+    <t>le_disconnect(string device_name)</t>
+  </si>
+  <si>
+    <t>le_send(string device_name, string message)</t>
+  </si>
+  <si>
+    <t>le_ask(string device_name, string message, int timeout_ms)</t>
+  </si>
+  <si>
+    <t>infile_scale(int column, float scale, ...)</t>
+  </si>
+  <si>
+    <t>movel_single_axis(int axis, float daxis)</t>
+  </si>
+  <si>
+    <t>movel_rot_only(float rx, ry, rz)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">free_drive(bool is_on, int 0=base|1=tcp|2=part, bool axis1, axis2, … axis 6) </t>
+  </si>
+  <si>
+    <t>set_part_geometry(string FLAT|CYLINDER|SPHERE, float diam_mm)</t>
+  </si>
+  <si>
+    <t>save_position(string position_name)</t>
+  </si>
+  <si>
+    <t>system_position(string position_name, boolean True|False)</t>
+  </si>
+  <si>
+    <t>move_joint(string position_name)</t>
+  </si>
+  <si>
+    <t>move_linear(strig position_name)</t>
+  </si>
+  <si>
+    <t>clear_positions()</t>
+  </si>
+  <si>
+    <t>clear_variables()</t>
+  </si>
+  <si>
+    <t>import_variables(string filename)</t>
+  </si>
+  <si>
+    <t>system_variable(string var_name, bool is_system)</t>
+  </si>
+  <si>
+    <t>clear_variables</t>
+  </si>
+  <si>
+    <t>import_variables</t>
+  </si>
+  <si>
+    <t>set_door_closed_input(int dig_in, int state)</t>
+  </si>
+  <si>
+    <t>Testing/import_test_data.txt</t>
   </si>
 </sst>
 </file>
@@ -1333,20 +1330,20 @@
   </sheetPr>
   <dimension ref="A1:AC1009"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A21" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G39" sqref="G39"/>
+    <sheetView workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="66.42578125" customWidth="1"/>
+    <col min="1" max="1" width="76.28515625" customWidth="1"/>
     <col min="2" max="2" width="10.85546875" style="11" customWidth="1"/>
     <col min="3" max="3" width="8.5703125" style="11" customWidth="1"/>
     <col min="4" max="4" width="9.85546875" style="11" customWidth="1"/>
     <col min="5" max="5" width="13.42578125" style="35" customWidth="1"/>
     <col min="6" max="6" width="27.85546875" customWidth="1"/>
-    <col min="7" max="7" width="27.28515625" customWidth="1"/>
+    <col min="7" max="7" width="38.28515625" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="44.85546875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -1360,10 +1357,10 @@
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
       <c r="E1" s="39" t="s">
-        <v>218</v>
+        <v>202</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G1" s="37"/>
       <c r="H1" s="37" t="s">
@@ -1383,10 +1380,10 @@
       </c>
       <c r="E2" s="39"/>
       <c r="F2" s="13" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H2" s="37"/>
     </row>
@@ -1419,7 +1416,7 @@
         <v>6</v>
       </c>
       <c r="F4" s="20" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G4" s="20"/>
       <c r="H4" s="19"/>
@@ -1441,7 +1438,7 @@
         <v>6</v>
       </c>
       <c r="F5" s="20" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G5" s="20"/>
       <c r="H5" s="19"/>
@@ -1463,14 +1460,14 @@
         <v>6</v>
       </c>
       <c r="F6" s="20" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G6" s="20"/>
       <c r="H6" s="19"/>
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>207</v>
+        <v>192</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>6</v>
@@ -1485,14 +1482,14 @@
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>168</v>
+        <v>163</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
     </row>
     <row r="8" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>205</v>
+        <v>190</v>
       </c>
       <c r="B8" s="27" t="s">
         <v>6</v>
@@ -1507,16 +1504,16 @@
         <v>6</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>217</v>
+        <v>201</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>215</v>
+        <v>199</v>
       </c>
       <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>208</v>
+        <v>193</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>6</v>
@@ -1531,16 +1528,16 @@
         <v>6</v>
       </c>
       <c r="F9" s="28" t="s">
-        <v>170</v>
+        <v>165</v>
       </c>
       <c r="G9" s="29" t="s">
-        <v>169</v>
+        <v>164</v>
       </c>
       <c r="H9" s="28"/>
     </row>
     <row r="10" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A10" s="20" t="s">
-        <v>206</v>
+        <v>191</v>
       </c>
       <c r="B10" s="27" t="s">
         <v>6</v>
@@ -1555,16 +1552,16 @@
         <v>6</v>
       </c>
       <c r="F10" s="28" t="s">
-        <v>171</v>
+        <v>166</v>
       </c>
       <c r="G10" s="29" t="s">
-        <v>172</v>
+        <v>167</v>
       </c>
       <c r="H10" s="28"/>
     </row>
     <row r="11" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>204</v>
+        <v>189</v>
       </c>
       <c r="B11" s="27" t="s">
         <v>6</v>
@@ -1579,14 +1576,14 @@
         <v>6</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>226</v>
+        <v>208</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>210</v>
+        <v>194</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>6</v>
@@ -1601,14 +1598,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>227</v>
+        <v>209</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>211</v>
+        <v>195</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>6</v>
@@ -1623,7 +1620,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>228</v>
+        <v>210</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="28"/>
@@ -1652,7 +1649,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>173</v>
+        <v>280</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>6</v>
@@ -1663,14 +1660,14 @@
         <v>6</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>175</v>
+        <v>283</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>209</v>
+        <v>281</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>6</v>
@@ -1681,16 +1678,16 @@
         <v>6</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>176</v>
+        <v>284</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>178</v>
+        <v>286</v>
       </c>
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>174</v>
+        <v>282</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>6</v>
@@ -1701,7 +1698,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>175</v>
+        <v>283</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
@@ -1723,7 +1720,7 @@
         <v>6</v>
       </c>
       <c r="F19" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G19" s="19"/>
       <c r="H19" s="19"/>
@@ -1745,7 +1742,7 @@
         <v>6</v>
       </c>
       <c r="F20" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G20" s="19"/>
       <c r="H20" s="19"/>
@@ -1767,7 +1764,7 @@
         <v>6</v>
       </c>
       <c r="F21" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G21" s="19"/>
       <c r="H21" s="19"/>
@@ -1789,14 +1786,14 @@
         <v>6</v>
       </c>
       <c r="F22" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G22" s="19"/>
       <c r="H22" s="19"/>
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>274</v>
+        <v>249</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>6</v>
@@ -1807,14 +1804,14 @@
         <v>6</v>
       </c>
       <c r="F23" s="28" t="s">
-        <v>190</v>
+        <v>179</v>
       </c>
       <c r="G23" s="19"/>
       <c r="H23" s="19"/>
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>212</v>
+        <v>196</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27" t="s">
@@ -1827,14 +1824,14 @@
         <v>6</v>
       </c>
       <c r="F24" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G24" s="19"/>
       <c r="H24" s="19"/>
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>213</v>
+        <v>197</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27" t="s">
@@ -1847,14 +1844,14 @@
         <v>6</v>
       </c>
       <c r="F25" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G25" s="19"/>
       <c r="H25" s="19"/>
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>214</v>
+        <v>198</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27" t="s">
@@ -1867,7 +1864,7 @@
         <v>6</v>
       </c>
       <c r="F26" s="28" t="s">
-        <v>181</v>
+        <v>171</v>
       </c>
       <c r="G26" s="19"/>
       <c r="H26" s="19"/>
@@ -1884,7 +1881,7 @@
     </row>
     <row r="28" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A28" s="24" t="s">
-        <v>189</v>
+        <v>178</v>
       </c>
       <c r="B28" s="25"/>
       <c r="C28" s="25"/>
@@ -1896,7 +1893,7 @@
     </row>
     <row r="29" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A29" s="20" t="s">
-        <v>184</v>
+        <v>173</v>
       </c>
       <c r="B29" s="27" t="s">
         <v>6</v>
@@ -1911,14 +1908,14 @@
         <v>6</v>
       </c>
       <c r="F29" s="20" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G29" s="19"/>
       <c r="H29" s="19"/>
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>182</v>
+        <v>262</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>6</v>
@@ -1933,7 +1930,7 @@
         <v>6</v>
       </c>
       <c r="F30" s="20" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G30" s="19"/>
       <c r="H30" s="19"/>
@@ -1955,7 +1952,7 @@
         <v>6</v>
       </c>
       <c r="F31" s="20" t="s">
-        <v>186</v>
+        <v>175</v>
       </c>
       <c r="G31" s="19"/>
       <c r="H31" s="19"/>
@@ -1972,7 +1969,7 @@
     </row>
     <row r="33" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A33" s="24" t="s">
-        <v>188</v>
+        <v>177</v>
       </c>
       <c r="B33" s="25"/>
       <c r="C33" s="25"/>
@@ -1984,7 +1981,7 @@
     </row>
     <row r="34" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>183</v>
+        <v>172</v>
       </c>
       <c r="B34" s="27" t="s">
         <v>6</v>
@@ -1999,14 +1996,14 @@
         <v>6</v>
       </c>
       <c r="F34" s="20" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G34" s="19"/>
       <c r="H34" s="19"/>
     </row>
     <row r="35" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>185</v>
+        <v>174</v>
       </c>
       <c r="B35" s="27" t="s">
         <v>6</v>
@@ -2021,7 +2018,7 @@
         <v>6</v>
       </c>
       <c r="F35" s="28" t="s">
-        <v>187</v>
+        <v>176</v>
       </c>
       <c r="G35" s="19"/>
       <c r="H35" s="19"/>
@@ -2038,7 +2035,7 @@
     </row>
     <row r="37" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A37" s="24" t="s">
-        <v>19</v>
+        <v>17</v>
       </c>
       <c r="B37" s="25"/>
       <c r="C37" s="25"/>
@@ -2050,7 +2047,7 @@
     </row>
     <row r="38" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>278</v>
+        <v>253</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>6</v>
@@ -2065,14 +2062,14 @@
         <v>6</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>280</v>
+        <v>255</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>283</v>
+        <v>258</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>6</v>
@@ -2083,16 +2080,18 @@
       <c r="D39" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E39" s="27"/>
-      <c r="F39" s="20"/>
+      <c r="E39" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F39" s="20" t="s">
+        <v>255</v>
+      </c>
       <c r="G39" s="19"/>
-      <c r="H39" s="19" t="s">
-        <v>287</v>
-      </c>
+      <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>279</v>
+        <v>254</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>6</v>
@@ -2107,14 +2106,14 @@
         <v>6</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>281</v>
+        <v>256</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>284</v>
+        <v>259</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>6</v>
@@ -2125,16 +2124,18 @@
       <c r="D41" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E41" s="27"/>
-      <c r="F41" s="20"/>
+      <c r="E41" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F41" s="20" t="s">
+        <v>256</v>
+      </c>
       <c r="G41" s="19"/>
-      <c r="H41" s="19" t="s">
-        <v>287</v>
-      </c>
+      <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>286</v>
+        <v>261</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>6</v>
@@ -2149,14 +2150,14 @@
         <v>6</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>282</v>
+        <v>257</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
     </row>
     <row r="43" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>285</v>
+        <v>260</v>
       </c>
       <c r="B43" s="27" t="s">
         <v>6</v>
@@ -2167,14 +2168,18 @@
       <c r="D43" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="E43" s="27"/>
-      <c r="F43" s="20"/>
+      <c r="E43" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F43" s="20" t="s">
+        <v>257</v>
+      </c>
       <c r="G43" s="19"/>
       <c r="H43" s="19"/>
     </row>
     <row r="44" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="B44" s="27" t="s">
         <v>6</v>
@@ -2189,14 +2194,14 @@
         <v>6</v>
       </c>
       <c r="F44" s="20" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="G44" s="19"/>
       <c r="H44" s="19"/>
     </row>
     <row r="45" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="B45" s="27" t="s">
         <v>6</v>
@@ -2211,14 +2216,14 @@
         <v>6</v>
       </c>
       <c r="F45" s="20" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="G45" s="19"/>
       <c r="H45" s="19"/>
     </row>
     <row r="46" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>22</v>
+        <v>20</v>
       </c>
       <c r="B46" s="33" t="s">
         <v>6</v>
@@ -2233,7 +2238,7 @@
         <v>6</v>
       </c>
       <c r="F46" s="20" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="G46" s="30"/>
       <c r="H46" s="30"/>
@@ -2261,7 +2266,7 @@
     </row>
     <row r="47" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>23</v>
+        <v>21</v>
       </c>
       <c r="B47" s="27" t="s">
         <v>6</v>
@@ -2272,14 +2277,14 @@
         <v>6</v>
       </c>
       <c r="F47" s="20" t="s">
-        <v>194</v>
+        <v>181</v>
       </c>
       <c r="G47" s="19"/>
       <c r="H47" s="19"/>
     </row>
     <row r="48" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A48" s="20" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="B48" s="27" t="s">
         <v>6</v>
@@ -2294,14 +2299,14 @@
         <v>6</v>
       </c>
       <c r="F48" s="20" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="G48" s="19"/>
       <c r="H48" s="19"/>
     </row>
     <row r="49" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A49" s="20" t="s">
-        <v>25</v>
+        <v>23</v>
       </c>
       <c r="B49" s="27" t="s">
         <v>6</v>
@@ -2316,14 +2321,14 @@
         <v>6</v>
       </c>
       <c r="F49" s="20" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="G49" s="19"/>
       <c r="H49" s="19"/>
     </row>
     <row r="50" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>26</v>
+        <v>24</v>
       </c>
       <c r="B50" s="27" t="s">
         <v>6</v>
@@ -2338,14 +2343,14 @@
         <v>6</v>
       </c>
       <c r="F50" s="20" t="s">
-        <v>195</v>
+        <v>182</v>
       </c>
       <c r="G50" s="19"/>
       <c r="H50" s="19"/>
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>191</v>
+        <v>263</v>
       </c>
       <c r="B51" s="27" t="s">
         <v>6</v>
@@ -2360,14 +2365,14 @@
         <v>6</v>
       </c>
       <c r="F51" s="20" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="G51" s="19"/>
       <c r="H51" s="19"/>
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>224</v>
+        <v>264</v>
       </c>
       <c r="B52" s="27" t="s">
         <v>6</v>
@@ -2378,14 +2383,14 @@
         <v>6</v>
       </c>
       <c r="F52" s="20" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G52" s="19"/>
       <c r="H52" s="19"/>
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>225</v>
+        <v>265</v>
       </c>
       <c r="B53" s="27" t="s">
         <v>6</v>
@@ -2396,14 +2401,14 @@
         <v>6</v>
       </c>
       <c r="F53" s="20" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G53" s="19"/>
       <c r="H53" s="19"/>
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>222</v>
+        <v>206</v>
       </c>
       <c r="B54" s="27"/>
       <c r="C54" s="27" t="s">
@@ -2416,14 +2421,14 @@
         <v>6</v>
       </c>
       <c r="F54" s="20" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G54" s="19"/>
       <c r="H54" s="19"/>
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>223</v>
+        <v>207</v>
       </c>
       <c r="B55" s="27"/>
       <c r="C55" s="27" t="s">
@@ -2436,7 +2441,7 @@
         <v>6</v>
       </c>
       <c r="F55" s="20" t="s">
-        <v>180</v>
+        <v>170</v>
       </c>
       <c r="G55" s="19"/>
       <c r="H55" s="19"/>
@@ -2465,7 +2470,7 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>197</v>
+        <v>266</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>6</v>
@@ -2480,14 +2485,14 @@
         <v>6</v>
       </c>
       <c r="F58" s="28" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G58" s="19"/>
       <c r="H58" s="28"/>
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>198</v>
+        <v>267</v>
       </c>
       <c r="B59" s="27" t="s">
         <v>6</v>
@@ -2502,14 +2507,14 @@
         <v>6</v>
       </c>
       <c r="F59" s="28" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G59" s="19"/>
       <c r="H59" s="28"/>
     </row>
     <row r="60" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>199</v>
+        <v>184</v>
       </c>
       <c r="B60" s="27" t="s">
         <v>6</v>
@@ -2524,14 +2529,14 @@
         <v>6</v>
       </c>
       <c r="F60" s="28" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G60" s="19"/>
       <c r="H60" s="28"/>
     </row>
     <row r="61" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>200</v>
+        <v>185</v>
       </c>
       <c r="B61" s="27" t="s">
         <v>6</v>
@@ -2546,14 +2551,14 @@
         <v>6</v>
       </c>
       <c r="F61" s="28" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G61" s="19"/>
       <c r="H61" s="28"/>
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>17</v>
+        <v>268</v>
       </c>
       <c r="B62" s="27" t="s">
         <v>6</v>
@@ -2568,14 +2573,14 @@
         <v>6</v>
       </c>
       <c r="F62" s="28" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G62" s="19"/>
       <c r="H62" s="28"/>
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>18</v>
+        <v>269</v>
       </c>
       <c r="B63" s="27" t="s">
         <v>6</v>
@@ -2590,7 +2595,7 @@
         <v>6</v>
       </c>
       <c r="F63" s="28" t="s">
-        <v>202</v>
+        <v>187</v>
       </c>
       <c r="G63" s="19"/>
       <c r="H63" s="28"/>
@@ -2607,7 +2612,7 @@
     </row>
     <row r="65" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A65" s="24" t="s">
-        <v>27</v>
+        <v>25</v>
       </c>
       <c r="B65" s="25"/>
       <c r="C65" s="25"/>
@@ -2619,7 +2624,7 @@
     </row>
     <row r="66" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A66" s="20" t="s">
-        <v>192</v>
+        <v>180</v>
       </c>
       <c r="B66" s="27" t="s">
         <v>6</v>
@@ -2630,14 +2635,14 @@
         <v>6</v>
       </c>
       <c r="F66" s="20" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G66" s="19"/>
       <c r="H66" s="19"/>
     </row>
     <row r="67" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A67" s="20" t="s">
-        <v>28</v>
+        <v>26</v>
       </c>
       <c r="B67" s="27" t="s">
         <v>6</v>
@@ -2648,14 +2653,14 @@
         <v>6</v>
       </c>
       <c r="F67" s="20" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G67" s="19"/>
       <c r="H67" s="19"/>
     </row>
     <row r="68" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>29</v>
+        <v>27</v>
       </c>
       <c r="B68" s="27" t="s">
         <v>6</v>
@@ -2666,14 +2671,14 @@
         <v>6</v>
       </c>
       <c r="F68" s="20" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G68" s="19"/>
       <c r="H68" s="19"/>
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>193</v>
+        <v>270</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>6</v>
@@ -2684,7 +2689,7 @@
         <v>6</v>
       </c>
       <c r="F69" s="20" t="s">
-        <v>201</v>
+        <v>186</v>
       </c>
       <c r="G69" s="19"/>
       <c r="H69" s="19"/>
@@ -2701,7 +2706,7 @@
     </row>
     <row r="71" spans="1:8" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A71" s="24" t="s">
-        <v>30</v>
+        <v>28</v>
       </c>
       <c r="B71" s="25"/>
       <c r="C71" s="25"/>
@@ -2713,7 +2718,7 @@
     </row>
     <row r="72" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A72" s="20" t="s">
-        <v>203</v>
+        <v>188</v>
       </c>
       <c r="B72" s="27" t="s">
         <v>6</v>
@@ -2721,7 +2726,7 @@
       <c r="C72" s="27"/>
       <c r="D72" s="27"/>
       <c r="E72" s="32" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
@@ -8367,16 +8372,16 @@
   <sheetPr>
     <outlinePr summaryBelow="0" summaryRight="0"/>
   </sheetPr>
-  <dimension ref="A1:AD1077"/>
+  <dimension ref="A1:AD1078"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <pane ySplit="2" topLeftCell="A96" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="F113" sqref="F113"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
+      <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="1" max="1" width="95.42578125" style="9" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="102.140625" style="9" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="14.28515625" customWidth="1"/>
     <col min="3" max="3" width="10.85546875" customWidth="1"/>
     <col min="4" max="4" width="8.5703125" customWidth="1"/>
@@ -8392,7 +8397,7 @@
         <v>0</v>
       </c>
       <c r="B1" s="39" t="s">
-        <v>164</v>
+        <v>159</v>
       </c>
       <c r="C1" s="37" t="s">
         <v>1</v>
@@ -8400,10 +8405,10 @@
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="39" t="s">
-        <v>219</v>
+        <v>203</v>
       </c>
       <c r="G1" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="H1" s="37"/>
       <c r="I1" s="37" t="s">
@@ -8445,10 +8450,10 @@
       </c>
       <c r="F2" s="39"/>
       <c r="G2" s="13" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="H2" s="14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="I2" s="37"/>
       <c r="J2" s="1"/>
@@ -8475,7 +8480,7 @@
     </row>
     <row r="3" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>258</v>
+        <v>234</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -8488,7 +8493,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>262</v>
+        <v>237</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="27" t="s">
@@ -8520,7 +8525,7 @@
     </row>
     <row r="6" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A6" s="24" t="s">
-        <v>39</v>
+        <v>37</v>
       </c>
       <c r="B6" s="25"/>
       <c r="C6" s="25"/>
@@ -8533,10 +8538,10 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>263</v>
+        <v>238</v>
       </c>
       <c r="B7" s="26" t="s">
-        <v>40</v>
+        <v>38</v>
       </c>
       <c r="C7" s="27" t="s">
         <v>6</v>
@@ -8556,10 +8561,10 @@
     </row>
     <row r="8" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A8" s="20" t="s">
-        <v>41</v>
+        <v>39</v>
       </c>
       <c r="B8" s="26" t="s">
-        <v>42</v>
+        <v>40</v>
       </c>
       <c r="C8" s="27" t="s">
         <v>6</v>
@@ -8579,10 +8584,10 @@
     </row>
     <row r="9" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>43</v>
+        <v>41</v>
       </c>
       <c r="B9" s="26" t="s">
-        <v>44</v>
+        <v>42</v>
       </c>
       <c r="C9" s="27" t="s">
         <v>6</v>
@@ -8613,10 +8618,10 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>264</v>
+        <v>239</v>
       </c>
       <c r="B11" s="26" t="s">
-        <v>45</v>
+        <v>43</v>
       </c>
       <c r="C11" s="27" t="s">
         <v>6</v>
@@ -8636,10 +8641,10 @@
     </row>
     <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>61</v>
+        <v>271</v>
       </c>
       <c r="B12" s="26" t="s">
-        <v>62</v>
+        <v>59</v>
       </c>
       <c r="C12" s="27" t="s">
         <v>6</v>
@@ -8659,10 +8664,10 @@
     </row>
     <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>63</v>
+        <v>272</v>
       </c>
       <c r="B13" s="26" t="s">
-        <v>64</v>
+        <v>60</v>
       </c>
       <c r="C13" s="27" t="s">
         <v>6</v>
@@ -8682,10 +8687,10 @@
     </row>
     <row r="14" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A14" s="20" t="s">
-        <v>46</v>
+        <v>44</v>
       </c>
       <c r="B14" s="26" t="s">
-        <v>47</v>
+        <v>45</v>
       </c>
       <c r="C14" s="27" t="s">
         <v>6</v>
@@ -8705,10 +8710,10 @@
     </row>
     <row r="15" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A15" s="20" t="s">
-        <v>48</v>
+        <v>46</v>
       </c>
       <c r="B15" s="26" t="s">
-        <v>49</v>
+        <v>47</v>
       </c>
       <c r="C15" s="27" t="s">
         <v>6</v>
@@ -8739,10 +8744,10 @@
     </row>
     <row r="17" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>50</v>
+        <v>48</v>
       </c>
       <c r="B17" s="26" t="s">
-        <v>51</v>
+        <v>49</v>
       </c>
       <c r="C17" s="27" t="s">
         <v>6</v>
@@ -8762,10 +8767,10 @@
     </row>
     <row r="18" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>52</v>
+        <v>50</v>
       </c>
       <c r="B18" s="26" t="s">
-        <v>53</v>
+        <v>51</v>
       </c>
       <c r="C18" s="27" t="s">
         <v>6</v>
@@ -8796,10 +8801,10 @@
     </row>
     <row r="20" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A20" s="20" t="s">
-        <v>55</v>
+        <v>53</v>
       </c>
       <c r="B20" s="26" t="s">
-        <v>56</v>
+        <v>54</v>
       </c>
       <c r="C20" s="27" t="s">
         <v>6</v>
@@ -8819,10 +8824,10 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>276</v>
+        <v>251</v>
       </c>
       <c r="B21" s="26" t="s">
-        <v>54</v>
+        <v>52</v>
       </c>
       <c r="C21" s="27" t="s">
         <v>6</v>
@@ -8842,10 +8847,10 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>277</v>
+        <v>252</v>
       </c>
       <c r="B22" s="26" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C22" s="27" t="s">
         <v>6</v>
@@ -8865,10 +8870,10 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>240</v>
+        <v>273</v>
       </c>
       <c r="B23" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C23" s="27" t="s">
         <v>6</v>
@@ -8882,9 +8887,7 @@
       <c r="F23" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G23" s="20" t="s">
-        <v>261</v>
-      </c>
+      <c r="G23" s="20"/>
       <c r="H23" s="21"/>
       <c r="I23" s="19"/>
     </row>
@@ -8901,7 +8904,7 @@
     </row>
     <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>259</v>
+        <v>235</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -8914,10 +8917,10 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>265</v>
+        <v>240</v>
       </c>
       <c r="B26" s="26" t="s">
-        <v>58</v>
+        <v>56</v>
       </c>
       <c r="C26" s="27" t="s">
         <v>6</v>
@@ -8937,10 +8940,10 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>266</v>
+        <v>241</v>
       </c>
       <c r="B27" s="26" t="s">
-        <v>59</v>
+        <v>57</v>
       </c>
       <c r="C27" s="27" t="s">
         <v>6</v>
@@ -8960,10 +8963,10 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>267</v>
+        <v>242</v>
       </c>
       <c r="B28" s="26" t="s">
-        <v>60</v>
+        <v>58</v>
       </c>
       <c r="C28" s="27" t="s">
         <v>6</v>
@@ -8994,7 +8997,7 @@
     </row>
     <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>260</v>
+        <v>236</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -9007,10 +9010,10 @@
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>268</v>
+        <v>243</v>
       </c>
       <c r="B31" s="26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C31" s="27" t="s">
         <v>6</v>
@@ -9030,10 +9033,10 @@
     </row>
     <row r="32" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A32" s="20" t="s">
-        <v>66</v>
+        <v>62</v>
       </c>
       <c r="B32" s="26" t="s">
-        <v>65</v>
+        <v>61</v>
       </c>
       <c r="C32" s="27" t="s">
         <v>6</v>
@@ -9053,10 +9056,10 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>269</v>
+        <v>244</v>
       </c>
       <c r="B33" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C33" s="27" t="s">
         <v>6</v>
@@ -9076,10 +9079,10 @@
     </row>
     <row r="34" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A34" s="20" t="s">
-        <v>68</v>
+        <v>64</v>
       </c>
       <c r="B34" s="26" t="s">
-        <v>67</v>
+        <v>63</v>
       </c>
       <c r="C34" s="27" t="s">
         <v>6</v>
@@ -9099,10 +9102,10 @@
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>270</v>
+        <v>245</v>
       </c>
       <c r="B35" s="26" t="s">
-        <v>69</v>
+        <v>65</v>
       </c>
       <c r="C35" s="27" t="s">
         <v>6</v>
@@ -9122,10 +9125,10 @@
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>271</v>
+        <v>246</v>
       </c>
       <c r="B36" s="26" t="s">
-        <v>70</v>
+        <v>66</v>
       </c>
       <c r="C36" s="27" t="s">
         <v>6</v>
@@ -9156,7 +9159,7 @@
     </row>
     <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>257</v>
+        <v>233</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -9169,7 +9172,7 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>251</v>
+        <v>231</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="27" t="s">
@@ -9190,19 +9193,19 @@
     </row>
     <row r="40" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>82</v>
+        <v>77</v>
       </c>
       <c r="B40" s="26" t="s">
-        <v>83</v>
+        <v>78</v>
       </c>
       <c r="C40" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F40" s="27" t="s">
         <v>6</v>
@@ -9213,19 +9216,19 @@
     </row>
     <row r="41" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>84</v>
+        <v>79</v>
       </c>
       <c r="B41" s="26" t="s">
-        <v>85</v>
+        <v>80</v>
       </c>
       <c r="C41" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>6</v>
@@ -9236,19 +9239,19 @@
     </row>
     <row r="42" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>86</v>
+        <v>81</v>
       </c>
       <c r="B42" s="26" t="s">
-        <v>87</v>
+        <v>82</v>
       </c>
       <c r="C42" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>6</v>
@@ -9259,19 +9262,19 @@
     </row>
     <row r="43" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>88</v>
+        <v>83</v>
       </c>
       <c r="B43" s="26" t="s">
-        <v>89</v>
+        <v>84</v>
       </c>
       <c r="C43" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>6</v>
@@ -9282,10 +9285,10 @@
     </row>
     <row r="44" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A44" s="20" t="s">
-        <v>90</v>
+        <v>85</v>
       </c>
       <c r="B44" s="26" t="s">
-        <v>91</v>
+        <v>86</v>
       </c>
       <c r="C44" s="27" t="s">
         <v>6</v>
@@ -9303,10 +9306,10 @@
     </row>
     <row r="45" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A45" s="20" t="s">
-        <v>92</v>
+        <v>87</v>
       </c>
       <c r="B45" s="26" t="s">
-        <v>93</v>
+        <v>88</v>
       </c>
       <c r="C45" s="27" t="s">
         <v>6</v>
@@ -9324,10 +9327,10 @@
     </row>
     <row r="46" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A46" s="20" t="s">
-        <v>94</v>
+        <v>89</v>
       </c>
       <c r="B46" s="26" t="s">
-        <v>95</v>
+        <v>90</v>
       </c>
       <c r="C46" s="27" t="s">
         <v>6</v>
@@ -9345,10 +9348,10 @@
     </row>
     <row r="47" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A47" s="20" t="s">
-        <v>96</v>
+        <v>91</v>
       </c>
       <c r="B47" s="26" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C47" s="27" t="s">
         <v>6</v>
@@ -9377,7 +9380,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
-        <v>256</v>
+        <v>232</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="27"/>
@@ -9390,7 +9393,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>239</v>
+        <v>275</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="27" t="s">
@@ -9406,14 +9409,14 @@
         <v>6</v>
       </c>
       <c r="G50" s="20"/>
-      <c r="H50" s="21"/>
+      <c r="H50" s="19"/>
       <c r="I50" s="19"/>
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>252</v>
-      </c>
-      <c r="B51" s="26"/>
+        <v>276</v>
+      </c>
+      <c r="B51" s="18"/>
       <c r="C51" s="27" t="s">
         <v>6</v>
       </c>
@@ -9432,7 +9435,7 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>253</v>
+        <v>279</v>
       </c>
       <c r="B52" s="18"/>
       <c r="C52" s="27" t="s">
@@ -9453,7 +9456,7 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>254</v>
+        <v>277</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="27" t="s">
@@ -9474,7 +9477,7 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>255</v>
+        <v>278</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="27" t="s">
@@ -9495,7 +9498,7 @@
     </row>
     <row r="55" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>36</v>
+        <v>34</v>
       </c>
       <c r="B55" s="26"/>
       <c r="C55" s="27" t="s">
@@ -9516,7 +9519,7 @@
     </row>
     <row r="56" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A56" s="20" t="s">
-        <v>37</v>
+        <v>35</v>
       </c>
       <c r="B56" s="26"/>
       <c r="C56" s="27" t="s">
@@ -9548,7 +9551,7 @@
     </row>
     <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
-        <v>275</v>
+        <v>250</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -9559,13 +9562,11 @@
       <c r="H58" s="16"/>
       <c r="I58" s="16"/>
     </row>
-    <row r="59" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>235</v>
-      </c>
-      <c r="B59" s="26" t="s">
-        <v>71</v>
-      </c>
+        <v>274</v>
+      </c>
+      <c r="B59" s="26"/>
       <c r="C59" s="27" t="s">
         <v>6</v>
       </c>
@@ -9578,17 +9579,13 @@
       <c r="F59" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G59" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="H59" s="19"/>
-      <c r="I59" s="19" t="s">
-        <v>234</v>
-      </c>
+      <c r="G59" s="20"/>
+      <c r="H59" s="21"/>
+      <c r="I59" s="19"/>
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>236</v>
+        <v>248</v>
       </c>
       <c r="B60" s="26" t="s">
         <v>72</v>
@@ -9603,20 +9600,20 @@
         <v>6</v>
       </c>
       <c r="F60" s="27" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="H60" s="19"/>
+        <v>213</v>
+      </c>
+      <c r="H60" s="21"/>
       <c r="I60" s="19"/>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>272</v>
+        <v>217</v>
       </c>
       <c r="B61" s="26" t="s">
-        <v>73</v>
+        <v>67</v>
       </c>
       <c r="C61" s="27" t="s">
         <v>6</v>
@@ -9631,17 +9628,19 @@
         <v>6</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="H61" s="19"/>
-      <c r="I61" s="19"/>
+      <c r="I61" s="19" t="s">
+        <v>216</v>
+      </c>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>237</v>
+        <v>218</v>
       </c>
       <c r="B62" s="26" t="s">
-        <v>74</v>
+        <v>68</v>
       </c>
       <c r="C62" s="27" t="s">
         <v>6</v>
@@ -9656,17 +9655,17 @@
         <v>6</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>238</v>
+        <v>247</v>
       </c>
       <c r="B63" s="26" t="s">
-        <v>75</v>
+        <v>69</v>
       </c>
       <c r="C63" s="27" t="s">
         <v>6</v>
@@ -9681,17 +9680,17 @@
         <v>6</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>231</v>
+        <v>213</v>
       </c>
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>273</v>
+        <v>219</v>
       </c>
       <c r="B64" s="26" t="s">
-        <v>76</v>
+        <v>70</v>
       </c>
       <c r="C64" s="27" t="s">
         <v>6</v>
@@ -9703,74 +9702,78 @@
         <v>6</v>
       </c>
       <c r="F64" s="27" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>231</v>
-      </c>
-      <c r="H64" s="21"/>
+        <v>213</v>
+      </c>
+      <c r="H64" s="19"/>
       <c r="I64" s="19"/>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A65" s="20"/>
-      <c r="B65" s="26"/>
-      <c r="C65" s="27"/>
-      <c r="D65" s="27"/>
-      <c r="E65" s="27"/>
-      <c r="F65" s="27"/>
-      <c r="G65" s="20"/>
+      <c r="A65" s="20" t="s">
+        <v>220</v>
+      </c>
+      <c r="B65" s="26" t="s">
+        <v>71</v>
+      </c>
+      <c r="C65" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D65" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E65" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F65" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="20" t="s">
+        <v>213</v>
+      </c>
       <c r="H65" s="19"/>
       <c r="I65" s="19"/>
     </row>
-    <row r="66" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A66" s="24" t="s">
-        <v>77</v>
-      </c>
-      <c r="B66" s="25"/>
-      <c r="C66" s="25"/>
-      <c r="D66" s="25"/>
-      <c r="E66" s="25"/>
-      <c r="F66" s="25"/>
+    <row r="66" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A66" s="20"/>
+      <c r="B66" s="26"/>
+      <c r="C66" s="27"/>
+      <c r="D66" s="27"/>
+      <c r="E66" s="27"/>
+      <c r="F66" s="27"/>
       <c r="G66" s="20"/>
-      <c r="H66" s="16"/>
-      <c r="I66" s="16"/>
-    </row>
-    <row r="67" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A67" s="20" t="s">
-        <v>78</v>
-      </c>
-      <c r="B67" s="26" t="s">
-        <v>79</v>
-      </c>
-      <c r="C67" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D67" s="27"/>
-      <c r="E67" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F67" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="H66" s="19"/>
+      <c r="I66" s="19"/>
+    </row>
+    <row r="67" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A67" s="24" t="s">
+        <v>73</v>
+      </c>
+      <c r="B67" s="25"/>
+      <c r="C67" s="25"/>
+      <c r="D67" s="25"/>
+      <c r="E67" s="25"/>
+      <c r="F67" s="25"/>
       <c r="G67" s="20"/>
-      <c r="H67" s="19"/>
-      <c r="I67" s="19"/>
+      <c r="H67" s="16"/>
+      <c r="I67" s="16"/>
     </row>
     <row r="68" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A68" s="20" t="s">
-        <v>80</v>
+        <v>74</v>
       </c>
       <c r="B68" s="26" t="s">
-        <v>81</v>
+        <v>75</v>
       </c>
       <c r="C68" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D68" s="27" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="E68" s="27" t="s">
-        <v>216</v>
+        <v>6</v>
       </c>
       <c r="F68" s="27" t="s">
         <v>6</v>
@@ -9781,19 +9784,19 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>97</v>
+        <v>285</v>
       </c>
       <c r="B69" s="26" t="s">
-        <v>98</v>
+        <v>76</v>
       </c>
       <c r="C69" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F69" s="27" t="s">
         <v>6</v>
@@ -9803,58 +9806,58 @@
       <c r="I69" s="19"/>
     </row>
     <row r="70" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A70" s="20"/>
-      <c r="B70" s="26"/>
-      <c r="C70" s="27"/>
-      <c r="D70" s="27"/>
-      <c r="E70" s="27"/>
-      <c r="F70" s="27"/>
+      <c r="A70" s="20" t="s">
+        <v>92</v>
+      </c>
+      <c r="B70" s="26" t="s">
+        <v>93</v>
+      </c>
+      <c r="C70" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D70" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E70" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="F70" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G70" s="20"/>
       <c r="H70" s="19"/>
       <c r="I70" s="19"/>
     </row>
-    <row r="71" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A71" s="24" t="s">
-        <v>31</v>
-      </c>
-      <c r="B71" s="25"/>
-      <c r="C71" s="25"/>
-      <c r="D71" s="25"/>
-      <c r="E71" s="25"/>
-      <c r="F71" s="25"/>
+    <row r="71" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A71" s="20"/>
+      <c r="B71" s="26"/>
+      <c r="C71" s="27"/>
+      <c r="D71" s="27"/>
+      <c r="E71" s="27"/>
+      <c r="F71" s="27"/>
       <c r="G71" s="20"/>
-      <c r="H71" s="24"/>
-      <c r="I71" s="16"/>
-    </row>
-    <row r="72" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A72" s="20" t="s">
-        <v>32</v>
-      </c>
-      <c r="B72" s="26" t="s">
-        <v>33</v>
-      </c>
-      <c r="C72" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D72" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E72" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F72" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="H71" s="19"/>
+      <c r="I71" s="19"/>
+    </row>
+    <row r="72" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A72" s="24" t="s">
+        <v>29</v>
+      </c>
+      <c r="B72" s="25"/>
+      <c r="C72" s="25"/>
+      <c r="D72" s="25"/>
+      <c r="E72" s="25"/>
+      <c r="F72" s="25"/>
       <c r="G72" s="20"/>
-      <c r="H72" s="20"/>
-      <c r="I72" s="19"/>
+      <c r="H72" s="24"/>
+      <c r="I72" s="16"/>
     </row>
     <row r="73" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A73" s="20" t="s">
-        <v>34</v>
-      </c>
-      <c r="B73" s="26">
-        <v>98</v>
+        <v>30</v>
+      </c>
+      <c r="B73" s="26" t="s">
+        <v>31</v>
       </c>
       <c r="C73" s="27" t="s">
         <v>6</v>
@@ -9869,15 +9872,15 @@
         <v>6</v>
       </c>
       <c r="G73" s="20"/>
-      <c r="H73" s="29"/>
+      <c r="H73" s="20"/>
       <c r="I73" s="19"/>
     </row>
     <row r="74" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A74" s="20" t="s">
-        <v>35</v>
+        <v>32</v>
       </c>
       <c r="B74" s="26">
-        <v>99</v>
+        <v>98</v>
       </c>
       <c r="C74" s="27" t="s">
         <v>6</v>
@@ -9896,58 +9899,58 @@
       <c r="I74" s="19"/>
     </row>
     <row r="75" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
-      <c r="A75" s="20"/>
-      <c r="B75" s="26"/>
-      <c r="C75" s="27"/>
-      <c r="D75" s="27"/>
-      <c r="E75" s="27"/>
-      <c r="F75" s="27"/>
+      <c r="A75" s="20" t="s">
+        <v>33</v>
+      </c>
+      <c r="B75" s="26">
+        <v>99</v>
+      </c>
+      <c r="C75" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D75" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E75" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F75" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G75" s="20"/>
       <c r="H75" s="29"/>
       <c r="I75" s="19"/>
     </row>
-    <row r="76" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A76" s="24" t="s">
-        <v>124</v>
-      </c>
-      <c r="B76" s="25"/>
-      <c r="C76" s="25"/>
-      <c r="D76" s="25"/>
-      <c r="E76" s="25"/>
-      <c r="F76" s="25"/>
+    <row r="76" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
+      <c r="A76" s="20"/>
+      <c r="B76" s="26"/>
+      <c r="C76" s="27"/>
+      <c r="D76" s="27"/>
+      <c r="E76" s="27"/>
+      <c r="F76" s="27"/>
       <c r="G76" s="20"/>
-      <c r="H76" s="16"/>
-      <c r="I76" s="16"/>
-    </row>
-    <row r="77" spans="1:9" ht="30" x14ac:dyDescent="0.2">
-      <c r="A77" s="31" t="s">
-        <v>233</v>
-      </c>
-      <c r="B77" s="26" t="s">
-        <v>142</v>
-      </c>
-      <c r="C77" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D77" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E77" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F77" s="27" t="s">
-        <v>6</v>
-      </c>
+      <c r="H76" s="29"/>
+      <c r="I76" s="19"/>
+    </row>
+    <row r="77" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A77" s="24" t="s">
+        <v>119</v>
+      </c>
+      <c r="B77" s="25"/>
+      <c r="C77" s="25"/>
+      <c r="D77" s="25"/>
+      <c r="E77" s="25"/>
+      <c r="F77" s="25"/>
       <c r="G77" s="20"/>
-      <c r="H77" s="19"/>
-      <c r="I77" s="19"/>
+      <c r="H77" s="16"/>
+      <c r="I77" s="16"/>
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="31" t="s">
-        <v>125</v>
+        <v>215</v>
       </c>
       <c r="B78" s="26" t="s">
-        <v>126</v>
+        <v>137</v>
       </c>
       <c r="C78" s="27" t="s">
         <v>6</v>
@@ -9961,15 +9964,16 @@
       <c r="F78" s="27" t="s">
         <v>6</v>
       </c>
+      <c r="G78" s="20"/>
       <c r="H78" s="19"/>
       <c r="I78" s="19"/>
     </row>
-    <row r="79" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="79" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A79" s="31" t="s">
-        <v>127</v>
+        <v>120</v>
       </c>
       <c r="B79" s="26" t="s">
-        <v>128</v>
+        <v>121</v>
       </c>
       <c r="C79" s="27" t="s">
         <v>6</v>
@@ -9983,16 +9987,15 @@
       <c r="F79" s="27" t="s">
         <v>6</v>
       </c>
-      <c r="G79" s="20"/>
       <c r="H79" s="19"/>
       <c r="I79" s="19"/>
     </row>
     <row r="80" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A80" s="31" t="s">
-        <v>129</v>
+        <v>122</v>
       </c>
       <c r="B80" s="26" t="s">
-        <v>130</v>
+        <v>123</v>
       </c>
       <c r="C80" s="27" t="s">
         <v>6</v>
@@ -10010,12 +10013,12 @@
       <c r="H80" s="19"/>
       <c r="I80" s="19"/>
     </row>
-    <row r="81" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="81" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A81" s="31" t="s">
-        <v>131</v>
+        <v>124</v>
       </c>
       <c r="B81" s="26" t="s">
-        <v>132</v>
+        <v>125</v>
       </c>
       <c r="C81" s="27" t="s">
         <v>6</v>
@@ -10035,10 +10038,10 @@
     </row>
     <row r="82" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A82" s="31" t="s">
-        <v>133</v>
+        <v>126</v>
       </c>
       <c r="B82" s="26" t="s">
-        <v>134</v>
+        <v>127</v>
       </c>
       <c r="C82" s="27" t="s">
         <v>6</v>
@@ -10058,10 +10061,10 @@
     </row>
     <row r="83" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A83" s="31" t="s">
-        <v>135</v>
+        <v>128</v>
       </c>
       <c r="B83" s="26" t="s">
-        <v>136</v>
+        <v>129</v>
       </c>
       <c r="C83" s="27" t="s">
         <v>6</v>
@@ -10079,12 +10082,12 @@
       <c r="H83" s="19"/>
       <c r="I83" s="19"/>
     </row>
-    <row r="84" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+    <row r="84" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A84" s="31" t="s">
-        <v>137</v>
+        <v>130</v>
       </c>
       <c r="B84" s="26" t="s">
-        <v>138</v>
+        <v>131</v>
       </c>
       <c r="C84" s="27" t="s">
         <v>6</v>
@@ -10102,12 +10105,12 @@
       <c r="H84" s="19"/>
       <c r="I84" s="19"/>
     </row>
-    <row r="85" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A85" s="20" t="s">
-        <v>139</v>
+    <row r="85" spans="1:9" ht="30" x14ac:dyDescent="0.2">
+      <c r="A85" s="31" t="s">
+        <v>132</v>
       </c>
       <c r="B85" s="26" t="s">
-        <v>140</v>
+        <v>133</v>
       </c>
       <c r="C85" s="27" t="s">
         <v>6</v>
@@ -10126,60 +10129,58 @@
       <c r="I85" s="19"/>
     </row>
     <row r="86" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A86" s="20"/>
-      <c r="B86" s="26"/>
-      <c r="C86" s="27"/>
-      <c r="D86" s="27"/>
-      <c r="E86" s="27"/>
-      <c r="F86" s="27"/>
+      <c r="A86" s="20" t="s">
+        <v>134</v>
+      </c>
+      <c r="B86" s="26" t="s">
+        <v>135</v>
+      </c>
+      <c r="C86" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D86" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E86" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F86" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G86" s="20"/>
       <c r="H86" s="19"/>
       <c r="I86" s="19"/>
     </row>
-    <row r="87" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A87" s="24" t="s">
-        <v>141</v>
-      </c>
-      <c r="B87" s="25"/>
-      <c r="C87" s="25"/>
-      <c r="D87" s="25"/>
-      <c r="E87" s="25"/>
-      <c r="F87" s="25"/>
+    <row r="87" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="A87" s="20"/>
+      <c r="B87" s="26"/>
+      <c r="C87" s="27"/>
+      <c r="D87" s="27"/>
+      <c r="E87" s="27"/>
+      <c r="F87" s="27"/>
       <c r="G87" s="20"/>
-      <c r="H87" s="16"/>
-      <c r="I87" s="16"/>
-    </row>
-    <row r="88" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A88" s="20" t="s">
-        <v>241</v>
-      </c>
-      <c r="B88" s="26" t="s">
-        <v>143</v>
-      </c>
-      <c r="C88" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D88" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="E88" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="F88" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="G88" s="20" t="s">
-        <v>232</v>
-      </c>
-      <c r="H88" s="19"/>
-      <c r="I88" s="19"/>
+      <c r="H87" s="19"/>
+      <c r="I87" s="19"/>
+    </row>
+    <row r="88" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A88" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="B88" s="25"/>
+      <c r="C88" s="25"/>
+      <c r="D88" s="25"/>
+      <c r="E88" s="25"/>
+      <c r="F88" s="25"/>
+      <c r="G88" s="20"/>
+      <c r="H88" s="16"/>
+      <c r="I88" s="16"/>
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
-        <v>242</v>
+        <v>221</v>
       </c>
       <c r="B89" s="26" t="s">
-        <v>144</v>
+        <v>138</v>
       </c>
       <c r="C89" s="27" t="s">
         <v>6</v>
@@ -10194,17 +10195,17 @@
         <v>6</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
-        <v>243</v>
+        <v>222</v>
       </c>
       <c r="B90" s="26" t="s">
-        <v>145</v>
+        <v>139</v>
       </c>
       <c r="C90" s="27" t="s">
         <v>6</v>
@@ -10219,17 +10220,17 @@
         <v>6</v>
       </c>
       <c r="G90" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
-        <v>244</v>
+        <v>223</v>
       </c>
       <c r="B91" s="26" t="s">
-        <v>146</v>
+        <v>140</v>
       </c>
       <c r="C91" s="27" t="s">
         <v>6</v>
@@ -10244,17 +10245,17 @@
         <v>6</v>
       </c>
       <c r="G91" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
-        <v>245</v>
+        <v>224</v>
       </c>
       <c r="B92" s="26" t="s">
-        <v>147</v>
+        <v>141</v>
       </c>
       <c r="C92" s="27" t="s">
         <v>6</v>
@@ -10269,17 +10270,17 @@
         <v>6</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
       <c r="B93" s="26" t="s">
-        <v>148</v>
+        <v>142</v>
       </c>
       <c r="C93" s="27" t="s">
         <v>6</v>
@@ -10294,17 +10295,17 @@
         <v>6</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
-        <v>230</v>
+        <v>211</v>
       </c>
       <c r="B94" s="26" t="s">
-        <v>149</v>
+        <v>143</v>
       </c>
       <c r="C94" s="27" t="s">
         <v>6</v>
@@ -10319,17 +10320,17 @@
         <v>6</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
-        <v>246</v>
+        <v>212</v>
       </c>
       <c r="B95" s="26" t="s">
-        <v>150</v>
+        <v>144</v>
       </c>
       <c r="C95" s="27" t="s">
         <v>6</v>
@@ -10344,17 +10345,17 @@
         <v>6</v>
       </c>
       <c r="G95" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>247</v>
+        <v>226</v>
       </c>
       <c r="B96" s="26" t="s">
-        <v>151</v>
+        <v>145</v>
       </c>
       <c r="C96" s="27" t="s">
         <v>6</v>
@@ -10369,17 +10370,17 @@
         <v>6</v>
       </c>
       <c r="G96" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
-        <v>248</v>
+        <v>227</v>
       </c>
       <c r="B97" s="26" t="s">
-        <v>152</v>
+        <v>146</v>
       </c>
       <c r="C97" s="27" t="s">
         <v>6</v>
@@ -10394,17 +10395,17 @@
         <v>6</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A98" s="31" t="s">
-        <v>249</v>
+      <c r="A98" s="20" t="s">
+        <v>228</v>
       </c>
       <c r="B98" s="26" t="s">
-        <v>153</v>
+        <v>147</v>
       </c>
       <c r="C98" s="27" t="s">
         <v>6</v>
@@ -10419,17 +10420,17 @@
         <v>6</v>
       </c>
       <c r="G98" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H98" s="19"/>
       <c r="I98" s="19"/>
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A99" s="20" t="s">
-        <v>250</v>
+      <c r="A99" s="31" t="s">
+        <v>229</v>
       </c>
       <c r="B99" s="26" t="s">
-        <v>154</v>
+        <v>148</v>
       </c>
       <c r="C99" s="27" t="s">
         <v>6</v>
@@ -10444,72 +10445,74 @@
         <v>6</v>
       </c>
       <c r="G99" s="20" t="s">
-        <v>232</v>
+        <v>214</v>
       </c>
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B100" s="7"/>
-      <c r="C100" s="7"/>
-      <c r="D100" s="8"/>
-      <c r="E100" s="8"/>
-      <c r="F100" s="8"/>
-    </row>
-    <row r="101" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
-      <c r="A101" s="24" t="s">
-        <v>99</v>
-      </c>
-      <c r="B101" s="25"/>
-      <c r="C101" s="25"/>
-      <c r="D101" s="25"/>
-      <c r="E101" s="25"/>
-      <c r="F101" s="25"/>
-      <c r="G101" s="20"/>
-      <c r="H101" s="16"/>
-      <c r="I101" s="16"/>
-    </row>
-    <row r="102" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A102" s="20" t="s">
-        <v>100</v>
-      </c>
-      <c r="B102" s="26" t="s">
-        <v>101</v>
-      </c>
-      <c r="C102" s="27" t="s">
-        <v>6</v>
-      </c>
-      <c r="D102" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="E102" s="27" t="s">
-        <v>216</v>
-      </c>
-      <c r="F102" s="27" t="s">
-        <v>216</v>
-      </c>
+      <c r="A100" s="20" t="s">
+        <v>230</v>
+      </c>
+      <c r="B100" s="26" t="s">
+        <v>149</v>
+      </c>
+      <c r="C100" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D100" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="E100" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="F100" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="G100" s="20" t="s">
+        <v>214</v>
+      </c>
+      <c r="H100" s="19"/>
+      <c r="I100" s="19"/>
+    </row>
+    <row r="101" spans="1:9" ht="15" x14ac:dyDescent="0.2">
+      <c r="B101" s="7"/>
+      <c r="C101" s="7"/>
+      <c r="D101" s="8"/>
+      <c r="E101" s="8"/>
+      <c r="F101" s="8"/>
+    </row>
+    <row r="102" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
+      <c r="A102" s="24" t="s">
+        <v>94</v>
+      </c>
+      <c r="B102" s="25"/>
+      <c r="C102" s="25"/>
+      <c r="D102" s="25"/>
+      <c r="E102" s="25"/>
+      <c r="F102" s="25"/>
       <c r="G102" s="20"/>
-      <c r="H102" s="19"/>
-      <c r="I102" s="19"/>
+      <c r="H102" s="16"/>
+      <c r="I102" s="16"/>
     </row>
     <row r="103" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A103" s="20" t="s">
-        <v>102</v>
+        <v>95</v>
       </c>
       <c r="B103" s="26" t="s">
-        <v>103</v>
+        <v>96</v>
       </c>
       <c r="C103" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F103" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G103" s="20"/>
       <c r="H103" s="19"/>
@@ -10517,22 +10520,22 @@
     </row>
     <row r="104" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A104" s="20" t="s">
-        <v>104</v>
+        <v>97</v>
       </c>
       <c r="B104" s="26" t="s">
-        <v>105</v>
+        <v>98</v>
       </c>
       <c r="C104" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F104" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G104" s="20"/>
       <c r="H104" s="19"/>
@@ -10540,22 +10543,22 @@
     </row>
     <row r="105" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A105" s="20" t="s">
-        <v>106</v>
+        <v>99</v>
       </c>
       <c r="B105" s="26" t="s">
-        <v>107</v>
+        <v>100</v>
       </c>
       <c r="C105" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D105" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F105" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G105" s="20"/>
       <c r="H105" s="19"/>
@@ -10563,22 +10566,22 @@
     </row>
     <row r="106" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A106" s="20" t="s">
-        <v>108</v>
+        <v>101</v>
       </c>
       <c r="B106" s="26" t="s">
-        <v>109</v>
+        <v>102</v>
       </c>
       <c r="C106" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F106" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G106" s="20"/>
       <c r="H106" s="19"/>
@@ -10586,22 +10589,22 @@
     </row>
     <row r="107" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A107" s="20" t="s">
-        <v>110</v>
+        <v>103</v>
       </c>
       <c r="B107" s="26" t="s">
-        <v>111</v>
+        <v>104</v>
       </c>
       <c r="C107" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F107" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G107" s="20"/>
       <c r="H107" s="19"/>
@@ -10609,22 +10612,22 @@
     </row>
     <row r="108" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A108" s="20" t="s">
-        <v>112</v>
+        <v>105</v>
       </c>
       <c r="B108" s="26" t="s">
-        <v>113</v>
+        <v>106</v>
       </c>
       <c r="C108" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D108" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G108" s="20"/>
       <c r="H108" s="19"/>
@@ -10632,22 +10635,22 @@
     </row>
     <row r="109" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A109" s="20" t="s">
-        <v>114</v>
+        <v>107</v>
       </c>
       <c r="B109" s="26" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C109" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F109" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G109" s="20"/>
       <c r="H109" s="19"/>
@@ -10655,22 +10658,22 @@
     </row>
     <row r="110" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A110" s="20" t="s">
-        <v>116</v>
+        <v>109</v>
       </c>
       <c r="B110" s="26" t="s">
-        <v>117</v>
+        <v>110</v>
       </c>
       <c r="C110" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D110" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F110" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="G110" s="20"/>
       <c r="H110" s="19"/>
@@ -10678,22 +10681,22 @@
     </row>
     <row r="111" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A111" s="20" t="s">
-        <v>118</v>
+        <v>111</v>
       </c>
       <c r="B111" s="26" t="s">
-        <v>119</v>
+        <v>112</v>
       </c>
       <c r="C111" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D111" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F111" s="27" t="s">
-        <v>6</v>
+        <v>200</v>
       </c>
       <c r="G111" s="20"/>
       <c r="H111" s="19"/>
@@ -10701,19 +10704,19 @@
     </row>
     <row r="112" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A112" s="20" t="s">
-        <v>120</v>
+        <v>113</v>
       </c>
       <c r="B112" s="26" t="s">
-        <v>121</v>
+        <v>114</v>
       </c>
       <c r="C112" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D112" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F112" s="27" t="s">
         <v>6</v>
@@ -10724,19 +10727,19 @@
     </row>
     <row r="113" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A113" s="20" t="s">
-        <v>122</v>
+        <v>115</v>
       </c>
       <c r="B113" s="26" t="s">
-        <v>123</v>
+        <v>116</v>
       </c>
       <c r="C113" s="27" t="s">
         <v>6</v>
       </c>
       <c r="D113" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="F113" s="27" t="s">
         <v>6</v>
@@ -10746,22 +10749,38 @@
       <c r="I113" s="19"/>
     </row>
     <row r="114" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="A114" s="20"/>
-      <c r="B114" s="26"/>
-      <c r="C114" s="27"/>
-      <c r="D114" s="27"/>
-      <c r="E114" s="27"/>
-      <c r="F114" s="27"/>
+      <c r="A114" s="20" t="s">
+        <v>117</v>
+      </c>
+      <c r="B114" s="26" t="s">
+        <v>118</v>
+      </c>
+      <c r="C114" s="27" t="s">
+        <v>6</v>
+      </c>
+      <c r="D114" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="E114" s="27" t="s">
+        <v>200</v>
+      </c>
+      <c r="F114" s="27" t="s">
+        <v>6</v>
+      </c>
       <c r="G114" s="20"/>
       <c r="H114" s="19"/>
       <c r="I114" s="19"/>
     </row>
     <row r="115" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B115" s="7"/>
-      <c r="C115" s="7"/>
-      <c r="D115" s="8"/>
-      <c r="E115" s="8"/>
-      <c r="F115" s="8"/>
+      <c r="A115" s="20"/>
+      <c r="B115" s="26"/>
+      <c r="C115" s="27"/>
+      <c r="D115" s="27"/>
+      <c r="E115" s="27"/>
+      <c r="F115" s="27"/>
+      <c r="G115" s="20"/>
+      <c r="H115" s="19"/>
+      <c r="I115" s="19"/>
     </row>
     <row r="116" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="B116" s="7"/>
@@ -10792,8 +10811,8 @@
       <c r="F119" s="8"/>
     </row>
     <row r="120" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B120" s="8"/>
-      <c r="C120" s="8"/>
+      <c r="B120" s="7"/>
+      <c r="C120" s="7"/>
       <c r="D120" s="8"/>
       <c r="E120" s="8"/>
       <c r="F120" s="8"/>
@@ -10806,15 +10825,15 @@
       <c r="F121" s="8"/>
     </row>
     <row r="122" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B122" s="7"/>
-      <c r="C122" s="7"/>
+      <c r="B122" s="8"/>
+      <c r="C122" s="8"/>
       <c r="D122" s="8"/>
       <c r="E122" s="8"/>
       <c r="F122" s="8"/>
     </row>
     <row r="123" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B123" s="8"/>
-      <c r="C123" s="8"/>
+      <c r="B123" s="7"/>
+      <c r="C123" s="7"/>
       <c r="D123" s="8"/>
       <c r="E123" s="8"/>
       <c r="F123" s="8"/>
@@ -10827,8 +10846,8 @@
       <c r="F124" s="8"/>
     </row>
     <row r="125" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B125" s="7"/>
-      <c r="C125" s="7"/>
+      <c r="B125" s="8"/>
+      <c r="C125" s="8"/>
       <c r="D125" s="8"/>
       <c r="E125" s="8"/>
       <c r="F125" s="8"/>
@@ -10841,7 +10860,7 @@
       <c r="F126" s="8"/>
     </row>
     <row r="127" spans="1:9" ht="15" x14ac:dyDescent="0.2">
-      <c r="B127" s="8"/>
+      <c r="B127" s="7"/>
       <c r="C127" s="7"/>
       <c r="D127" s="8"/>
       <c r="E127" s="8"/>
@@ -10870,7 +10889,7 @@
     </row>
     <row r="131" spans="2:6" ht="15" x14ac:dyDescent="0.2">
       <c r="B131" s="8"/>
-      <c r="C131" s="8"/>
+      <c r="C131" s="7"/>
       <c r="D131" s="8"/>
       <c r="E131" s="8"/>
       <c r="F131" s="8"/>
@@ -17496,6 +17515,13 @@
       <c r="D1077" s="8"/>
       <c r="E1077" s="8"/>
       <c r="F1077" s="8"/>
+    </row>
+    <row r="1078" spans="2:6" ht="15" x14ac:dyDescent="0.2">
+      <c r="B1078" s="8"/>
+      <c r="C1078" s="8"/>
+      <c r="D1078" s="8"/>
+      <c r="E1078" s="8"/>
+      <c r="F1078" s="8"/>
     </row>
   </sheetData>
   <mergeCells count="6">
@@ -17545,10 +17571,10 @@
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="39" t="s">
-        <v>220</v>
+        <v>204</v>
       </c>
       <c r="F1" s="37" t="s">
-        <v>167</v>
+        <v>162</v>
       </c>
       <c r="G1" s="37"/>
       <c r="H1" s="37" t="s">
@@ -17589,10 +17615,10 @@
       </c>
       <c r="E2" s="39"/>
       <c r="F2" s="13" t="s">
-        <v>179</v>
+        <v>169</v>
       </c>
       <c r="G2" s="14" t="s">
-        <v>177</v>
+        <v>168</v>
       </c>
       <c r="H2" s="37"/>
       <c r="I2" s="1"/>
@@ -17619,7 +17645,7 @@
     </row>
     <row r="3" spans="1:29" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="15" t="s">
-        <v>165</v>
+        <v>160</v>
       </c>
       <c r="B3" s="15"/>
       <c r="C3" s="15"/>
@@ -17652,7 +17678,7 @@
     </row>
     <row r="4" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A4" s="17" t="s">
-        <v>155</v>
+        <v>150</v>
       </c>
       <c r="B4" s="18" t="s">
         <v>6</v>
@@ -17672,7 +17698,7 @@
     </row>
     <row r="5" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A5" s="17" t="s">
-        <v>156</v>
+        <v>151</v>
       </c>
       <c r="B5" s="18" t="s">
         <v>6</v>
@@ -17692,7 +17718,7 @@
     </row>
     <row r="6" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A6" s="17" t="s">
-        <v>157</v>
+        <v>152</v>
       </c>
       <c r="B6" s="18" t="s">
         <v>6</v>
@@ -17712,16 +17738,16 @@
     </row>
     <row r="7" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A7" s="17" t="s">
-        <v>158</v>
+        <v>153</v>
       </c>
       <c r="B7" s="18" t="s">
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>216</v>
+        <v>200</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>6</v>
@@ -17732,7 +17758,7 @@
     </row>
     <row r="8" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A8" s="17" t="s">
-        <v>159</v>
+        <v>154</v>
       </c>
       <c r="B8" s="18" t="s">
         <v>6</v>
@@ -17762,7 +17788,7 @@
     </row>
     <row r="10" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A10" s="16" t="s">
-        <v>166</v>
+        <v>161</v>
       </c>
       <c r="B10" s="23"/>
       <c r="C10" s="23"/>
@@ -17774,7 +17800,7 @@
     </row>
     <row r="11" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A11" s="17" t="s">
-        <v>160</v>
+        <v>155</v>
       </c>
       <c r="B11" s="18"/>
       <c r="C11" s="18"/>
@@ -17788,7 +17814,7 @@
     </row>
     <row r="12" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A12" s="17" t="s">
-        <v>161</v>
+        <v>156</v>
       </c>
       <c r="B12" s="18"/>
       <c r="C12" s="18"/>
@@ -17802,7 +17828,7 @@
     </row>
     <row r="13" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A13" s="17" t="s">
-        <v>162</v>
+        <v>157</v>
       </c>
       <c r="B13" s="18"/>
       <c r="C13" s="18"/>
@@ -17816,7 +17842,7 @@
     </row>
     <row r="14" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A14" s="17" t="s">
-        <v>163</v>
+        <v>158</v>
       </c>
       <c r="B14" s="18"/>
       <c r="C14" s="18"/>
@@ -17830,7 +17856,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>221</v>
+        <v>205</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>

</xml_diff>

<commit_message>
LEonardRoot set as system variable in all 3 engines sysLanguage, sysLeonardRoot, sysSequenceFilename sysSequencePath, sysStartTime
</commit_message>
<xml_diff>
--- a/MasterFiles/Documentation/Complete Statement List.xlsx
+++ b/MasterFiles/Documentation/Complete Statement List.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\nedlecky\GitHub\LEonard\MasterFiles\Documentation\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B85D2788-939E-4B01-AE2C-99B904A2A056}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CD4FA46-8AC3-47D9-9FA2-AE73F274423F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="48015" yWindow="1950" windowWidth="24810" windowHeight="19560" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="51345" yWindow="1200" windowWidth="24810" windowHeight="19560" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Main" sheetId="1" r:id="rId1"/>
@@ -22,7 +22,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="287">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="911" uniqueCount="288">
   <si>
     <t>Statement</t>
   </si>
@@ -603,9 +603,6 @@
     <t>exec_python(string filename)</t>
   </si>
   <si>
-    <t>le_language [this is a system variable]</t>
-  </si>
-  <si>
     <t>exec_java(string filename)</t>
   </si>
   <si>
@@ -888,6 +885,12 @@
   </si>
   <si>
     <t>Testing/import_test_data.txt</t>
+  </si>
+  <si>
+    <t>sysSystemVariables</t>
+  </si>
+  <si>
+    <t>sysvar</t>
   </si>
 </sst>
 </file>
@@ -1330,9 +1333,9 @@
   </sheetPr>
   <dimension ref="A1:AC1009"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
-      <selection pane="bottomLeft" activeCell="G29" sqref="G29"/>
+      <selection pane="bottomLeft" activeCell="F7" sqref="F7"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="12.5703125" defaultRowHeight="15.75" customHeight="1" x14ac:dyDescent="0.2"/>
@@ -1357,7 +1360,7 @@
       <c r="C1" s="38"/>
       <c r="D1" s="38"/>
       <c r="E1" s="39" t="s">
-        <v>202</v>
+        <v>201</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>162</v>
@@ -1467,7 +1470,7 @@
     </row>
     <row r="7" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>192</v>
+        <v>286</v>
       </c>
       <c r="B7" s="27" t="s">
         <v>6</v>
@@ -1482,7 +1485,7 @@
         <v>6</v>
       </c>
       <c r="F7" s="20" t="s">
-        <v>163</v>
+        <v>287</v>
       </c>
       <c r="G7" s="20"/>
       <c r="H7" s="19"/>
@@ -1504,16 +1507,16 @@
         <v>6</v>
       </c>
       <c r="F8" s="28" t="s">
-        <v>201</v>
+        <v>200</v>
       </c>
       <c r="G8" s="29" t="s">
-        <v>199</v>
+        <v>198</v>
       </c>
       <c r="H8" s="28"/>
     </row>
     <row r="9" spans="1:8" ht="30" x14ac:dyDescent="0.2">
       <c r="A9" s="20" t="s">
-        <v>193</v>
+        <v>192</v>
       </c>
       <c r="B9" s="27" t="s">
         <v>6</v>
@@ -1576,14 +1579,14 @@
         <v>6</v>
       </c>
       <c r="F11" s="28" t="s">
-        <v>208</v>
+        <v>207</v>
       </c>
       <c r="G11" s="19"/>
       <c r="H11" s="28"/>
     </row>
     <row r="12" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>194</v>
+        <v>193</v>
       </c>
       <c r="B12" s="27" t="s">
         <v>6</v>
@@ -1598,14 +1601,14 @@
         <v>6</v>
       </c>
       <c r="F12" s="28" t="s">
-        <v>209</v>
+        <v>208</v>
       </c>
       <c r="G12" s="19"/>
       <c r="H12" s="28"/>
     </row>
     <row r="13" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>195</v>
+        <v>194</v>
       </c>
       <c r="B13" s="27" t="s">
         <v>6</v>
@@ -1620,7 +1623,7 @@
         <v>6</v>
       </c>
       <c r="F13" s="28" t="s">
-        <v>210</v>
+        <v>209</v>
       </c>
       <c r="G13" s="19"/>
       <c r="H13" s="28"/>
@@ -1649,7 +1652,7 @@
     </row>
     <row r="16" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A16" s="20" t="s">
-        <v>280</v>
+        <v>279</v>
       </c>
       <c r="B16" s="27" t="s">
         <v>6</v>
@@ -1660,14 +1663,14 @@
         <v>6</v>
       </c>
       <c r="F16" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G16" s="19"/>
       <c r="H16" s="19"/>
     </row>
     <row r="17" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A17" s="20" t="s">
-        <v>281</v>
+        <v>280</v>
       </c>
       <c r="B17" s="27" t="s">
         <v>6</v>
@@ -1678,16 +1681,16 @@
         <v>6</v>
       </c>
       <c r="F17" s="20" t="s">
-        <v>284</v>
+        <v>283</v>
       </c>
       <c r="G17" s="20" t="s">
-        <v>286</v>
+        <v>285</v>
       </c>
       <c r="H17" s="20"/>
     </row>
     <row r="18" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A18" s="20" t="s">
-        <v>282</v>
+        <v>281</v>
       </c>
       <c r="B18" s="27" t="s">
         <v>6</v>
@@ -1698,7 +1701,7 @@
         <v>6</v>
       </c>
       <c r="F18" s="20" t="s">
-        <v>283</v>
+        <v>282</v>
       </c>
       <c r="G18" s="19"/>
       <c r="H18" s="19"/>
@@ -1793,7 +1796,7 @@
     </row>
     <row r="23" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>249</v>
+        <v>248</v>
       </c>
       <c r="B23" s="27" t="s">
         <v>6</v>
@@ -1811,7 +1814,7 @@
     </row>
     <row r="24" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A24" s="20" t="s">
-        <v>196</v>
+        <v>195</v>
       </c>
       <c r="B24" s="27"/>
       <c r="C24" s="27" t="s">
@@ -1831,7 +1834,7 @@
     </row>
     <row r="25" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A25" s="20" t="s">
-        <v>197</v>
+        <v>196</v>
       </c>
       <c r="B25" s="27"/>
       <c r="C25" s="27" t="s">
@@ -1851,7 +1854,7 @@
     </row>
     <row r="26" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>198</v>
+        <v>197</v>
       </c>
       <c r="B26" s="27"/>
       <c r="C26" s="27" t="s">
@@ -1915,7 +1918,7 @@
     </row>
     <row r="30" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A30" s="20" t="s">
-        <v>262</v>
+        <v>261</v>
       </c>
       <c r="B30" s="27" t="s">
         <v>6</v>
@@ -2047,7 +2050,7 @@
     </row>
     <row r="38" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A38" s="20" t="s">
-        <v>253</v>
+        <v>252</v>
       </c>
       <c r="B38" s="27" t="s">
         <v>6</v>
@@ -2062,14 +2065,14 @@
         <v>6</v>
       </c>
       <c r="F38" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G38" s="19"/>
       <c r="H38" s="19"/>
     </row>
     <row r="39" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>258</v>
+        <v>257</v>
       </c>
       <c r="B39" s="27" t="s">
         <v>6</v>
@@ -2084,14 +2087,14 @@
         <v>6</v>
       </c>
       <c r="F39" s="20" t="s">
-        <v>255</v>
+        <v>254</v>
       </c>
       <c r="G39" s="19"/>
       <c r="H39" s="19"/>
     </row>
     <row r="40" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A40" s="20" t="s">
-        <v>254</v>
+        <v>253</v>
       </c>
       <c r="B40" s="27" t="s">
         <v>6</v>
@@ -2106,14 +2109,14 @@
         <v>6</v>
       </c>
       <c r="F40" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G40" s="19"/>
       <c r="H40" s="19"/>
     </row>
     <row r="41" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A41" s="20" t="s">
-        <v>259</v>
+        <v>258</v>
       </c>
       <c r="B41" s="27" t="s">
         <v>6</v>
@@ -2128,14 +2131,14 @@
         <v>6</v>
       </c>
       <c r="F41" s="20" t="s">
-        <v>256</v>
+        <v>255</v>
       </c>
       <c r="G41" s="19"/>
       <c r="H41" s="19"/>
     </row>
     <row r="42" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A42" s="20" t="s">
-        <v>261</v>
+        <v>260</v>
       </c>
       <c r="B42" s="27" t="s">
         <v>6</v>
@@ -2150,14 +2153,14 @@
         <v>6</v>
       </c>
       <c r="F42" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G42" s="19"/>
       <c r="H42" s="19"/>
     </row>
     <row r="43" spans="1:29" ht="15" x14ac:dyDescent="0.2">
       <c r="A43" s="20" t="s">
-        <v>260</v>
+        <v>259</v>
       </c>
       <c r="B43" s="27" t="s">
         <v>6</v>
@@ -2172,7 +2175,7 @@
         <v>6</v>
       </c>
       <c r="F43" s="20" t="s">
-        <v>257</v>
+        <v>256</v>
       </c>
       <c r="G43" s="19"/>
       <c r="H43" s="19"/>
@@ -2350,7 +2353,7 @@
     </row>
     <row r="51" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>263</v>
+        <v>262</v>
       </c>
       <c r="B51" s="27" t="s">
         <v>6</v>
@@ -2372,7 +2375,7 @@
     </row>
     <row r="52" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>264</v>
+        <v>263</v>
       </c>
       <c r="B52" s="27" t="s">
         <v>6</v>
@@ -2390,7 +2393,7 @@
     </row>
     <row r="53" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>265</v>
+        <v>264</v>
       </c>
       <c r="B53" s="27" t="s">
         <v>6</v>
@@ -2408,7 +2411,7 @@
     </row>
     <row r="54" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>206</v>
+        <v>205</v>
       </c>
       <c r="B54" s="27"/>
       <c r="C54" s="27" t="s">
@@ -2428,7 +2431,7 @@
     </row>
     <row r="55" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A55" s="20" t="s">
-        <v>207</v>
+        <v>206</v>
       </c>
       <c r="B55" s="27"/>
       <c r="C55" s="27" t="s">
@@ -2470,7 +2473,7 @@
     </row>
     <row r="58" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A58" s="20" t="s">
-        <v>266</v>
+        <v>265</v>
       </c>
       <c r="B58" s="27" t="s">
         <v>6</v>
@@ -2492,7 +2495,7 @@
     </row>
     <row r="59" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>267</v>
+        <v>266</v>
       </c>
       <c r="B59" s="27" t="s">
         <v>6</v>
@@ -2558,7 +2561,7 @@
     </row>
     <row r="62" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>268</v>
+        <v>267</v>
       </c>
       <c r="B62" s="27" t="s">
         <v>6</v>
@@ -2580,7 +2583,7 @@
     </row>
     <row r="63" spans="1:8" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>269</v>
+        <v>268</v>
       </c>
       <c r="B63" s="27" t="s">
         <v>6</v>
@@ -2678,7 +2681,7 @@
     </row>
     <row r="69" spans="1:8" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>270</v>
+        <v>269</v>
       </c>
       <c r="B69" s="27" t="s">
         <v>6</v>
@@ -2726,7 +2729,7 @@
       <c r="C72" s="27"/>
       <c r="D72" s="27"/>
       <c r="E72" s="32" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F72" s="19"/>
       <c r="G72" s="19"/>
@@ -8374,7 +8377,7 @@
   </sheetPr>
   <dimension ref="A1:AD1078"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <pane ySplit="2" topLeftCell="A3" activePane="bottomLeft" state="frozen"/>
       <selection pane="bottomLeft" activeCell="G70" sqref="G70"/>
     </sheetView>
@@ -8405,7 +8408,7 @@
       <c r="D1" s="37"/>
       <c r="E1" s="37"/>
       <c r="F1" s="39" t="s">
-        <v>203</v>
+        <v>202</v>
       </c>
       <c r="G1" s="37" t="s">
         <v>162</v>
@@ -8480,7 +8483,7 @@
     </row>
     <row r="3" spans="1:30" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A3" s="24" t="s">
-        <v>234</v>
+        <v>233</v>
       </c>
       <c r="B3" s="25"/>
       <c r="C3" s="25"/>
@@ -8493,7 +8496,7 @@
     </row>
     <row r="4" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A4" s="20" t="s">
-        <v>237</v>
+        <v>236</v>
       </c>
       <c r="B4" s="26"/>
       <c r="C4" s="27" t="s">
@@ -8538,7 +8541,7 @@
     </row>
     <row r="7" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A7" s="20" t="s">
-        <v>238</v>
+        <v>237</v>
       </c>
       <c r="B7" s="26" t="s">
         <v>38</v>
@@ -8618,7 +8621,7 @@
     </row>
     <row r="11" spans="1:30" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A11" s="20" t="s">
-        <v>239</v>
+        <v>238</v>
       </c>
       <c r="B11" s="26" t="s">
         <v>43</v>
@@ -8641,7 +8644,7 @@
     </row>
     <row r="12" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A12" s="20" t="s">
-        <v>271</v>
+        <v>270</v>
       </c>
       <c r="B12" s="26" t="s">
         <v>59</v>
@@ -8664,7 +8667,7 @@
     </row>
     <row r="13" spans="1:30" ht="15" x14ac:dyDescent="0.2">
       <c r="A13" s="20" t="s">
-        <v>272</v>
+        <v>271</v>
       </c>
       <c r="B13" s="26" t="s">
         <v>60</v>
@@ -8824,7 +8827,7 @@
     </row>
     <row r="21" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A21" s="20" t="s">
-        <v>251</v>
+        <v>250</v>
       </c>
       <c r="B21" s="26" t="s">
         <v>52</v>
@@ -8847,7 +8850,7 @@
     </row>
     <row r="22" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A22" s="20" t="s">
-        <v>252</v>
+        <v>251</v>
       </c>
       <c r="B22" s="26" t="s">
         <v>55</v>
@@ -8870,7 +8873,7 @@
     </row>
     <row r="23" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A23" s="20" t="s">
-        <v>273</v>
+        <v>272</v>
       </c>
       <c r="B23" s="26" t="s">
         <v>36</v>
@@ -8904,7 +8907,7 @@
     </row>
     <row r="25" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A25" s="24" t="s">
-        <v>235</v>
+        <v>234</v>
       </c>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -8917,7 +8920,7 @@
     </row>
     <row r="26" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A26" s="20" t="s">
-        <v>240</v>
+        <v>239</v>
       </c>
       <c r="B26" s="26" t="s">
         <v>56</v>
@@ -8940,7 +8943,7 @@
     </row>
     <row r="27" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A27" s="20" t="s">
-        <v>241</v>
+        <v>240</v>
       </c>
       <c r="B27" s="26" t="s">
         <v>57</v>
@@ -8963,7 +8966,7 @@
     </row>
     <row r="28" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A28" s="20" t="s">
-        <v>242</v>
+        <v>241</v>
       </c>
       <c r="B28" s="26" t="s">
         <v>58</v>
@@ -8997,7 +9000,7 @@
     </row>
     <row r="30" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A30" s="24" t="s">
-        <v>236</v>
+        <v>235</v>
       </c>
       <c r="B30" s="25"/>
       <c r="C30" s="25"/>
@@ -9010,7 +9013,7 @@
     </row>
     <row r="31" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A31" s="20" t="s">
-        <v>243</v>
+        <v>242</v>
       </c>
       <c r="B31" s="26" t="s">
         <v>61</v>
@@ -9056,7 +9059,7 @@
     </row>
     <row r="33" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A33" s="20" t="s">
-        <v>244</v>
+        <v>243</v>
       </c>
       <c r="B33" s="26" t="s">
         <v>63</v>
@@ -9102,7 +9105,7 @@
     </row>
     <row r="35" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A35" s="20" t="s">
-        <v>245</v>
+        <v>244</v>
       </c>
       <c r="B35" s="26" t="s">
         <v>65</v>
@@ -9125,7 +9128,7 @@
     </row>
     <row r="36" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A36" s="20" t="s">
-        <v>246</v>
+        <v>245</v>
       </c>
       <c r="B36" s="26" t="s">
         <v>66</v>
@@ -9159,7 +9162,7 @@
     </row>
     <row r="38" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A38" s="24" t="s">
-        <v>233</v>
+        <v>232</v>
       </c>
       <c r="B38" s="25"/>
       <c r="C38" s="25"/>
@@ -9172,7 +9175,7 @@
     </row>
     <row r="39" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A39" s="20" t="s">
-        <v>231</v>
+        <v>230</v>
       </c>
       <c r="B39" s="26"/>
       <c r="C39" s="27" t="s">
@@ -9202,10 +9205,10 @@
         <v>6</v>
       </c>
       <c r="D40" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E40" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F40" s="27" t="s">
         <v>6</v>
@@ -9225,10 +9228,10 @@
         <v>6</v>
       </c>
       <c r="D41" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E41" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F41" s="27" t="s">
         <v>6</v>
@@ -9248,10 +9251,10 @@
         <v>6</v>
       </c>
       <c r="D42" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E42" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F42" s="27" t="s">
         <v>6</v>
@@ -9271,10 +9274,10 @@
         <v>6</v>
       </c>
       <c r="D43" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E43" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F43" s="27" t="s">
         <v>6</v>
@@ -9380,7 +9383,7 @@
     </row>
     <row r="49" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A49" s="24" t="s">
-        <v>232</v>
+        <v>231</v>
       </c>
       <c r="B49" s="26"/>
       <c r="C49" s="27"/>
@@ -9393,7 +9396,7 @@
     </row>
     <row r="50" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A50" s="20" t="s">
-        <v>275</v>
+        <v>274</v>
       </c>
       <c r="B50" s="26"/>
       <c r="C50" s="27" t="s">
@@ -9414,7 +9417,7 @@
     </row>
     <row r="51" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A51" s="20" t="s">
-        <v>276</v>
+        <v>275</v>
       </c>
       <c r="B51" s="18"/>
       <c r="C51" s="27" t="s">
@@ -9435,7 +9438,7 @@
     </row>
     <row r="52" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A52" s="20" t="s">
-        <v>279</v>
+        <v>278</v>
       </c>
       <c r="B52" s="18"/>
       <c r="C52" s="27" t="s">
@@ -9456,7 +9459,7 @@
     </row>
     <row r="53" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A53" s="20" t="s">
-        <v>277</v>
+        <v>276</v>
       </c>
       <c r="B53" s="26"/>
       <c r="C53" s="27" t="s">
@@ -9477,7 +9480,7 @@
     </row>
     <row r="54" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A54" s="20" t="s">
-        <v>278</v>
+        <v>277</v>
       </c>
       <c r="B54" s="26"/>
       <c r="C54" s="27" t="s">
@@ -9551,7 +9554,7 @@
     </row>
     <row r="58" spans="1:9" ht="16.5" x14ac:dyDescent="0.25">
       <c r="A58" s="24" t="s">
-        <v>250</v>
+        <v>249</v>
       </c>
       <c r="B58" s="25"/>
       <c r="C58" s="25"/>
@@ -9564,7 +9567,7 @@
     </row>
     <row r="59" spans="1:9" ht="15.75" customHeight="1" x14ac:dyDescent="0.2">
       <c r="A59" s="20" t="s">
-        <v>274</v>
+        <v>273</v>
       </c>
       <c r="B59" s="26"/>
       <c r="C59" s="27" t="s">
@@ -9585,7 +9588,7 @@
     </row>
     <row r="60" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A60" s="20" t="s">
-        <v>248</v>
+        <v>247</v>
       </c>
       <c r="B60" s="26" t="s">
         <v>72</v>
@@ -9600,17 +9603,17 @@
         <v>6</v>
       </c>
       <c r="F60" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G60" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H60" s="21"/>
       <c r="I60" s="19"/>
     </row>
     <row r="61" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A61" s="20" t="s">
-        <v>217</v>
+        <v>216</v>
       </c>
       <c r="B61" s="26" t="s">
         <v>67</v>
@@ -9628,16 +9631,16 @@
         <v>6</v>
       </c>
       <c r="G61" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H61" s="19"/>
       <c r="I61" s="19" t="s">
-        <v>216</v>
+        <v>215</v>
       </c>
     </row>
     <row r="62" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A62" s="20" t="s">
-        <v>218</v>
+        <v>217</v>
       </c>
       <c r="B62" s="26" t="s">
         <v>68</v>
@@ -9655,14 +9658,14 @@
         <v>6</v>
       </c>
       <c r="G62" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H62" s="19"/>
       <c r="I62" s="19"/>
     </row>
     <row r="63" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A63" s="20" t="s">
-        <v>247</v>
+        <v>246</v>
       </c>
       <c r="B63" s="26" t="s">
         <v>69</v>
@@ -9680,14 +9683,14 @@
         <v>6</v>
       </c>
       <c r="G63" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H63" s="19"/>
       <c r="I63" s="19"/>
     </row>
     <row r="64" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A64" s="20" t="s">
-        <v>219</v>
+        <v>218</v>
       </c>
       <c r="B64" s="26" t="s">
         <v>70</v>
@@ -9705,14 +9708,14 @@
         <v>6</v>
       </c>
       <c r="G64" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H64" s="19"/>
       <c r="I64" s="19"/>
     </row>
     <row r="65" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A65" s="20" t="s">
-        <v>220</v>
+        <v>219</v>
       </c>
       <c r="B65" s="26" t="s">
         <v>71</v>
@@ -9730,7 +9733,7 @@
         <v>6</v>
       </c>
       <c r="G65" s="20" t="s">
-        <v>213</v>
+        <v>212</v>
       </c>
       <c r="H65" s="19"/>
       <c r="I65" s="19"/>
@@ -9784,7 +9787,7 @@
     </row>
     <row r="69" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A69" s="20" t="s">
-        <v>285</v>
+        <v>284</v>
       </c>
       <c r="B69" s="26" t="s">
         <v>76</v>
@@ -9793,10 +9796,10 @@
         <v>6</v>
       </c>
       <c r="D69" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E69" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F69" s="27" t="s">
         <v>6</v>
@@ -9816,10 +9819,10 @@
         <v>6</v>
       </c>
       <c r="D70" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E70" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F70" s="27" t="s">
         <v>6</v>
@@ -9947,7 +9950,7 @@
     </row>
     <row r="78" spans="1:9" ht="30" x14ac:dyDescent="0.2">
       <c r="A78" s="31" t="s">
-        <v>215</v>
+        <v>214</v>
       </c>
       <c r="B78" s="26" t="s">
         <v>137</v>
@@ -10177,7 +10180,7 @@
     </row>
     <row r="89" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A89" s="20" t="s">
-        <v>221</v>
+        <v>220</v>
       </c>
       <c r="B89" s="26" t="s">
         <v>138</v>
@@ -10195,14 +10198,14 @@
         <v>6</v>
       </c>
       <c r="G89" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H89" s="19"/>
       <c r="I89" s="19"/>
     </row>
     <row r="90" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A90" s="20" t="s">
-        <v>222</v>
+        <v>221</v>
       </c>
       <c r="B90" s="26" t="s">
         <v>139</v>
@@ -10220,14 +10223,14 @@
         <v>6</v>
       </c>
       <c r="G90" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H90" s="19"/>
       <c r="I90" s="19"/>
     </row>
     <row r="91" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A91" s="20" t="s">
-        <v>223</v>
+        <v>222</v>
       </c>
       <c r="B91" s="26" t="s">
         <v>140</v>
@@ -10245,14 +10248,14 @@
         <v>6</v>
       </c>
       <c r="G91" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H91" s="19"/>
       <c r="I91" s="19"/>
     </row>
     <row r="92" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A92" s="20" t="s">
-        <v>224</v>
+        <v>223</v>
       </c>
       <c r="B92" s="26" t="s">
         <v>141</v>
@@ -10270,14 +10273,14 @@
         <v>6</v>
       </c>
       <c r="G92" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H92" s="19"/>
       <c r="I92" s="19"/>
     </row>
     <row r="93" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A93" s="20" t="s">
-        <v>225</v>
+        <v>224</v>
       </c>
       <c r="B93" s="26" t="s">
         <v>142</v>
@@ -10295,14 +10298,14 @@
         <v>6</v>
       </c>
       <c r="G93" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H93" s="19"/>
       <c r="I93" s="19"/>
     </row>
     <row r="94" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A94" s="20" t="s">
-        <v>211</v>
+        <v>210</v>
       </c>
       <c r="B94" s="26" t="s">
         <v>143</v>
@@ -10320,14 +10323,14 @@
         <v>6</v>
       </c>
       <c r="G94" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H94" s="19"/>
       <c r="I94" s="19"/>
     </row>
     <row r="95" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A95" s="20" t="s">
-        <v>212</v>
+        <v>211</v>
       </c>
       <c r="B95" s="26" t="s">
         <v>144</v>
@@ -10345,14 +10348,14 @@
         <v>6</v>
       </c>
       <c r="G95" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H95" s="19"/>
       <c r="I95" s="19"/>
     </row>
     <row r="96" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A96" s="20" t="s">
-        <v>226</v>
+        <v>225</v>
       </c>
       <c r="B96" s="26" t="s">
         <v>145</v>
@@ -10370,14 +10373,14 @@
         <v>6</v>
       </c>
       <c r="G96" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H96" s="19"/>
       <c r="I96" s="19"/>
     </row>
     <row r="97" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A97" s="20" t="s">
-        <v>227</v>
+        <v>226</v>
       </c>
       <c r="B97" s="26" t="s">
         <v>146</v>
@@ -10395,14 +10398,14 @@
         <v>6</v>
       </c>
       <c r="G97" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H97" s="19"/>
       <c r="I97" s="19"/>
     </row>
     <row r="98" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A98" s="20" t="s">
-        <v>228</v>
+        <v>227</v>
       </c>
       <c r="B98" s="26" t="s">
         <v>147</v>
@@ -10420,14 +10423,14 @@
         <v>6</v>
       </c>
       <c r="G98" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H98" s="19"/>
       <c r="I98" s="19"/>
     </row>
     <row r="99" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A99" s="31" t="s">
-        <v>229</v>
+        <v>228</v>
       </c>
       <c r="B99" s="26" t="s">
         <v>148</v>
@@ -10445,14 +10448,14 @@
         <v>6</v>
       </c>
       <c r="G99" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H99" s="19"/>
       <c r="I99" s="19"/>
     </row>
     <row r="100" spans="1:9" ht="15" x14ac:dyDescent="0.2">
       <c r="A100" s="20" t="s">
-        <v>230</v>
+        <v>229</v>
       </c>
       <c r="B100" s="26" t="s">
         <v>149</v>
@@ -10470,7 +10473,7 @@
         <v>6</v>
       </c>
       <c r="G100" s="20" t="s">
-        <v>214</v>
+        <v>213</v>
       </c>
       <c r="H100" s="19"/>
       <c r="I100" s="19"/>
@@ -10506,13 +10509,13 @@
         <v>6</v>
       </c>
       <c r="D103" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E103" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F103" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G103" s="20"/>
       <c r="H103" s="19"/>
@@ -10529,13 +10532,13 @@
         <v>6</v>
       </c>
       <c r="D104" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E104" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F104" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G104" s="20"/>
       <c r="H104" s="19"/>
@@ -10552,13 +10555,13 @@
         <v>6</v>
       </c>
       <c r="D105" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E105" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F105" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G105" s="20"/>
       <c r="H105" s="19"/>
@@ -10575,13 +10578,13 @@
         <v>6</v>
       </c>
       <c r="D106" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E106" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F106" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G106" s="20"/>
       <c r="H106" s="19"/>
@@ -10598,13 +10601,13 @@
         <v>6</v>
       </c>
       <c r="D107" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E107" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F107" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G107" s="20"/>
       <c r="H107" s="19"/>
@@ -10621,13 +10624,13 @@
         <v>6</v>
       </c>
       <c r="D108" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E108" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F108" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G108" s="20"/>
       <c r="H108" s="19"/>
@@ -10644,13 +10647,13 @@
         <v>6</v>
       </c>
       <c r="D109" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E109" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F109" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G109" s="20"/>
       <c r="H109" s="19"/>
@@ -10667,13 +10670,13 @@
         <v>6</v>
       </c>
       <c r="D110" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E110" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F110" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G110" s="20"/>
       <c r="H110" s="19"/>
@@ -10690,13 +10693,13 @@
         <v>6</v>
       </c>
       <c r="D111" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E111" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F111" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="G111" s="20"/>
       <c r="H111" s="19"/>
@@ -10713,10 +10716,10 @@
         <v>6</v>
       </c>
       <c r="D112" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E112" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F112" s="27" t="s">
         <v>6</v>
@@ -10736,10 +10739,10 @@
         <v>6</v>
       </c>
       <c r="D113" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E113" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F113" s="27" t="s">
         <v>6</v>
@@ -10759,10 +10762,10 @@
         <v>6</v>
       </c>
       <c r="D114" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E114" s="27" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="F114" s="27" t="s">
         <v>6</v>
@@ -17571,7 +17574,7 @@
       <c r="C1" s="37"/>
       <c r="D1" s="37"/>
       <c r="E1" s="39" t="s">
-        <v>204</v>
+        <v>203</v>
       </c>
       <c r="F1" s="37" t="s">
         <v>162</v>
@@ -17744,10 +17747,10 @@
         <v>6</v>
       </c>
       <c r="C7" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="D7" s="18" t="s">
-        <v>200</v>
+        <v>199</v>
       </c>
       <c r="E7" s="36" t="s">
         <v>6</v>
@@ -17856,7 +17859,7 @@
     </row>
     <row r="15" spans="1:29" ht="15.75" customHeight="1" x14ac:dyDescent="0.25">
       <c r="A15" s="17" t="s">
-        <v>205</v>
+        <v>204</v>
       </c>
       <c r="B15" s="18"/>
       <c r="C15" s="18"/>

</xml_diff>